<commit_message>
Working for SecurityHeadersFilter 2
</commit_message>
<xml_diff>
--- a/conf/messages.xlsx
+++ b/conf/messages.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1204" uniqueCount="1150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1213" uniqueCount="1159">
   <si>
     <t>key</t>
   </si>
@@ -3810,6 +3810,42 @@
   </si>
   <si>
     <t>Version</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>cut</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Cut</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>カット</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>コピー</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Copy</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>copy</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ペースト</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Paste</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>paste</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -4284,10 +4320,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G458"/>
+  <dimension ref="A1:G461"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A436" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B444" sqref="B444"/>
+    <sheetView tabSelected="1" topLeftCell="A358" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="M380" sqref="M380"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -6689,65 +6725,65 @@
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A269" s="1" t="s">
-        <v>469</v>
+        <v>1155</v>
       </c>
       <c r="B269" s="1" t="s">
-        <v>470</v>
+        <v>1154</v>
       </c>
       <c r="D269" s="1" t="s">
-        <v>471</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A270" s="1" t="s">
-        <v>780</v>
+        <v>469</v>
       </c>
       <c r="B270" s="1" t="s">
-        <v>781</v>
+        <v>470</v>
       </c>
       <c r="D270" s="1" t="s">
-        <v>782</v>
+        <v>471</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A271" s="1" t="s">
-        <v>580</v>
+        <v>780</v>
       </c>
       <c r="B271" s="1" t="s">
-        <v>581</v>
+        <v>781</v>
       </c>
       <c r="D271" s="1" t="s">
-        <v>582</v>
+        <v>782</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A272" s="1" t="s">
-        <v>538</v>
+        <v>1150</v>
       </c>
       <c r="B272" s="1" t="s">
-        <v>539</v>
+        <v>1151</v>
       </c>
       <c r="D272" s="1" t="s">
-        <v>540</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A273" s="1" t="s">
-        <v>535</v>
+        <v>580</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>536</v>
+        <v>581</v>
       </c>
       <c r="D273" s="1" t="s">
-        <v>537</v>
+        <v>582</v>
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A274" s="1" t="s">
-        <v>1020</v>
+        <v>538</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>1021</v>
+        <v>539</v>
       </c>
       <c r="D274" s="1" t="s">
         <v>540</v>
@@ -6755,2007 +6791,2040 @@
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A275" s="1" t="s">
-        <v>1</v>
+        <v>535</v>
       </c>
       <c r="B275" s="1" t="s">
-        <v>5</v>
+        <v>536</v>
       </c>
       <c r="D275" s="1" t="s">
-        <v>222</v>
+        <v>537</v>
       </c>
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A276" s="1" t="s">
-        <v>478</v>
+        <v>1020</v>
       </c>
       <c r="B276" s="1" t="s">
-        <v>479</v>
+        <v>1021</v>
       </c>
       <c r="D276" s="1" t="s">
-        <v>480</v>
+        <v>540</v>
       </c>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A277" s="1" t="s">
-        <v>669</v>
+        <v>1</v>
       </c>
       <c r="B277" s="1" t="s">
-        <v>670</v>
+        <v>5</v>
       </c>
       <c r="D277" s="1" t="s">
-        <v>671</v>
+        <v>222</v>
       </c>
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A278" s="1" t="s">
-        <v>508</v>
+        <v>478</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>509</v>
+        <v>479</v>
       </c>
       <c r="D278" s="1" t="s">
-        <v>510</v>
+        <v>480</v>
       </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A279" s="1" t="s">
-        <v>852</v>
+        <v>669</v>
       </c>
       <c r="B279" s="1" t="s">
-        <v>853</v>
+        <v>670</v>
       </c>
       <c r="D279" s="1" t="s">
-        <v>854</v>
+        <v>671</v>
       </c>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A280" s="1" t="s">
-        <v>645</v>
+        <v>508</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>646</v>
+        <v>509</v>
       </c>
       <c r="D280" s="1" t="s">
-        <v>647</v>
+        <v>510</v>
       </c>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A281" s="1" t="s">
-        <v>790</v>
+        <v>852</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>791</v>
+        <v>853</v>
       </c>
       <c r="D281" s="1" t="s">
-        <v>792</v>
+        <v>854</v>
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A282" s="1" t="s">
-        <v>681</v>
+        <v>645</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>682</v>
+        <v>646</v>
       </c>
       <c r="D282" s="1" t="s">
-        <v>683</v>
+        <v>647</v>
       </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A283" s="1" t="s">
-        <v>425</v>
+        <v>790</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>426</v>
+        <v>791</v>
       </c>
       <c r="D283" s="1" t="s">
-        <v>427</v>
+        <v>792</v>
       </c>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A284" s="1" t="s">
-        <v>948</v>
+        <v>681</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>949</v>
+        <v>682</v>
       </c>
       <c r="D284" s="1" t="s">
-        <v>950</v>
+        <v>683</v>
       </c>
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A285" s="1" t="s">
-        <v>571</v>
+        <v>425</v>
       </c>
       <c r="B285" s="1" t="s">
-        <v>572</v>
+        <v>426</v>
       </c>
       <c r="D285" s="1" t="s">
-        <v>573</v>
+        <v>427</v>
       </c>
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A286" s="1" t="s">
-        <v>520</v>
+        <v>948</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>521</v>
+        <v>949</v>
       </c>
       <c r="D286" s="1" t="s">
-        <v>522</v>
+        <v>950</v>
       </c>
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A287" s="1" t="s">
-        <v>523</v>
+        <v>571</v>
       </c>
       <c r="B287" s="1" t="s">
-        <v>524</v>
+        <v>572</v>
       </c>
       <c r="D287" s="1" t="s">
-        <v>525</v>
+        <v>573</v>
       </c>
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A288" s="1" t="s">
-        <v>1037</v>
+        <v>520</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>1038</v>
+        <v>521</v>
       </c>
       <c r="D288" s="1" t="s">
-        <v>1039</v>
+        <v>522</v>
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A289" s="1" t="s">
-        <v>493</v>
+        <v>523</v>
       </c>
       <c r="B289" s="1" t="s">
-        <v>494</v>
+        <v>524</v>
       </c>
       <c r="D289" s="1" t="s">
-        <v>495</v>
+        <v>525</v>
       </c>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A290" s="1" t="s">
-        <v>774</v>
+        <v>1037</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>24</v>
+        <v>1038</v>
       </c>
       <c r="D290" s="1" t="s">
-        <v>775</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A291" s="1" t="s">
-        <v>463</v>
+        <v>493</v>
       </c>
       <c r="B291" s="1" t="s">
-        <v>464</v>
+        <v>494</v>
       </c>
       <c r="D291" s="1" t="s">
-        <v>465</v>
+        <v>495</v>
       </c>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A292" s="1" t="s">
-        <v>610</v>
+        <v>774</v>
       </c>
       <c r="B292" s="1" t="s">
-        <v>611</v>
+        <v>24</v>
       </c>
       <c r="D292" s="1" t="s">
-        <v>612</v>
+        <v>775</v>
       </c>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A293" s="1" t="s">
-        <v>795</v>
+        <v>463</v>
       </c>
       <c r="B293" s="1" t="s">
-        <v>796</v>
+        <v>464</v>
       </c>
       <c r="D293" s="1" t="s">
-        <v>797</v>
+        <v>465</v>
       </c>
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A294" s="1" t="s">
-        <v>583</v>
+        <v>610</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>584</v>
+        <v>611</v>
       </c>
       <c r="D294" s="1" t="s">
-        <v>585</v>
+        <v>612</v>
       </c>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A295" s="1" t="s">
-        <v>1013</v>
+        <v>795</v>
       </c>
       <c r="B295" s="1" t="s">
-        <v>1014</v>
+        <v>796</v>
       </c>
       <c r="D295" s="1" t="s">
-        <v>1015</v>
+        <v>797</v>
       </c>
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A296" s="1" t="s">
-        <v>804</v>
+        <v>583</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>805</v>
+        <v>584</v>
       </c>
       <c r="D296" s="1" t="s">
-        <v>806</v>
+        <v>585</v>
       </c>
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A297" s="1" t="s">
-        <v>457</v>
+        <v>1013</v>
       </c>
       <c r="B297" s="1" t="s">
-        <v>458</v>
+        <v>1014</v>
       </c>
       <c r="D297" s="1" t="s">
-        <v>459</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A298" s="1" t="s">
-        <v>840</v>
+        <v>804</v>
       </c>
       <c r="B298" s="1" t="s">
-        <v>841</v>
+        <v>805</v>
       </c>
       <c r="D298" s="1" t="s">
-        <v>842</v>
+        <v>806</v>
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A299" s="1" t="s">
-        <v>1043</v>
+        <v>457</v>
       </c>
       <c r="B299" s="1" t="s">
-        <v>1044</v>
+        <v>458</v>
       </c>
       <c r="D299" s="1" t="s">
-        <v>1045</v>
+        <v>459</v>
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A300" s="1" t="s">
-        <v>716</v>
+        <v>840</v>
       </c>
       <c r="B300" s="1" t="s">
-        <v>717</v>
+        <v>841</v>
       </c>
       <c r="D300" s="1" t="s">
-        <v>718</v>
+        <v>842</v>
       </c>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A301" s="1" t="s">
-        <v>719</v>
+        <v>1043</v>
       </c>
       <c r="B301" s="1" t="s">
-        <v>720</v>
+        <v>1044</v>
       </c>
       <c r="D301" s="1" t="s">
-        <v>721</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A302" s="1" t="s">
-        <v>616</v>
+        <v>716</v>
       </c>
       <c r="B302" s="1" t="s">
-        <v>617</v>
+        <v>717</v>
       </c>
       <c r="D302" s="1" t="s">
-        <v>618</v>
+        <v>718</v>
       </c>
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A303" s="1" t="s">
-        <v>586</v>
+        <v>719</v>
       </c>
       <c r="B303" s="1" t="s">
-        <v>587</v>
+        <v>720</v>
       </c>
       <c r="D303" s="1" t="s">
-        <v>588</v>
+        <v>721</v>
       </c>
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A304" s="1" t="s">
-        <v>613</v>
+        <v>616</v>
       </c>
       <c r="B304" s="1" t="s">
-        <v>614</v>
+        <v>617</v>
       </c>
       <c r="D304" s="1" t="s">
-        <v>615</v>
+        <v>618</v>
       </c>
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A305" s="1" t="s">
-        <v>757</v>
+        <v>586</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>758</v>
+        <v>587</v>
       </c>
       <c r="D305" s="1" t="s">
-        <v>759</v>
+        <v>588</v>
       </c>
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A306" s="1" t="s">
-        <v>895</v>
+        <v>613</v>
       </c>
       <c r="B306" s="1" t="s">
-        <v>896</v>
+        <v>614</v>
+      </c>
+      <c r="D306" s="1" t="s">
+        <v>615</v>
       </c>
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A307" s="1" t="s">
-        <v>702</v>
+        <v>757</v>
       </c>
       <c r="B307" s="1" t="s">
-        <v>703</v>
+        <v>758</v>
       </c>
       <c r="D307" s="1" t="s">
-        <v>704</v>
+        <v>759</v>
       </c>
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A308" s="1" t="s">
-        <v>684</v>
+        <v>895</v>
       </c>
       <c r="B308" s="1" t="s">
-        <v>685</v>
-      </c>
-      <c r="D308" s="1" t="s">
-        <v>686</v>
+        <v>896</v>
       </c>
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A309" s="1" t="s">
-        <v>793</v>
+        <v>702</v>
       </c>
       <c r="B309" s="1" t="s">
-        <v>794</v>
+        <v>703</v>
       </c>
       <c r="D309" s="1" t="s">
-        <v>963</v>
+        <v>704</v>
       </c>
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A310" s="1" t="s">
-        <v>776</v>
+        <v>684</v>
       </c>
       <c r="B310" s="1" t="s">
-        <v>777</v>
+        <v>685</v>
       </c>
       <c r="D310" s="1" t="s">
-        <v>433</v>
+        <v>686</v>
       </c>
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A311" s="1" t="s">
-        <v>834</v>
+        <v>793</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>835</v>
+        <v>794</v>
       </c>
       <c r="D311" s="1" t="s">
-        <v>836</v>
+        <v>963</v>
       </c>
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A312" s="1" t="s">
-        <v>639</v>
+        <v>776</v>
       </c>
       <c r="B312" s="1" t="s">
-        <v>640</v>
+        <v>777</v>
       </c>
       <c r="D312" s="1" t="s">
-        <v>641</v>
+        <v>433</v>
       </c>
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A313" s="1" t="s">
-        <v>553</v>
+        <v>834</v>
       </c>
       <c r="B313" s="1" t="s">
-        <v>554</v>
+        <v>835</v>
       </c>
       <c r="D313" s="1" t="s">
-        <v>555</v>
+        <v>836</v>
       </c>
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A314" s="1" t="s">
-        <v>960</v>
+        <v>639</v>
       </c>
       <c r="B314" s="1" t="s">
-        <v>961</v>
+        <v>640</v>
       </c>
       <c r="D314" s="1" t="s">
-        <v>962</v>
+        <v>641</v>
       </c>
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A315" s="1" t="s">
-        <v>1032</v>
+        <v>553</v>
       </c>
       <c r="B315" s="1" t="s">
-        <v>1031</v>
+        <v>554</v>
       </c>
       <c r="D315" s="1" t="s">
-        <v>1033</v>
+        <v>555</v>
       </c>
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A316" s="1" t="s">
-        <v>696</v>
+        <v>960</v>
       </c>
       <c r="B316" s="1" t="s">
-        <v>697</v>
+        <v>961</v>
       </c>
       <c r="D316" s="1" t="s">
-        <v>698</v>
+        <v>962</v>
       </c>
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A317" s="1" t="s">
-        <v>678</v>
+        <v>1032</v>
       </c>
       <c r="B317" s="1" t="s">
-        <v>679</v>
+        <v>1031</v>
       </c>
       <c r="D317" s="1" t="s">
-        <v>680</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A318" s="1" t="s">
-        <v>876</v>
+        <v>696</v>
       </c>
       <c r="B318" s="1" t="s">
-        <v>877</v>
+        <v>697</v>
       </c>
       <c r="D318" s="1" t="s">
-        <v>878</v>
+        <v>698</v>
       </c>
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A319" s="1" t="s">
-        <v>959</v>
+        <v>678</v>
       </c>
       <c r="B319" s="1" t="s">
-        <v>958</v>
+        <v>679</v>
       </c>
       <c r="D319" s="1" t="s">
-        <v>760</v>
+        <v>680</v>
       </c>
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A320" s="1" t="s">
-        <v>1010</v>
+        <v>876</v>
       </c>
       <c r="B320" s="1" t="s">
-        <v>1011</v>
+        <v>877</v>
       </c>
       <c r="D320" s="1" t="s">
-        <v>955</v>
+        <v>878</v>
       </c>
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A321" s="1" t="s">
-        <v>887</v>
+        <v>959</v>
       </c>
       <c r="B321" s="1" t="s">
-        <v>888</v>
+        <v>958</v>
+      </c>
+      <c r="D321" s="1" t="s">
+        <v>760</v>
       </c>
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A322" s="1" t="s">
-        <v>858</v>
+        <v>1010</v>
       </c>
       <c r="B322" s="1" t="s">
-        <v>859</v>
+        <v>1011</v>
       </c>
       <c r="D322" s="1" t="s">
-        <v>860</v>
+        <v>955</v>
       </c>
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A323" s="1" t="s">
-        <v>885</v>
+        <v>887</v>
       </c>
       <c r="B323" s="1" t="s">
-        <v>886</v>
+        <v>888</v>
       </c>
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A324" s="1" t="s">
-        <v>754</v>
+        <v>858</v>
       </c>
       <c r="B324" s="1" t="s">
-        <v>755</v>
+        <v>859</v>
       </c>
       <c r="D324" s="1" t="s">
-        <v>756</v>
+        <v>860</v>
       </c>
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A325" s="1" t="s">
-        <v>574</v>
+        <v>885</v>
       </c>
       <c r="B325" s="1" t="s">
-        <v>575</v>
-      </c>
-      <c r="D325" s="1" t="s">
-        <v>576</v>
+        <v>886</v>
       </c>
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A326" s="1" t="s">
-        <v>778</v>
+        <v>754</v>
       </c>
       <c r="B326" s="1" t="s">
-        <v>779</v>
+        <v>755</v>
       </c>
       <c r="D326" s="1" t="s">
-        <v>576</v>
+        <v>756</v>
       </c>
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A327" s="1" t="s">
-        <v>511</v>
+        <v>574</v>
       </c>
       <c r="B327" s="1" t="s">
-        <v>512</v>
+        <v>575</v>
       </c>
       <c r="D327" s="1" t="s">
-        <v>513</v>
+        <v>576</v>
       </c>
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A328" s="1" t="s">
-        <v>986</v>
+        <v>778</v>
       </c>
       <c r="B328" s="1" t="s">
-        <v>917</v>
+        <v>779</v>
       </c>
       <c r="D328" s="1" t="s">
-        <v>980</v>
+        <v>576</v>
       </c>
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A329" s="1" t="s">
-        <v>985</v>
+        <v>511</v>
       </c>
       <c r="B329" s="1" t="s">
-        <v>918</v>
+        <v>512</v>
       </c>
       <c r="D329" s="1" t="s">
-        <v>979</v>
+        <v>513</v>
       </c>
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A330" s="1" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="B330" s="1" t="s">
-        <v>915</v>
+        <v>917</v>
       </c>
       <c r="D330" s="1" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A331" s="1" t="s">
-        <v>988</v>
+        <v>985</v>
       </c>
       <c r="B331" s="1" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="D331" s="1" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
     </row>
     <row r="332" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A332" s="1" t="s">
-        <v>761</v>
+        <v>987</v>
       </c>
       <c r="B332" s="1" t="s">
-        <v>762</v>
+        <v>915</v>
       </c>
       <c r="D332" s="1" t="s">
-        <v>763</v>
+        <v>982</v>
       </c>
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A333" s="1" t="s">
-        <v>889</v>
+        <v>988</v>
       </c>
       <c r="B333" s="1" t="s">
-        <v>890</v>
+        <v>916</v>
+      </c>
+      <c r="D333" s="1" t="s">
+        <v>981</v>
       </c>
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A334" s="1" t="s">
-        <v>891</v>
+        <v>761</v>
       </c>
       <c r="B334" s="1" t="s">
-        <v>892</v>
+        <v>762</v>
+      </c>
+      <c r="D334" s="1" t="s">
+        <v>763</v>
       </c>
     </row>
     <row r="335" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A335" s="1" t="s">
-        <v>969</v>
+        <v>889</v>
       </c>
       <c r="B335" s="1" t="s">
-        <v>926</v>
-      </c>
-      <c r="D335" s="1" t="s">
-        <v>912</v>
+        <v>890</v>
       </c>
     </row>
     <row r="336" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A336" s="1" t="s">
-        <v>0</v>
+        <v>891</v>
       </c>
       <c r="B336" s="1" t="s">
-        <v>711</v>
-      </c>
-      <c r="D336" s="1" t="s">
-        <v>712</v>
+        <v>892</v>
       </c>
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A337" s="1" t="s">
-        <v>812</v>
+        <v>969</v>
       </c>
       <c r="B337" s="1" t="s">
-        <v>813</v>
+        <v>926</v>
       </c>
       <c r="D337" s="1" t="s">
-        <v>901</v>
+        <v>912</v>
       </c>
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A338" s="1" t="s">
-        <v>589</v>
+        <v>0</v>
       </c>
       <c r="B338" s="1" t="s">
-        <v>590</v>
+        <v>711</v>
       </c>
       <c r="D338" s="1" t="s">
-        <v>591</v>
+        <v>712</v>
       </c>
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A339" s="1" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="B339" s="1" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="D339" s="1" t="s">
-        <v>528</v>
+        <v>901</v>
       </c>
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A340" s="1" t="s">
-        <v>944</v>
+        <v>589</v>
       </c>
       <c r="B340" s="1" t="s">
-        <v>942</v>
+        <v>590</v>
       </c>
       <c r="D340" s="1" t="s">
-        <v>943</v>
+        <v>591</v>
       </c>
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A341" s="1" t="s">
-        <v>807</v>
+        <v>814</v>
       </c>
       <c r="B341" s="1" t="s">
-        <v>808</v>
+        <v>815</v>
       </c>
       <c r="D341" s="1" t="s">
-        <v>809</v>
+        <v>528</v>
       </c>
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A342" s="1" t="s">
-        <v>1072</v>
+        <v>944</v>
       </c>
       <c r="B342" s="1" t="s">
-        <v>1073</v>
+        <v>942</v>
       </c>
       <c r="D342" s="1" t="s">
-        <v>786</v>
+        <v>943</v>
       </c>
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A343" s="1" t="s">
-        <v>870</v>
+        <v>807</v>
       </c>
       <c r="B343" s="1" t="s">
-        <v>871</v>
+        <v>808</v>
       </c>
       <c r="D343" s="1" t="s">
-        <v>872</v>
+        <v>809</v>
       </c>
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A344" s="1" t="s">
-        <v>642</v>
+        <v>1072</v>
       </c>
       <c r="B344" s="1" t="s">
-        <v>643</v>
+        <v>1073</v>
       </c>
       <c r="D344" s="1" t="s">
-        <v>644</v>
+        <v>786</v>
       </c>
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A345" s="1" t="s">
-        <v>529</v>
+        <v>870</v>
       </c>
       <c r="B345" s="1" t="s">
-        <v>530</v>
+        <v>871</v>
       </c>
       <c r="D345" s="1" t="s">
-        <v>531</v>
+        <v>872</v>
       </c>
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A346" s="1" t="s">
-        <v>437</v>
+        <v>642</v>
       </c>
       <c r="B346" s="1" t="s">
-        <v>438</v>
+        <v>643</v>
       </c>
       <c r="D346" s="1" t="s">
-        <v>439</v>
+        <v>644</v>
       </c>
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A347" s="1" t="s">
-        <v>440</v>
+        <v>529</v>
       </c>
       <c r="B347" s="1" t="s">
-        <v>441</v>
+        <v>530</v>
       </c>
       <c r="D347" s="1" t="s">
-        <v>442</v>
+        <v>531</v>
       </c>
     </row>
     <row r="348" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A348" s="1" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
       <c r="B348" s="1" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="D348" s="1" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A349" s="1" t="s">
-        <v>810</v>
+        <v>440</v>
       </c>
       <c r="B349" s="1" t="s">
-        <v>811</v>
+        <v>441</v>
       </c>
       <c r="D349" s="1" t="s">
-        <v>995</v>
+        <v>442</v>
       </c>
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A350" s="1" t="s">
-        <v>648</v>
+        <v>443</v>
       </c>
       <c r="B350" s="1" t="s">
-        <v>649</v>
+        <v>444</v>
       </c>
       <c r="D350" s="1" t="s">
-        <v>650</v>
+        <v>445</v>
       </c>
     </row>
     <row r="351" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A351" s="1" t="s">
-        <v>930</v>
+        <v>810</v>
       </c>
       <c r="B351" s="1" t="s">
-        <v>931</v>
+        <v>811</v>
       </c>
       <c r="D351" s="1" t="s">
-        <v>932</v>
+        <v>995</v>
       </c>
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A352" s="1" t="s">
-        <v>996</v>
+        <v>648</v>
       </c>
       <c r="B352" s="1" t="s">
-        <v>997</v>
+        <v>649</v>
       </c>
       <c r="D352" s="1" t="s">
-        <v>998</v>
+        <v>650</v>
       </c>
     </row>
     <row r="353" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A353" s="1" t="s">
-        <v>999</v>
+        <v>930</v>
       </c>
       <c r="B353" s="1" t="s">
-        <v>1000</v>
+        <v>931</v>
       </c>
       <c r="D353" s="1" t="s">
-        <v>1001</v>
+        <v>932</v>
       </c>
     </row>
     <row r="354" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A354" s="1" t="s">
-        <v>1006</v>
+        <v>996</v>
       </c>
       <c r="B354" s="1" t="s">
-        <v>731</v>
+        <v>997</v>
       </c>
       <c r="D354" s="1" t="s">
-        <v>732</v>
+        <v>998</v>
       </c>
     </row>
     <row r="355" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A355" s="1" t="s">
-        <v>855</v>
+        <v>999</v>
       </c>
       <c r="B355" s="1" t="s">
-        <v>856</v>
+        <v>1000</v>
       </c>
       <c r="D355" s="1" t="s">
-        <v>857</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="356" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A356" s="1" t="s">
-        <v>666</v>
+        <v>1006</v>
       </c>
       <c r="B356" s="1" t="s">
-        <v>667</v>
+        <v>731</v>
       </c>
       <c r="D356" s="1" t="s">
-        <v>668</v>
+        <v>732</v>
       </c>
     </row>
     <row r="357" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A357" s="1" t="s">
-        <v>967</v>
+        <v>855</v>
       </c>
       <c r="B357" s="1" t="s">
-        <v>928</v>
+        <v>856</v>
       </c>
       <c r="D357" s="1" t="s">
-        <v>911</v>
+        <v>857</v>
       </c>
     </row>
     <row r="358" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A358" s="1" t="s">
-        <v>1002</v>
+        <v>666</v>
       </c>
       <c r="B358" s="1" t="s">
-        <v>1003</v>
+        <v>667</v>
       </c>
       <c r="D358" s="1" t="s">
-        <v>1004</v>
+        <v>668</v>
       </c>
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A359" s="1" t="s">
-        <v>1007</v>
+        <v>967</v>
       </c>
       <c r="B359" s="1" t="s">
-        <v>1008</v>
+        <v>928</v>
       </c>
       <c r="D359" s="1" t="s">
-        <v>1009</v>
+        <v>911</v>
       </c>
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A360" s="1" t="s">
-        <v>1022</v>
+        <v>1002</v>
       </c>
       <c r="B360" s="1" t="s">
-        <v>1023</v>
+        <v>1003</v>
       </c>
       <c r="D360" s="1" t="s">
-        <v>1024</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A361" s="1" t="s">
-        <v>431</v>
+        <v>1007</v>
       </c>
       <c r="B361" s="1" t="s">
-        <v>432</v>
+        <v>1008</v>
       </c>
       <c r="D361" s="1" t="s">
-        <v>433</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="362" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A362" s="1" t="s">
-        <v>434</v>
+        <v>1022</v>
       </c>
       <c r="B362" s="1" t="s">
-        <v>435</v>
+        <v>1023</v>
       </c>
       <c r="D362" s="1" t="s">
-        <v>436</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="363" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A363" s="1" t="s">
-        <v>601</v>
+        <v>431</v>
       </c>
       <c r="B363" s="1" t="s">
-        <v>602</v>
+        <v>432</v>
       </c>
       <c r="D363" s="1" t="s">
-        <v>603</v>
+        <v>433</v>
       </c>
     </row>
     <row r="364" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A364" s="1" t="s">
-        <v>595</v>
+        <v>434</v>
       </c>
       <c r="B364" s="1" t="s">
-        <v>596</v>
+        <v>435</v>
       </c>
       <c r="D364" s="1" t="s">
-        <v>597</v>
+        <v>436</v>
       </c>
     </row>
     <row r="365" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A365" s="1" t="s">
-        <v>672</v>
+        <v>601</v>
       </c>
       <c r="B365" s="1" t="s">
-        <v>673</v>
+        <v>602</v>
       </c>
       <c r="D365" s="1" t="s">
-        <v>674</v>
+        <v>603</v>
       </c>
     </row>
     <row r="366" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A366" s="1" t="s">
-        <v>446</v>
+        <v>595</v>
       </c>
       <c r="B366" s="1" t="s">
-        <v>447</v>
+        <v>596</v>
       </c>
       <c r="D366" s="1" t="s">
-        <v>447</v>
+        <v>597</v>
       </c>
     </row>
     <row r="367" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A367" s="1" t="s">
-        <v>598</v>
+        <v>672</v>
       </c>
       <c r="B367" s="1" t="s">
-        <v>599</v>
+        <v>673</v>
       </c>
       <c r="D367" s="1" t="s">
-        <v>600</v>
+        <v>674</v>
       </c>
     </row>
     <row r="368" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A368" s="1" t="s">
-        <v>544</v>
+        <v>446</v>
       </c>
       <c r="B368" s="1" t="s">
-        <v>545</v>
+        <v>447</v>
       </c>
       <c r="D368" s="1" t="s">
-        <v>546</v>
+        <v>447</v>
       </c>
     </row>
     <row r="369" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A369" s="1" t="s">
-        <v>466</v>
+        <v>598</v>
       </c>
       <c r="B369" s="1" t="s">
-        <v>467</v>
+        <v>599</v>
       </c>
       <c r="D369" s="1" t="s">
-        <v>468</v>
+        <v>600</v>
       </c>
     </row>
     <row r="370" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A370" s="1" t="s">
-        <v>621</v>
+        <v>544</v>
       </c>
       <c r="B370" s="1" t="s">
-        <v>622</v>
+        <v>545</v>
       </c>
       <c r="D370" s="1" t="s">
-        <v>623</v>
+        <v>546</v>
       </c>
     </row>
     <row r="371" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A371" s="1" t="s">
-        <v>404</v>
+        <v>466</v>
       </c>
       <c r="B371" s="1" t="s">
-        <v>405</v>
+        <v>467</v>
       </c>
       <c r="D371" s="1" t="s">
-        <v>406</v>
+        <v>468</v>
       </c>
     </row>
     <row r="372" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A372" s="1" t="s">
-        <v>407</v>
+        <v>621</v>
       </c>
       <c r="B372" s="1" t="s">
-        <v>408</v>
+        <v>622</v>
       </c>
       <c r="D372" s="1" t="s">
-        <v>409</v>
+        <v>623</v>
       </c>
     </row>
     <row r="373" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A373" s="1" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="B373" s="1" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="D373" s="1" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
     </row>
     <row r="374" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A374" s="1" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="B374" s="1" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="D374" s="1" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
     </row>
     <row r="375" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A375" s="1" t="s">
-        <v>849</v>
+        <v>410</v>
       </c>
       <c r="B375" s="1" t="s">
-        <v>850</v>
+        <v>411</v>
       </c>
       <c r="D375" s="1" t="s">
-        <v>851</v>
+        <v>412</v>
       </c>
     </row>
     <row r="376" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A376" s="1" t="s">
-        <v>828</v>
+        <v>413</v>
       </c>
       <c r="B376" s="1" t="s">
-        <v>829</v>
+        <v>414</v>
       </c>
       <c r="D376" s="1" t="s">
-        <v>830</v>
+        <v>415</v>
       </c>
     </row>
     <row r="377" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A377" s="1" t="s">
-        <v>831</v>
+        <v>849</v>
       </c>
       <c r="B377" s="1" t="s">
-        <v>832</v>
+        <v>850</v>
       </c>
       <c r="D377" s="1" t="s">
-        <v>833</v>
+        <v>851</v>
       </c>
     </row>
     <row r="378" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A378" s="1" t="s">
-        <v>728</v>
+        <v>828</v>
       </c>
       <c r="B378" s="1" t="s">
-        <v>729</v>
+        <v>829</v>
       </c>
       <c r="D378" s="1" t="s">
-        <v>730</v>
+        <v>830</v>
       </c>
     </row>
     <row r="379" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A379" s="1" t="s">
-        <v>725</v>
+        <v>831</v>
       </c>
       <c r="B379" s="1" t="s">
-        <v>726</v>
+        <v>832</v>
       </c>
       <c r="D379" s="1" t="s">
-        <v>727</v>
+        <v>833</v>
       </c>
     </row>
     <row r="380" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A380" s="1" t="s">
-        <v>517</v>
+        <v>1158</v>
       </c>
       <c r="B380" s="1" t="s">
-        <v>518</v>
+        <v>1157</v>
       </c>
       <c r="D380" s="1" t="s">
-        <v>519</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="381" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A381" s="1" t="s">
-        <v>592</v>
+        <v>728</v>
       </c>
       <c r="B381" s="1" t="s">
-        <v>593</v>
+        <v>729</v>
       </c>
       <c r="D381" s="1" t="s">
-        <v>594</v>
+        <v>730</v>
       </c>
     </row>
     <row r="382" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A382" s="1" t="s">
-        <v>675</v>
+        <v>725</v>
       </c>
       <c r="B382" s="1" t="s">
-        <v>676</v>
+        <v>726</v>
       </c>
       <c r="D382" s="1" t="s">
-        <v>677</v>
+        <v>727</v>
       </c>
     </row>
     <row r="383" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A383" s="1" t="s">
-        <v>655</v>
+        <v>517</v>
       </c>
       <c r="B383" s="1" t="s">
-        <v>656</v>
+        <v>518</v>
       </c>
       <c r="D383" s="1" t="s">
-        <v>1036</v>
+        <v>519</v>
       </c>
     </row>
     <row r="384" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A384" s="1" t="s">
-        <v>1046</v>
+        <v>592</v>
       </c>
       <c r="B384" s="1" t="s">
-        <v>1047</v>
+        <v>593</v>
       </c>
       <c r="D384" s="1" t="s">
-        <v>1048</v>
+        <v>594</v>
       </c>
     </row>
     <row r="385" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A385" s="1" t="s">
-        <v>1029</v>
+        <v>675</v>
       </c>
       <c r="B385" s="1" t="s">
-        <v>1028</v>
+        <v>676</v>
       </c>
       <c r="D385" s="1" t="s">
-        <v>1030</v>
+        <v>677</v>
       </c>
     </row>
     <row r="386" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A386" s="1" t="s">
-        <v>843</v>
+        <v>655</v>
       </c>
       <c r="B386" s="1" t="s">
-        <v>844</v>
+        <v>656</v>
       </c>
       <c r="D386" s="1" t="s">
-        <v>845</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="387" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A387" s="1" t="s">
-        <v>867</v>
+        <v>1046</v>
       </c>
       <c r="B387" s="1" t="s">
-        <v>868</v>
+        <v>1047</v>
       </c>
       <c r="D387" s="1" t="s">
-        <v>869</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="388" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A388" s="1" t="s">
-        <v>472</v>
+        <v>1029</v>
       </c>
       <c r="B388" s="1" t="s">
-        <v>473</v>
+        <v>1028</v>
       </c>
       <c r="D388" s="1" t="s">
-        <v>474</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="389" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A389" s="1" t="s">
-        <v>976</v>
+        <v>843</v>
       </c>
       <c r="B389" s="1" t="s">
-        <v>923</v>
+        <v>844</v>
       </c>
       <c r="D389" s="1" t="s">
-        <v>1005</v>
+        <v>845</v>
       </c>
     </row>
     <row r="390" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A390" s="1" t="s">
-        <v>559</v>
+        <v>867</v>
       </c>
       <c r="B390" s="1" t="s">
-        <v>560</v>
+        <v>868</v>
       </c>
       <c r="D390" s="1" t="s">
-        <v>561</v>
+        <v>869</v>
       </c>
     </row>
     <row r="391" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A391" s="1" t="s">
-        <v>973</v>
+        <v>472</v>
       </c>
       <c r="B391" s="1" t="s">
-        <v>922</v>
+        <v>473</v>
       </c>
       <c r="D391" s="1" t="s">
-        <v>975</v>
+        <v>474</v>
       </c>
     </row>
     <row r="392" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A392" s="1" t="s">
-        <v>496</v>
+        <v>976</v>
       </c>
       <c r="B392" s="1" t="s">
-        <v>497</v>
+        <v>923</v>
       </c>
       <c r="D392" s="1" t="s">
-        <v>498</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="393" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A393" s="1" t="s">
-        <v>992</v>
+        <v>559</v>
       </c>
       <c r="B393" s="1" t="s">
-        <v>993</v>
+        <v>560</v>
       </c>
       <c r="D393" s="1" t="s">
-        <v>994</v>
+        <v>561</v>
       </c>
     </row>
     <row r="394" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A394" s="1" t="s">
-        <v>984</v>
+        <v>973</v>
       </c>
       <c r="B394" s="1" t="s">
-        <v>920</v>
+        <v>922</v>
       </c>
       <c r="D394" s="1" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
     </row>
     <row r="395" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A395" s="1" t="s">
-        <v>983</v>
+        <v>496</v>
       </c>
       <c r="B395" s="1" t="s">
-        <v>919</v>
+        <v>497</v>
       </c>
       <c r="D395" s="1" t="s">
-        <v>978</v>
+        <v>498</v>
       </c>
     </row>
     <row r="396" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A396" s="1" t="s">
-        <v>902</v>
+        <v>992</v>
       </c>
       <c r="B396" s="1" t="s">
-        <v>903</v>
+        <v>993</v>
       </c>
       <c r="D396" s="1" t="s">
-        <v>904</v>
+        <v>994</v>
       </c>
     </row>
     <row r="397" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A397" s="1" t="s">
-        <v>481</v>
+        <v>984</v>
       </c>
       <c r="B397" s="1" t="s">
-        <v>482</v>
+        <v>920</v>
       </c>
       <c r="D397" s="1" t="s">
-        <v>483</v>
+        <v>977</v>
       </c>
     </row>
     <row r="398" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A398" s="1" t="s">
-        <v>1074</v>
+        <v>983</v>
       </c>
       <c r="B398" s="1" t="s">
-        <v>1075</v>
+        <v>919</v>
       </c>
       <c r="D398" s="1" t="s">
-        <v>1015</v>
+        <v>978</v>
       </c>
     </row>
     <row r="399" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A399" s="1" t="s">
-        <v>499</v>
+        <v>902</v>
       </c>
       <c r="B399" s="1" t="s">
-        <v>500</v>
+        <v>903</v>
       </c>
       <c r="D399" s="1" t="s">
-        <v>501</v>
+        <v>904</v>
       </c>
     </row>
     <row r="400" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A400" s="1" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="B400" s="1" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="D400" s="1" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="401" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A401" s="1" t="s">
-        <v>487</v>
+        <v>1074</v>
       </c>
       <c r="B401" s="1" t="s">
-        <v>488</v>
+        <v>1075</v>
       </c>
       <c r="D401" s="1" t="s">
-        <v>489</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="402" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A402" s="1" t="s">
-        <v>945</v>
+        <v>499</v>
       </c>
       <c r="B402" s="1" t="s">
-        <v>946</v>
+        <v>500</v>
       </c>
       <c r="D402" s="1" t="s">
-        <v>947</v>
+        <v>501</v>
       </c>
     </row>
     <row r="403" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A403" s="1" t="s">
-        <v>705</v>
+        <v>484</v>
       </c>
       <c r="B403" s="1" t="s">
-        <v>706</v>
+        <v>485</v>
       </c>
       <c r="D403" s="1" t="s">
-        <v>707</v>
+        <v>486</v>
       </c>
     </row>
     <row r="404" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A404" s="1" t="s">
-        <v>801</v>
+        <v>487</v>
       </c>
       <c r="B404" s="1" t="s">
-        <v>802</v>
+        <v>488</v>
       </c>
       <c r="D404" s="1" t="s">
-        <v>803</v>
+        <v>489</v>
       </c>
     </row>
     <row r="405" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A405" s="1" t="s">
-        <v>532</v>
+        <v>945</v>
       </c>
       <c r="B405" s="1" t="s">
-        <v>533</v>
+        <v>946</v>
       </c>
       <c r="D405" s="1" t="s">
-        <v>534</v>
+        <v>947</v>
       </c>
     </row>
     <row r="406" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A406" s="1" t="s">
-        <v>502</v>
+        <v>705</v>
       </c>
       <c r="B406" s="1" t="s">
-        <v>503</v>
+        <v>706</v>
       </c>
       <c r="D406" s="1" t="s">
-        <v>504</v>
+        <v>707</v>
       </c>
     </row>
     <row r="407" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A407" s="1" t="s">
-        <v>416</v>
+        <v>801</v>
       </c>
       <c r="B407" s="1" t="s">
-        <v>417</v>
+        <v>802</v>
       </c>
       <c r="D407" s="1" t="s">
-        <v>418</v>
+        <v>803</v>
       </c>
     </row>
     <row r="408" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A408" s="1" t="s">
-        <v>505</v>
+        <v>532</v>
       </c>
       <c r="B408" s="1" t="s">
-        <v>506</v>
+        <v>533</v>
       </c>
       <c r="D408" s="1" t="s">
-        <v>507</v>
+        <v>534</v>
       </c>
     </row>
     <row r="409" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A409" s="1" t="s">
-        <v>722</v>
+        <v>502</v>
       </c>
       <c r="B409" s="1" t="s">
-        <v>723</v>
+        <v>503</v>
       </c>
       <c r="D409" s="1" t="s">
-        <v>724</v>
+        <v>504</v>
       </c>
     </row>
     <row r="410" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A410" s="1" t="s">
-        <v>556</v>
+        <v>416</v>
       </c>
       <c r="B410" s="1" t="s">
-        <v>557</v>
+        <v>417</v>
       </c>
       <c r="D410" s="1" t="s">
-        <v>558</v>
+        <v>418</v>
       </c>
     </row>
     <row r="411" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A411" s="1" t="s">
-        <v>562</v>
+        <v>505</v>
       </c>
       <c r="B411" s="1" t="s">
-        <v>563</v>
+        <v>506</v>
       </c>
       <c r="D411" s="1" t="s">
-        <v>564</v>
+        <v>507</v>
       </c>
     </row>
     <row r="412" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A412" s="1" t="s">
-        <v>550</v>
+        <v>722</v>
       </c>
       <c r="B412" s="1" t="s">
-        <v>551</v>
+        <v>723</v>
       </c>
       <c r="D412" s="1" t="s">
-        <v>552</v>
+        <v>724</v>
       </c>
     </row>
     <row r="413" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A413" s="1" t="s">
-        <v>764</v>
+        <v>556</v>
       </c>
       <c r="B413" s="1" t="s">
-        <v>765</v>
+        <v>557</v>
       </c>
       <c r="D413" s="1" t="s">
-        <v>552</v>
+        <v>558</v>
       </c>
     </row>
     <row r="414" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A414" s="1" t="s">
-        <v>619</v>
+        <v>562</v>
       </c>
       <c r="B414" s="1" t="s">
-        <v>620</v>
+        <v>563</v>
       </c>
       <c r="D414" s="1" t="s">
-        <v>1012</v>
+        <v>564</v>
       </c>
     </row>
     <row r="415" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A415" s="1" t="s">
-        <v>607</v>
+        <v>550</v>
       </c>
       <c r="B415" s="1" t="s">
-        <v>608</v>
+        <v>551</v>
       </c>
       <c r="D415" s="1" t="s">
-        <v>609</v>
+        <v>552</v>
       </c>
     </row>
     <row r="416" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A416" s="1" t="s">
-        <v>451</v>
+        <v>764</v>
       </c>
       <c r="B416" s="1" t="s">
-        <v>452</v>
+        <v>765</v>
       </c>
       <c r="D416" s="1" t="s">
-        <v>453</v>
+        <v>552</v>
       </c>
     </row>
     <row r="417" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A417" s="1" t="s">
-        <v>690</v>
+        <v>619</v>
       </c>
       <c r="B417" s="1" t="s">
-        <v>691</v>
+        <v>620</v>
       </c>
       <c r="D417" s="1" t="s">
-        <v>692</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="418" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A418" s="1" t="s">
-        <v>454</v>
+        <v>607</v>
       </c>
       <c r="B418" s="1" t="s">
-        <v>455</v>
+        <v>608</v>
       </c>
       <c r="D418" s="1" t="s">
-        <v>456</v>
+        <v>609</v>
       </c>
     </row>
     <row r="419" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A419" s="1" t="s">
-        <v>766</v>
+        <v>451</v>
       </c>
       <c r="B419" s="1" t="s">
-        <v>767</v>
+        <v>452</v>
       </c>
       <c r="D419" s="1" t="s">
-        <v>768</v>
+        <v>453</v>
       </c>
     </row>
     <row r="420" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A420" s="1" t="s">
-        <v>1052</v>
+        <v>690</v>
       </c>
       <c r="B420" s="1" t="s">
-        <v>1053</v>
+        <v>691</v>
       </c>
       <c r="D420" s="1" t="s">
-        <v>1054</v>
+        <v>692</v>
       </c>
     </row>
     <row r="421" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A421" s="1" t="s">
-        <v>822</v>
+        <v>454</v>
       </c>
       <c r="B421" s="1" t="s">
-        <v>823</v>
+        <v>455</v>
       </c>
       <c r="D421" s="1" t="s">
-        <v>824</v>
+        <v>456</v>
       </c>
     </row>
     <row r="422" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A422" s="1" t="s">
-        <v>422</v>
+        <v>766</v>
       </c>
       <c r="B422" s="1" t="s">
-        <v>423</v>
+        <v>767</v>
       </c>
       <c r="D422" s="1" t="s">
-        <v>424</v>
+        <v>768</v>
       </c>
     </row>
     <row r="423" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A423" s="1" t="s">
-        <v>1017</v>
+        <v>1052</v>
       </c>
       <c r="B423" s="1" t="s">
-        <v>1018</v>
+        <v>1053</v>
       </c>
       <c r="D423" s="1" t="s">
-        <v>1019</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="424" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A424" s="1" t="s">
-        <v>745</v>
+        <v>822</v>
       </c>
       <c r="B424" s="1" t="s">
-        <v>746</v>
+        <v>823</v>
       </c>
       <c r="D424" s="1" t="s">
-        <v>747</v>
+        <v>824</v>
       </c>
     </row>
     <row r="425" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A425" s="1" t="s">
-        <v>906</v>
+        <v>422</v>
       </c>
       <c r="B425" s="1" t="s">
-        <v>905</v>
+        <v>423</v>
       </c>
       <c r="D425" s="1" t="s">
-        <v>907</v>
+        <v>424</v>
       </c>
     </row>
     <row r="426" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A426" s="1" t="s">
-        <v>908</v>
+        <v>1017</v>
       </c>
       <c r="B426" s="1" t="s">
-        <v>909</v>
+        <v>1018</v>
       </c>
       <c r="D426" s="1" t="s">
-        <v>910</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="427" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A427" s="1" t="s">
-        <v>541</v>
+        <v>745</v>
       </c>
       <c r="B427" s="1" t="s">
-        <v>542</v>
+        <v>746</v>
       </c>
       <c r="D427" s="1" t="s">
-        <v>543</v>
+        <v>747</v>
       </c>
     </row>
     <row r="428" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A428" s="1" t="s">
-        <v>663</v>
+        <v>906</v>
       </c>
       <c r="B428" s="1" t="s">
-        <v>664</v>
+        <v>905</v>
       </c>
       <c r="D428" s="1" t="s">
-        <v>665</v>
+        <v>907</v>
       </c>
     </row>
     <row r="429" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A429" s="1" t="s">
-        <v>693</v>
+        <v>908</v>
       </c>
       <c r="B429" s="1" t="s">
-        <v>694</v>
+        <v>909</v>
       </c>
       <c r="D429" s="1" t="s">
-        <v>695</v>
+        <v>910</v>
       </c>
     </row>
     <row r="430" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A430" s="1" t="s">
-        <v>968</v>
+        <v>541</v>
       </c>
       <c r="B430" s="1" t="s">
-        <v>927</v>
+        <v>542</v>
       </c>
       <c r="D430" s="1" t="s">
-        <v>913</v>
+        <v>543</v>
       </c>
     </row>
     <row r="431" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A431" s="1" t="s">
-        <v>787</v>
+        <v>663</v>
       </c>
       <c r="B431" s="1" t="s">
-        <v>788</v>
+        <v>664</v>
       </c>
       <c r="D431" s="1" t="s">
-        <v>789</v>
+        <v>665</v>
       </c>
     </row>
     <row r="432" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A432" s="1" t="s">
-        <v>624</v>
+        <v>693</v>
       </c>
       <c r="B432" s="1" t="s">
-        <v>625</v>
+        <v>694</v>
       </c>
       <c r="D432" s="1" t="s">
-        <v>626</v>
+        <v>695</v>
       </c>
     </row>
     <row r="433" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A433" s="1" t="s">
-        <v>837</v>
+        <v>968</v>
       </c>
       <c r="B433" s="1" t="s">
-        <v>838</v>
+        <v>927</v>
       </c>
       <c r="D433" s="1" t="s">
-        <v>839</v>
+        <v>913</v>
       </c>
     </row>
     <row r="434" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A434" s="1" t="s">
-        <v>687</v>
+        <v>787</v>
       </c>
       <c r="B434" s="1" t="s">
-        <v>688</v>
+        <v>788</v>
       </c>
       <c r="D434" s="1" t="s">
-        <v>689</v>
+        <v>789</v>
       </c>
     </row>
     <row r="435" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A435" s="1" t="s">
-        <v>897</v>
+        <v>624</v>
       </c>
       <c r="B435" s="1" t="s">
-        <v>898</v>
+        <v>625</v>
+      </c>
+      <c r="D435" s="1" t="s">
+        <v>626</v>
       </c>
     </row>
     <row r="436" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A436" s="1" t="s">
-        <v>972</v>
+        <v>837</v>
       </c>
       <c r="B436" s="1" t="s">
-        <v>921</v>
+        <v>838</v>
       </c>
       <c r="D436" s="1" t="s">
-        <v>974</v>
+        <v>839</v>
       </c>
     </row>
     <row r="437" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A437" s="1" t="s">
-        <v>951</v>
+        <v>687</v>
       </c>
       <c r="B437" s="1" t="s">
-        <v>952</v>
+        <v>688</v>
       </c>
       <c r="D437" s="1" t="s">
-        <v>953</v>
+        <v>689</v>
       </c>
     </row>
     <row r="438" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A438" s="1" t="s">
-        <v>475</v>
+        <v>897</v>
       </c>
       <c r="B438" s="1" t="s">
-        <v>476</v>
-      </c>
-      <c r="D438" s="1" t="s">
-        <v>477</v>
+        <v>898</v>
       </c>
     </row>
     <row r="439" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A439" s="1" t="s">
-        <v>568</v>
+        <v>972</v>
       </c>
       <c r="B439" s="1" t="s">
-        <v>569</v>
+        <v>921</v>
       </c>
       <c r="D439" s="1" t="s">
-        <v>570</v>
+        <v>974</v>
       </c>
     </row>
     <row r="440" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A440" s="1" t="s">
-        <v>769</v>
+        <v>951</v>
       </c>
       <c r="B440" s="1" t="s">
-        <v>770</v>
+        <v>952</v>
       </c>
       <c r="D440" s="1" t="s">
-        <v>771</v>
+        <v>953</v>
       </c>
     </row>
     <row r="441" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A441" s="1" t="s">
-        <v>772</v>
+        <v>475</v>
       </c>
       <c r="B441" s="1" t="s">
-        <v>773</v>
+        <v>476</v>
       </c>
       <c r="D441" s="1" t="s">
-        <v>355</v>
+        <v>477</v>
       </c>
     </row>
     <row r="442" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A442" s="1" t="s">
-        <v>713</v>
+        <v>568</v>
       </c>
       <c r="B442" s="1" t="s">
-        <v>714</v>
+        <v>569</v>
       </c>
       <c r="D442" s="1" t="s">
-        <v>715</v>
+        <v>570</v>
       </c>
     </row>
     <row r="443" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A443" s="1" t="s">
-        <v>882</v>
+        <v>769</v>
       </c>
       <c r="B443" s="1" t="s">
-        <v>883</v>
+        <v>770</v>
       </c>
       <c r="D443" s="1" t="s">
-        <v>884</v>
+        <v>771</v>
       </c>
     </row>
     <row r="444" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A444" s="1" t="s">
-        <v>1148</v>
+        <v>772</v>
       </c>
       <c r="B444" s="1" t="s">
-        <v>1149</v>
+        <v>773</v>
       </c>
       <c r="D444" s="1" t="s">
-        <v>1147</v>
+        <v>355</v>
       </c>
     </row>
     <row r="445" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A445" s="1" t="s">
-        <v>954</v>
+        <v>713</v>
       </c>
       <c r="B445" s="1" t="s">
-        <v>956</v>
+        <v>714</v>
       </c>
       <c r="D445" s="1" t="s">
-        <v>957</v>
+        <v>715</v>
       </c>
     </row>
     <row r="446" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A446" s="1" t="s">
-        <v>748</v>
+        <v>882</v>
       </c>
       <c r="B446" s="1" t="s">
-        <v>749</v>
+        <v>883</v>
       </c>
       <c r="D446" s="1" t="s">
-        <v>750</v>
+        <v>884</v>
       </c>
     </row>
     <row r="447" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A447" s="1" t="s">
-        <v>577</v>
+        <v>1148</v>
       </c>
       <c r="B447" s="1" t="s">
-        <v>578</v>
+        <v>1149</v>
       </c>
       <c r="D447" s="1" t="s">
-        <v>579</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="448" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A448" s="1" t="s">
-        <v>825</v>
+        <v>954</v>
       </c>
       <c r="B448" s="1" t="s">
-        <v>826</v>
+        <v>956</v>
       </c>
       <c r="D448" s="1" t="s">
-        <v>827</v>
+        <v>957</v>
       </c>
     </row>
     <row r="449" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A449" s="1" t="s">
-        <v>1025</v>
+        <v>748</v>
       </c>
       <c r="B449" s="1" t="s">
-        <v>1026</v>
+        <v>749</v>
       </c>
       <c r="D449" s="1" t="s">
-        <v>1027</v>
+        <v>750</v>
       </c>
     </row>
     <row r="450" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A450" s="1" t="s">
-        <v>428</v>
+        <v>577</v>
       </c>
       <c r="B450" s="1" t="s">
-        <v>429</v>
+        <v>578</v>
       </c>
       <c r="D450" s="1" t="s">
-        <v>430</v>
+        <v>579</v>
       </c>
     </row>
     <row r="451" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A451" s="1" t="s">
-        <v>627</v>
+        <v>825</v>
       </c>
       <c r="B451" s="1" t="s">
-        <v>628</v>
+        <v>826</v>
       </c>
       <c r="D451" s="1" t="s">
-        <v>629</v>
+        <v>827</v>
       </c>
     </row>
     <row r="452" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A452" s="1" t="s">
-        <v>419</v>
+        <v>1025</v>
       </c>
       <c r="B452" s="1" t="s">
-        <v>420</v>
+        <v>1026</v>
       </c>
       <c r="D452" s="1" t="s">
-        <v>421</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="453" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A453" s="1" t="s">
-        <v>933</v>
+        <v>428</v>
       </c>
       <c r="B453" s="1" t="s">
-        <v>934</v>
+        <v>429</v>
       </c>
       <c r="D453" s="1" t="s">
-        <v>935</v>
+        <v>430</v>
       </c>
     </row>
     <row r="454" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A454" s="1" t="s">
-        <v>736</v>
+        <v>627</v>
       </c>
       <c r="B454" s="1" t="s">
-        <v>737</v>
+        <v>628</v>
       </c>
       <c r="D454" s="1" t="s">
-        <v>738</v>
+        <v>629</v>
       </c>
     </row>
     <row r="455" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A455" s="1" t="s">
-        <v>739</v>
+        <v>419</v>
       </c>
       <c r="B455" s="1" t="s">
-        <v>740</v>
+        <v>420</v>
       </c>
       <c r="D455" s="1" t="s">
-        <v>741</v>
+        <v>421</v>
       </c>
     </row>
     <row r="456" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A456" s="1" t="s">
-        <v>742</v>
+        <v>933</v>
       </c>
       <c r="B456" s="1" t="s">
-        <v>743</v>
+        <v>934</v>
       </c>
       <c r="D456" s="1" t="s">
-        <v>744</v>
+        <v>935</v>
       </c>
     </row>
     <row r="457" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A457" s="1" t="s">
-        <v>630</v>
+        <v>736</v>
       </c>
       <c r="B457" s="1" t="s">
-        <v>631</v>
+        <v>737</v>
       </c>
       <c r="D457" s="1" t="s">
-        <v>632</v>
+        <v>738</v>
       </c>
     </row>
     <row r="458" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A458" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="B458" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="D458" s="1" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="459" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A459" s="1" t="s">
+        <v>742</v>
+      </c>
+      <c r="B459" s="1" t="s">
+        <v>743</v>
+      </c>
+      <c r="D459" s="1" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="460" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A460" s="1" t="s">
+        <v>630</v>
+      </c>
+      <c r="B460" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="D460" s="1" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="461" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A461" s="1" t="s">
         <v>633</v>
       </c>
-      <c r="B458" s="1" t="s">
+      <c r="B461" s="1" t="s">
         <v>634</v>
       </c>
-      <c r="D458" s="1" t="s">
+      <c r="D461" s="1" t="s">
         <v>635</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Working for SecurityHeadersFilter 4
</commit_message>
<xml_diff>
--- a/conf/messages.xlsx
+++ b/conf/messages.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1213" uniqueCount="1159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1212" uniqueCount="1160">
   <si>
     <t>key</t>
   </si>
@@ -759,9 +759,6 @@
   </si>
   <si>
     <t>Japanese</t>
-  </si>
-  <si>
-    <t>ckeditor.lang</t>
   </si>
   <si>
     <t>parsley.lang</t>
@@ -3846,6 +3843,14 @@
   </si>
   <si>
     <t>paste</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>summernote.lang</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ja-JP</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -4322,8 +4327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G461"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A358" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="M380" sqref="M380"/>
+    <sheetView tabSelected="1" topLeftCell="A151" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A163" sqref="A163:XFD163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -4369,10 +4374,10 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>899</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>900</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
@@ -4382,7 +4387,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>9</v>
@@ -4422,7 +4427,7 @@
         <v>16</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
@@ -4433,7 +4438,7 @@
         <v>18</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
@@ -4444,7 +4449,7 @@
         <v>20</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
@@ -4455,7 +4460,7 @@
         <v>22</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
@@ -4477,7 +4482,7 @@
         <v>27</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
@@ -4493,7 +4498,7 @@
         <v>30</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
@@ -4690,7 +4695,7 @@
         <v>81</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
@@ -4909,7 +4914,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A66" s="1" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.15">
@@ -4919,7 +4924,7 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A69" s="1" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>137</v>
@@ -4930,7 +4935,7 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A70" s="1" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>139</v>
@@ -4941,54 +4946,54 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A71" s="1" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A72" s="1" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A73" s="1" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>143</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A74" s="1" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="B74" s="1" t="s">
+        <v>1097</v>
+      </c>
+      <c r="D74" s="1" t="s">
         <v>1098</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>1099</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A75" s="1" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>144</v>
@@ -4996,18 +5001,18 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A76" s="1" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A77" s="1" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>141</v>
@@ -5018,7 +5023,7 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A78" s="1" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>142</v>
@@ -5029,54 +5034,54 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A79" s="1" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A80" s="1" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A81" s="1" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A82" s="1" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A83" s="1" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>147</v>
@@ -5084,7 +5089,7 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A84" s="1" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>148</v>
@@ -5095,10 +5100,10 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A85" s="1" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>150</v>
@@ -5106,51 +5111,51 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A86" s="1" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A87" s="1" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="B87" s="1" t="s">
+        <v>1122</v>
+      </c>
+      <c r="D87" s="1" t="s">
         <v>1123</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>1124</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A88" s="1" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A89" s="1" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A90" s="1" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>151</v>
@@ -5166,7 +5171,7 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A93" s="1" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.15">
@@ -5182,7 +5187,7 @@
         <v>154</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.15">
@@ -5198,24 +5203,24 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A98" s="1" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B98" s="1" t="s">
         <v>1055</v>
       </c>
-      <c r="B98" s="1" t="s">
-        <v>1056</v>
-      </c>
       <c r="D98" s="1" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A99" s="1" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B99" s="1" t="s">
         <v>1057</v>
       </c>
-      <c r="B99" s="1" t="s">
-        <v>1058</v>
-      </c>
       <c r="D99" s="1" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.15">
@@ -5253,24 +5258,24 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A104" s="1" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A105" s="1" t="s">
+        <v>1061</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>1065</v>
+      </c>
+      <c r="D105" s="1" t="s">
         <v>1062</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>1066</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>1063</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.15">
@@ -5458,10 +5463,10 @@
         <v>212</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.15">
@@ -5469,10 +5474,10 @@
         <v>213</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.15">
@@ -5564,7 +5569,7 @@
         <v>230</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.15">
@@ -5634,29 +5639,26 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A162" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="B162" s="1" t="s">
-        <v>235</v>
+        <v>1158</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>236</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A163" s="1" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="B163" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A164" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B164" s="1" t="s">
         <v>235</v>
@@ -5667,7 +5669,7 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A165" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B165" s="1" t="s">
         <v>235</v>
@@ -5681,7 +5683,7 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A166" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B166" s="1" t="s">
         <v>2</v>
@@ -5692,13 +5694,13 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A167" s="1" t="s">
+        <v>935</v>
+      </c>
+      <c r="B167" s="1" t="s">
         <v>936</v>
       </c>
-      <c r="B167" s="1" t="s">
+      <c r="D167" s="1" t="s">
         <v>937</v>
-      </c>
-      <c r="D167" s="1" t="s">
-        <v>938</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.15">
@@ -5708,95 +5710,95 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A171" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>154</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A172" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B172" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="B172" s="1" t="s">
+      <c r="D172" s="1" t="s">
         <v>250</v>
-      </c>
-      <c r="D172" s="1" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A173" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B173" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="B173" s="1" t="s">
-        <v>253</v>
-      </c>
       <c r="D173" s="1" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A174" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B174" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D174" s="1" t="s">
         <v>250</v>
-      </c>
-      <c r="D174" s="1" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A175" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B175" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="B175" s="1" t="s">
+      <c r="D175" s="1" t="s">
         <v>256</v>
-      </c>
-      <c r="D175" s="1" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A176" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B176" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="B176" s="1" t="s">
+      <c r="D176" s="1" t="s">
         <v>259</v>
-      </c>
-      <c r="D176" s="1" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A177" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B177" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="B177" s="1" t="s">
+      <c r="D177" s="1" t="s">
         <v>262</v>
-      </c>
-      <c r="D177" s="1" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A178" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B178" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="B178" s="1" t="s">
+      <c r="D178" s="1" t="s">
         <v>265</v>
-      </c>
-      <c r="D178" s="1" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A179" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B179" s="1" t="s">
         <v>156</v>
@@ -5807,476 +5809,476 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A180" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B180" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="B180" s="3" t="s">
-        <v>269</v>
-      </c>
       <c r="D180" s="1" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A181" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B181" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="B181" s="1" t="s">
-        <v>271</v>
-      </c>
       <c r="D181" s="1" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A182" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B182" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="B182" s="1" t="s">
+      <c r="D182" s="1" t="s">
         <v>273</v>
-      </c>
-      <c r="D182" s="1" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A183" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B183" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="B183" s="1" t="s">
+      <c r="D183" s="1" t="s">
         <v>276</v>
-      </c>
-      <c r="D183" s="1" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A184" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B184" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="B184" s="1" t="s">
+      <c r="D184" s="1" t="s">
         <v>279</v>
-      </c>
-      <c r="D184" s="1" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A185" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B185" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="B185" s="1" t="s">
+      <c r="D185" s="1" t="s">
         <v>282</v>
-      </c>
-      <c r="D185" s="1" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A186" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B186" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="B186" s="1" t="s">
+      <c r="D186" s="1" t="s">
         <v>285</v>
-      </c>
-      <c r="D186" s="1" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A187" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B187" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="B187" s="1" t="s">
+      <c r="D187" s="1" t="s">
         <v>288</v>
-      </c>
-      <c r="D187" s="1" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A189" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B189" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="B189" s="1" t="s">
+      <c r="D189" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="D189" s="1" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A190" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B190" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="B190" s="1" t="s">
+      <c r="D190" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="D190" s="1" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A191" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B191" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="B191" s="1" t="s">
+      <c r="D191" s="1" t="s">
         <v>297</v>
-      </c>
-      <c r="D191" s="1" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A192" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B192" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="B192" s="1" t="s">
+      <c r="D192" s="1" t="s">
         <v>300</v>
-      </c>
-      <c r="D192" s="1" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A193" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B193" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="B193" s="1" t="s">
+      <c r="D193" s="1" t="s">
         <v>303</v>
-      </c>
-      <c r="D193" s="1" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A194" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="B194" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="B194" s="1" t="s">
+      <c r="D194" s="1" t="s">
         <v>306</v>
-      </c>
-      <c r="D194" s="1" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A195" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B195" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="B195" s="1" t="s">
+      <c r="D195" s="1" t="s">
         <v>309</v>
-      </c>
-      <c r="D195" s="1" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A196" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B196" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="B196" s="1" t="s">
+      <c r="D196" s="1" t="s">
         <v>312</v>
-      </c>
-      <c r="D196" s="1" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A197" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="B197" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="B197" s="1" t="s">
+      <c r="D197" s="1" t="s">
         <v>315</v>
-      </c>
-      <c r="D197" s="1" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A199" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="B199" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="B199" s="1" t="s">
+      <c r="D199" s="1" t="s">
         <v>318</v>
-      </c>
-      <c r="D199" s="1" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A200" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="B200" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="B200" s="1" t="s">
+      <c r="D200" s="1" t="s">
         <v>321</v>
-      </c>
-      <c r="D200" s="1" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A201" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B201" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="B201" s="1" t="s">
+      <c r="D201" s="1" t="s">
         <v>324</v>
-      </c>
-      <c r="D201" s="1" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A202" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B202" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="B202" s="1" t="s">
+      <c r="D202" s="1" t="s">
         <v>327</v>
-      </c>
-      <c r="D202" s="1" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A203" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="B203" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="B203" s="1" t="s">
+      <c r="D203" s="1" t="s">
         <v>330</v>
-      </c>
-      <c r="D203" s="1" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A204" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="B204" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="B204" s="1" t="s">
+      <c r="D204" s="1" t="s">
         <v>333</v>
-      </c>
-      <c r="D204" s="1" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A205" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B205" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="B205" s="1" t="s">
+      <c r="D205" s="1" t="s">
         <v>336</v>
-      </c>
-      <c r="D205" s="1" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A206" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="B206" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="B206" s="1" t="s">
+      <c r="D206" s="1" t="s">
         <v>339</v>
-      </c>
-      <c r="D206" s="1" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A207" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B207" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="B207" s="1" t="s">
+      <c r="D207" s="1" t="s">
         <v>342</v>
-      </c>
-      <c r="D207" s="1" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A208" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="B208" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="B208" s="1" t="s">
+      <c r="D208" s="1" t="s">
         <v>345</v>
-      </c>
-      <c r="D208" s="1" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A209" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="B209" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="B209" s="1" t="s">
+      <c r="D209" s="1" t="s">
         <v>348</v>
-      </c>
-      <c r="D209" s="1" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A210" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B210" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="B210" s="1" t="s">
+      <c r="D210" s="1" t="s">
         <v>351</v>
-      </c>
-      <c r="D210" s="1" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A212" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="B212" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="B212" s="1" t="s">
+      <c r="D212" s="1" t="s">
         <v>354</v>
-      </c>
-      <c r="D212" s="1" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A213" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B213" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="B213" s="1" t="s">
+      <c r="D213" s="1" t="s">
         <v>357</v>
-      </c>
-      <c r="D213" s="1" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A214" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="B214" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="B214" s="1" t="s">
+      <c r="D214" s="1" t="s">
         <v>360</v>
-      </c>
-      <c r="D214" s="1" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A215" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B215" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="B215" s="1" t="s">
+      <c r="D215" s="1" t="s">
         <v>363</v>
-      </c>
-      <c r="D215" s="1" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A216" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="B216" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="B216" s="1" t="s">
+      <c r="D216" s="1" t="s">
         <v>366</v>
-      </c>
-      <c r="D216" s="1" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A217" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="B217" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="B217" s="1" t="s">
+      <c r="D217" s="1" t="s">
         <v>369</v>
-      </c>
-      <c r="D217" s="1" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A218" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="B218" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="B218" s="1" t="s">
+      <c r="D218" s="1" t="s">
         <v>372</v>
-      </c>
-      <c r="D218" s="1" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A219" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="B219" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="B219" s="1" t="s">
+      <c r="D219" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="D219" s="1" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A220" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="B220" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="B220" s="1" t="s">
+      <c r="D220" s="1" t="s">
         <v>378</v>
-      </c>
-      <c r="D220" s="1" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A222" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="B222" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="B222" s="1" t="s">
+      <c r="D222" s="1" t="s">
         <v>381</v>
-      </c>
-      <c r="D222" s="1" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A223" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="B223" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="B223" s="1" t="s">
+      <c r="D223" s="1" t="s">
         <v>384</v>
-      </c>
-      <c r="D223" s="1" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A224" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="B224" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="B224" s="1" t="s">
+      <c r="D224" s="1" t="s">
         <v>387</v>
-      </c>
-      <c r="D224" s="1" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A225" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="B225" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="B225" s="1" t="s">
+      <c r="D225" s="1" t="s">
         <v>390</v>
-      </c>
-      <c r="D225" s="1" t="s">
-        <v>391</v>
       </c>
       <c r="G225" s="1"/>
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A226" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="B226" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="B226" s="1" t="s">
+      <c r="D226" s="1" t="s">
         <v>393</v>
-      </c>
-      <c r="D226" s="1" t="s">
-        <v>394</v>
       </c>
       <c r="G226" s="1"/>
     </row>
@@ -6294,521 +6296,521 @@
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A230" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="B230" s="1" t="s">
         <v>733</v>
       </c>
-      <c r="B230" s="1" t="s">
+      <c r="D230" s="1" t="s">
         <v>734</v>
-      </c>
-      <c r="D230" s="1" t="s">
-        <v>735</v>
       </c>
       <c r="G230" s="1"/>
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A231" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="B231" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="B231" s="1" t="s">
+      <c r="D231" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="D231" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="G231" s="1"/>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A232" s="1" t="s">
+        <v>988</v>
+      </c>
+      <c r="B232" s="1" t="s">
         <v>989</v>
       </c>
-      <c r="B232" s="1" t="s">
+      <c r="D232" s="1" t="s">
         <v>990</v>
-      </c>
-      <c r="D232" s="1" t="s">
-        <v>991</v>
       </c>
       <c r="G232" s="1"/>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A233" s="1" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="D233" s="1" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A234" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="B234" s="1" t="s">
         <v>604</v>
       </c>
-      <c r="B234" s="1" t="s">
+      <c r="D234" s="1" t="s">
         <v>605</v>
-      </c>
-      <c r="D234" s="1" t="s">
-        <v>606</v>
       </c>
       <c r="G234" s="1"/>
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A235" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="B235" s="1" t="s">
         <v>651</v>
       </c>
-      <c r="B235" s="1" t="s">
+      <c r="D235" s="1" t="s">
         <v>652</v>
-      </c>
-      <c r="D235" s="1" t="s">
-        <v>653</v>
       </c>
       <c r="G235" s="1"/>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A236" s="1" t="s">
+        <v>845</v>
+      </c>
+      <c r="B236" s="1" t="s">
         <v>846</v>
       </c>
-      <c r="B236" s="1" t="s">
+      <c r="D236" s="1" t="s">
         <v>847</v>
-      </c>
-      <c r="D236" s="1" t="s">
-        <v>848</v>
       </c>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A237" s="1" t="s">
+        <v>815</v>
+      </c>
+      <c r="B237" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="B237" s="1" t="s">
+      <c r="D237" s="1" t="s">
         <v>817</v>
-      </c>
-      <c r="D237" s="1" t="s">
-        <v>818</v>
       </c>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A238" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="B238" s="1" t="s">
         <v>526</v>
       </c>
-      <c r="B238" s="1" t="s">
-        <v>527</v>
-      </c>
       <c r="D238" s="1" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A239" s="1" t="s">
+        <v>938</v>
+      </c>
+      <c r="B239" s="1" t="s">
         <v>939</v>
       </c>
-      <c r="B239" s="1" t="s">
+      <c r="D239" s="1" t="s">
         <v>940</v>
-      </c>
-      <c r="D239" s="1" t="s">
-        <v>941</v>
       </c>
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A240" s="1" t="s">
+        <v>750</v>
+      </c>
+      <c r="B240" s="1" t="s">
         <v>751</v>
       </c>
-      <c r="B240" s="1" t="s">
+      <c r="D240" s="1" t="s">
         <v>752</v>
-      </c>
-      <c r="D240" s="1" t="s">
-        <v>753</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A241" s="1" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="D241" s="1" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A242" s="1" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="B242" s="1" t="s">
+        <v>1076</v>
+      </c>
+      <c r="D242" s="1" t="s">
         <v>1077</v>
-      </c>
-      <c r="D242" s="1" t="s">
-        <v>1078</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A243" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="B243" s="1" t="s">
         <v>660</v>
       </c>
-      <c r="B243" s="1" t="s">
+      <c r="D243" s="1" t="s">
         <v>661</v>
-      </c>
-      <c r="D243" s="1" t="s">
-        <v>662</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A244" s="1" t="s">
+        <v>892</v>
+      </c>
+      <c r="B244" s="1" t="s">
         <v>893</v>
-      </c>
-      <c r="B244" s="1" t="s">
-        <v>894</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A245" s="1" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="D245" s="1" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A246" s="1" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B246" s="1" t="s">
         <v>1081</v>
       </c>
-      <c r="B246" s="1" t="s">
+      <c r="D246" s="1" t="s">
         <v>1082</v>
-      </c>
-      <c r="D246" s="1" t="s">
-        <v>1083</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A247" s="1" t="s">
+        <v>797</v>
+      </c>
+      <c r="B247" s="1" t="s">
         <v>798</v>
       </c>
-      <c r="B247" s="1" t="s">
+      <c r="D247" s="1" t="s">
         <v>799</v>
-      </c>
-      <c r="D247" s="1" t="s">
-        <v>800</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A248" s="1" t="s">
+        <v>860</v>
+      </c>
+      <c r="B248" s="1" t="s">
         <v>861</v>
       </c>
-      <c r="B248" s="1" t="s">
+      <c r="D248" s="1" t="s">
         <v>862</v>
-      </c>
-      <c r="D248" s="1" t="s">
-        <v>863</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A249" s="1" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B249" s="1" t="s">
         <v>1040</v>
       </c>
-      <c r="B249" s="1" t="s">
+      <c r="D249" s="1" t="s">
         <v>1041</v>
-      </c>
-      <c r="D249" s="1" t="s">
-        <v>1042</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A250" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="B250" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="B250" s="1" t="s">
+      <c r="D250" s="1" t="s">
         <v>449</v>
-      </c>
-      <c r="D250" s="1" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A251" s="1" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B251" s="1" t="s">
         <v>1049</v>
       </c>
-      <c r="B251" s="1" t="s">
+      <c r="D251" s="1" t="s">
         <v>1050</v>
-      </c>
-      <c r="D251" s="1" t="s">
-        <v>1051</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A252" s="1" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="D252" s="1" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A253" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B253" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="B253" s="1" t="s">
+      <c r="D253" s="1" t="s">
         <v>491</v>
-      </c>
-      <c r="D253" s="1" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A254" s="1" t="s">
+        <v>878</v>
+      </c>
+      <c r="B254" s="1" t="s">
         <v>879</v>
       </c>
-      <c r="B254" s="1" t="s">
+      <c r="D254" s="1" t="s">
         <v>880</v>
-      </c>
-      <c r="D254" s="1" t="s">
-        <v>881</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A255" s="1" t="s">
+        <v>863</v>
+      </c>
+      <c r="B255" s="1" t="s">
         <v>864</v>
       </c>
-      <c r="B255" s="1" t="s">
+      <c r="D255" s="1" t="s">
         <v>865</v>
-      </c>
-      <c r="D255" s="1" t="s">
-        <v>866</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A256" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="B256" s="1" t="s">
         <v>565</v>
       </c>
-      <c r="B256" s="1" t="s">
+      <c r="D256" s="1" t="s">
         <v>566</v>
-      </c>
-      <c r="D256" s="1" t="s">
-        <v>567</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A257" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="B257" s="1" t="s">
         <v>547</v>
       </c>
-      <c r="B257" s="1" t="s">
+      <c r="D257" s="1" t="s">
         <v>548</v>
-      </c>
-      <c r="D257" s="1" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A258" s="1" t="s">
+        <v>872</v>
+      </c>
+      <c r="B258" s="1" t="s">
         <v>873</v>
       </c>
-      <c r="B258" s="1" t="s">
+      <c r="D258" s="1" t="s">
         <v>874</v>
-      </c>
-      <c r="D258" s="1" t="s">
-        <v>875</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A259" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="B259" s="1" t="s">
         <v>708</v>
       </c>
-      <c r="B259" s="1" t="s">
+      <c r="D259" s="1" t="s">
         <v>709</v>
-      </c>
-      <c r="D259" s="1" t="s">
-        <v>710</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A260" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="B260" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="B260" s="1" t="s">
+      <c r="D260" s="1" t="s">
         <v>396</v>
-      </c>
-      <c r="D260" s="1" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A261" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="B261" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="B261" s="1" t="s">
+      <c r="D261" s="1" t="s">
         <v>399</v>
-      </c>
-      <c r="D261" s="1" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A262" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="B262" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="B262" s="1" t="s">
+      <c r="D262" s="1" t="s">
         <v>402</v>
-      </c>
-      <c r="D262" s="1" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A263" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="B263" s="1" t="s">
         <v>460</v>
       </c>
-      <c r="B263" s="1" t="s">
+      <c r="D263" s="1" t="s">
         <v>461</v>
-      </c>
-      <c r="D263" s="1" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A264" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="B264" s="1" t="s">
         <v>819</v>
       </c>
-      <c r="B264" s="1" t="s">
+      <c r="D264" s="1" t="s">
         <v>820</v>
-      </c>
-      <c r="D264" s="1" t="s">
-        <v>821</v>
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A265" s="1" t="s">
+        <v>635</v>
+      </c>
+      <c r="B265" s="1" t="s">
         <v>636</v>
       </c>
-      <c r="B265" s="1" t="s">
+      <c r="D265" s="1" t="s">
         <v>637</v>
-      </c>
-      <c r="D265" s="1" t="s">
-        <v>638</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A266" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="B266" s="1" t="s">
         <v>657</v>
       </c>
-      <c r="B266" s="1" t="s">
+      <c r="D266" s="1" t="s">
         <v>658</v>
-      </c>
-      <c r="D266" s="1" t="s">
-        <v>659</v>
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A267" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="B267" s="1" t="s">
         <v>783</v>
       </c>
-      <c r="B267" s="1" t="s">
+      <c r="D267" s="1" t="s">
         <v>784</v>
-      </c>
-      <c r="D267" s="1" t="s">
-        <v>785</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A268" s="1" t="s">
+        <v>698</v>
+      </c>
+      <c r="B268" s="1" t="s">
         <v>699</v>
       </c>
-      <c r="B268" s="1" t="s">
+      <c r="D268" s="1" t="s">
         <v>700</v>
-      </c>
-      <c r="D268" s="1" t="s">
-        <v>701</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A269" s="1" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B269" s="1" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="D269" s="1" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A270" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="B270" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="B270" s="1" t="s">
+      <c r="D270" s="1" t="s">
         <v>470</v>
-      </c>
-      <c r="D270" s="1" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A271" s="1" t="s">
+        <v>779</v>
+      </c>
+      <c r="B271" s="1" t="s">
         <v>780</v>
       </c>
-      <c r="B271" s="1" t="s">
+      <c r="D271" s="1" t="s">
         <v>781</v>
-      </c>
-      <c r="D271" s="1" t="s">
-        <v>782</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A272" s="1" t="s">
+        <v>1149</v>
+      </c>
+      <c r="B272" s="1" t="s">
         <v>1150</v>
       </c>
-      <c r="B272" s="1" t="s">
+      <c r="D272" s="1" t="s">
         <v>1151</v>
-      </c>
-      <c r="D272" s="1" t="s">
-        <v>1152</v>
       </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A273" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="B273" s="1" t="s">
         <v>580</v>
       </c>
-      <c r="B273" s="1" t="s">
+      <c r="D273" s="1" t="s">
         <v>581</v>
-      </c>
-      <c r="D273" s="1" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A274" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="B274" s="1" t="s">
         <v>538</v>
       </c>
-      <c r="B274" s="1" t="s">
+      <c r="D274" s="1" t="s">
         <v>539</v>
-      </c>
-      <c r="D274" s="1" t="s">
-        <v>540</v>
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A275" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="B275" s="1" t="s">
         <v>535</v>
       </c>
-      <c r="B275" s="1" t="s">
+      <c r="D275" s="1" t="s">
         <v>536</v>
-      </c>
-      <c r="D275" s="1" t="s">
-        <v>537</v>
       </c>
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A276" s="1" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B276" s="1" t="s">
         <v>1020</v>
       </c>
-      <c r="B276" s="1" t="s">
-        <v>1021</v>
-      </c>
       <c r="D276" s="1" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.15">
@@ -6824,647 +6826,647 @@
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A278" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="B278" s="1" t="s">
         <v>478</v>
       </c>
-      <c r="B278" s="1" t="s">
+      <c r="D278" s="1" t="s">
         <v>479</v>
-      </c>
-      <c r="D278" s="1" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A279" s="1" t="s">
+        <v>668</v>
+      </c>
+      <c r="B279" s="1" t="s">
         <v>669</v>
       </c>
-      <c r="B279" s="1" t="s">
+      <c r="D279" s="1" t="s">
         <v>670</v>
-      </c>
-      <c r="D279" s="1" t="s">
-        <v>671</v>
       </c>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A280" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="B280" s="1" t="s">
         <v>508</v>
       </c>
-      <c r="B280" s="1" t="s">
+      <c r="D280" s="1" t="s">
         <v>509</v>
-      </c>
-      <c r="D280" s="1" t="s">
-        <v>510</v>
       </c>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A281" s="1" t="s">
+        <v>851</v>
+      </c>
+      <c r="B281" s="1" t="s">
         <v>852</v>
       </c>
-      <c r="B281" s="1" t="s">
+      <c r="D281" s="1" t="s">
         <v>853</v>
-      </c>
-      <c r="D281" s="1" t="s">
-        <v>854</v>
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A282" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="B282" s="1" t="s">
         <v>645</v>
       </c>
-      <c r="B282" s="1" t="s">
+      <c r="D282" s="1" t="s">
         <v>646</v>
-      </c>
-      <c r="D282" s="1" t="s">
-        <v>647</v>
       </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A283" s="1" t="s">
+        <v>789</v>
+      </c>
+      <c r="B283" s="1" t="s">
         <v>790</v>
       </c>
-      <c r="B283" s="1" t="s">
+      <c r="D283" s="1" t="s">
         <v>791</v>
-      </c>
-      <c r="D283" s="1" t="s">
-        <v>792</v>
       </c>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A284" s="1" t="s">
+        <v>680</v>
+      </c>
+      <c r="B284" s="1" t="s">
         <v>681</v>
       </c>
-      <c r="B284" s="1" t="s">
+      <c r="D284" s="1" t="s">
         <v>682</v>
-      </c>
-      <c r="D284" s="1" t="s">
-        <v>683</v>
       </c>
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A285" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="B285" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="B285" s="1" t="s">
+      <c r="D285" s="1" t="s">
         <v>426</v>
-      </c>
-      <c r="D285" s="1" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A286" s="1" t="s">
+        <v>947</v>
+      </c>
+      <c r="B286" s="1" t="s">
         <v>948</v>
       </c>
-      <c r="B286" s="1" t="s">
+      <c r="D286" s="1" t="s">
         <v>949</v>
-      </c>
-      <c r="D286" s="1" t="s">
-        <v>950</v>
       </c>
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A287" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="B287" s="1" t="s">
         <v>571</v>
       </c>
-      <c r="B287" s="1" t="s">
+      <c r="D287" s="1" t="s">
         <v>572</v>
-      </c>
-      <c r="D287" s="1" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A288" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="B288" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="B288" s="1" t="s">
+      <c r="D288" s="1" t="s">
         <v>521</v>
-      </c>
-      <c r="D288" s="1" t="s">
-        <v>522</v>
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A289" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="B289" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="B289" s="1" t="s">
+      <c r="D289" s="1" t="s">
         <v>524</v>
-      </c>
-      <c r="D289" s="1" t="s">
-        <v>525</v>
       </c>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A290" s="1" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B290" s="1" t="s">
         <v>1037</v>
       </c>
-      <c r="B290" s="1" t="s">
+      <c r="D290" s="1" t="s">
         <v>1038</v>
-      </c>
-      <c r="D290" s="1" t="s">
-        <v>1039</v>
       </c>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A291" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="B291" s="1" t="s">
         <v>493</v>
       </c>
-      <c r="B291" s="1" t="s">
+      <c r="D291" s="1" t="s">
         <v>494</v>
-      </c>
-      <c r="D291" s="1" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A292" s="1" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="B292" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D292" s="1" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A293" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="B293" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="B293" s="1" t="s">
+      <c r="D293" s="1" t="s">
         <v>464</v>
-      </c>
-      <c r="D293" s="1" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A294" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="B294" s="1" t="s">
         <v>610</v>
       </c>
-      <c r="B294" s="1" t="s">
+      <c r="D294" s="1" t="s">
         <v>611</v>
-      </c>
-      <c r="D294" s="1" t="s">
-        <v>612</v>
       </c>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A295" s="1" t="s">
+        <v>794</v>
+      </c>
+      <c r="B295" s="1" t="s">
         <v>795</v>
       </c>
-      <c r="B295" s="1" t="s">
+      <c r="D295" s="1" t="s">
         <v>796</v>
-      </c>
-      <c r="D295" s="1" t="s">
-        <v>797</v>
       </c>
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A296" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="B296" s="1" t="s">
         <v>583</v>
       </c>
-      <c r="B296" s="1" t="s">
+      <c r="D296" s="1" t="s">
         <v>584</v>
-      </c>
-      <c r="D296" s="1" t="s">
-        <v>585</v>
       </c>
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A297" s="1" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B297" s="1" t="s">
         <v>1013</v>
       </c>
-      <c r="B297" s="1" t="s">
+      <c r="D297" s="1" t="s">
         <v>1014</v>
-      </c>
-      <c r="D297" s="1" t="s">
-        <v>1015</v>
       </c>
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A298" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="B298" s="1" t="s">
         <v>804</v>
       </c>
-      <c r="B298" s="1" t="s">
+      <c r="D298" s="1" t="s">
         <v>805</v>
-      </c>
-      <c r="D298" s="1" t="s">
-        <v>806</v>
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A299" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="B299" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="B299" s="1" t="s">
+      <c r="D299" s="1" t="s">
         <v>458</v>
-      </c>
-      <c r="D299" s="1" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A300" s="1" t="s">
+        <v>839</v>
+      </c>
+      <c r="B300" s="1" t="s">
         <v>840</v>
       </c>
-      <c r="B300" s="1" t="s">
+      <c r="D300" s="1" t="s">
         <v>841</v>
-      </c>
-      <c r="D300" s="1" t="s">
-        <v>842</v>
       </c>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A301" s="1" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B301" s="1" t="s">
         <v>1043</v>
       </c>
-      <c r="B301" s="1" t="s">
+      <c r="D301" s="1" t="s">
         <v>1044</v>
-      </c>
-      <c r="D301" s="1" t="s">
-        <v>1045</v>
       </c>
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A302" s="1" t="s">
+        <v>715</v>
+      </c>
+      <c r="B302" s="1" t="s">
         <v>716</v>
       </c>
-      <c r="B302" s="1" t="s">
+      <c r="D302" s="1" t="s">
         <v>717</v>
-      </c>
-      <c r="D302" s="1" t="s">
-        <v>718</v>
       </c>
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A303" s="1" t="s">
+        <v>718</v>
+      </c>
+      <c r="B303" s="1" t="s">
         <v>719</v>
       </c>
-      <c r="B303" s="1" t="s">
+      <c r="D303" s="1" t="s">
         <v>720</v>
-      </c>
-      <c r="D303" s="1" t="s">
-        <v>721</v>
       </c>
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A304" s="1" t="s">
+        <v>615</v>
+      </c>
+      <c r="B304" s="1" t="s">
         <v>616</v>
       </c>
-      <c r="B304" s="1" t="s">
+      <c r="D304" s="1" t="s">
         <v>617</v>
-      </c>
-      <c r="D304" s="1" t="s">
-        <v>618</v>
       </c>
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A305" s="1" t="s">
+        <v>585</v>
+      </c>
+      <c r="B305" s="1" t="s">
         <v>586</v>
       </c>
-      <c r="B305" s="1" t="s">
+      <c r="D305" s="1" t="s">
         <v>587</v>
-      </c>
-      <c r="D305" s="1" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A306" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="B306" s="1" t="s">
         <v>613</v>
       </c>
-      <c r="B306" s="1" t="s">
+      <c r="D306" s="1" t="s">
         <v>614</v>
-      </c>
-      <c r="D306" s="1" t="s">
-        <v>615</v>
       </c>
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A307" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="B307" s="1" t="s">
         <v>757</v>
       </c>
-      <c r="B307" s="1" t="s">
+      <c r="D307" s="1" t="s">
         <v>758</v>
-      </c>
-      <c r="D307" s="1" t="s">
-        <v>759</v>
       </c>
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A308" s="1" t="s">
+        <v>894</v>
+      </c>
+      <c r="B308" s="1" t="s">
         <v>895</v>
-      </c>
-      <c r="B308" s="1" t="s">
-        <v>896</v>
       </c>
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A309" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="B309" s="1" t="s">
         <v>702</v>
       </c>
-      <c r="B309" s="1" t="s">
+      <c r="D309" s="1" t="s">
         <v>703</v>
-      </c>
-      <c r="D309" s="1" t="s">
-        <v>704</v>
       </c>
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A310" s="1" t="s">
+        <v>683</v>
+      </c>
+      <c r="B310" s="1" t="s">
         <v>684</v>
       </c>
-      <c r="B310" s="1" t="s">
+      <c r="D310" s="1" t="s">
         <v>685</v>
-      </c>
-      <c r="D310" s="1" t="s">
-        <v>686</v>
       </c>
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A311" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="B311" s="1" t="s">
         <v>793</v>
       </c>
-      <c r="B311" s="1" t="s">
-        <v>794</v>
-      </c>
       <c r="D311" s="1" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A312" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="B312" s="1" t="s">
         <v>776</v>
       </c>
-      <c r="B312" s="1" t="s">
-        <v>777</v>
-      </c>
       <c r="D312" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A313" s="1" t="s">
+        <v>833</v>
+      </c>
+      <c r="B313" s="1" t="s">
         <v>834</v>
       </c>
-      <c r="B313" s="1" t="s">
+      <c r="D313" s="1" t="s">
         <v>835</v>
-      </c>
-      <c r="D313" s="1" t="s">
-        <v>836</v>
       </c>
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A314" s="1" t="s">
+        <v>638</v>
+      </c>
+      <c r="B314" s="1" t="s">
         <v>639</v>
       </c>
-      <c r="B314" s="1" t="s">
+      <c r="D314" s="1" t="s">
         <v>640</v>
-      </c>
-      <c r="D314" s="1" t="s">
-        <v>641</v>
       </c>
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A315" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="B315" s="1" t="s">
         <v>553</v>
       </c>
-      <c r="B315" s="1" t="s">
+      <c r="D315" s="1" t="s">
         <v>554</v>
-      </c>
-      <c r="D315" s="1" t="s">
-        <v>555</v>
       </c>
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A316" s="1" t="s">
+        <v>959</v>
+      </c>
+      <c r="B316" s="1" t="s">
         <v>960</v>
       </c>
-      <c r="B316" s="1" t="s">
+      <c r="D316" s="1" t="s">
         <v>961</v>
-      </c>
-      <c r="D316" s="1" t="s">
-        <v>962</v>
       </c>
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A317" s="1" t="s">
+        <v>1031</v>
+      </c>
+      <c r="B317" s="1" t="s">
+        <v>1030</v>
+      </c>
+      <c r="D317" s="1" t="s">
         <v>1032</v>
-      </c>
-      <c r="B317" s="1" t="s">
-        <v>1031</v>
-      </c>
-      <c r="D317" s="1" t="s">
-        <v>1033</v>
       </c>
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A318" s="1" t="s">
+        <v>695</v>
+      </c>
+      <c r="B318" s="1" t="s">
         <v>696</v>
       </c>
-      <c r="B318" s="1" t="s">
+      <c r="D318" s="1" t="s">
         <v>697</v>
-      </c>
-      <c r="D318" s="1" t="s">
-        <v>698</v>
       </c>
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A319" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="B319" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="B319" s="1" t="s">
+      <c r="D319" s="1" t="s">
         <v>679</v>
-      </c>
-      <c r="D319" s="1" t="s">
-        <v>680</v>
       </c>
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A320" s="1" t="s">
+        <v>875</v>
+      </c>
+      <c r="B320" s="1" t="s">
         <v>876</v>
       </c>
-      <c r="B320" s="1" t="s">
+      <c r="D320" s="1" t="s">
         <v>877</v>
-      </c>
-      <c r="D320" s="1" t="s">
-        <v>878</v>
       </c>
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A321" s="1" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="B321" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="D321" s="1" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A322" s="1" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B322" s="1" t="s">
         <v>1010</v>
       </c>
-      <c r="B322" s="1" t="s">
-        <v>1011</v>
-      </c>
       <c r="D322" s="1" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A323" s="1" t="s">
+        <v>886</v>
+      </c>
+      <c r="B323" s="1" t="s">
         <v>887</v>
-      </c>
-      <c r="B323" s="1" t="s">
-        <v>888</v>
       </c>
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A324" s="1" t="s">
+        <v>857</v>
+      </c>
+      <c r="B324" s="1" t="s">
         <v>858</v>
       </c>
-      <c r="B324" s="1" t="s">
+      <c r="D324" s="1" t="s">
         <v>859</v>
-      </c>
-      <c r="D324" s="1" t="s">
-        <v>860</v>
       </c>
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A325" s="1" t="s">
+        <v>884</v>
+      </c>
+      <c r="B325" s="1" t="s">
         <v>885</v>
-      </c>
-      <c r="B325" s="1" t="s">
-        <v>886</v>
       </c>
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A326" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="B326" s="1" t="s">
         <v>754</v>
       </c>
-      <c r="B326" s="1" t="s">
+      <c r="D326" s="1" t="s">
         <v>755</v>
-      </c>
-      <c r="D326" s="1" t="s">
-        <v>756</v>
       </c>
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A327" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="B327" s="1" t="s">
         <v>574</v>
       </c>
-      <c r="B327" s="1" t="s">
+      <c r="D327" s="1" t="s">
         <v>575</v>
-      </c>
-      <c r="D327" s="1" t="s">
-        <v>576</v>
       </c>
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A328" s="1" t="s">
+        <v>777</v>
+      </c>
+      <c r="B328" s="1" t="s">
         <v>778</v>
       </c>
-      <c r="B328" s="1" t="s">
-        <v>779</v>
-      </c>
       <c r="D328" s="1" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A329" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="B329" s="1" t="s">
         <v>511</v>
       </c>
-      <c r="B329" s="1" t="s">
+      <c r="D329" s="1" t="s">
         <v>512</v>
-      </c>
-      <c r="D329" s="1" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A330" s="1" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="B330" s="1" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="D330" s="1" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A331" s="1" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="B331" s="1" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="D331" s="1" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="332" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A332" s="1" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="B332" s="1" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D332" s="1" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A333" s="1" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="B333" s="1" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D333" s="1" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A334" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="B334" s="1" t="s">
         <v>761</v>
       </c>
-      <c r="B334" s="1" t="s">
+      <c r="D334" s="1" t="s">
         <v>762</v>
-      </c>
-      <c r="D334" s="1" t="s">
-        <v>763</v>
       </c>
     </row>
     <row r="335" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A335" s="1" t="s">
+        <v>888</v>
+      </c>
+      <c r="B335" s="1" t="s">
         <v>889</v>
-      </c>
-      <c r="B335" s="1" t="s">
-        <v>890</v>
       </c>
     </row>
     <row r="336" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A336" s="1" t="s">
+        <v>890</v>
+      </c>
+      <c r="B336" s="1" t="s">
         <v>891</v>
-      </c>
-      <c r="B336" s="1" t="s">
-        <v>892</v>
       </c>
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A337" s="1" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="B337" s="1" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="D337" s="1" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.15">
@@ -7472,1360 +7474,1360 @@
         <v>0</v>
       </c>
       <c r="B338" s="1" t="s">
+        <v>710</v>
+      </c>
+      <c r="D338" s="1" t="s">
         <v>711</v>
-      </c>
-      <c r="D338" s="1" t="s">
-        <v>712</v>
       </c>
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A339" s="1" t="s">
+        <v>811</v>
+      </c>
+      <c r="B339" s="1" t="s">
         <v>812</v>
       </c>
-      <c r="B339" s="1" t="s">
-        <v>813</v>
-      </c>
       <c r="D339" s="1" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A340" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="B340" s="1" t="s">
         <v>589</v>
       </c>
-      <c r="B340" s="1" t="s">
+      <c r="D340" s="1" t="s">
         <v>590</v>
-      </c>
-      <c r="D340" s="1" t="s">
-        <v>591</v>
       </c>
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A341" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="B341" s="1" t="s">
         <v>814</v>
       </c>
-      <c r="B341" s="1" t="s">
-        <v>815</v>
-      </c>
       <c r="D341" s="1" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A342" s="1" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="B342" s="1" t="s">
+        <v>941</v>
+      </c>
+      <c r="D342" s="1" t="s">
         <v>942</v>
-      </c>
-      <c r="D342" s="1" t="s">
-        <v>943</v>
       </c>
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A343" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="B343" s="1" t="s">
         <v>807</v>
       </c>
-      <c r="B343" s="1" t="s">
+      <c r="D343" s="1" t="s">
         <v>808</v>
-      </c>
-      <c r="D343" s="1" t="s">
-        <v>809</v>
       </c>
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A344" s="1" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B344" s="1" t="s">
         <v>1072</v>
       </c>
-      <c r="B344" s="1" t="s">
-        <v>1073</v>
-      </c>
       <c r="D344" s="1" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A345" s="1" t="s">
+        <v>869</v>
+      </c>
+      <c r="B345" s="1" t="s">
         <v>870</v>
       </c>
-      <c r="B345" s="1" t="s">
+      <c r="D345" s="1" t="s">
         <v>871</v>
-      </c>
-      <c r="D345" s="1" t="s">
-        <v>872</v>
       </c>
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A346" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="B346" s="1" t="s">
         <v>642</v>
       </c>
-      <c r="B346" s="1" t="s">
+      <c r="D346" s="1" t="s">
         <v>643</v>
-      </c>
-      <c r="D346" s="1" t="s">
-        <v>644</v>
       </c>
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A347" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="B347" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="B347" s="1" t="s">
+      <c r="D347" s="1" t="s">
         <v>530</v>
-      </c>
-      <c r="D347" s="1" t="s">
-        <v>531</v>
       </c>
     </row>
     <row r="348" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A348" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="B348" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="B348" s="1" t="s">
+      <c r="D348" s="1" t="s">
         <v>438</v>
-      </c>
-      <c r="D348" s="1" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A349" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="B349" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="B349" s="1" t="s">
+      <c r="D349" s="1" t="s">
         <v>441</v>
-      </c>
-      <c r="D349" s="1" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A350" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="B350" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="B350" s="1" t="s">
+      <c r="D350" s="1" t="s">
         <v>444</v>
-      </c>
-      <c r="D350" s="1" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="351" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A351" s="1" t="s">
+        <v>809</v>
+      </c>
+      <c r="B351" s="1" t="s">
         <v>810</v>
       </c>
-      <c r="B351" s="1" t="s">
-        <v>811</v>
-      </c>
       <c r="D351" s="1" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A352" s="1" t="s">
+        <v>647</v>
+      </c>
+      <c r="B352" s="1" t="s">
         <v>648</v>
       </c>
-      <c r="B352" s="1" t="s">
+      <c r="D352" s="1" t="s">
         <v>649</v>
-      </c>
-      <c r="D352" s="1" t="s">
-        <v>650</v>
       </c>
     </row>
     <row r="353" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A353" s="1" t="s">
+        <v>929</v>
+      </c>
+      <c r="B353" s="1" t="s">
         <v>930</v>
       </c>
-      <c r="B353" s="1" t="s">
+      <c r="D353" s="1" t="s">
         <v>931</v>
-      </c>
-      <c r="D353" s="1" t="s">
-        <v>932</v>
       </c>
     </row>
     <row r="354" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A354" s="1" t="s">
+        <v>995</v>
+      </c>
+      <c r="B354" s="1" t="s">
         <v>996</v>
       </c>
-      <c r="B354" s="1" t="s">
+      <c r="D354" s="1" t="s">
         <v>997</v>
-      </c>
-      <c r="D354" s="1" t="s">
-        <v>998</v>
       </c>
     </row>
     <row r="355" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A355" s="1" t="s">
+        <v>998</v>
+      </c>
+      <c r="B355" s="1" t="s">
         <v>999</v>
       </c>
-      <c r="B355" s="1" t="s">
+      <c r="D355" s="1" t="s">
         <v>1000</v>
-      </c>
-      <c r="D355" s="1" t="s">
-        <v>1001</v>
       </c>
     </row>
     <row r="356" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A356" s="1" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="B356" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="D356" s="1" t="s">
         <v>731</v>
-      </c>
-      <c r="D356" s="1" t="s">
-        <v>732</v>
       </c>
     </row>
     <row r="357" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A357" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="B357" s="1" t="s">
         <v>855</v>
       </c>
-      <c r="B357" s="1" t="s">
+      <c r="D357" s="1" t="s">
         <v>856</v>
-      </c>
-      <c r="D357" s="1" t="s">
-        <v>857</v>
       </c>
     </row>
     <row r="358" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A358" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="B358" s="1" t="s">
         <v>666</v>
       </c>
-      <c r="B358" s="1" t="s">
+      <c r="D358" s="1" t="s">
         <v>667</v>
-      </c>
-      <c r="D358" s="1" t="s">
-        <v>668</v>
       </c>
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A359" s="1" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="B359" s="1" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="D359" s="1" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A360" s="1" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B360" s="1" t="s">
         <v>1002</v>
       </c>
-      <c r="B360" s="1" t="s">
+      <c r="D360" s="1" t="s">
         <v>1003</v>
-      </c>
-      <c r="D360" s="1" t="s">
-        <v>1004</v>
       </c>
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A361" s="1" t="s">
+        <v>1006</v>
+      </c>
+      <c r="B361" s="1" t="s">
         <v>1007</v>
       </c>
-      <c r="B361" s="1" t="s">
+      <c r="D361" s="1" t="s">
         <v>1008</v>
-      </c>
-      <c r="D361" s="1" t="s">
-        <v>1009</v>
       </c>
     </row>
     <row r="362" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A362" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="B362" s="1" t="s">
         <v>1022</v>
       </c>
-      <c r="B362" s="1" t="s">
+      <c r="D362" s="1" t="s">
         <v>1023</v>
-      </c>
-      <c r="D362" s="1" t="s">
-        <v>1024</v>
       </c>
     </row>
     <row r="363" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A363" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="B363" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="B363" s="1" t="s">
+      <c r="D363" s="1" t="s">
         <v>432</v>
-      </c>
-      <c r="D363" s="1" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="364" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A364" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="B364" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="B364" s="1" t="s">
+      <c r="D364" s="1" t="s">
         <v>435</v>
-      </c>
-      <c r="D364" s="1" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="365" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A365" s="1" t="s">
+        <v>600</v>
+      </c>
+      <c r="B365" s="1" t="s">
         <v>601</v>
       </c>
-      <c r="B365" s="1" t="s">
+      <c r="D365" s="1" t="s">
         <v>602</v>
-      </c>
-      <c r="D365" s="1" t="s">
-        <v>603</v>
       </c>
     </row>
     <row r="366" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A366" s="1" t="s">
+        <v>594</v>
+      </c>
+      <c r="B366" s="1" t="s">
         <v>595</v>
       </c>
-      <c r="B366" s="1" t="s">
+      <c r="D366" s="1" t="s">
         <v>596</v>
-      </c>
-      <c r="D366" s="1" t="s">
-        <v>597</v>
       </c>
     </row>
     <row r="367" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A367" s="1" t="s">
+        <v>671</v>
+      </c>
+      <c r="B367" s="1" t="s">
         <v>672</v>
       </c>
-      <c r="B367" s="1" t="s">
+      <c r="D367" s="1" t="s">
         <v>673</v>
-      </c>
-      <c r="D367" s="1" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="368" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A368" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="B368" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="B368" s="1" t="s">
-        <v>447</v>
-      </c>
       <c r="D368" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="369" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A369" s="1" t="s">
+        <v>597</v>
+      </c>
+      <c r="B369" s="1" t="s">
         <v>598</v>
       </c>
-      <c r="B369" s="1" t="s">
+      <c r="D369" s="1" t="s">
         <v>599</v>
-      </c>
-      <c r="D369" s="1" t="s">
-        <v>600</v>
       </c>
     </row>
     <row r="370" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A370" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="B370" s="1" t="s">
         <v>544</v>
       </c>
-      <c r="B370" s="1" t="s">
+      <c r="D370" s="1" t="s">
         <v>545</v>
-      </c>
-      <c r="D370" s="1" t="s">
-        <v>546</v>
       </c>
     </row>
     <row r="371" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A371" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="B371" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="B371" s="1" t="s">
+      <c r="D371" s="1" t="s">
         <v>467</v>
-      </c>
-      <c r="D371" s="1" t="s">
-        <v>468</v>
       </c>
     </row>
     <row r="372" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A372" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="B372" s="1" t="s">
         <v>621</v>
       </c>
-      <c r="B372" s="1" t="s">
+      <c r="D372" s="1" t="s">
         <v>622</v>
-      </c>
-      <c r="D372" s="1" t="s">
-        <v>623</v>
       </c>
     </row>
     <row r="373" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A373" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B373" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="B373" s="1" t="s">
+      <c r="D373" s="1" t="s">
         <v>405</v>
-      </c>
-      <c r="D373" s="1" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="374" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A374" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="B374" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="B374" s="1" t="s">
+      <c r="D374" s="1" t="s">
         <v>408</v>
-      </c>
-      <c r="D374" s="1" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="375" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A375" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B375" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="B375" s="1" t="s">
+      <c r="D375" s="1" t="s">
         <v>411</v>
-      </c>
-      <c r="D375" s="1" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="376" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A376" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="B376" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="B376" s="1" t="s">
+      <c r="D376" s="1" t="s">
         <v>414</v>
-      </c>
-      <c r="D376" s="1" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="377" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A377" s="1" t="s">
+        <v>848</v>
+      </c>
+      <c r="B377" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="B377" s="1" t="s">
+      <c r="D377" s="1" t="s">
         <v>850</v>
-      </c>
-      <c r="D377" s="1" t="s">
-        <v>851</v>
       </c>
     </row>
     <row r="378" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A378" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="B378" s="1" t="s">
         <v>828</v>
       </c>
-      <c r="B378" s="1" t="s">
+      <c r="D378" s="1" t="s">
         <v>829</v>
-      </c>
-      <c r="D378" s="1" t="s">
-        <v>830</v>
       </c>
     </row>
     <row r="379" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A379" s="1" t="s">
+        <v>830</v>
+      </c>
+      <c r="B379" s="1" t="s">
         <v>831</v>
       </c>
-      <c r="B379" s="1" t="s">
+      <c r="D379" s="1" t="s">
         <v>832</v>
-      </c>
-      <c r="D379" s="1" t="s">
-        <v>833</v>
       </c>
     </row>
     <row r="380" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A380" s="1" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="B380" s="1" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="D380" s="1" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="381" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A381" s="1" t="s">
+        <v>727</v>
+      </c>
+      <c r="B381" s="1" t="s">
         <v>728</v>
       </c>
-      <c r="B381" s="1" t="s">
+      <c r="D381" s="1" t="s">
         <v>729</v>
-      </c>
-      <c r="D381" s="1" t="s">
-        <v>730</v>
       </c>
     </row>
     <row r="382" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A382" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="B382" s="1" t="s">
         <v>725</v>
       </c>
-      <c r="B382" s="1" t="s">
+      <c r="D382" s="1" t="s">
         <v>726</v>
-      </c>
-      <c r="D382" s="1" t="s">
-        <v>727</v>
       </c>
     </row>
     <row r="383" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A383" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="B383" s="1" t="s">
         <v>517</v>
       </c>
-      <c r="B383" s="1" t="s">
+      <c r="D383" s="1" t="s">
         <v>518</v>
-      </c>
-      <c r="D383" s="1" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="384" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A384" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="B384" s="1" t="s">
         <v>592</v>
       </c>
-      <c r="B384" s="1" t="s">
+      <c r="D384" s="1" t="s">
         <v>593</v>
-      </c>
-      <c r="D384" s="1" t="s">
-        <v>594</v>
       </c>
     </row>
     <row r="385" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A385" s="1" t="s">
+        <v>674</v>
+      </c>
+      <c r="B385" s="1" t="s">
         <v>675</v>
       </c>
-      <c r="B385" s="1" t="s">
+      <c r="D385" s="1" t="s">
         <v>676</v>
-      </c>
-      <c r="D385" s="1" t="s">
-        <v>677</v>
       </c>
     </row>
     <row r="386" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A386" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="B386" s="1" t="s">
         <v>655</v>
       </c>
-      <c r="B386" s="1" t="s">
-        <v>656</v>
-      </c>
       <c r="D386" s="1" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="387" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A387" s="1" t="s">
+        <v>1045</v>
+      </c>
+      <c r="B387" s="1" t="s">
         <v>1046</v>
       </c>
-      <c r="B387" s="1" t="s">
+      <c r="D387" s="1" t="s">
         <v>1047</v>
-      </c>
-      <c r="D387" s="1" t="s">
-        <v>1048</v>
       </c>
     </row>
     <row r="388" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A388" s="1" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B388" s="1" t="s">
+        <v>1027</v>
+      </c>
+      <c r="D388" s="1" t="s">
         <v>1029</v>
-      </c>
-      <c r="B388" s="1" t="s">
-        <v>1028</v>
-      </c>
-      <c r="D388" s="1" t="s">
-        <v>1030</v>
       </c>
     </row>
     <row r="389" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A389" s="1" t="s">
+        <v>842</v>
+      </c>
+      <c r="B389" s="1" t="s">
         <v>843</v>
       </c>
-      <c r="B389" s="1" t="s">
+      <c r="D389" s="1" t="s">
         <v>844</v>
-      </c>
-      <c r="D389" s="1" t="s">
-        <v>845</v>
       </c>
     </row>
     <row r="390" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A390" s="1" t="s">
+        <v>866</v>
+      </c>
+      <c r="B390" s="1" t="s">
         <v>867</v>
       </c>
-      <c r="B390" s="1" t="s">
+      <c r="D390" s="1" t="s">
         <v>868</v>
-      </c>
-      <c r="D390" s="1" t="s">
-        <v>869</v>
       </c>
     </row>
     <row r="391" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A391" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="B391" s="1" t="s">
         <v>472</v>
       </c>
-      <c r="B391" s="1" t="s">
+      <c r="D391" s="1" t="s">
         <v>473</v>
-      </c>
-      <c r="D391" s="1" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="392" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A392" s="1" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="B392" s="1" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D392" s="1" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="393" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A393" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="B393" s="1" t="s">
         <v>559</v>
       </c>
-      <c r="B393" s="1" t="s">
+      <c r="D393" s="1" t="s">
         <v>560</v>
-      </c>
-      <c r="D393" s="1" t="s">
-        <v>561</v>
       </c>
     </row>
     <row r="394" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A394" s="1" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="B394" s="1" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D394" s="1" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="395" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A395" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="B395" s="1" t="s">
         <v>496</v>
       </c>
-      <c r="B395" s="1" t="s">
+      <c r="D395" s="1" t="s">
         <v>497</v>
-      </c>
-      <c r="D395" s="1" t="s">
-        <v>498</v>
       </c>
     </row>
     <row r="396" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A396" s="1" t="s">
+        <v>991</v>
+      </c>
+      <c r="B396" s="1" t="s">
         <v>992</v>
       </c>
-      <c r="B396" s="1" t="s">
+      <c r="D396" s="1" t="s">
         <v>993</v>
-      </c>
-      <c r="D396" s="1" t="s">
-        <v>994</v>
       </c>
     </row>
     <row r="397" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A397" s="1" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="B397" s="1" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="D397" s="1" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="398" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A398" s="1" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="B398" s="1" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="D398" s="1" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="399" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A399" s="1" t="s">
+        <v>901</v>
+      </c>
+      <c r="B399" s="1" t="s">
         <v>902</v>
       </c>
-      <c r="B399" s="1" t="s">
+      <c r="D399" s="1" t="s">
         <v>903</v>
-      </c>
-      <c r="D399" s="1" t="s">
-        <v>904</v>
       </c>
     </row>
     <row r="400" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A400" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="B400" s="1" t="s">
         <v>481</v>
       </c>
-      <c r="B400" s="1" t="s">
+      <c r="D400" s="1" t="s">
         <v>482</v>
-      </c>
-      <c r="D400" s="1" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="401" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A401" s="1" t="s">
+        <v>1073</v>
+      </c>
+      <c r="B401" s="1" t="s">
         <v>1074</v>
       </c>
-      <c r="B401" s="1" t="s">
-        <v>1075</v>
-      </c>
       <c r="D401" s="1" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="402" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A402" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="B402" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="B402" s="1" t="s">
+      <c r="D402" s="1" t="s">
         <v>500</v>
-      </c>
-      <c r="D402" s="1" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="403" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A403" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="B403" s="1" t="s">
         <v>484</v>
       </c>
-      <c r="B403" s="1" t="s">
+      <c r="D403" s="1" t="s">
         <v>485</v>
-      </c>
-      <c r="D403" s="1" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="404" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A404" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="B404" s="1" t="s">
         <v>487</v>
       </c>
-      <c r="B404" s="1" t="s">
+      <c r="D404" s="1" t="s">
         <v>488</v>
-      </c>
-      <c r="D404" s="1" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="405" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A405" s="1" t="s">
+        <v>944</v>
+      </c>
+      <c r="B405" s="1" t="s">
         <v>945</v>
       </c>
-      <c r="B405" s="1" t="s">
+      <c r="D405" s="1" t="s">
         <v>946</v>
-      </c>
-      <c r="D405" s="1" t="s">
-        <v>947</v>
       </c>
     </row>
     <row r="406" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A406" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="B406" s="1" t="s">
         <v>705</v>
       </c>
-      <c r="B406" s="1" t="s">
+      <c r="D406" s="1" t="s">
         <v>706</v>
-      </c>
-      <c r="D406" s="1" t="s">
-        <v>707</v>
       </c>
     </row>
     <row r="407" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A407" s="1" t="s">
+        <v>800</v>
+      </c>
+      <c r="B407" s="1" t="s">
         <v>801</v>
       </c>
-      <c r="B407" s="1" t="s">
+      <c r="D407" s="1" t="s">
         <v>802</v>
-      </c>
-      <c r="D407" s="1" t="s">
-        <v>803</v>
       </c>
     </row>
     <row r="408" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A408" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="B408" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="B408" s="1" t="s">
+      <c r="D408" s="1" t="s">
         <v>533</v>
-      </c>
-      <c r="D408" s="1" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="409" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A409" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="B409" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="B409" s="1" t="s">
+      <c r="D409" s="1" t="s">
         <v>503</v>
-      </c>
-      <c r="D409" s="1" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="410" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A410" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="B410" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="B410" s="1" t="s">
+      <c r="D410" s="1" t="s">
         <v>417</v>
-      </c>
-      <c r="D410" s="1" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="411" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A411" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="B411" s="1" t="s">
         <v>505</v>
       </c>
-      <c r="B411" s="1" t="s">
+      <c r="D411" s="1" t="s">
         <v>506</v>
-      </c>
-      <c r="D411" s="1" t="s">
-        <v>507</v>
       </c>
     </row>
     <row r="412" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A412" s="1" t="s">
+        <v>721</v>
+      </c>
+      <c r="B412" s="1" t="s">
         <v>722</v>
       </c>
-      <c r="B412" s="1" t="s">
+      <c r="D412" s="1" t="s">
         <v>723</v>
-      </c>
-      <c r="D412" s="1" t="s">
-        <v>724</v>
       </c>
     </row>
     <row r="413" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A413" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="B413" s="1" t="s">
         <v>556</v>
       </c>
-      <c r="B413" s="1" t="s">
+      <c r="D413" s="1" t="s">
         <v>557</v>
-      </c>
-      <c r="D413" s="1" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="414" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A414" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="B414" s="1" t="s">
         <v>562</v>
       </c>
-      <c r="B414" s="1" t="s">
+      <c r="D414" s="1" t="s">
         <v>563</v>
-      </c>
-      <c r="D414" s="1" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="415" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A415" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="B415" s="1" t="s">
         <v>550</v>
       </c>
-      <c r="B415" s="1" t="s">
+      <c r="D415" s="1" t="s">
         <v>551</v>
-      </c>
-      <c r="D415" s="1" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="416" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A416" s="1" t="s">
+        <v>763</v>
+      </c>
+      <c r="B416" s="1" t="s">
         <v>764</v>
       </c>
-      <c r="B416" s="1" t="s">
-        <v>765</v>
-      </c>
       <c r="D416" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="417" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A417" s="1" t="s">
+        <v>618</v>
+      </c>
+      <c r="B417" s="1" t="s">
         <v>619</v>
       </c>
-      <c r="B417" s="1" t="s">
-        <v>620</v>
-      </c>
       <c r="D417" s="1" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="418" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A418" s="1" t="s">
+        <v>606</v>
+      </c>
+      <c r="B418" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="B418" s="1" t="s">
+      <c r="D418" s="1" t="s">
         <v>608</v>
-      </c>
-      <c r="D418" s="1" t="s">
-        <v>609</v>
       </c>
     </row>
     <row r="419" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A419" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="B419" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="B419" s="1" t="s">
+      <c r="D419" s="1" t="s">
         <v>452</v>
-      </c>
-      <c r="D419" s="1" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="420" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A420" s="1" t="s">
+        <v>689</v>
+      </c>
+      <c r="B420" s="1" t="s">
         <v>690</v>
       </c>
-      <c r="B420" s="1" t="s">
+      <c r="D420" s="1" t="s">
         <v>691</v>
-      </c>
-      <c r="D420" s="1" t="s">
-        <v>692</v>
       </c>
     </row>
     <row r="421" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A421" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="B421" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="B421" s="1" t="s">
+      <c r="D421" s="1" t="s">
         <v>455</v>
-      </c>
-      <c r="D421" s="1" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="422" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A422" s="1" t="s">
+        <v>765</v>
+      </c>
+      <c r="B422" s="1" t="s">
         <v>766</v>
       </c>
-      <c r="B422" s="1" t="s">
+      <c r="D422" s="1" t="s">
         <v>767</v>
-      </c>
-      <c r="D422" s="1" t="s">
-        <v>768</v>
       </c>
     </row>
     <row r="423" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A423" s="1" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B423" s="1" t="s">
         <v>1052</v>
       </c>
-      <c r="B423" s="1" t="s">
+      <c r="D423" s="1" t="s">
         <v>1053</v>
-      </c>
-      <c r="D423" s="1" t="s">
-        <v>1054</v>
       </c>
     </row>
     <row r="424" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A424" s="1" t="s">
+        <v>821</v>
+      </c>
+      <c r="B424" s="1" t="s">
         <v>822</v>
       </c>
-      <c r="B424" s="1" t="s">
+      <c r="D424" s="1" t="s">
         <v>823</v>
-      </c>
-      <c r="D424" s="1" t="s">
-        <v>824</v>
       </c>
     </row>
     <row r="425" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A425" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="B425" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="B425" s="1" t="s">
+      <c r="D425" s="1" t="s">
         <v>423</v>
-      </c>
-      <c r="D425" s="1" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="426" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A426" s="1" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B426" s="1" t="s">
         <v>1017</v>
       </c>
-      <c r="B426" s="1" t="s">
+      <c r="D426" s="1" t="s">
         <v>1018</v>
-      </c>
-      <c r="D426" s="1" t="s">
-        <v>1019</v>
       </c>
     </row>
     <row r="427" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A427" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="B427" s="1" t="s">
         <v>745</v>
       </c>
-      <c r="B427" s="1" t="s">
+      <c r="D427" s="1" t="s">
         <v>746</v>
-      </c>
-      <c r="D427" s="1" t="s">
-        <v>747</v>
       </c>
     </row>
     <row r="428" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A428" s="1" t="s">
+        <v>905</v>
+      </c>
+      <c r="B428" s="1" t="s">
+        <v>904</v>
+      </c>
+      <c r="D428" s="1" t="s">
         <v>906</v>
-      </c>
-      <c r="B428" s="1" t="s">
-        <v>905</v>
-      </c>
-      <c r="D428" s="1" t="s">
-        <v>907</v>
       </c>
     </row>
     <row r="429" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A429" s="1" t="s">
+        <v>907</v>
+      </c>
+      <c r="B429" s="1" t="s">
         <v>908</v>
       </c>
-      <c r="B429" s="1" t="s">
+      <c r="D429" s="1" t="s">
         <v>909</v>
-      </c>
-      <c r="D429" s="1" t="s">
-        <v>910</v>
       </c>
     </row>
     <row r="430" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A430" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="B430" s="1" t="s">
         <v>541</v>
       </c>
-      <c r="B430" s="1" t="s">
+      <c r="D430" s="1" t="s">
         <v>542</v>
-      </c>
-      <c r="D430" s="1" t="s">
-        <v>543</v>
       </c>
     </row>
     <row r="431" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A431" s="1" t="s">
+        <v>662</v>
+      </c>
+      <c r="B431" s="1" t="s">
         <v>663</v>
       </c>
-      <c r="B431" s="1" t="s">
+      <c r="D431" s="1" t="s">
         <v>664</v>
-      </c>
-      <c r="D431" s="1" t="s">
-        <v>665</v>
       </c>
     </row>
     <row r="432" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A432" s="1" t="s">
+        <v>692</v>
+      </c>
+      <c r="B432" s="1" t="s">
         <v>693</v>
       </c>
-      <c r="B432" s="1" t="s">
+      <c r="D432" s="1" t="s">
         <v>694</v>
-      </c>
-      <c r="D432" s="1" t="s">
-        <v>695</v>
       </c>
     </row>
     <row r="433" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A433" s="1" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="B433" s="1" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="D433" s="1" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="434" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A434" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B434" s="1" t="s">
         <v>787</v>
       </c>
-      <c r="B434" s="1" t="s">
+      <c r="D434" s="1" t="s">
         <v>788</v>
-      </c>
-      <c r="D434" s="1" t="s">
-        <v>789</v>
       </c>
     </row>
     <row r="435" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A435" s="1" t="s">
+        <v>623</v>
+      </c>
+      <c r="B435" s="1" t="s">
         <v>624</v>
       </c>
-      <c r="B435" s="1" t="s">
+      <c r="D435" s="1" t="s">
         <v>625</v>
-      </c>
-      <c r="D435" s="1" t="s">
-        <v>626</v>
       </c>
     </row>
     <row r="436" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A436" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="B436" s="1" t="s">
         <v>837</v>
       </c>
-      <c r="B436" s="1" t="s">
+      <c r="D436" s="1" t="s">
         <v>838</v>
-      </c>
-      <c r="D436" s="1" t="s">
-        <v>839</v>
       </c>
     </row>
     <row r="437" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A437" s="1" t="s">
+        <v>686</v>
+      </c>
+      <c r="B437" s="1" t="s">
         <v>687</v>
       </c>
-      <c r="B437" s="1" t="s">
+      <c r="D437" s="1" t="s">
         <v>688</v>
-      </c>
-      <c r="D437" s="1" t="s">
-        <v>689</v>
       </c>
     </row>
     <row r="438" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A438" s="1" t="s">
+        <v>896</v>
+      </c>
+      <c r="B438" s="1" t="s">
         <v>897</v>
-      </c>
-      <c r="B438" s="1" t="s">
-        <v>898</v>
       </c>
     </row>
     <row r="439" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A439" s="1" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="B439" s="1" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="D439" s="1" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="440" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A440" s="1" t="s">
+        <v>950</v>
+      </c>
+      <c r="B440" s="1" t="s">
         <v>951</v>
       </c>
-      <c r="B440" s="1" t="s">
+      <c r="D440" s="1" t="s">
         <v>952</v>
-      </c>
-      <c r="D440" s="1" t="s">
-        <v>953</v>
       </c>
     </row>
     <row r="441" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A441" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="B441" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="B441" s="1" t="s">
+      <c r="D441" s="1" t="s">
         <v>476</v>
-      </c>
-      <c r="D441" s="1" t="s">
-        <v>477</v>
       </c>
     </row>
     <row r="442" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A442" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="B442" s="1" t="s">
         <v>568</v>
       </c>
-      <c r="B442" s="1" t="s">
+      <c r="D442" s="1" t="s">
         <v>569</v>
-      </c>
-      <c r="D442" s="1" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="443" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A443" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="B443" s="1" t="s">
         <v>769</v>
       </c>
-      <c r="B443" s="1" t="s">
+      <c r="D443" s="1" t="s">
         <v>770</v>
-      </c>
-      <c r="D443" s="1" t="s">
-        <v>771</v>
       </c>
     </row>
     <row r="444" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A444" s="1" t="s">
+        <v>771</v>
+      </c>
+      <c r="B444" s="1" t="s">
         <v>772</v>
       </c>
-      <c r="B444" s="1" t="s">
-        <v>773</v>
-      </c>
       <c r="D444" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="445" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A445" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="B445" s="1" t="s">
         <v>713</v>
       </c>
-      <c r="B445" s="1" t="s">
+      <c r="D445" s="1" t="s">
         <v>714</v>
-      </c>
-      <c r="D445" s="1" t="s">
-        <v>715</v>
       </c>
     </row>
     <row r="446" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A446" s="1" t="s">
+        <v>881</v>
+      </c>
+      <c r="B446" s="1" t="s">
         <v>882</v>
       </c>
-      <c r="B446" s="1" t="s">
+      <c r="D446" s="1" t="s">
         <v>883</v>
-      </c>
-      <c r="D446" s="1" t="s">
-        <v>884</v>
       </c>
     </row>
     <row r="447" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A447" s="1" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B447" s="1" t="s">
         <v>1148</v>
       </c>
-      <c r="B447" s="1" t="s">
-        <v>1149</v>
-      </c>
       <c r="D447" s="1" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="448" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A448" s="1" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="B448" s="1" t="s">
+        <v>955</v>
+      </c>
+      <c r="D448" s="1" t="s">
         <v>956</v>
-      </c>
-      <c r="D448" s="1" t="s">
-        <v>957</v>
       </c>
     </row>
     <row r="449" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A449" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="B449" s="1" t="s">
         <v>748</v>
       </c>
-      <c r="B449" s="1" t="s">
+      <c r="D449" s="1" t="s">
         <v>749</v>
-      </c>
-      <c r="D449" s="1" t="s">
-        <v>750</v>
       </c>
     </row>
     <row r="450" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A450" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="B450" s="1" t="s">
         <v>577</v>
       </c>
-      <c r="B450" s="1" t="s">
+      <c r="D450" s="1" t="s">
         <v>578</v>
-      </c>
-      <c r="D450" s="1" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="451" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A451" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="B451" s="1" t="s">
         <v>825</v>
       </c>
-      <c r="B451" s="1" t="s">
+      <c r="D451" s="1" t="s">
         <v>826</v>
-      </c>
-      <c r="D451" s="1" t="s">
-        <v>827</v>
       </c>
     </row>
     <row r="452" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A452" s="1" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B452" s="1" t="s">
         <v>1025</v>
       </c>
-      <c r="B452" s="1" t="s">
+      <c r="D452" s="1" t="s">
         <v>1026</v>
-      </c>
-      <c r="D452" s="1" t="s">
-        <v>1027</v>
       </c>
     </row>
     <row r="453" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A453" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="B453" s="1" t="s">
         <v>428</v>
       </c>
-      <c r="B453" s="1" t="s">
+      <c r="D453" s="1" t="s">
         <v>429</v>
-      </c>
-      <c r="D453" s="1" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="454" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A454" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="B454" s="1" t="s">
         <v>627</v>
       </c>
-      <c r="B454" s="1" t="s">
+      <c r="D454" s="1" t="s">
         <v>628</v>
-      </c>
-      <c r="D454" s="1" t="s">
-        <v>629</v>
       </c>
     </row>
     <row r="455" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A455" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="B455" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="B455" s="1" t="s">
+      <c r="D455" s="1" t="s">
         <v>420</v>
-      </c>
-      <c r="D455" s="1" t="s">
-        <v>421</v>
       </c>
     </row>
     <row r="456" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A456" s="1" t="s">
+        <v>932</v>
+      </c>
+      <c r="B456" s="1" t="s">
         <v>933</v>
       </c>
-      <c r="B456" s="1" t="s">
+      <c r="D456" s="1" t="s">
         <v>934</v>
-      </c>
-      <c r="D456" s="1" t="s">
-        <v>935</v>
       </c>
     </row>
     <row r="457" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A457" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="B457" s="1" t="s">
         <v>736</v>
       </c>
-      <c r="B457" s="1" t="s">
+      <c r="D457" s="1" t="s">
         <v>737</v>
-      </c>
-      <c r="D457" s="1" t="s">
-        <v>738</v>
       </c>
     </row>
     <row r="458" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A458" s="1" t="s">
+        <v>738</v>
+      </c>
+      <c r="B458" s="1" t="s">
         <v>739</v>
       </c>
-      <c r="B458" s="1" t="s">
+      <c r="D458" s="1" t="s">
         <v>740</v>
-      </c>
-      <c r="D458" s="1" t="s">
-        <v>741</v>
       </c>
     </row>
     <row r="459" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A459" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="B459" s="1" t="s">
         <v>742</v>
       </c>
-      <c r="B459" s="1" t="s">
+      <c r="D459" s="1" t="s">
         <v>743</v>
-      </c>
-      <c r="D459" s="1" t="s">
-        <v>744</v>
       </c>
     </row>
     <row r="460" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A460" s="1" t="s">
+        <v>629</v>
+      </c>
+      <c r="B460" s="1" t="s">
         <v>630</v>
       </c>
-      <c r="B460" s="1" t="s">
+      <c r="D460" s="1" t="s">
         <v>631</v>
-      </c>
-      <c r="D460" s="1" t="s">
-        <v>632</v>
       </c>
     </row>
     <row r="461" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A461" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="B461" s="1" t="s">
         <v>633</v>
       </c>
-      <c r="B461" s="1" t="s">
+      <c r="D461" s="1" t="s">
         <v>634</v>
-      </c>
-      <c r="D461" s="1" t="s">
-        <v>635</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working for SecurityHeadersFilter 5
</commit_message>
<xml_diff>
--- a/conf/messages.xlsx
+++ b/conf/messages.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1212" uniqueCount="1160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1215" uniqueCount="1163">
   <si>
     <t>key</t>
   </si>
@@ -3851,6 +3851,21 @@
   </si>
   <si>
     <t>ja-JP</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>写真</t>
+    <rPh sb="0" eb="2">
+      <t>シャシn</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>photo</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Photo</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -4325,10 +4340,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G461"/>
+  <dimension ref="A1:G462"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A163" sqref="A163:XFD163"/>
+    <sheetView tabSelected="1" topLeftCell="A368" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E388" sqref="E388"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -7944,395 +7959,395 @@
     </row>
     <row r="381" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A381" s="1" t="s">
-        <v>727</v>
+        <v>1161</v>
       </c>
       <c r="B381" s="1" t="s">
-        <v>728</v>
+        <v>1162</v>
       </c>
       <c r="D381" s="1" t="s">
-        <v>729</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="382" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A382" s="1" t="s">
-        <v>724</v>
+        <v>727</v>
       </c>
       <c r="B382" s="1" t="s">
-        <v>725</v>
+        <v>728</v>
       </c>
       <c r="D382" s="1" t="s">
-        <v>726</v>
+        <v>729</v>
       </c>
     </row>
     <row r="383" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A383" s="1" t="s">
-        <v>516</v>
+        <v>724</v>
       </c>
       <c r="B383" s="1" t="s">
-        <v>517</v>
+        <v>725</v>
       </c>
       <c r="D383" s="1" t="s">
-        <v>518</v>
+        <v>726</v>
       </c>
     </row>
     <row r="384" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A384" s="1" t="s">
-        <v>591</v>
+        <v>516</v>
       </c>
       <c r="B384" s="1" t="s">
-        <v>592</v>
+        <v>517</v>
       </c>
       <c r="D384" s="1" t="s">
-        <v>593</v>
+        <v>518</v>
       </c>
     </row>
     <row r="385" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A385" s="1" t="s">
-        <v>674</v>
+        <v>591</v>
       </c>
       <c r="B385" s="1" t="s">
-        <v>675</v>
+        <v>592</v>
       </c>
       <c r="D385" s="1" t="s">
-        <v>676</v>
+        <v>593</v>
       </c>
     </row>
     <row r="386" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A386" s="1" t="s">
-        <v>654</v>
+        <v>674</v>
       </c>
       <c r="B386" s="1" t="s">
-        <v>655</v>
+        <v>675</v>
       </c>
       <c r="D386" s="1" t="s">
-        <v>1035</v>
+        <v>676</v>
       </c>
     </row>
     <row r="387" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A387" s="1" t="s">
-        <v>1045</v>
+        <v>654</v>
       </c>
       <c r="B387" s="1" t="s">
-        <v>1046</v>
+        <v>655</v>
       </c>
       <c r="D387" s="1" t="s">
-        <v>1047</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="388" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A388" s="1" t="s">
-        <v>1028</v>
+        <v>1045</v>
       </c>
       <c r="B388" s="1" t="s">
-        <v>1027</v>
+        <v>1046</v>
       </c>
       <c r="D388" s="1" t="s">
-        <v>1029</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="389" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A389" s="1" t="s">
-        <v>842</v>
+        <v>1028</v>
       </c>
       <c r="B389" s="1" t="s">
-        <v>843</v>
+        <v>1027</v>
       </c>
       <c r="D389" s="1" t="s">
-        <v>844</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="390" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A390" s="1" t="s">
-        <v>866</v>
+        <v>842</v>
       </c>
       <c r="B390" s="1" t="s">
-        <v>867</v>
+        <v>843</v>
       </c>
       <c r="D390" s="1" t="s">
-        <v>868</v>
+        <v>844</v>
       </c>
     </row>
     <row r="391" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A391" s="1" t="s">
-        <v>471</v>
+        <v>866</v>
       </c>
       <c r="B391" s="1" t="s">
-        <v>472</v>
+        <v>867</v>
       </c>
       <c r="D391" s="1" t="s">
-        <v>473</v>
+        <v>868</v>
       </c>
     </row>
     <row r="392" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A392" s="1" t="s">
-        <v>975</v>
+        <v>471</v>
       </c>
       <c r="B392" s="1" t="s">
-        <v>922</v>
+        <v>472</v>
       </c>
       <c r="D392" s="1" t="s">
-        <v>1004</v>
+        <v>473</v>
       </c>
     </row>
     <row r="393" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A393" s="1" t="s">
-        <v>558</v>
+        <v>975</v>
       </c>
       <c r="B393" s="1" t="s">
-        <v>559</v>
+        <v>922</v>
       </c>
       <c r="D393" s="1" t="s">
-        <v>560</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="394" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A394" s="1" t="s">
-        <v>972</v>
+        <v>558</v>
       </c>
       <c r="B394" s="1" t="s">
-        <v>921</v>
+        <v>559</v>
       </c>
       <c r="D394" s="1" t="s">
-        <v>974</v>
+        <v>560</v>
       </c>
     </row>
     <row r="395" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A395" s="1" t="s">
-        <v>495</v>
+        <v>972</v>
       </c>
       <c r="B395" s="1" t="s">
-        <v>496</v>
+        <v>921</v>
       </c>
       <c r="D395" s="1" t="s">
-        <v>497</v>
+        <v>974</v>
       </c>
     </row>
     <row r="396" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A396" s="1" t="s">
-        <v>991</v>
+        <v>495</v>
       </c>
       <c r="B396" s="1" t="s">
-        <v>992</v>
+        <v>496</v>
       </c>
       <c r="D396" s="1" t="s">
-        <v>993</v>
+        <v>497</v>
       </c>
     </row>
     <row r="397" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A397" s="1" t="s">
-        <v>983</v>
+        <v>991</v>
       </c>
       <c r="B397" s="1" t="s">
-        <v>919</v>
+        <v>992</v>
       </c>
       <c r="D397" s="1" t="s">
-        <v>976</v>
+        <v>993</v>
       </c>
     </row>
     <row r="398" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A398" s="1" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="B398" s="1" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="D398" s="1" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="399" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A399" s="1" t="s">
-        <v>901</v>
+        <v>982</v>
       </c>
       <c r="B399" s="1" t="s">
-        <v>902</v>
+        <v>918</v>
       </c>
       <c r="D399" s="1" t="s">
-        <v>903</v>
+        <v>977</v>
       </c>
     </row>
     <row r="400" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A400" s="1" t="s">
-        <v>480</v>
+        <v>901</v>
       </c>
       <c r="B400" s="1" t="s">
-        <v>481</v>
+        <v>902</v>
       </c>
       <c r="D400" s="1" t="s">
-        <v>482</v>
+        <v>903</v>
       </c>
     </row>
     <row r="401" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A401" s="1" t="s">
-        <v>1073</v>
+        <v>480</v>
       </c>
       <c r="B401" s="1" t="s">
-        <v>1074</v>
+        <v>481</v>
       </c>
       <c r="D401" s="1" t="s">
-        <v>1014</v>
+        <v>482</v>
       </c>
     </row>
     <row r="402" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A402" s="1" t="s">
-        <v>498</v>
+        <v>1073</v>
       </c>
       <c r="B402" s="1" t="s">
-        <v>499</v>
+        <v>1074</v>
       </c>
       <c r="D402" s="1" t="s">
-        <v>500</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="403" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A403" s="1" t="s">
-        <v>483</v>
+        <v>498</v>
       </c>
       <c r="B403" s="1" t="s">
-        <v>484</v>
+        <v>499</v>
       </c>
       <c r="D403" s="1" t="s">
-        <v>485</v>
+        <v>500</v>
       </c>
     </row>
     <row r="404" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A404" s="1" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="B404" s="1" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="D404" s="1" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
     </row>
     <row r="405" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A405" s="1" t="s">
-        <v>944</v>
+        <v>486</v>
       </c>
       <c r="B405" s="1" t="s">
-        <v>945</v>
+        <v>487</v>
       </c>
       <c r="D405" s="1" t="s">
-        <v>946</v>
+        <v>488</v>
       </c>
     </row>
     <row r="406" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A406" s="1" t="s">
-        <v>704</v>
+        <v>944</v>
       </c>
       <c r="B406" s="1" t="s">
-        <v>705</v>
+        <v>945</v>
       </c>
       <c r="D406" s="1" t="s">
-        <v>706</v>
+        <v>946</v>
       </c>
     </row>
     <row r="407" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A407" s="1" t="s">
-        <v>800</v>
+        <v>704</v>
       </c>
       <c r="B407" s="1" t="s">
-        <v>801</v>
+        <v>705</v>
       </c>
       <c r="D407" s="1" t="s">
-        <v>802</v>
+        <v>706</v>
       </c>
     </row>
     <row r="408" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A408" s="1" t="s">
-        <v>531</v>
+        <v>800</v>
       </c>
       <c r="B408" s="1" t="s">
-        <v>532</v>
+        <v>801</v>
       </c>
       <c r="D408" s="1" t="s">
-        <v>533</v>
+        <v>802</v>
       </c>
     </row>
     <row r="409" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A409" s="1" t="s">
-        <v>501</v>
+        <v>531</v>
       </c>
       <c r="B409" s="1" t="s">
-        <v>502</v>
+        <v>532</v>
       </c>
       <c r="D409" s="1" t="s">
-        <v>503</v>
+        <v>533</v>
       </c>
     </row>
     <row r="410" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A410" s="1" t="s">
-        <v>415</v>
+        <v>501</v>
       </c>
       <c r="B410" s="1" t="s">
-        <v>416</v>
+        <v>502</v>
       </c>
       <c r="D410" s="1" t="s">
-        <v>417</v>
+        <v>503</v>
       </c>
     </row>
     <row r="411" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A411" s="1" t="s">
-        <v>504</v>
+        <v>415</v>
       </c>
       <c r="B411" s="1" t="s">
-        <v>505</v>
+        <v>416</v>
       </c>
       <c r="D411" s="1" t="s">
-        <v>506</v>
+        <v>417</v>
       </c>
     </row>
     <row r="412" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A412" s="1" t="s">
-        <v>721</v>
+        <v>504</v>
       </c>
       <c r="B412" s="1" t="s">
-        <v>722</v>
+        <v>505</v>
       </c>
       <c r="D412" s="1" t="s">
-        <v>723</v>
+        <v>506</v>
       </c>
     </row>
     <row r="413" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A413" s="1" t="s">
-        <v>555</v>
+        <v>721</v>
       </c>
       <c r="B413" s="1" t="s">
-        <v>556</v>
+        <v>722</v>
       </c>
       <c r="D413" s="1" t="s">
-        <v>557</v>
+        <v>723</v>
       </c>
     </row>
     <row r="414" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A414" s="1" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="B414" s="1" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
       <c r="D414" s="1" t="s">
-        <v>563</v>
+        <v>557</v>
       </c>
     </row>
     <row r="415" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A415" s="1" t="s">
-        <v>549</v>
+        <v>561</v>
       </c>
       <c r="B415" s="1" t="s">
-        <v>550</v>
+        <v>562</v>
       </c>
       <c r="D415" s="1" t="s">
-        <v>551</v>
+        <v>563</v>
       </c>
     </row>
     <row r="416" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A416" s="1" t="s">
-        <v>763</v>
+        <v>549</v>
       </c>
       <c r="B416" s="1" t="s">
-        <v>764</v>
+        <v>550</v>
       </c>
       <c r="D416" s="1" t="s">
         <v>551</v>
@@ -8340,493 +8355,504 @@
     </row>
     <row r="417" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A417" s="1" t="s">
-        <v>618</v>
+        <v>763</v>
       </c>
       <c r="B417" s="1" t="s">
-        <v>619</v>
+        <v>764</v>
       </c>
       <c r="D417" s="1" t="s">
-        <v>1011</v>
+        <v>551</v>
       </c>
     </row>
     <row r="418" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A418" s="1" t="s">
-        <v>606</v>
+        <v>618</v>
       </c>
       <c r="B418" s="1" t="s">
-        <v>607</v>
+        <v>619</v>
       </c>
       <c r="D418" s="1" t="s">
-        <v>608</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="419" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A419" s="1" t="s">
-        <v>450</v>
+        <v>606</v>
       </c>
       <c r="B419" s="1" t="s">
-        <v>451</v>
+        <v>607</v>
       </c>
       <c r="D419" s="1" t="s">
-        <v>452</v>
+        <v>608</v>
       </c>
     </row>
     <row r="420" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A420" s="1" t="s">
-        <v>689</v>
+        <v>450</v>
       </c>
       <c r="B420" s="1" t="s">
-        <v>690</v>
+        <v>451</v>
       </c>
       <c r="D420" s="1" t="s">
-        <v>691</v>
+        <v>452</v>
       </c>
     </row>
     <row r="421" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A421" s="1" t="s">
-        <v>453</v>
+        <v>689</v>
       </c>
       <c r="B421" s="1" t="s">
-        <v>454</v>
+        <v>690</v>
       </c>
       <c r="D421" s="1" t="s">
-        <v>455</v>
+        <v>691</v>
       </c>
     </row>
     <row r="422" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A422" s="1" t="s">
-        <v>765</v>
+        <v>453</v>
       </c>
       <c r="B422" s="1" t="s">
-        <v>766</v>
+        <v>454</v>
       </c>
       <c r="D422" s="1" t="s">
-        <v>767</v>
+        <v>455</v>
       </c>
     </row>
     <row r="423" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A423" s="1" t="s">
-        <v>1051</v>
+        <v>765</v>
       </c>
       <c r="B423" s="1" t="s">
-        <v>1052</v>
+        <v>766</v>
       </c>
       <c r="D423" s="1" t="s">
-        <v>1053</v>
+        <v>767</v>
       </c>
     </row>
     <row r="424" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A424" s="1" t="s">
-        <v>821</v>
+        <v>1051</v>
       </c>
       <c r="B424" s="1" t="s">
-        <v>822</v>
+        <v>1052</v>
       </c>
       <c r="D424" s="1" t="s">
-        <v>823</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="425" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A425" s="1" t="s">
-        <v>421</v>
+        <v>821</v>
       </c>
       <c r="B425" s="1" t="s">
-        <v>422</v>
+        <v>822</v>
       </c>
       <c r="D425" s="1" t="s">
-        <v>423</v>
+        <v>823</v>
       </c>
     </row>
     <row r="426" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A426" s="1" t="s">
-        <v>1016</v>
+        <v>421</v>
       </c>
       <c r="B426" s="1" t="s">
-        <v>1017</v>
+        <v>422</v>
       </c>
       <c r="D426" s="1" t="s">
-        <v>1018</v>
+        <v>423</v>
       </c>
     </row>
     <row r="427" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A427" s="1" t="s">
-        <v>744</v>
+        <v>1016</v>
       </c>
       <c r="B427" s="1" t="s">
-        <v>745</v>
+        <v>1017</v>
       </c>
       <c r="D427" s="1" t="s">
-        <v>746</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="428" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A428" s="1" t="s">
-        <v>905</v>
+        <v>744</v>
       </c>
       <c r="B428" s="1" t="s">
-        <v>904</v>
+        <v>745</v>
       </c>
       <c r="D428" s="1" t="s">
-        <v>906</v>
+        <v>746</v>
       </c>
     </row>
     <row r="429" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A429" s="1" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="B429" s="1" t="s">
-        <v>908</v>
+        <v>904</v>
       </c>
       <c r="D429" s="1" t="s">
-        <v>909</v>
+        <v>906</v>
       </c>
     </row>
     <row r="430" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A430" s="1" t="s">
-        <v>540</v>
+        <v>907</v>
       </c>
       <c r="B430" s="1" t="s">
-        <v>541</v>
+        <v>908</v>
       </c>
       <c r="D430" s="1" t="s">
-        <v>542</v>
+        <v>909</v>
       </c>
     </row>
     <row r="431" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A431" s="1" t="s">
-        <v>662</v>
+        <v>540</v>
       </c>
       <c r="B431" s="1" t="s">
-        <v>663</v>
+        <v>541</v>
       </c>
       <c r="D431" s="1" t="s">
-        <v>664</v>
+        <v>542</v>
       </c>
     </row>
     <row r="432" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A432" s="1" t="s">
-        <v>692</v>
+        <v>662</v>
       </c>
       <c r="B432" s="1" t="s">
-        <v>693</v>
+        <v>663</v>
       </c>
       <c r="D432" s="1" t="s">
-        <v>694</v>
+        <v>664</v>
       </c>
     </row>
     <row r="433" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A433" s="1" t="s">
-        <v>967</v>
+        <v>692</v>
       </c>
       <c r="B433" s="1" t="s">
-        <v>926</v>
+        <v>693</v>
       </c>
       <c r="D433" s="1" t="s">
-        <v>912</v>
+        <v>694</v>
       </c>
     </row>
     <row r="434" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A434" s="1" t="s">
-        <v>786</v>
+        <v>967</v>
       </c>
       <c r="B434" s="1" t="s">
-        <v>787</v>
+        <v>926</v>
       </c>
       <c r="D434" s="1" t="s">
-        <v>788</v>
+        <v>912</v>
       </c>
     </row>
     <row r="435" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A435" s="1" t="s">
-        <v>623</v>
+        <v>786</v>
       </c>
       <c r="B435" s="1" t="s">
-        <v>624</v>
+        <v>787</v>
       </c>
       <c r="D435" s="1" t="s">
-        <v>625</v>
+        <v>788</v>
       </c>
     </row>
     <row r="436" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A436" s="1" t="s">
-        <v>836</v>
+        <v>623</v>
       </c>
       <c r="B436" s="1" t="s">
-        <v>837</v>
+        <v>624</v>
       </c>
       <c r="D436" s="1" t="s">
-        <v>838</v>
+        <v>625</v>
       </c>
     </row>
     <row r="437" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A437" s="1" t="s">
-        <v>686</v>
+        <v>836</v>
       </c>
       <c r="B437" s="1" t="s">
-        <v>687</v>
+        <v>837</v>
       </c>
       <c r="D437" s="1" t="s">
-        <v>688</v>
+        <v>838</v>
       </c>
     </row>
     <row r="438" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A438" s="1" t="s">
-        <v>896</v>
+        <v>686</v>
       </c>
       <c r="B438" s="1" t="s">
-        <v>897</v>
+        <v>687</v>
+      </c>
+      <c r="D438" s="1" t="s">
+        <v>688</v>
       </c>
     </row>
     <row r="439" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A439" s="1" t="s">
-        <v>971</v>
+        <v>896</v>
       </c>
       <c r="B439" s="1" t="s">
-        <v>920</v>
-      </c>
-      <c r="D439" s="1" t="s">
-        <v>973</v>
+        <v>897</v>
       </c>
     </row>
     <row r="440" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A440" s="1" t="s">
-        <v>950</v>
+        <v>971</v>
       </c>
       <c r="B440" s="1" t="s">
-        <v>951</v>
+        <v>920</v>
       </c>
       <c r="D440" s="1" t="s">
-        <v>952</v>
+        <v>973</v>
       </c>
     </row>
     <row r="441" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A441" s="1" t="s">
-        <v>474</v>
+        <v>950</v>
       </c>
       <c r="B441" s="1" t="s">
-        <v>475</v>
+        <v>951</v>
       </c>
       <c r="D441" s="1" t="s">
-        <v>476</v>
+        <v>952</v>
       </c>
     </row>
     <row r="442" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A442" s="1" t="s">
-        <v>567</v>
+        <v>474</v>
       </c>
       <c r="B442" s="1" t="s">
-        <v>568</v>
+        <v>475</v>
       </c>
       <c r="D442" s="1" t="s">
-        <v>569</v>
+        <v>476</v>
       </c>
     </row>
     <row r="443" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A443" s="1" t="s">
-        <v>768</v>
+        <v>567</v>
       </c>
       <c r="B443" s="1" t="s">
-        <v>769</v>
+        <v>568</v>
       </c>
       <c r="D443" s="1" t="s">
-        <v>770</v>
+        <v>569</v>
       </c>
     </row>
     <row r="444" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A444" s="1" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="B444" s="1" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="D444" s="1" t="s">
-        <v>354</v>
+        <v>770</v>
       </c>
     </row>
     <row r="445" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A445" s="1" t="s">
-        <v>712</v>
+        <v>771</v>
       </c>
       <c r="B445" s="1" t="s">
-        <v>713</v>
+        <v>772</v>
       </c>
       <c r="D445" s="1" t="s">
-        <v>714</v>
+        <v>354</v>
       </c>
     </row>
     <row r="446" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A446" s="1" t="s">
-        <v>881</v>
+        <v>712</v>
       </c>
       <c r="B446" s="1" t="s">
-        <v>882</v>
+        <v>713</v>
       </c>
       <c r="D446" s="1" t="s">
-        <v>883</v>
+        <v>714</v>
       </c>
     </row>
     <row r="447" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A447" s="1" t="s">
-        <v>1147</v>
+        <v>881</v>
       </c>
       <c r="B447" s="1" t="s">
-        <v>1148</v>
+        <v>882</v>
       </c>
       <c r="D447" s="1" t="s">
-        <v>1146</v>
+        <v>883</v>
       </c>
     </row>
     <row r="448" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A448" s="1" t="s">
-        <v>953</v>
+        <v>1147</v>
       </c>
       <c r="B448" s="1" t="s">
-        <v>955</v>
+        <v>1148</v>
       </c>
       <c r="D448" s="1" t="s">
-        <v>956</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="449" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A449" s="1" t="s">
-        <v>747</v>
+        <v>953</v>
       </c>
       <c r="B449" s="1" t="s">
-        <v>748</v>
+        <v>955</v>
       </c>
       <c r="D449" s="1" t="s">
-        <v>749</v>
+        <v>956</v>
       </c>
     </row>
     <row r="450" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A450" s="1" t="s">
-        <v>576</v>
+        <v>747</v>
       </c>
       <c r="B450" s="1" t="s">
-        <v>577</v>
+        <v>748</v>
       </c>
       <c r="D450" s="1" t="s">
-        <v>578</v>
+        <v>749</v>
       </c>
     </row>
     <row r="451" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A451" s="1" t="s">
-        <v>824</v>
+        <v>576</v>
       </c>
       <c r="B451" s="1" t="s">
-        <v>825</v>
+        <v>577</v>
       </c>
       <c r="D451" s="1" t="s">
-        <v>826</v>
+        <v>578</v>
       </c>
     </row>
     <row r="452" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A452" s="1" t="s">
-        <v>1024</v>
+        <v>824</v>
       </c>
       <c r="B452" s="1" t="s">
-        <v>1025</v>
+        <v>825</v>
       </c>
       <c r="D452" s="1" t="s">
-        <v>1026</v>
+        <v>826</v>
       </c>
     </row>
     <row r="453" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A453" s="1" t="s">
-        <v>427</v>
+        <v>1024</v>
       </c>
       <c r="B453" s="1" t="s">
-        <v>428</v>
+        <v>1025</v>
       </c>
       <c r="D453" s="1" t="s">
-        <v>429</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="454" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A454" s="1" t="s">
-        <v>626</v>
+        <v>427</v>
       </c>
       <c r="B454" s="1" t="s">
-        <v>627</v>
+        <v>428</v>
       </c>
       <c r="D454" s="1" t="s">
-        <v>628</v>
+        <v>429</v>
       </c>
     </row>
     <row r="455" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A455" s="1" t="s">
-        <v>418</v>
+        <v>626</v>
       </c>
       <c r="B455" s="1" t="s">
-        <v>419</v>
+        <v>627</v>
       </c>
       <c r="D455" s="1" t="s">
-        <v>420</v>
+        <v>628</v>
       </c>
     </row>
     <row r="456" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A456" s="1" t="s">
-        <v>932</v>
+        <v>418</v>
       </c>
       <c r="B456" s="1" t="s">
-        <v>933</v>
+        <v>419</v>
       </c>
       <c r="D456" s="1" t="s">
-        <v>934</v>
+        <v>420</v>
       </c>
     </row>
     <row r="457" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A457" s="1" t="s">
-        <v>735</v>
+        <v>932</v>
       </c>
       <c r="B457" s="1" t="s">
-        <v>736</v>
+        <v>933</v>
       </c>
       <c r="D457" s="1" t="s">
-        <v>737</v>
+        <v>934</v>
       </c>
     </row>
     <row r="458" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A458" s="1" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
       <c r="B458" s="1" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="D458" s="1" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
     </row>
     <row r="459" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A459" s="1" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="B459" s="1" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
       <c r="D459" s="1" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
     </row>
     <row r="460" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A460" s="1" t="s">
-        <v>629</v>
+        <v>741</v>
       </c>
       <c r="B460" s="1" t="s">
-        <v>630</v>
+        <v>742</v>
       </c>
       <c r="D460" s="1" t="s">
-        <v>631</v>
+        <v>743</v>
       </c>
     </row>
     <row r="461" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A461" s="1" t="s">
+        <v>629</v>
+      </c>
+      <c r="B461" s="1" t="s">
+        <v>630</v>
+      </c>
+      <c r="D461" s="1" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="462" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A462" s="1" t="s">
         <v>632</v>
       </c>
-      <c r="B461" s="1" t="s">
+      <c r="B462" s="1" t="s">
         <v>633</v>
       </c>
-      <c r="D461" s="1" t="s">
+      <c r="D462" s="1" t="s">
         <v>634</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Follow Play Framework v2.6.7
</commit_message>
<xml_diff>
--- a/conf/messages.xlsx
+++ b/conf/messages.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1215" uniqueCount="1163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="1205">
   <si>
     <t>key</t>
   </si>
@@ -3866,6 +3866,202 @@
   </si>
   <si>
     <t>Photo</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>batch</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Batch</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>restart</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Restart</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>再開</t>
+    <rPh sb="0" eb="2">
+      <t>サイカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>parameter</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Parameter</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>パラメーター</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>stop</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Stop</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>停止</t>
+    <rPh sb="0" eb="2">
+      <t>テイsh</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>一括処理</t>
+    <rPh sb="0" eb="4">
+      <t>イッカt</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>reload</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Reload</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>再読込</t>
+    <rPh sb="0" eb="1">
+      <t>サイ</t>
+    </rPh>
+    <rPh sb="1" eb="3">
+      <t>ヨm</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Before</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>After</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>after</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>before</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ビフォー</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>アフター</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>started</t>
+  </si>
+  <si>
+    <t>starting</t>
+  </si>
+  <si>
+    <t>stopped</t>
+  </si>
+  <si>
+    <t>stopping</t>
+  </si>
+  <si>
+    <t>completed</t>
+  </si>
+  <si>
+    <t>failed</t>
+  </si>
+  <si>
+    <t>abandoned</t>
+  </si>
+  <si>
+    <t>Started</t>
+  </si>
+  <si>
+    <t>Starting</t>
+  </si>
+  <si>
+    <t>Stopped</t>
+  </si>
+  <si>
+    <t>Stopping</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>Abandoned</t>
+  </si>
+  <si>
+    <t>開始済</t>
+    <rPh sb="0" eb="3">
+      <t>カイsh</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>開始中</t>
+    <rPh sb="0" eb="3">
+      <t>カイsh</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>停止済</t>
+    <rPh sb="0" eb="3">
+      <t>テイsh</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>停止中</t>
+    <rPh sb="0" eb="3">
+      <t>テイsh</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>完了済</t>
+    <rPh sb="0" eb="2">
+      <t>カンリョ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ズm</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>失敗済</t>
+    <rPh sb="0" eb="2">
+      <t>シッパ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ズm</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>破棄済</t>
+    <rPh sb="0" eb="3">
+      <t>ハキズm</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -3927,8 +4123,78 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="65">
+  <cellStyleXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4000,7 +4266,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="65">
+  <cellStyles count="135">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
@@ -4033,6 +4299,41 @@
     <cellStyle name="ハイパーリンク" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="133" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
@@ -4066,6 +4367,41 @@
     <cellStyle name="表示済みのハイパーリンク" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="134" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -4340,10 +4676,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G462"/>
+  <dimension ref="A1:G476"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A368" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E388" sqref="E388"/>
+    <sheetView tabSelected="1" topLeftCell="A272" workbookViewId="0">
+      <selection activeCell="E304" sqref="E304"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -6311,2548 +6647,2703 @@
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A230" s="1" t="s">
-        <v>732</v>
+        <v>1190</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>733</v>
+        <v>1197</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>734</v>
-      </c>
-      <c r="G230" s="1"/>
+        <v>1204</v>
+      </c>
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A231" s="1" t="s">
-        <v>513</v>
+        <v>732</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>514</v>
+        <v>733</v>
       </c>
       <c r="D231" s="1" t="s">
-        <v>515</v>
+        <v>734</v>
       </c>
       <c r="G231" s="1"/>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A232" s="1" t="s">
-        <v>988</v>
+        <v>513</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>989</v>
+        <v>514</v>
       </c>
       <c r="D232" s="1" t="s">
-        <v>990</v>
+        <v>515</v>
       </c>
       <c r="G232" s="1"/>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A233" s="1" t="s">
-        <v>970</v>
+        <v>988</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>923</v>
+        <v>989</v>
       </c>
       <c r="D233" s="1" t="s">
-        <v>964</v>
-      </c>
+        <v>990</v>
+      </c>
+      <c r="G233" s="1"/>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A234" s="1" t="s">
-        <v>603</v>
+        <v>1180</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>604</v>
+        <v>1179</v>
       </c>
       <c r="D234" s="1" t="s">
-        <v>605</v>
+        <v>1183</v>
       </c>
       <c r="G234" s="1"/>
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A235" s="1" t="s">
-        <v>650</v>
+        <v>970</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>651</v>
+        <v>923</v>
       </c>
       <c r="D235" s="1" t="s">
-        <v>652</v>
-      </c>
-      <c r="G235" s="1"/>
+        <v>964</v>
+      </c>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A236" s="1" t="s">
-        <v>845</v>
+        <v>603</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>846</v>
+        <v>604</v>
       </c>
       <c r="D236" s="1" t="s">
-        <v>847</v>
-      </c>
+        <v>605</v>
+      </c>
+      <c r="G236" s="1"/>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A237" s="1" t="s">
-        <v>815</v>
+        <v>650</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>816</v>
+        <v>651</v>
       </c>
       <c r="D237" s="1" t="s">
-        <v>817</v>
-      </c>
+        <v>652</v>
+      </c>
+      <c r="G237" s="1"/>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A238" s="1" t="s">
-        <v>525</v>
+        <v>845</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>526</v>
+        <v>846</v>
       </c>
       <c r="D238" s="1" t="s">
-        <v>963</v>
+        <v>847</v>
       </c>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A239" s="1" t="s">
-        <v>938</v>
+        <v>815</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>939</v>
+        <v>816</v>
       </c>
       <c r="D239" s="1" t="s">
-        <v>940</v>
+        <v>817</v>
       </c>
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A240" s="1" t="s">
-        <v>750</v>
+        <v>525</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>751</v>
+        <v>526</v>
       </c>
       <c r="D240" s="1" t="s">
-        <v>752</v>
+        <v>963</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A241" s="1" t="s">
-        <v>1079</v>
+        <v>938</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>1075</v>
+        <v>939</v>
       </c>
       <c r="D241" s="1" t="s">
-        <v>653</v>
+        <v>940</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A242" s="1" t="s">
-        <v>1078</v>
+        <v>750</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>1076</v>
+        <v>751</v>
       </c>
       <c r="D242" s="1" t="s">
-        <v>1077</v>
+        <v>752</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A243" s="1" t="s">
-        <v>659</v>
+        <v>1079</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>660</v>
+        <v>1075</v>
       </c>
       <c r="D243" s="1" t="s">
-        <v>661</v>
+        <v>653</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A244" s="1" t="s">
-        <v>892</v>
+        <v>1078</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>893</v>
+        <v>1076</v>
+      </c>
+      <c r="D244" s="1" t="s">
+        <v>1077</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A245" s="1" t="s">
-        <v>965</v>
+        <v>659</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>928</v>
+        <v>660</v>
       </c>
       <c r="D245" s="1" t="s">
-        <v>913</v>
+        <v>661</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A246" s="1" t="s">
-        <v>1080</v>
+        <v>1163</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>1081</v>
+        <v>1164</v>
       </c>
       <c r="D246" s="1" t="s">
-        <v>1082</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A247" s="1" t="s">
-        <v>797</v>
+        <v>1181</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>798</v>
+        <v>1178</v>
       </c>
       <c r="D247" s="1" t="s">
-        <v>799</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A248" s="1" t="s">
-        <v>860</v>
+        <v>892</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>861</v>
-      </c>
-      <c r="D248" s="1" t="s">
-        <v>862</v>
+        <v>893</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A249" s="1" t="s">
-        <v>1039</v>
+        <v>965</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>1040</v>
+        <v>928</v>
       </c>
       <c r="D249" s="1" t="s">
-        <v>1041</v>
+        <v>913</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A250" s="1" t="s">
-        <v>447</v>
+        <v>1080</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>448</v>
+        <v>1081</v>
       </c>
       <c r="D250" s="1" t="s">
-        <v>449</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A251" s="1" t="s">
-        <v>1048</v>
+        <v>797</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>1049</v>
+        <v>798</v>
       </c>
       <c r="D251" s="1" t="s">
-        <v>1050</v>
+        <v>799</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A252" s="1" t="s">
-        <v>969</v>
+        <v>860</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>924</v>
+        <v>861</v>
       </c>
       <c r="D252" s="1" t="s">
-        <v>910</v>
+        <v>862</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A253" s="1" t="s">
-        <v>489</v>
+        <v>1039</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>490</v>
+        <v>1040</v>
       </c>
       <c r="D253" s="1" t="s">
-        <v>491</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A254" s="1" t="s">
-        <v>878</v>
+        <v>447</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>879</v>
+        <v>448</v>
       </c>
       <c r="D254" s="1" t="s">
-        <v>880</v>
+        <v>449</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A255" s="1" t="s">
-        <v>863</v>
+        <v>1048</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>864</v>
+        <v>1049</v>
       </c>
       <c r="D255" s="1" t="s">
-        <v>865</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A256" s="1" t="s">
-        <v>564</v>
+        <v>969</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>565</v>
+        <v>924</v>
       </c>
       <c r="D256" s="1" t="s">
-        <v>566</v>
+        <v>910</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A257" s="1" t="s">
-        <v>546</v>
+        <v>489</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>547</v>
+        <v>490</v>
       </c>
       <c r="D257" s="1" t="s">
-        <v>548</v>
+        <v>491</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A258" s="1" t="s">
-        <v>872</v>
+        <v>878</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>873</v>
+        <v>879</v>
       </c>
       <c r="D258" s="1" t="s">
-        <v>874</v>
+        <v>880</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A259" s="1" t="s">
-        <v>707</v>
+        <v>863</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>708</v>
+        <v>864</v>
       </c>
       <c r="D259" s="1" t="s">
-        <v>709</v>
+        <v>865</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A260" s="1" t="s">
-        <v>394</v>
+        <v>564</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>395</v>
+        <v>565</v>
       </c>
       <c r="D260" s="1" t="s">
-        <v>396</v>
+        <v>566</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A261" s="1" t="s">
-        <v>397</v>
+        <v>546</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>398</v>
+        <v>547</v>
       </c>
       <c r="D261" s="1" t="s">
-        <v>399</v>
+        <v>548</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A262" s="1" t="s">
-        <v>400</v>
+        <v>872</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>401</v>
+        <v>873</v>
       </c>
       <c r="D262" s="1" t="s">
-        <v>402</v>
+        <v>874</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A263" s="1" t="s">
-        <v>459</v>
+        <v>707</v>
       </c>
       <c r="B263" s="1" t="s">
-        <v>460</v>
+        <v>708</v>
       </c>
       <c r="D263" s="1" t="s">
-        <v>461</v>
+        <v>709</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A264" s="1" t="s">
-        <v>818</v>
+        <v>394</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>819</v>
+        <v>395</v>
       </c>
       <c r="D264" s="1" t="s">
-        <v>820</v>
+        <v>396</v>
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A265" s="1" t="s">
-        <v>635</v>
+        <v>397</v>
       </c>
       <c r="B265" s="1" t="s">
-        <v>636</v>
+        <v>398</v>
       </c>
       <c r="D265" s="1" t="s">
-        <v>637</v>
+        <v>399</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A266" s="1" t="s">
-        <v>656</v>
+        <v>400</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>657</v>
+        <v>401</v>
       </c>
       <c r="D266" s="1" t="s">
-        <v>658</v>
+        <v>402</v>
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A267" s="1" t="s">
-        <v>782</v>
+        <v>459</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>783</v>
+        <v>460</v>
       </c>
       <c r="D267" s="1" t="s">
-        <v>784</v>
+        <v>461</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A268" s="1" t="s">
-        <v>698</v>
+        <v>1188</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>699</v>
+        <v>1195</v>
       </c>
       <c r="D268" s="1" t="s">
-        <v>700</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A269" s="1" t="s">
-        <v>1154</v>
+        <v>818</v>
       </c>
       <c r="B269" s="1" t="s">
-        <v>1153</v>
+        <v>819</v>
       </c>
       <c r="D269" s="1" t="s">
-        <v>1152</v>
+        <v>820</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A270" s="1" t="s">
-        <v>468</v>
+        <v>635</v>
       </c>
       <c r="B270" s="1" t="s">
-        <v>469</v>
+        <v>636</v>
       </c>
       <c r="D270" s="1" t="s">
-        <v>470</v>
+        <v>637</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A271" s="1" t="s">
-        <v>779</v>
+        <v>656</v>
       </c>
       <c r="B271" s="1" t="s">
-        <v>780</v>
+        <v>657</v>
       </c>
       <c r="D271" s="1" t="s">
-        <v>781</v>
+        <v>658</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A272" s="1" t="s">
-        <v>1149</v>
+        <v>782</v>
       </c>
       <c r="B272" s="1" t="s">
-        <v>1150</v>
+        <v>783</v>
       </c>
       <c r="D272" s="1" t="s">
-        <v>1151</v>
+        <v>784</v>
       </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A273" s="1" t="s">
-        <v>579</v>
+        <v>698</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>580</v>
+        <v>699</v>
       </c>
       <c r="D273" s="1" t="s">
-        <v>581</v>
+        <v>700</v>
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A274" s="1" t="s">
-        <v>537</v>
+        <v>1154</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>538</v>
+        <v>1153</v>
       </c>
       <c r="D274" s="1" t="s">
-        <v>539</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A275" s="1" t="s">
-        <v>534</v>
+        <v>468</v>
       </c>
       <c r="B275" s="1" t="s">
-        <v>535</v>
+        <v>469</v>
       </c>
       <c r="D275" s="1" t="s">
-        <v>536</v>
+        <v>470</v>
       </c>
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A276" s="1" t="s">
-        <v>1019</v>
+        <v>779</v>
       </c>
       <c r="B276" s="1" t="s">
-        <v>1020</v>
+        <v>780</v>
       </c>
       <c r="D276" s="1" t="s">
-        <v>539</v>
+        <v>781</v>
       </c>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A277" s="1" t="s">
-        <v>1</v>
+        <v>1149</v>
       </c>
       <c r="B277" s="1" t="s">
-        <v>5</v>
+        <v>1150</v>
       </c>
       <c r="D277" s="1" t="s">
-        <v>222</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A278" s="1" t="s">
-        <v>477</v>
+        <v>579</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>478</v>
+        <v>580</v>
       </c>
       <c r="D278" s="1" t="s">
-        <v>479</v>
+        <v>581</v>
       </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A279" s="1" t="s">
-        <v>668</v>
+        <v>537</v>
       </c>
       <c r="B279" s="1" t="s">
-        <v>669</v>
+        <v>538</v>
       </c>
       <c r="D279" s="1" t="s">
-        <v>670</v>
+        <v>539</v>
       </c>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A280" s="1" t="s">
-        <v>507</v>
+        <v>534</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>508</v>
+        <v>535</v>
       </c>
       <c r="D280" s="1" t="s">
-        <v>509</v>
+        <v>536</v>
       </c>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A281" s="1" t="s">
-        <v>851</v>
+        <v>1019</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>852</v>
+        <v>1020</v>
       </c>
       <c r="D281" s="1" t="s">
-        <v>853</v>
+        <v>539</v>
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A282" s="1" t="s">
-        <v>644</v>
+        <v>1</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>645</v>
+        <v>5</v>
       </c>
       <c r="D282" s="1" t="s">
-        <v>646</v>
+        <v>222</v>
       </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A283" s="1" t="s">
-        <v>789</v>
+        <v>477</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>790</v>
+        <v>478</v>
       </c>
       <c r="D283" s="1" t="s">
-        <v>791</v>
+        <v>479</v>
       </c>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A284" s="1" t="s">
-        <v>680</v>
+        <v>668</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>681</v>
+        <v>669</v>
       </c>
       <c r="D284" s="1" t="s">
-        <v>682</v>
+        <v>670</v>
       </c>
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A285" s="1" t="s">
-        <v>424</v>
+        <v>507</v>
       </c>
       <c r="B285" s="1" t="s">
-        <v>425</v>
+        <v>508</v>
       </c>
       <c r="D285" s="1" t="s">
-        <v>426</v>
+        <v>509</v>
       </c>
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A286" s="1" t="s">
-        <v>947</v>
+        <v>851</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>948</v>
+        <v>852</v>
       </c>
       <c r="D286" s="1" t="s">
-        <v>949</v>
+        <v>853</v>
       </c>
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A287" s="1" t="s">
-        <v>570</v>
+        <v>644</v>
       </c>
       <c r="B287" s="1" t="s">
-        <v>571</v>
+        <v>645</v>
       </c>
       <c r="D287" s="1" t="s">
-        <v>572</v>
+        <v>646</v>
       </c>
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A288" s="1" t="s">
-        <v>519</v>
+        <v>789</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>520</v>
+        <v>790</v>
       </c>
       <c r="D288" s="1" t="s">
-        <v>521</v>
+        <v>791</v>
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A289" s="1" t="s">
-        <v>522</v>
+        <v>680</v>
       </c>
       <c r="B289" s="1" t="s">
-        <v>523</v>
+        <v>681</v>
       </c>
       <c r="D289" s="1" t="s">
-        <v>524</v>
+        <v>682</v>
       </c>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A290" s="1" t="s">
-        <v>1036</v>
+        <v>424</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>1037</v>
+        <v>425</v>
       </c>
       <c r="D290" s="1" t="s">
-        <v>1038</v>
+        <v>426</v>
       </c>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A291" s="1" t="s">
-        <v>492</v>
+        <v>947</v>
       </c>
       <c r="B291" s="1" t="s">
-        <v>493</v>
+        <v>948</v>
       </c>
       <c r="D291" s="1" t="s">
-        <v>494</v>
+        <v>949</v>
       </c>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A292" s="1" t="s">
-        <v>773</v>
+        <v>570</v>
       </c>
       <c r="B292" s="1" t="s">
-        <v>24</v>
+        <v>571</v>
       </c>
       <c r="D292" s="1" t="s">
-        <v>774</v>
+        <v>572</v>
       </c>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A293" s="1" t="s">
-        <v>462</v>
+        <v>519</v>
       </c>
       <c r="B293" s="1" t="s">
-        <v>463</v>
+        <v>520</v>
       </c>
       <c r="D293" s="1" t="s">
-        <v>464</v>
+        <v>521</v>
       </c>
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A294" s="1" t="s">
-        <v>609</v>
+        <v>522</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>610</v>
+        <v>523</v>
       </c>
       <c r="D294" s="1" t="s">
-        <v>611</v>
+        <v>524</v>
       </c>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A295" s="1" t="s">
-        <v>794</v>
+        <v>1036</v>
       </c>
       <c r="B295" s="1" t="s">
-        <v>795</v>
+        <v>1037</v>
       </c>
       <c r="D295" s="1" t="s">
-        <v>796</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A296" s="1" t="s">
-        <v>582</v>
+        <v>492</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>583</v>
+        <v>493</v>
       </c>
       <c r="D296" s="1" t="s">
-        <v>584</v>
+        <v>494</v>
       </c>
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A297" s="1" t="s">
-        <v>1012</v>
+        <v>773</v>
       </c>
       <c r="B297" s="1" t="s">
-        <v>1013</v>
+        <v>24</v>
       </c>
       <c r="D297" s="1" t="s">
-        <v>1014</v>
+        <v>774</v>
       </c>
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A298" s="1" t="s">
-        <v>803</v>
+        <v>462</v>
       </c>
       <c r="B298" s="1" t="s">
-        <v>804</v>
+        <v>463</v>
       </c>
       <c r="D298" s="1" t="s">
-        <v>805</v>
+        <v>464</v>
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A299" s="1" t="s">
-        <v>456</v>
+        <v>609</v>
       </c>
       <c r="B299" s="1" t="s">
-        <v>457</v>
+        <v>610</v>
       </c>
       <c r="D299" s="1" t="s">
-        <v>458</v>
+        <v>611</v>
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A300" s="1" t="s">
-        <v>839</v>
+        <v>794</v>
       </c>
       <c r="B300" s="1" t="s">
-        <v>840</v>
+        <v>795</v>
       </c>
       <c r="D300" s="1" t="s">
-        <v>841</v>
+        <v>796</v>
       </c>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A301" s="1" t="s">
-        <v>1042</v>
+        <v>582</v>
       </c>
       <c r="B301" s="1" t="s">
-        <v>1043</v>
+        <v>583</v>
       </c>
       <c r="D301" s="1" t="s">
-        <v>1044</v>
+        <v>584</v>
       </c>
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A302" s="1" t="s">
-        <v>715</v>
+        <v>1012</v>
       </c>
       <c r="B302" s="1" t="s">
-        <v>716</v>
+        <v>1013</v>
       </c>
       <c r="D302" s="1" t="s">
-        <v>717</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A303" s="1" t="s">
-        <v>718</v>
+        <v>803</v>
       </c>
       <c r="B303" s="1" t="s">
-        <v>719</v>
+        <v>804</v>
       </c>
       <c r="D303" s="1" t="s">
-        <v>720</v>
+        <v>805</v>
       </c>
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A304" s="1" t="s">
-        <v>615</v>
+        <v>1189</v>
       </c>
       <c r="B304" s="1" t="s">
-        <v>616</v>
+        <v>1196</v>
       </c>
       <c r="D304" s="1" t="s">
-        <v>617</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A305" s="1" t="s">
-        <v>585</v>
+        <v>456</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>586</v>
+        <v>457</v>
       </c>
       <c r="D305" s="1" t="s">
-        <v>587</v>
+        <v>458</v>
       </c>
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A306" s="1" t="s">
-        <v>612</v>
+        <v>839</v>
       </c>
       <c r="B306" s="1" t="s">
-        <v>613</v>
+        <v>840</v>
       </c>
       <c r="D306" s="1" t="s">
-        <v>614</v>
+        <v>841</v>
       </c>
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A307" s="1" t="s">
-        <v>756</v>
+        <v>1042</v>
       </c>
       <c r="B307" s="1" t="s">
-        <v>757</v>
+        <v>1043</v>
       </c>
       <c r="D307" s="1" t="s">
-        <v>758</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A308" s="1" t="s">
-        <v>894</v>
+        <v>715</v>
       </c>
       <c r="B308" s="1" t="s">
-        <v>895</v>
+        <v>716</v>
+      </c>
+      <c r="D308" s="1" t="s">
+        <v>717</v>
       </c>
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A309" s="1" t="s">
-        <v>701</v>
+        <v>718</v>
       </c>
       <c r="B309" s="1" t="s">
-        <v>702</v>
+        <v>719</v>
       </c>
       <c r="D309" s="1" t="s">
-        <v>703</v>
+        <v>720</v>
       </c>
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A310" s="1" t="s">
-        <v>683</v>
+        <v>615</v>
       </c>
       <c r="B310" s="1" t="s">
-        <v>684</v>
+        <v>616</v>
       </c>
       <c r="D310" s="1" t="s">
-        <v>685</v>
+        <v>617</v>
       </c>
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A311" s="1" t="s">
-        <v>792</v>
+        <v>585</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>793</v>
+        <v>586</v>
       </c>
       <c r="D311" s="1" t="s">
-        <v>962</v>
+        <v>587</v>
       </c>
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A312" s="1" t="s">
-        <v>775</v>
+        <v>612</v>
       </c>
       <c r="B312" s="1" t="s">
-        <v>776</v>
+        <v>613</v>
       </c>
       <c r="D312" s="1" t="s">
-        <v>432</v>
+        <v>614</v>
       </c>
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A313" s="1" t="s">
-        <v>833</v>
+        <v>756</v>
       </c>
       <c r="B313" s="1" t="s">
-        <v>834</v>
+        <v>757</v>
       </c>
       <c r="D313" s="1" t="s">
-        <v>835</v>
+        <v>758</v>
       </c>
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A314" s="1" t="s">
-        <v>638</v>
+        <v>894</v>
       </c>
       <c r="B314" s="1" t="s">
-        <v>639</v>
-      </c>
-      <c r="D314" s="1" t="s">
-        <v>640</v>
+        <v>895</v>
       </c>
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A315" s="1" t="s">
-        <v>552</v>
+        <v>701</v>
       </c>
       <c r="B315" s="1" t="s">
-        <v>553</v>
+        <v>702</v>
       </c>
       <c r="D315" s="1" t="s">
-        <v>554</v>
+        <v>703</v>
       </c>
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A316" s="1" t="s">
-        <v>959</v>
+        <v>683</v>
       </c>
       <c r="B316" s="1" t="s">
-        <v>960</v>
+        <v>684</v>
       </c>
       <c r="D316" s="1" t="s">
-        <v>961</v>
+        <v>685</v>
       </c>
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A317" s="1" t="s">
-        <v>1031</v>
+        <v>792</v>
       </c>
       <c r="B317" s="1" t="s">
-        <v>1030</v>
+        <v>793</v>
       </c>
       <c r="D317" s="1" t="s">
-        <v>1032</v>
+        <v>962</v>
       </c>
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A318" s="1" t="s">
-        <v>695</v>
+        <v>775</v>
       </c>
       <c r="B318" s="1" t="s">
-        <v>696</v>
+        <v>776</v>
       </c>
       <c r="D318" s="1" t="s">
-        <v>697</v>
+        <v>432</v>
       </c>
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A319" s="1" t="s">
-        <v>677</v>
+        <v>833</v>
       </c>
       <c r="B319" s="1" t="s">
-        <v>678</v>
+        <v>834</v>
       </c>
       <c r="D319" s="1" t="s">
-        <v>679</v>
+        <v>835</v>
       </c>
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A320" s="1" t="s">
-        <v>875</v>
+        <v>638</v>
       </c>
       <c r="B320" s="1" t="s">
-        <v>876</v>
+        <v>639</v>
       </c>
       <c r="D320" s="1" t="s">
-        <v>877</v>
+        <v>640</v>
       </c>
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A321" s="1" t="s">
-        <v>958</v>
+        <v>552</v>
       </c>
       <c r="B321" s="1" t="s">
-        <v>957</v>
+        <v>553</v>
       </c>
       <c r="D321" s="1" t="s">
-        <v>759</v>
+        <v>554</v>
       </c>
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A322" s="1" t="s">
-        <v>1009</v>
+        <v>959</v>
       </c>
       <c r="B322" s="1" t="s">
-        <v>1010</v>
+        <v>960</v>
       </c>
       <c r="D322" s="1" t="s">
-        <v>954</v>
+        <v>961</v>
       </c>
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A323" s="1" t="s">
-        <v>886</v>
+        <v>1031</v>
       </c>
       <c r="B323" s="1" t="s">
-        <v>887</v>
+        <v>1030</v>
+      </c>
+      <c r="D323" s="1" t="s">
+        <v>1032</v>
       </c>
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A324" s="1" t="s">
-        <v>857</v>
+        <v>695</v>
       </c>
       <c r="B324" s="1" t="s">
-        <v>858</v>
+        <v>696</v>
       </c>
       <c r="D324" s="1" t="s">
-        <v>859</v>
+        <v>697</v>
       </c>
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A325" s="1" t="s">
-        <v>884</v>
+        <v>677</v>
       </c>
       <c r="B325" s="1" t="s">
-        <v>885</v>
+        <v>678</v>
+      </c>
+      <c r="D325" s="1" t="s">
+        <v>679</v>
       </c>
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A326" s="1" t="s">
-        <v>753</v>
+        <v>875</v>
       </c>
       <c r="B326" s="1" t="s">
-        <v>754</v>
+        <v>876</v>
       </c>
       <c r="D326" s="1" t="s">
-        <v>755</v>
+        <v>877</v>
       </c>
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A327" s="1" t="s">
-        <v>573</v>
+        <v>958</v>
       </c>
       <c r="B327" s="1" t="s">
-        <v>574</v>
+        <v>957</v>
       </c>
       <c r="D327" s="1" t="s">
-        <v>575</v>
+        <v>759</v>
       </c>
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A328" s="1" t="s">
-        <v>777</v>
+        <v>1009</v>
       </c>
       <c r="B328" s="1" t="s">
-        <v>778</v>
+        <v>1010</v>
       </c>
       <c r="D328" s="1" t="s">
-        <v>575</v>
+        <v>954</v>
       </c>
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A329" s="1" t="s">
-        <v>510</v>
+        <v>886</v>
       </c>
       <c r="B329" s="1" t="s">
-        <v>511</v>
-      </c>
-      <c r="D329" s="1" t="s">
-        <v>512</v>
+        <v>887</v>
       </c>
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A330" s="1" t="s">
-        <v>985</v>
+        <v>857</v>
       </c>
       <c r="B330" s="1" t="s">
-        <v>916</v>
+        <v>858</v>
       </c>
       <c r="D330" s="1" t="s">
-        <v>979</v>
+        <v>859</v>
       </c>
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A331" s="1" t="s">
-        <v>984</v>
+        <v>884</v>
       </c>
       <c r="B331" s="1" t="s">
-        <v>917</v>
-      </c>
-      <c r="D331" s="1" t="s">
-        <v>978</v>
+        <v>885</v>
       </c>
     </row>
     <row r="332" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A332" s="1" t="s">
-        <v>986</v>
+        <v>753</v>
       </c>
       <c r="B332" s="1" t="s">
-        <v>914</v>
+        <v>754</v>
       </c>
       <c r="D332" s="1" t="s">
-        <v>981</v>
+        <v>755</v>
       </c>
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A333" s="1" t="s">
-        <v>987</v>
+        <v>573</v>
       </c>
       <c r="B333" s="1" t="s">
-        <v>915</v>
+        <v>574</v>
       </c>
       <c r="D333" s="1" t="s">
-        <v>980</v>
+        <v>575</v>
       </c>
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A334" s="1" t="s">
-        <v>760</v>
+        <v>777</v>
       </c>
       <c r="B334" s="1" t="s">
-        <v>761</v>
+        <v>778</v>
       </c>
       <c r="D334" s="1" t="s">
-        <v>762</v>
+        <v>575</v>
       </c>
     </row>
     <row r="335" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A335" s="1" t="s">
-        <v>888</v>
+        <v>510</v>
       </c>
       <c r="B335" s="1" t="s">
-        <v>889</v>
+        <v>511</v>
+      </c>
+      <c r="D335" s="1" t="s">
+        <v>512</v>
       </c>
     </row>
     <row r="336" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A336" s="1" t="s">
-        <v>890</v>
+        <v>985</v>
       </c>
       <c r="B336" s="1" t="s">
-        <v>891</v>
+        <v>916</v>
+      </c>
+      <c r="D336" s="1" t="s">
+        <v>979</v>
       </c>
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A337" s="1" t="s">
-        <v>968</v>
+        <v>984</v>
       </c>
       <c r="B337" s="1" t="s">
-        <v>925</v>
+        <v>917</v>
       </c>
       <c r="D337" s="1" t="s">
-        <v>911</v>
+        <v>978</v>
       </c>
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A338" s="1" t="s">
-        <v>0</v>
+        <v>986</v>
       </c>
       <c r="B338" s="1" t="s">
-        <v>710</v>
+        <v>914</v>
       </c>
       <c r="D338" s="1" t="s">
-        <v>711</v>
+        <v>981</v>
       </c>
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A339" s="1" t="s">
-        <v>811</v>
+        <v>987</v>
       </c>
       <c r="B339" s="1" t="s">
-        <v>812</v>
+        <v>915</v>
       </c>
       <c r="D339" s="1" t="s">
-        <v>900</v>
+        <v>980</v>
       </c>
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A340" s="1" t="s">
-        <v>588</v>
+        <v>760</v>
       </c>
       <c r="B340" s="1" t="s">
-        <v>589</v>
+        <v>761</v>
       </c>
       <c r="D340" s="1" t="s">
-        <v>590</v>
+        <v>762</v>
       </c>
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A341" s="1" t="s">
-        <v>813</v>
+        <v>888</v>
       </c>
       <c r="B341" s="1" t="s">
-        <v>814</v>
-      </c>
-      <c r="D341" s="1" t="s">
-        <v>527</v>
+        <v>889</v>
       </c>
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A342" s="1" t="s">
-        <v>943</v>
+        <v>890</v>
       </c>
       <c r="B342" s="1" t="s">
-        <v>941</v>
-      </c>
-      <c r="D342" s="1" t="s">
-        <v>942</v>
+        <v>891</v>
       </c>
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A343" s="1" t="s">
-        <v>806</v>
+        <v>968</v>
       </c>
       <c r="B343" s="1" t="s">
-        <v>807</v>
+        <v>925</v>
       </c>
       <c r="D343" s="1" t="s">
-        <v>808</v>
+        <v>911</v>
       </c>
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A344" s="1" t="s">
-        <v>1071</v>
+        <v>0</v>
       </c>
       <c r="B344" s="1" t="s">
-        <v>1072</v>
+        <v>710</v>
       </c>
       <c r="D344" s="1" t="s">
-        <v>785</v>
+        <v>711</v>
       </c>
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A345" s="1" t="s">
-        <v>869</v>
+        <v>811</v>
       </c>
       <c r="B345" s="1" t="s">
-        <v>870</v>
+        <v>812</v>
       </c>
       <c r="D345" s="1" t="s">
-        <v>871</v>
+        <v>900</v>
       </c>
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A346" s="1" t="s">
-        <v>641</v>
+        <v>588</v>
       </c>
       <c r="B346" s="1" t="s">
-        <v>642</v>
+        <v>589</v>
       </c>
       <c r="D346" s="1" t="s">
-        <v>643</v>
+        <v>590</v>
       </c>
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A347" s="1" t="s">
-        <v>528</v>
+        <v>813</v>
       </c>
       <c r="B347" s="1" t="s">
-        <v>529</v>
+        <v>814</v>
       </c>
       <c r="D347" s="1" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="348" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A348" s="1" t="s">
-        <v>436</v>
+        <v>943</v>
       </c>
       <c r="B348" s="1" t="s">
-        <v>437</v>
+        <v>941</v>
       </c>
       <c r="D348" s="1" t="s">
-        <v>438</v>
+        <v>942</v>
       </c>
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A349" s="1" t="s">
-        <v>439</v>
+        <v>806</v>
       </c>
       <c r="B349" s="1" t="s">
-        <v>440</v>
+        <v>807</v>
       </c>
       <c r="D349" s="1" t="s">
-        <v>441</v>
+        <v>808</v>
       </c>
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A350" s="1" t="s">
-        <v>442</v>
+        <v>1071</v>
       </c>
       <c r="B350" s="1" t="s">
-        <v>443</v>
+        <v>1072</v>
       </c>
       <c r="D350" s="1" t="s">
-        <v>444</v>
+        <v>785</v>
       </c>
     </row>
     <row r="351" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A351" s="1" t="s">
-        <v>809</v>
+        <v>869</v>
       </c>
       <c r="B351" s="1" t="s">
-        <v>810</v>
+        <v>870</v>
       </c>
       <c r="D351" s="1" t="s">
-        <v>994</v>
+        <v>871</v>
       </c>
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A352" s="1" t="s">
-        <v>647</v>
+        <v>641</v>
       </c>
       <c r="B352" s="1" t="s">
-        <v>648</v>
+        <v>642</v>
       </c>
       <c r="D352" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
     </row>
     <row r="353" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A353" s="1" t="s">
-        <v>929</v>
+        <v>528</v>
       </c>
       <c r="B353" s="1" t="s">
-        <v>930</v>
+        <v>529</v>
       </c>
       <c r="D353" s="1" t="s">
-        <v>931</v>
+        <v>530</v>
       </c>
     </row>
     <row r="354" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A354" s="1" t="s">
-        <v>995</v>
+        <v>436</v>
       </c>
       <c r="B354" s="1" t="s">
-        <v>996</v>
+        <v>437</v>
       </c>
       <c r="D354" s="1" t="s">
-        <v>997</v>
+        <v>438</v>
       </c>
     </row>
     <row r="355" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A355" s="1" t="s">
-        <v>998</v>
+        <v>439</v>
       </c>
       <c r="B355" s="1" t="s">
-        <v>999</v>
+        <v>440</v>
       </c>
       <c r="D355" s="1" t="s">
-        <v>1000</v>
+        <v>441</v>
       </c>
     </row>
     <row r="356" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A356" s="1" t="s">
-        <v>1005</v>
+        <v>442</v>
       </c>
       <c r="B356" s="1" t="s">
-        <v>730</v>
+        <v>443</v>
       </c>
       <c r="D356" s="1" t="s">
-        <v>731</v>
+        <v>444</v>
       </c>
     </row>
     <row r="357" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A357" s="1" t="s">
-        <v>854</v>
+        <v>809</v>
       </c>
       <c r="B357" s="1" t="s">
-        <v>855</v>
+        <v>810</v>
       </c>
       <c r="D357" s="1" t="s">
-        <v>856</v>
+        <v>994</v>
       </c>
     </row>
     <row r="358" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A358" s="1" t="s">
-        <v>665</v>
+        <v>647</v>
       </c>
       <c r="B358" s="1" t="s">
-        <v>666</v>
+        <v>648</v>
       </c>
       <c r="D358" s="1" t="s">
-        <v>667</v>
+        <v>649</v>
       </c>
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A359" s="1" t="s">
-        <v>966</v>
+        <v>929</v>
       </c>
       <c r="B359" s="1" t="s">
-        <v>927</v>
+        <v>930</v>
       </c>
       <c r="D359" s="1" t="s">
-        <v>910</v>
+        <v>931</v>
       </c>
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A360" s="1" t="s">
-        <v>1001</v>
+        <v>995</v>
       </c>
       <c r="B360" s="1" t="s">
-        <v>1002</v>
+        <v>996</v>
       </c>
       <c r="D360" s="1" t="s">
-        <v>1003</v>
+        <v>997</v>
       </c>
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A361" s="1" t="s">
-        <v>1006</v>
+        <v>998</v>
       </c>
       <c r="B361" s="1" t="s">
-        <v>1007</v>
+        <v>999</v>
       </c>
       <c r="D361" s="1" t="s">
-        <v>1008</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="362" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A362" s="1" t="s">
-        <v>1021</v>
+        <v>1005</v>
       </c>
       <c r="B362" s="1" t="s">
-        <v>1022</v>
+        <v>730</v>
       </c>
       <c r="D362" s="1" t="s">
-        <v>1023</v>
+        <v>731</v>
       </c>
     </row>
     <row r="363" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A363" s="1" t="s">
-        <v>430</v>
+        <v>854</v>
       </c>
       <c r="B363" s="1" t="s">
-        <v>431</v>
+        <v>855</v>
       </c>
       <c r="D363" s="1" t="s">
-        <v>432</v>
+        <v>856</v>
       </c>
     </row>
     <row r="364" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A364" s="1" t="s">
-        <v>433</v>
+        <v>665</v>
       </c>
       <c r="B364" s="1" t="s">
-        <v>434</v>
+        <v>666</v>
       </c>
       <c r="D364" s="1" t="s">
-        <v>435</v>
+        <v>667</v>
       </c>
     </row>
     <row r="365" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A365" s="1" t="s">
-        <v>600</v>
+        <v>966</v>
       </c>
       <c r="B365" s="1" t="s">
-        <v>601</v>
+        <v>927</v>
       </c>
       <c r="D365" s="1" t="s">
-        <v>602</v>
+        <v>910</v>
       </c>
     </row>
     <row r="366" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A366" s="1" t="s">
-        <v>594</v>
+        <v>1001</v>
       </c>
       <c r="B366" s="1" t="s">
-        <v>595</v>
+        <v>1002</v>
       </c>
       <c r="D366" s="1" t="s">
-        <v>596</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="367" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A367" s="1" t="s">
-        <v>671</v>
+        <v>1006</v>
       </c>
       <c r="B367" s="1" t="s">
-        <v>672</v>
+        <v>1007</v>
       </c>
       <c r="D367" s="1" t="s">
-        <v>673</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="368" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A368" s="1" t="s">
-        <v>445</v>
+        <v>1021</v>
       </c>
       <c r="B368" s="1" t="s">
-        <v>446</v>
+        <v>1022</v>
       </c>
       <c r="D368" s="1" t="s">
-        <v>446</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="369" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A369" s="1" t="s">
-        <v>597</v>
+        <v>430</v>
       </c>
       <c r="B369" s="1" t="s">
-        <v>598</v>
+        <v>431</v>
       </c>
       <c r="D369" s="1" t="s">
-        <v>599</v>
+        <v>432</v>
       </c>
     </row>
     <row r="370" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A370" s="1" t="s">
-        <v>543</v>
+        <v>433</v>
       </c>
       <c r="B370" s="1" t="s">
-        <v>544</v>
+        <v>434</v>
       </c>
       <c r="D370" s="1" t="s">
-        <v>545</v>
+        <v>435</v>
       </c>
     </row>
     <row r="371" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A371" s="1" t="s">
-        <v>465</v>
+        <v>600</v>
       </c>
       <c r="B371" s="1" t="s">
-        <v>466</v>
+        <v>601</v>
       </c>
       <c r="D371" s="1" t="s">
-        <v>467</v>
+        <v>602</v>
       </c>
     </row>
     <row r="372" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A372" s="1" t="s">
-        <v>620</v>
+        <v>594</v>
       </c>
       <c r="B372" s="1" t="s">
-        <v>621</v>
+        <v>595</v>
       </c>
       <c r="D372" s="1" t="s">
-        <v>622</v>
+        <v>596</v>
       </c>
     </row>
     <row r="373" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A373" s="1" t="s">
-        <v>403</v>
+        <v>671</v>
       </c>
       <c r="B373" s="1" t="s">
-        <v>404</v>
+        <v>672</v>
       </c>
       <c r="D373" s="1" t="s">
-        <v>405</v>
+        <v>673</v>
       </c>
     </row>
     <row r="374" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A374" s="1" t="s">
-        <v>406</v>
+        <v>445</v>
       </c>
       <c r="B374" s="1" t="s">
-        <v>407</v>
+        <v>446</v>
       </c>
       <c r="D374" s="1" t="s">
-        <v>408</v>
+        <v>446</v>
       </c>
     </row>
     <row r="375" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A375" s="1" t="s">
-        <v>409</v>
+        <v>597</v>
       </c>
       <c r="B375" s="1" t="s">
-        <v>410</v>
+        <v>598</v>
       </c>
       <c r="D375" s="1" t="s">
-        <v>411</v>
+        <v>599</v>
       </c>
     </row>
     <row r="376" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A376" s="1" t="s">
-        <v>412</v>
+        <v>543</v>
       </c>
       <c r="B376" s="1" t="s">
-        <v>413</v>
+        <v>544</v>
       </c>
       <c r="D376" s="1" t="s">
-        <v>414</v>
+        <v>545</v>
       </c>
     </row>
     <row r="377" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A377" s="1" t="s">
-        <v>848</v>
+        <v>465</v>
       </c>
       <c r="B377" s="1" t="s">
-        <v>849</v>
+        <v>466</v>
       </c>
       <c r="D377" s="1" t="s">
-        <v>850</v>
+        <v>467</v>
       </c>
     </row>
     <row r="378" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A378" s="1" t="s">
-        <v>827</v>
+        <v>620</v>
       </c>
       <c r="B378" s="1" t="s">
-        <v>828</v>
+        <v>621</v>
       </c>
       <c r="D378" s="1" t="s">
-        <v>829</v>
+        <v>622</v>
       </c>
     </row>
     <row r="379" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A379" s="1" t="s">
-        <v>830</v>
+        <v>403</v>
       </c>
       <c r="B379" s="1" t="s">
-        <v>831</v>
+        <v>404</v>
       </c>
       <c r="D379" s="1" t="s">
-        <v>832</v>
+        <v>405</v>
       </c>
     </row>
     <row r="380" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A380" s="1" t="s">
-        <v>1157</v>
+        <v>406</v>
       </c>
       <c r="B380" s="1" t="s">
-        <v>1156</v>
+        <v>407</v>
       </c>
       <c r="D380" s="1" t="s">
-        <v>1155</v>
+        <v>408</v>
       </c>
     </row>
     <row r="381" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A381" s="1" t="s">
-        <v>1161</v>
+        <v>409</v>
       </c>
       <c r="B381" s="1" t="s">
-        <v>1162</v>
+        <v>410</v>
       </c>
       <c r="D381" s="1" t="s">
-        <v>1160</v>
+        <v>411</v>
       </c>
     </row>
     <row r="382" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A382" s="1" t="s">
-        <v>727</v>
+        <v>412</v>
       </c>
       <c r="B382" s="1" t="s">
-        <v>728</v>
+        <v>413</v>
       </c>
       <c r="D382" s="1" t="s">
-        <v>729</v>
+        <v>414</v>
       </c>
     </row>
     <row r="383" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A383" s="1" t="s">
-        <v>724</v>
+        <v>848</v>
       </c>
       <c r="B383" s="1" t="s">
-        <v>725</v>
+        <v>849</v>
       </c>
       <c r="D383" s="1" t="s">
-        <v>726</v>
+        <v>850</v>
       </c>
     </row>
     <row r="384" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A384" s="1" t="s">
-        <v>516</v>
+        <v>827</v>
       </c>
       <c r="B384" s="1" t="s">
-        <v>517</v>
+        <v>828</v>
       </c>
       <c r="D384" s="1" t="s">
-        <v>518</v>
+        <v>829</v>
       </c>
     </row>
     <row r="385" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A385" s="1" t="s">
-        <v>591</v>
+        <v>1168</v>
       </c>
       <c r="B385" s="1" t="s">
-        <v>592</v>
+        <v>1169</v>
       </c>
       <c r="D385" s="1" t="s">
-        <v>593</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="386" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A386" s="1" t="s">
-        <v>674</v>
+        <v>830</v>
       </c>
       <c r="B386" s="1" t="s">
-        <v>675</v>
+        <v>831</v>
       </c>
       <c r="D386" s="1" t="s">
-        <v>676</v>
+        <v>832</v>
       </c>
     </row>
     <row r="387" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A387" s="1" t="s">
-        <v>654</v>
+        <v>1157</v>
       </c>
       <c r="B387" s="1" t="s">
-        <v>655</v>
+        <v>1156</v>
       </c>
       <c r="D387" s="1" t="s">
-        <v>1035</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="388" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A388" s="1" t="s">
-        <v>1045</v>
+        <v>1161</v>
       </c>
       <c r="B388" s="1" t="s">
-        <v>1046</v>
+        <v>1162</v>
       </c>
       <c r="D388" s="1" t="s">
-        <v>1047</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="389" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A389" s="1" t="s">
-        <v>1028</v>
+        <v>727</v>
       </c>
       <c r="B389" s="1" t="s">
-        <v>1027</v>
+        <v>728</v>
       </c>
       <c r="D389" s="1" t="s">
-        <v>1029</v>
+        <v>729</v>
       </c>
     </row>
     <row r="390" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A390" s="1" t="s">
-        <v>842</v>
+        <v>724</v>
       </c>
       <c r="B390" s="1" t="s">
-        <v>843</v>
+        <v>725</v>
       </c>
       <c r="D390" s="1" t="s">
-        <v>844</v>
+        <v>726</v>
       </c>
     </row>
     <row r="391" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A391" s="1" t="s">
-        <v>866</v>
+        <v>516</v>
       </c>
       <c r="B391" s="1" t="s">
-        <v>867</v>
+        <v>517</v>
       </c>
       <c r="D391" s="1" t="s">
-        <v>868</v>
+        <v>518</v>
       </c>
     </row>
     <row r="392" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A392" s="1" t="s">
-        <v>471</v>
+        <v>591</v>
       </c>
       <c r="B392" s="1" t="s">
-        <v>472</v>
+        <v>592</v>
       </c>
       <c r="D392" s="1" t="s">
-        <v>473</v>
+        <v>593</v>
       </c>
     </row>
     <row r="393" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A393" s="1" t="s">
-        <v>975</v>
+        <v>674</v>
       </c>
       <c r="B393" s="1" t="s">
-        <v>922</v>
+        <v>675</v>
       </c>
       <c r="D393" s="1" t="s">
-        <v>1004</v>
+        <v>676</v>
       </c>
     </row>
     <row r="394" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A394" s="1" t="s">
-        <v>558</v>
+        <v>654</v>
       </c>
       <c r="B394" s="1" t="s">
-        <v>559</v>
+        <v>655</v>
       </c>
       <c r="D394" s="1" t="s">
-        <v>560</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="395" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A395" s="1" t="s">
-        <v>972</v>
+        <v>1045</v>
       </c>
       <c r="B395" s="1" t="s">
-        <v>921</v>
+        <v>1046</v>
       </c>
       <c r="D395" s="1" t="s">
-        <v>974</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="396" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A396" s="1" t="s">
-        <v>495</v>
+        <v>1028</v>
       </c>
       <c r="B396" s="1" t="s">
-        <v>496</v>
+        <v>1027</v>
       </c>
       <c r="D396" s="1" t="s">
-        <v>497</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="397" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A397" s="1" t="s">
-        <v>991</v>
+        <v>842</v>
       </c>
       <c r="B397" s="1" t="s">
-        <v>992</v>
+        <v>843</v>
       </c>
       <c r="D397" s="1" t="s">
-        <v>993</v>
+        <v>844</v>
       </c>
     </row>
     <row r="398" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A398" s="1" t="s">
-        <v>983</v>
+        <v>866</v>
       </c>
       <c r="B398" s="1" t="s">
-        <v>919</v>
+        <v>867</v>
       </c>
       <c r="D398" s="1" t="s">
-        <v>976</v>
+        <v>868</v>
       </c>
     </row>
     <row r="399" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A399" s="1" t="s">
-        <v>982</v>
+        <v>471</v>
       </c>
       <c r="B399" s="1" t="s">
-        <v>918</v>
+        <v>472</v>
       </c>
       <c r="D399" s="1" t="s">
-        <v>977</v>
+        <v>473</v>
       </c>
     </row>
     <row r="400" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A400" s="1" t="s">
-        <v>901</v>
+        <v>975</v>
       </c>
       <c r="B400" s="1" t="s">
-        <v>902</v>
+        <v>922</v>
       </c>
       <c r="D400" s="1" t="s">
-        <v>903</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="401" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A401" s="1" t="s">
-        <v>480</v>
+        <v>558</v>
       </c>
       <c r="B401" s="1" t="s">
-        <v>481</v>
+        <v>559</v>
       </c>
       <c r="D401" s="1" t="s">
-        <v>482</v>
+        <v>560</v>
       </c>
     </row>
     <row r="402" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A402" s="1" t="s">
-        <v>1073</v>
+        <v>972</v>
       </c>
       <c r="B402" s="1" t="s">
-        <v>1074</v>
+        <v>921</v>
       </c>
       <c r="D402" s="1" t="s">
-        <v>1014</v>
+        <v>974</v>
       </c>
     </row>
     <row r="403" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A403" s="1" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="B403" s="1" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="D403" s="1" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
     </row>
     <row r="404" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A404" s="1" t="s">
-        <v>483</v>
+        <v>1175</v>
       </c>
       <c r="B404" s="1" t="s">
-        <v>484</v>
+        <v>1176</v>
       </c>
       <c r="D404" s="1" t="s">
-        <v>485</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="405" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A405" s="1" t="s">
-        <v>486</v>
+        <v>991</v>
       </c>
       <c r="B405" s="1" t="s">
-        <v>487</v>
+        <v>992</v>
       </c>
       <c r="D405" s="1" t="s">
-        <v>488</v>
+        <v>993</v>
       </c>
     </row>
     <row r="406" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A406" s="1" t="s">
-        <v>944</v>
+        <v>983</v>
       </c>
       <c r="B406" s="1" t="s">
-        <v>945</v>
+        <v>919</v>
       </c>
       <c r="D406" s="1" t="s">
-        <v>946</v>
+        <v>976</v>
       </c>
     </row>
     <row r="407" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A407" s="1" t="s">
-        <v>704</v>
+        <v>982</v>
       </c>
       <c r="B407" s="1" t="s">
-        <v>705</v>
+        <v>918</v>
       </c>
       <c r="D407" s="1" t="s">
-        <v>706</v>
+        <v>977</v>
       </c>
     </row>
     <row r="408" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A408" s="1" t="s">
-        <v>800</v>
+        <v>901</v>
       </c>
       <c r="B408" s="1" t="s">
-        <v>801</v>
+        <v>902</v>
       </c>
       <c r="D408" s="1" t="s">
-        <v>802</v>
+        <v>903</v>
       </c>
     </row>
     <row r="409" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A409" s="1" t="s">
-        <v>531</v>
+        <v>480</v>
       </c>
       <c r="B409" s="1" t="s">
-        <v>532</v>
+        <v>481</v>
       </c>
       <c r="D409" s="1" t="s">
-        <v>533</v>
+        <v>482</v>
       </c>
     </row>
     <row r="410" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A410" s="1" t="s">
-        <v>501</v>
+        <v>1073</v>
       </c>
       <c r="B410" s="1" t="s">
-        <v>502</v>
+        <v>1074</v>
       </c>
       <c r="D410" s="1" t="s">
-        <v>503</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="411" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A411" s="1" t="s">
-        <v>415</v>
+        <v>498</v>
       </c>
       <c r="B411" s="1" t="s">
-        <v>416</v>
+        <v>499</v>
       </c>
       <c r="D411" s="1" t="s">
-        <v>417</v>
+        <v>500</v>
       </c>
     </row>
     <row r="412" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A412" s="1" t="s">
-        <v>504</v>
+        <v>483</v>
       </c>
       <c r="B412" s="1" t="s">
-        <v>505</v>
+        <v>484</v>
       </c>
       <c r="D412" s="1" t="s">
-        <v>506</v>
+        <v>485</v>
       </c>
     </row>
     <row r="413" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A413" s="1" t="s">
-        <v>721</v>
+        <v>1165</v>
       </c>
       <c r="B413" s="1" t="s">
-        <v>722</v>
+        <v>1166</v>
       </c>
       <c r="D413" s="1" t="s">
-        <v>723</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="414" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A414" s="1" t="s">
-        <v>555</v>
+        <v>486</v>
       </c>
       <c r="B414" s="1" t="s">
-        <v>556</v>
+        <v>487</v>
       </c>
       <c r="D414" s="1" t="s">
-        <v>557</v>
+        <v>488</v>
       </c>
     </row>
     <row r="415" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A415" s="1" t="s">
-        <v>561</v>
+        <v>944</v>
       </c>
       <c r="B415" s="1" t="s">
-        <v>562</v>
+        <v>945</v>
       </c>
       <c r="D415" s="1" t="s">
-        <v>563</v>
+        <v>946</v>
       </c>
     </row>
     <row r="416" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A416" s="1" t="s">
-        <v>549</v>
+        <v>704</v>
       </c>
       <c r="B416" s="1" t="s">
-        <v>550</v>
+        <v>705</v>
       </c>
       <c r="D416" s="1" t="s">
-        <v>551</v>
+        <v>706</v>
       </c>
     </row>
     <row r="417" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A417" s="1" t="s">
-        <v>763</v>
+        <v>800</v>
       </c>
       <c r="B417" s="1" t="s">
-        <v>764</v>
+        <v>801</v>
       </c>
       <c r="D417" s="1" t="s">
-        <v>551</v>
+        <v>802</v>
       </c>
     </row>
     <row r="418" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A418" s="1" t="s">
-        <v>618</v>
+        <v>531</v>
       </c>
       <c r="B418" s="1" t="s">
-        <v>619</v>
+        <v>532</v>
       </c>
       <c r="D418" s="1" t="s">
-        <v>1011</v>
+        <v>533</v>
       </c>
     </row>
     <row r="419" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A419" s="1" t="s">
-        <v>606</v>
+        <v>501</v>
       </c>
       <c r="B419" s="1" t="s">
-        <v>607</v>
+        <v>502</v>
       </c>
       <c r="D419" s="1" t="s">
-        <v>608</v>
+        <v>503</v>
       </c>
     </row>
     <row r="420" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A420" s="1" t="s">
-        <v>450</v>
+        <v>415</v>
       </c>
       <c r="B420" s="1" t="s">
-        <v>451</v>
+        <v>416</v>
       </c>
       <c r="D420" s="1" t="s">
-        <v>452</v>
+        <v>417</v>
       </c>
     </row>
     <row r="421" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A421" s="1" t="s">
-        <v>689</v>
+        <v>504</v>
       </c>
       <c r="B421" s="1" t="s">
-        <v>690</v>
+        <v>505</v>
       </c>
       <c r="D421" s="1" t="s">
-        <v>691</v>
+        <v>506</v>
       </c>
     </row>
     <row r="422" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A422" s="1" t="s">
-        <v>453</v>
+        <v>721</v>
       </c>
       <c r="B422" s="1" t="s">
-        <v>454</v>
+        <v>722</v>
       </c>
       <c r="D422" s="1" t="s">
-        <v>455</v>
+        <v>723</v>
       </c>
     </row>
     <row r="423" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A423" s="1" t="s">
-        <v>765</v>
+        <v>555</v>
       </c>
       <c r="B423" s="1" t="s">
-        <v>766</v>
+        <v>556</v>
       </c>
       <c r="D423" s="1" t="s">
-        <v>767</v>
+        <v>557</v>
       </c>
     </row>
     <row r="424" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A424" s="1" t="s">
-        <v>1051</v>
+        <v>561</v>
       </c>
       <c r="B424" s="1" t="s">
-        <v>1052</v>
+        <v>562</v>
       </c>
       <c r="D424" s="1" t="s">
-        <v>1053</v>
+        <v>563</v>
       </c>
     </row>
     <row r="425" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A425" s="1" t="s">
-        <v>821</v>
+        <v>549</v>
       </c>
       <c r="B425" s="1" t="s">
-        <v>822</v>
+        <v>550</v>
       </c>
       <c r="D425" s="1" t="s">
-        <v>823</v>
+        <v>551</v>
       </c>
     </row>
     <row r="426" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A426" s="1" t="s">
-        <v>421</v>
+        <v>763</v>
       </c>
       <c r="B426" s="1" t="s">
-        <v>422</v>
+        <v>764</v>
       </c>
       <c r="D426" s="1" t="s">
-        <v>423</v>
+        <v>551</v>
       </c>
     </row>
     <row r="427" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A427" s="1" t="s">
-        <v>1016</v>
+        <v>618</v>
       </c>
       <c r="B427" s="1" t="s">
-        <v>1017</v>
+        <v>619</v>
       </c>
       <c r="D427" s="1" t="s">
-        <v>1018</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="428" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A428" s="1" t="s">
-        <v>744</v>
+        <v>606</v>
       </c>
       <c r="B428" s="1" t="s">
-        <v>745</v>
+        <v>607</v>
       </c>
       <c r="D428" s="1" t="s">
-        <v>746</v>
+        <v>608</v>
       </c>
     </row>
     <row r="429" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A429" s="1" t="s">
-        <v>905</v>
+        <v>1184</v>
       </c>
       <c r="B429" s="1" t="s">
-        <v>904</v>
+        <v>1191</v>
       </c>
       <c r="D429" s="1" t="s">
-        <v>906</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="430" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A430" s="1" t="s">
-        <v>907</v>
+        <v>1185</v>
       </c>
       <c r="B430" s="1" t="s">
-        <v>908</v>
+        <v>1192</v>
       </c>
       <c r="D430" s="1" t="s">
-        <v>909</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="431" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A431" s="1" t="s">
-        <v>540</v>
+        <v>450</v>
       </c>
       <c r="B431" s="1" t="s">
-        <v>541</v>
+        <v>451</v>
       </c>
       <c r="D431" s="1" t="s">
-        <v>542</v>
+        <v>452</v>
       </c>
     </row>
     <row r="432" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A432" s="1" t="s">
-        <v>662</v>
+        <v>1171</v>
       </c>
       <c r="B432" s="1" t="s">
-        <v>663</v>
+        <v>1172</v>
       </c>
       <c r="D432" s="1" t="s">
-        <v>664</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="433" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A433" s="1" t="s">
-        <v>692</v>
+        <v>1186</v>
       </c>
       <c r="B433" s="1" t="s">
-        <v>693</v>
+        <v>1193</v>
       </c>
       <c r="D433" s="1" t="s">
-        <v>694</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="434" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A434" s="1" t="s">
-        <v>967</v>
+        <v>1187</v>
       </c>
       <c r="B434" s="1" t="s">
-        <v>926</v>
+        <v>1194</v>
       </c>
       <c r="D434" s="1" t="s">
-        <v>912</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="435" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A435" s="1" t="s">
-        <v>786</v>
+        <v>689</v>
       </c>
       <c r="B435" s="1" t="s">
-        <v>787</v>
+        <v>690</v>
       </c>
       <c r="D435" s="1" t="s">
-        <v>788</v>
+        <v>691</v>
       </c>
     </row>
     <row r="436" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A436" s="1" t="s">
-        <v>623</v>
+        <v>453</v>
       </c>
       <c r="B436" s="1" t="s">
-        <v>624</v>
+        <v>454</v>
       </c>
       <c r="D436" s="1" t="s">
-        <v>625</v>
+        <v>455</v>
       </c>
     </row>
     <row r="437" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A437" s="1" t="s">
-        <v>836</v>
+        <v>765</v>
       </c>
       <c r="B437" s="1" t="s">
-        <v>837</v>
+        <v>766</v>
       </c>
       <c r="D437" s="1" t="s">
-        <v>838</v>
+        <v>767</v>
       </c>
     </row>
     <row r="438" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A438" s="1" t="s">
-        <v>686</v>
+        <v>1051</v>
       </c>
       <c r="B438" s="1" t="s">
-        <v>687</v>
+        <v>1052</v>
       </c>
       <c r="D438" s="1" t="s">
-        <v>688</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="439" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A439" s="1" t="s">
-        <v>896</v>
+        <v>821</v>
       </c>
       <c r="B439" s="1" t="s">
-        <v>897</v>
+        <v>822</v>
+      </c>
+      <c r="D439" s="1" t="s">
+        <v>823</v>
       </c>
     </row>
     <row r="440" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A440" s="1" t="s">
-        <v>971</v>
+        <v>421</v>
       </c>
       <c r="B440" s="1" t="s">
-        <v>920</v>
+        <v>422</v>
       </c>
       <c r="D440" s="1" t="s">
-        <v>973</v>
+        <v>423</v>
       </c>
     </row>
     <row r="441" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A441" s="1" t="s">
-        <v>950</v>
+        <v>1016</v>
       </c>
       <c r="B441" s="1" t="s">
-        <v>951</v>
+        <v>1017</v>
       </c>
       <c r="D441" s="1" t="s">
-        <v>952</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="442" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A442" s="1" t="s">
-        <v>474</v>
+        <v>744</v>
       </c>
       <c r="B442" s="1" t="s">
-        <v>475</v>
+        <v>745</v>
       </c>
       <c r="D442" s="1" t="s">
-        <v>476</v>
+        <v>746</v>
       </c>
     </row>
     <row r="443" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A443" s="1" t="s">
-        <v>567</v>
+        <v>905</v>
       </c>
       <c r="B443" s="1" t="s">
-        <v>568</v>
+        <v>904</v>
       </c>
       <c r="D443" s="1" t="s">
-        <v>569</v>
+        <v>906</v>
       </c>
     </row>
     <row r="444" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A444" s="1" t="s">
-        <v>768</v>
+        <v>907</v>
       </c>
       <c r="B444" s="1" t="s">
-        <v>769</v>
+        <v>908</v>
       </c>
       <c r="D444" s="1" t="s">
-        <v>770</v>
+        <v>909</v>
       </c>
     </row>
     <row r="445" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A445" s="1" t="s">
-        <v>771</v>
+        <v>540</v>
       </c>
       <c r="B445" s="1" t="s">
-        <v>772</v>
+        <v>541</v>
       </c>
       <c r="D445" s="1" t="s">
-        <v>354</v>
+        <v>542</v>
       </c>
     </row>
     <row r="446" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A446" s="1" t="s">
-        <v>712</v>
+        <v>662</v>
       </c>
       <c r="B446" s="1" t="s">
-        <v>713</v>
+        <v>663</v>
       </c>
       <c r="D446" s="1" t="s">
-        <v>714</v>
+        <v>664</v>
       </c>
     </row>
     <row r="447" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A447" s="1" t="s">
-        <v>881</v>
+        <v>692</v>
       </c>
       <c r="B447" s="1" t="s">
-        <v>882</v>
+        <v>693</v>
       </c>
       <c r="D447" s="1" t="s">
-        <v>883</v>
+        <v>694</v>
       </c>
     </row>
     <row r="448" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A448" s="1" t="s">
-        <v>1147</v>
+        <v>967</v>
       </c>
       <c r="B448" s="1" t="s">
-        <v>1148</v>
+        <v>926</v>
       </c>
       <c r="D448" s="1" t="s">
-        <v>1146</v>
+        <v>912</v>
       </c>
     </row>
     <row r="449" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A449" s="1" t="s">
-        <v>953</v>
+        <v>786</v>
       </c>
       <c r="B449" s="1" t="s">
-        <v>955</v>
+        <v>787</v>
       </c>
       <c r="D449" s="1" t="s">
-        <v>956</v>
+        <v>788</v>
       </c>
     </row>
     <row r="450" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A450" s="1" t="s">
-        <v>747</v>
+        <v>623</v>
       </c>
       <c r="B450" s="1" t="s">
-        <v>748</v>
+        <v>624</v>
       </c>
       <c r="D450" s="1" t="s">
-        <v>749</v>
+        <v>625</v>
       </c>
     </row>
     <row r="451" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A451" s="1" t="s">
-        <v>576</v>
+        <v>836</v>
       </c>
       <c r="B451" s="1" t="s">
-        <v>577</v>
+        <v>837</v>
       </c>
       <c r="D451" s="1" t="s">
-        <v>578</v>
+        <v>838</v>
       </c>
     </row>
     <row r="452" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A452" s="1" t="s">
-        <v>824</v>
+        <v>686</v>
       </c>
       <c r="B452" s="1" t="s">
-        <v>825</v>
+        <v>687</v>
       </c>
       <c r="D452" s="1" t="s">
-        <v>826</v>
+        <v>688</v>
       </c>
     </row>
     <row r="453" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A453" s="1" t="s">
-        <v>1024</v>
+        <v>896</v>
       </c>
       <c r="B453" s="1" t="s">
-        <v>1025</v>
-      </c>
-      <c r="D453" s="1" t="s">
-        <v>1026</v>
+        <v>897</v>
       </c>
     </row>
     <row r="454" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A454" s="1" t="s">
-        <v>427</v>
+        <v>971</v>
       </c>
       <c r="B454" s="1" t="s">
-        <v>428</v>
+        <v>920</v>
       </c>
       <c r="D454" s="1" t="s">
-        <v>429</v>
+        <v>973</v>
       </c>
     </row>
     <row r="455" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A455" s="1" t="s">
-        <v>626</v>
+        <v>950</v>
       </c>
       <c r="B455" s="1" t="s">
-        <v>627</v>
+        <v>951</v>
       </c>
       <c r="D455" s="1" t="s">
-        <v>628</v>
+        <v>952</v>
       </c>
     </row>
     <row r="456" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A456" s="1" t="s">
-        <v>418</v>
+        <v>474</v>
       </c>
       <c r="B456" s="1" t="s">
-        <v>419</v>
+        <v>475</v>
       </c>
       <c r="D456" s="1" t="s">
-        <v>420</v>
+        <v>476</v>
       </c>
     </row>
     <row r="457" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A457" s="1" t="s">
-        <v>932</v>
+        <v>567</v>
       </c>
       <c r="B457" s="1" t="s">
-        <v>933</v>
+        <v>568</v>
       </c>
       <c r="D457" s="1" t="s">
-        <v>934</v>
+        <v>569</v>
       </c>
     </row>
     <row r="458" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A458" s="1" t="s">
-        <v>735</v>
+        <v>768</v>
       </c>
       <c r="B458" s="1" t="s">
-        <v>736</v>
+        <v>769</v>
       </c>
       <c r="D458" s="1" t="s">
-        <v>737</v>
+        <v>770</v>
       </c>
     </row>
     <row r="459" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A459" s="1" t="s">
-        <v>738</v>
+        <v>771</v>
       </c>
       <c r="B459" s="1" t="s">
-        <v>739</v>
+        <v>772</v>
       </c>
       <c r="D459" s="1" t="s">
-        <v>740</v>
+        <v>354</v>
       </c>
     </row>
     <row r="460" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A460" s="1" t="s">
-        <v>741</v>
+        <v>712</v>
       </c>
       <c r="B460" s="1" t="s">
-        <v>742</v>
+        <v>713</v>
       </c>
       <c r="D460" s="1" t="s">
-        <v>743</v>
+        <v>714</v>
       </c>
     </row>
     <row r="461" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A461" s="1" t="s">
-        <v>629</v>
+        <v>881</v>
       </c>
       <c r="B461" s="1" t="s">
-        <v>630</v>
+        <v>882</v>
       </c>
       <c r="D461" s="1" t="s">
-        <v>631</v>
+        <v>883</v>
       </c>
     </row>
     <row r="462" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A462" s="1" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B462" s="1" t="s">
+        <v>1148</v>
+      </c>
+      <c r="D462" s="1" t="s">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="463" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A463" s="1" t="s">
+        <v>953</v>
+      </c>
+      <c r="B463" s="1" t="s">
+        <v>955</v>
+      </c>
+      <c r="D463" s="1" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="464" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A464" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="B464" s="1" t="s">
+        <v>748</v>
+      </c>
+      <c r="D464" s="1" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="465" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A465" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="B465" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="D465" s="1" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="466" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A466" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="B466" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="D466" s="1" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="467" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A467" s="1" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B467" s="1" t="s">
+        <v>1025</v>
+      </c>
+      <c r="D467" s="1" t="s">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="468" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A468" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="B468" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="D468" s="1" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="469" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A469" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="B469" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="D469" s="1" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="470" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A470" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="B470" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="D470" s="1" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="471" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A471" s="1" t="s">
+        <v>932</v>
+      </c>
+      <c r="B471" s="1" t="s">
+        <v>933</v>
+      </c>
+      <c r="D471" s="1" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="472" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A472" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="B472" s="1" t="s">
+        <v>736</v>
+      </c>
+      <c r="D472" s="1" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="473" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A473" s="1" t="s">
+        <v>738</v>
+      </c>
+      <c r="B473" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="D473" s="1" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="474" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A474" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="B474" s="1" t="s">
+        <v>742</v>
+      </c>
+      <c r="D474" s="1" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="475" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A475" s="1" t="s">
+        <v>629</v>
+      </c>
+      <c r="B475" s="1" t="s">
+        <v>630</v>
+      </c>
+      <c r="D475" s="1" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="476" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A476" s="1" t="s">
         <v>632</v>
       </c>
-      <c r="B462" s="1" t="s">
+      <c r="B476" s="1" t="s">
         <v>633</v>
       </c>
-      <c r="D462" s="1" t="s">
+      <c r="D476" s="1" t="s">
         <v>634</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Follow Play Framework v2.6.10
</commit_message>
<xml_diff>
--- a/conf/messages.xlsx
+++ b/conf/messages.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1260" uniqueCount="1208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1266" uniqueCount="1214">
   <si>
     <t>key</t>
   </si>
@@ -4076,6 +4076,36 @@
     <t>概要</t>
     <rPh sb="0" eb="2">
       <t>ガイヨ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>full_text</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Full text</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>全文</t>
+    <rPh sb="0" eb="2">
+      <t>ゼンb</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>convert</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Convert</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>変換</t>
+    <rPh sb="0" eb="2">
+      <t>ヘンカn</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -4691,10 +4721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G477"/>
+  <dimension ref="A1:G479"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A275" workbookViewId="0">
-      <selection activeCell="D438" sqref="D438"/>
+    <sheetView tabSelected="1" topLeftCell="A265" workbookViewId="0">
+      <selection activeCell="J274" sqref="J274"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -7149,2227 +7179,2249 @@
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A274" s="1" t="s">
-        <v>1154</v>
+        <v>1211</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>1153</v>
+        <v>1212</v>
       </c>
       <c r="D274" s="1" t="s">
-        <v>1152</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A275" s="1" t="s">
-        <v>468</v>
+        <v>1154</v>
       </c>
       <c r="B275" s="1" t="s">
-        <v>469</v>
+        <v>1153</v>
       </c>
       <c r="D275" s="1" t="s">
-        <v>470</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A276" s="1" t="s">
-        <v>779</v>
+        <v>468</v>
       </c>
       <c r="B276" s="1" t="s">
-        <v>780</v>
+        <v>469</v>
       </c>
       <c r="D276" s="1" t="s">
-        <v>781</v>
+        <v>470</v>
       </c>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A277" s="1" t="s">
-        <v>1149</v>
+        <v>779</v>
       </c>
       <c r="B277" s="1" t="s">
-        <v>1150</v>
+        <v>780</v>
       </c>
       <c r="D277" s="1" t="s">
-        <v>1151</v>
+        <v>781</v>
       </c>
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A278" s="1" t="s">
-        <v>579</v>
+        <v>1149</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>580</v>
+        <v>1150</v>
       </c>
       <c r="D278" s="1" t="s">
-        <v>581</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A279" s="1" t="s">
-        <v>537</v>
+        <v>579</v>
       </c>
       <c r="B279" s="1" t="s">
-        <v>538</v>
+        <v>580</v>
       </c>
       <c r="D279" s="1" t="s">
-        <v>539</v>
+        <v>581</v>
       </c>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A280" s="1" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
       <c r="D280" s="1" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A281" s="1" t="s">
-        <v>1019</v>
+        <v>534</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>1020</v>
+        <v>535</v>
       </c>
       <c r="D281" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A282" s="1" t="s">
-        <v>1</v>
+        <v>1019</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>5</v>
+        <v>1020</v>
       </c>
       <c r="D282" s="1" t="s">
-        <v>222</v>
+        <v>539</v>
       </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A283" s="1" t="s">
-        <v>477</v>
+        <v>1</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>478</v>
+        <v>5</v>
       </c>
       <c r="D283" s="1" t="s">
-        <v>479</v>
+        <v>222</v>
       </c>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A284" s="1" t="s">
-        <v>668</v>
+        <v>477</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>669</v>
+        <v>478</v>
       </c>
       <c r="D284" s="1" t="s">
-        <v>670</v>
+        <v>479</v>
       </c>
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A285" s="1" t="s">
-        <v>507</v>
+        <v>668</v>
       </c>
       <c r="B285" s="1" t="s">
-        <v>508</v>
+        <v>669</v>
       </c>
       <c r="D285" s="1" t="s">
-        <v>509</v>
+        <v>670</v>
       </c>
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A286" s="1" t="s">
-        <v>851</v>
+        <v>507</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>852</v>
+        <v>508</v>
       </c>
       <c r="D286" s="1" t="s">
-        <v>853</v>
+        <v>509</v>
       </c>
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A287" s="1" t="s">
-        <v>644</v>
+        <v>851</v>
       </c>
       <c r="B287" s="1" t="s">
-        <v>645</v>
+        <v>852</v>
       </c>
       <c r="D287" s="1" t="s">
-        <v>646</v>
+        <v>853</v>
       </c>
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A288" s="1" t="s">
-        <v>789</v>
+        <v>644</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>790</v>
+        <v>645</v>
       </c>
       <c r="D288" s="1" t="s">
-        <v>791</v>
+        <v>646</v>
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A289" s="1" t="s">
-        <v>680</v>
+        <v>789</v>
       </c>
       <c r="B289" s="1" t="s">
-        <v>681</v>
+        <v>790</v>
       </c>
       <c r="D289" s="1" t="s">
-        <v>682</v>
+        <v>791</v>
       </c>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A290" s="1" t="s">
-        <v>424</v>
+        <v>680</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>425</v>
+        <v>681</v>
       </c>
       <c r="D290" s="1" t="s">
-        <v>426</v>
+        <v>682</v>
       </c>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A291" s="1" t="s">
-        <v>947</v>
+        <v>424</v>
       </c>
       <c r="B291" s="1" t="s">
-        <v>948</v>
+        <v>425</v>
       </c>
       <c r="D291" s="1" t="s">
-        <v>949</v>
+        <v>426</v>
       </c>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A292" s="1" t="s">
-        <v>570</v>
+        <v>947</v>
       </c>
       <c r="B292" s="1" t="s">
-        <v>571</v>
+        <v>948</v>
       </c>
       <c r="D292" s="1" t="s">
-        <v>572</v>
+        <v>949</v>
       </c>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A293" s="1" t="s">
-        <v>519</v>
+        <v>570</v>
       </c>
       <c r="B293" s="1" t="s">
-        <v>520</v>
+        <v>571</v>
       </c>
       <c r="D293" s="1" t="s">
-        <v>521</v>
+        <v>572</v>
       </c>
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A294" s="1" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="D294" s="1" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A295" s="1" t="s">
-        <v>1036</v>
+        <v>522</v>
       </c>
       <c r="B295" s="1" t="s">
-        <v>1037</v>
+        <v>523</v>
       </c>
       <c r="D295" s="1" t="s">
-        <v>1038</v>
+        <v>524</v>
       </c>
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A296" s="1" t="s">
-        <v>492</v>
+        <v>1036</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>493</v>
+        <v>1037</v>
       </c>
       <c r="D296" s="1" t="s">
-        <v>494</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A297" s="1" t="s">
-        <v>773</v>
+        <v>492</v>
       </c>
       <c r="B297" s="1" t="s">
-        <v>24</v>
+        <v>493</v>
       </c>
       <c r="D297" s="1" t="s">
-        <v>774</v>
+        <v>494</v>
       </c>
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A298" s="1" t="s">
-        <v>462</v>
+        <v>773</v>
       </c>
       <c r="B298" s="1" t="s">
-        <v>463</v>
+        <v>24</v>
       </c>
       <c r="D298" s="1" t="s">
-        <v>464</v>
+        <v>774</v>
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A299" s="1" t="s">
-        <v>609</v>
+        <v>462</v>
       </c>
       <c r="B299" s="1" t="s">
-        <v>610</v>
+        <v>463</v>
       </c>
       <c r="D299" s="1" t="s">
-        <v>611</v>
+        <v>464</v>
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A300" s="1" t="s">
-        <v>794</v>
+        <v>609</v>
       </c>
       <c r="B300" s="1" t="s">
-        <v>795</v>
+        <v>610</v>
       </c>
       <c r="D300" s="1" t="s">
-        <v>796</v>
+        <v>611</v>
       </c>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A301" s="1" t="s">
-        <v>582</v>
+        <v>794</v>
       </c>
       <c r="B301" s="1" t="s">
-        <v>583</v>
+        <v>795</v>
       </c>
       <c r="D301" s="1" t="s">
-        <v>584</v>
+        <v>796</v>
       </c>
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A302" s="1" t="s">
-        <v>1012</v>
+        <v>582</v>
       </c>
       <c r="B302" s="1" t="s">
-        <v>1013</v>
+        <v>583</v>
       </c>
       <c r="D302" s="1" t="s">
-        <v>1014</v>
+        <v>584</v>
       </c>
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A303" s="1" t="s">
-        <v>803</v>
+        <v>1012</v>
       </c>
       <c r="B303" s="1" t="s">
-        <v>804</v>
+        <v>1013</v>
       </c>
       <c r="D303" s="1" t="s">
-        <v>805</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A304" s="1" t="s">
-        <v>1189</v>
+        <v>803</v>
       </c>
       <c r="B304" s="1" t="s">
-        <v>1196</v>
+        <v>804</v>
       </c>
       <c r="D304" s="1" t="s">
-        <v>1203</v>
+        <v>805</v>
       </c>
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A305" s="1" t="s">
-        <v>456</v>
+        <v>1189</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>457</v>
+        <v>1196</v>
       </c>
       <c r="D305" s="1" t="s">
-        <v>458</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A306" s="1" t="s">
-        <v>839</v>
+        <v>456</v>
       </c>
       <c r="B306" s="1" t="s">
-        <v>840</v>
+        <v>457</v>
       </c>
       <c r="D306" s="1" t="s">
-        <v>841</v>
+        <v>458</v>
       </c>
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A307" s="1" t="s">
-        <v>1042</v>
+        <v>839</v>
       </c>
       <c r="B307" s="1" t="s">
-        <v>1043</v>
+        <v>840</v>
       </c>
       <c r="D307" s="1" t="s">
-        <v>1044</v>
+        <v>841</v>
       </c>
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A308" s="1" t="s">
-        <v>715</v>
+        <v>1042</v>
       </c>
       <c r="B308" s="1" t="s">
-        <v>716</v>
+        <v>1043</v>
       </c>
       <c r="D308" s="1" t="s">
-        <v>717</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A309" s="1" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
       <c r="B309" s="1" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
       <c r="D309" s="1" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A310" s="1" t="s">
-        <v>615</v>
+        <v>718</v>
       </c>
       <c r="B310" s="1" t="s">
-        <v>616</v>
+        <v>719</v>
       </c>
       <c r="D310" s="1" t="s">
-        <v>617</v>
+        <v>720</v>
       </c>
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A311" s="1" t="s">
-        <v>585</v>
+        <v>615</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>586</v>
+        <v>616</v>
       </c>
       <c r="D311" s="1" t="s">
-        <v>587</v>
+        <v>617</v>
       </c>
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A312" s="1" t="s">
-        <v>612</v>
+        <v>585</v>
       </c>
       <c r="B312" s="1" t="s">
-        <v>613</v>
+        <v>586</v>
       </c>
       <c r="D312" s="1" t="s">
-        <v>614</v>
+        <v>587</v>
       </c>
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A313" s="1" t="s">
-        <v>756</v>
+        <v>612</v>
       </c>
       <c r="B313" s="1" t="s">
-        <v>757</v>
+        <v>613</v>
       </c>
       <c r="D313" s="1" t="s">
-        <v>758</v>
+        <v>614</v>
       </c>
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A314" s="1" t="s">
-        <v>894</v>
+        <v>756</v>
       </c>
       <c r="B314" s="1" t="s">
-        <v>895</v>
+        <v>757</v>
+      </c>
+      <c r="D314" s="1" t="s">
+        <v>758</v>
       </c>
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A315" s="1" t="s">
-        <v>701</v>
+        <v>894</v>
       </c>
       <c r="B315" s="1" t="s">
-        <v>702</v>
-      </c>
-      <c r="D315" s="1" t="s">
-        <v>703</v>
+        <v>895</v>
       </c>
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A316" s="1" t="s">
-        <v>683</v>
+        <v>701</v>
       </c>
       <c r="B316" s="1" t="s">
-        <v>684</v>
+        <v>702</v>
       </c>
       <c r="D316" s="1" t="s">
-        <v>685</v>
+        <v>703</v>
       </c>
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A317" s="1" t="s">
-        <v>792</v>
+        <v>683</v>
       </c>
       <c r="B317" s="1" t="s">
-        <v>793</v>
+        <v>684</v>
       </c>
       <c r="D317" s="1" t="s">
-        <v>962</v>
+        <v>685</v>
       </c>
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A318" s="1" t="s">
-        <v>775</v>
+        <v>792</v>
       </c>
       <c r="B318" s="1" t="s">
-        <v>776</v>
+        <v>793</v>
       </c>
       <c r="D318" s="1" t="s">
-        <v>432</v>
+        <v>962</v>
       </c>
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A319" s="1" t="s">
-        <v>833</v>
+        <v>775</v>
       </c>
       <c r="B319" s="1" t="s">
-        <v>834</v>
+        <v>776</v>
       </c>
       <c r="D319" s="1" t="s">
-        <v>835</v>
+        <v>432</v>
       </c>
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A320" s="1" t="s">
-        <v>638</v>
+        <v>833</v>
       </c>
       <c r="B320" s="1" t="s">
-        <v>639</v>
+        <v>834</v>
       </c>
       <c r="D320" s="1" t="s">
-        <v>640</v>
+        <v>835</v>
       </c>
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A321" s="1" t="s">
-        <v>552</v>
+        <v>1208</v>
       </c>
       <c r="B321" s="1" t="s">
-        <v>553</v>
+        <v>1209</v>
       </c>
       <c r="D321" s="1" t="s">
-        <v>554</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A322" s="1" t="s">
-        <v>959</v>
+        <v>638</v>
       </c>
       <c r="B322" s="1" t="s">
-        <v>960</v>
+        <v>639</v>
       </c>
       <c r="D322" s="1" t="s">
-        <v>961</v>
+        <v>640</v>
       </c>
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A323" s="1" t="s">
-        <v>1031</v>
+        <v>552</v>
       </c>
       <c r="B323" s="1" t="s">
-        <v>1030</v>
+        <v>553</v>
       </c>
       <c r="D323" s="1" t="s">
-        <v>1032</v>
+        <v>554</v>
       </c>
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A324" s="1" t="s">
-        <v>695</v>
+        <v>959</v>
       </c>
       <c r="B324" s="1" t="s">
-        <v>696</v>
+        <v>960</v>
       </c>
       <c r="D324" s="1" t="s">
-        <v>697</v>
+        <v>961</v>
       </c>
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A325" s="1" t="s">
-        <v>677</v>
+        <v>1031</v>
       </c>
       <c r="B325" s="1" t="s">
-        <v>678</v>
+        <v>1030</v>
       </c>
       <c r="D325" s="1" t="s">
-        <v>679</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A326" s="1" t="s">
-        <v>875</v>
+        <v>695</v>
       </c>
       <c r="B326" s="1" t="s">
-        <v>876</v>
+        <v>696</v>
       </c>
       <c r="D326" s="1" t="s">
-        <v>877</v>
+        <v>697</v>
       </c>
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A327" s="1" t="s">
-        <v>958</v>
+        <v>677</v>
       </c>
       <c r="B327" s="1" t="s">
-        <v>957</v>
+        <v>678</v>
       </c>
       <c r="D327" s="1" t="s">
-        <v>759</v>
+        <v>679</v>
       </c>
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A328" s="1" t="s">
-        <v>1009</v>
+        <v>875</v>
       </c>
       <c r="B328" s="1" t="s">
-        <v>1010</v>
+        <v>876</v>
       </c>
       <c r="D328" s="1" t="s">
-        <v>954</v>
+        <v>877</v>
       </c>
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A329" s="1" t="s">
-        <v>886</v>
+        <v>958</v>
       </c>
       <c r="B329" s="1" t="s">
-        <v>887</v>
+        <v>957</v>
+      </c>
+      <c r="D329" s="1" t="s">
+        <v>759</v>
       </c>
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A330" s="1" t="s">
-        <v>857</v>
+        <v>1009</v>
       </c>
       <c r="B330" s="1" t="s">
-        <v>858</v>
+        <v>1010</v>
       </c>
       <c r="D330" s="1" t="s">
-        <v>859</v>
+        <v>954</v>
       </c>
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A331" s="1" t="s">
-        <v>884</v>
+        <v>886</v>
       </c>
       <c r="B331" s="1" t="s">
-        <v>885</v>
+        <v>887</v>
       </c>
     </row>
     <row r="332" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A332" s="1" t="s">
-        <v>753</v>
+        <v>857</v>
       </c>
       <c r="B332" s="1" t="s">
-        <v>754</v>
+        <v>858</v>
       </c>
       <c r="D332" s="1" t="s">
-        <v>755</v>
+        <v>859</v>
       </c>
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A333" s="1" t="s">
-        <v>573</v>
+        <v>884</v>
       </c>
       <c r="B333" s="1" t="s">
-        <v>574</v>
-      </c>
-      <c r="D333" s="1" t="s">
-        <v>575</v>
+        <v>885</v>
       </c>
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A334" s="1" t="s">
-        <v>777</v>
+        <v>753</v>
       </c>
       <c r="B334" s="1" t="s">
-        <v>778</v>
+        <v>754</v>
       </c>
       <c r="D334" s="1" t="s">
-        <v>575</v>
+        <v>755</v>
       </c>
     </row>
     <row r="335" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A335" s="1" t="s">
-        <v>510</v>
+        <v>573</v>
       </c>
       <c r="B335" s="1" t="s">
-        <v>511</v>
+        <v>574</v>
       </c>
       <c r="D335" s="1" t="s">
-        <v>512</v>
+        <v>575</v>
       </c>
     </row>
     <row r="336" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A336" s="1" t="s">
-        <v>985</v>
+        <v>777</v>
       </c>
       <c r="B336" s="1" t="s">
-        <v>916</v>
+        <v>778</v>
       </c>
       <c r="D336" s="1" t="s">
-        <v>979</v>
+        <v>575</v>
       </c>
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A337" s="1" t="s">
-        <v>984</v>
+        <v>510</v>
       </c>
       <c r="B337" s="1" t="s">
-        <v>917</v>
+        <v>511</v>
       </c>
       <c r="D337" s="1" t="s">
-        <v>978</v>
+        <v>512</v>
       </c>
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A338" s="1" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="B338" s="1" t="s">
-        <v>914</v>
+        <v>916</v>
       </c>
       <c r="D338" s="1" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A339" s="1" t="s">
-        <v>987</v>
+        <v>984</v>
       </c>
       <c r="B339" s="1" t="s">
-        <v>915</v>
+        <v>917</v>
       </c>
       <c r="D339" s="1" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A340" s="1" t="s">
-        <v>760</v>
+        <v>986</v>
       </c>
       <c r="B340" s="1" t="s">
-        <v>761</v>
+        <v>914</v>
       </c>
       <c r="D340" s="1" t="s">
-        <v>762</v>
+        <v>981</v>
       </c>
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A341" s="1" t="s">
-        <v>888</v>
+        <v>987</v>
       </c>
       <c r="B341" s="1" t="s">
-        <v>889</v>
+        <v>915</v>
+      </c>
+      <c r="D341" s="1" t="s">
+        <v>980</v>
       </c>
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A342" s="1" t="s">
-        <v>890</v>
+        <v>760</v>
       </c>
       <c r="B342" s="1" t="s">
-        <v>891</v>
+        <v>761</v>
+      </c>
+      <c r="D342" s="1" t="s">
+        <v>762</v>
       </c>
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A343" s="1" t="s">
-        <v>968</v>
+        <v>888</v>
       </c>
       <c r="B343" s="1" t="s">
-        <v>925</v>
-      </c>
-      <c r="D343" s="1" t="s">
-        <v>911</v>
+        <v>889</v>
       </c>
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A344" s="1" t="s">
-        <v>0</v>
+        <v>890</v>
       </c>
       <c r="B344" s="1" t="s">
-        <v>710</v>
-      </c>
-      <c r="D344" s="1" t="s">
-        <v>711</v>
+        <v>891</v>
       </c>
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A345" s="1" t="s">
-        <v>811</v>
+        <v>968</v>
       </c>
       <c r="B345" s="1" t="s">
-        <v>812</v>
+        <v>925</v>
       </c>
       <c r="D345" s="1" t="s">
-        <v>900</v>
+        <v>911</v>
       </c>
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A346" s="1" t="s">
-        <v>588</v>
+        <v>0</v>
       </c>
       <c r="B346" s="1" t="s">
-        <v>589</v>
+        <v>710</v>
       </c>
       <c r="D346" s="1" t="s">
-        <v>590</v>
+        <v>711</v>
       </c>
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A347" s="1" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="B347" s="1" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="D347" s="1" t="s">
-        <v>527</v>
+        <v>900</v>
       </c>
     </row>
     <row r="348" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A348" s="1" t="s">
-        <v>943</v>
+        <v>588</v>
       </c>
       <c r="B348" s="1" t="s">
-        <v>941</v>
+        <v>589</v>
       </c>
       <c r="D348" s="1" t="s">
-        <v>942</v>
+        <v>590</v>
       </c>
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A349" s="1" t="s">
-        <v>806</v>
+        <v>813</v>
       </c>
       <c r="B349" s="1" t="s">
-        <v>807</v>
+        <v>814</v>
       </c>
       <c r="D349" s="1" t="s">
-        <v>808</v>
+        <v>527</v>
       </c>
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A350" s="1" t="s">
-        <v>1071</v>
+        <v>943</v>
       </c>
       <c r="B350" s="1" t="s">
-        <v>1072</v>
+        <v>941</v>
       </c>
       <c r="D350" s="1" t="s">
-        <v>785</v>
+        <v>942</v>
       </c>
     </row>
     <row r="351" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A351" s="1" t="s">
-        <v>869</v>
+        <v>806</v>
       </c>
       <c r="B351" s="1" t="s">
-        <v>870</v>
+        <v>807</v>
       </c>
       <c r="D351" s="1" t="s">
-        <v>871</v>
+        <v>808</v>
       </c>
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A352" s="1" t="s">
-        <v>641</v>
+        <v>1071</v>
       </c>
       <c r="B352" s="1" t="s">
-        <v>642</v>
+        <v>1072</v>
       </c>
       <c r="D352" s="1" t="s">
-        <v>643</v>
+        <v>785</v>
       </c>
     </row>
     <row r="353" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A353" s="1" t="s">
-        <v>528</v>
+        <v>869</v>
       </c>
       <c r="B353" s="1" t="s">
-        <v>529</v>
+        <v>870</v>
       </c>
       <c r="D353" s="1" t="s">
-        <v>530</v>
+        <v>871</v>
       </c>
     </row>
     <row r="354" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A354" s="1" t="s">
-        <v>436</v>
+        <v>641</v>
       </c>
       <c r="B354" s="1" t="s">
-        <v>437</v>
+        <v>642</v>
       </c>
       <c r="D354" s="1" t="s">
-        <v>438</v>
+        <v>643</v>
       </c>
     </row>
     <row r="355" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A355" s="1" t="s">
-        <v>439</v>
+        <v>528</v>
       </c>
       <c r="B355" s="1" t="s">
-        <v>440</v>
+        <v>529</v>
       </c>
       <c r="D355" s="1" t="s">
-        <v>441</v>
+        <v>530</v>
       </c>
     </row>
     <row r="356" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A356" s="1" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
       <c r="B356" s="1" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
       <c r="D356" s="1" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
     </row>
     <row r="357" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A357" s="1" t="s">
-        <v>809</v>
+        <v>439</v>
       </c>
       <c r="B357" s="1" t="s">
-        <v>810</v>
+        <v>440</v>
       </c>
       <c r="D357" s="1" t="s">
-        <v>994</v>
+        <v>441</v>
       </c>
     </row>
     <row r="358" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A358" s="1" t="s">
-        <v>647</v>
+        <v>442</v>
       </c>
       <c r="B358" s="1" t="s">
-        <v>648</v>
+        <v>443</v>
       </c>
       <c r="D358" s="1" t="s">
-        <v>649</v>
+        <v>444</v>
       </c>
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A359" s="1" t="s">
-        <v>929</v>
+        <v>809</v>
       </c>
       <c r="B359" s="1" t="s">
-        <v>930</v>
+        <v>810</v>
       </c>
       <c r="D359" s="1" t="s">
-        <v>931</v>
+        <v>994</v>
       </c>
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A360" s="1" t="s">
-        <v>995</v>
+        <v>647</v>
       </c>
       <c r="B360" s="1" t="s">
-        <v>996</v>
+        <v>648</v>
       </c>
       <c r="D360" s="1" t="s">
-        <v>997</v>
+        <v>649</v>
       </c>
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A361" s="1" t="s">
-        <v>998</v>
+        <v>929</v>
       </c>
       <c r="B361" s="1" t="s">
-        <v>999</v>
+        <v>930</v>
       </c>
       <c r="D361" s="1" t="s">
-        <v>1000</v>
+        <v>931</v>
       </c>
     </row>
     <row r="362" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A362" s="1" t="s">
-        <v>1005</v>
+        <v>995</v>
       </c>
       <c r="B362" s="1" t="s">
-        <v>730</v>
+        <v>996</v>
       </c>
       <c r="D362" s="1" t="s">
-        <v>731</v>
+        <v>997</v>
       </c>
     </row>
     <row r="363" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A363" s="1" t="s">
-        <v>854</v>
+        <v>998</v>
       </c>
       <c r="B363" s="1" t="s">
-        <v>855</v>
+        <v>999</v>
       </c>
       <c r="D363" s="1" t="s">
-        <v>856</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="364" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A364" s="1" t="s">
-        <v>665</v>
+        <v>1005</v>
       </c>
       <c r="B364" s="1" t="s">
-        <v>666</v>
+        <v>730</v>
       </c>
       <c r="D364" s="1" t="s">
-        <v>667</v>
+        <v>731</v>
       </c>
     </row>
     <row r="365" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A365" s="1" t="s">
-        <v>966</v>
+        <v>854</v>
       </c>
       <c r="B365" s="1" t="s">
-        <v>927</v>
+        <v>855</v>
       </c>
       <c r="D365" s="1" t="s">
-        <v>910</v>
+        <v>856</v>
       </c>
     </row>
     <row r="366" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A366" s="1" t="s">
-        <v>1001</v>
+        <v>665</v>
       </c>
       <c r="B366" s="1" t="s">
-        <v>1002</v>
+        <v>666</v>
       </c>
       <c r="D366" s="1" t="s">
-        <v>1003</v>
+        <v>667</v>
       </c>
     </row>
     <row r="367" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A367" s="1" t="s">
-        <v>1006</v>
+        <v>966</v>
       </c>
       <c r="B367" s="1" t="s">
-        <v>1007</v>
+        <v>927</v>
       </c>
       <c r="D367" s="1" t="s">
-        <v>1008</v>
+        <v>910</v>
       </c>
     </row>
     <row r="368" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A368" s="1" t="s">
-        <v>1021</v>
+        <v>1001</v>
       </c>
       <c r="B368" s="1" t="s">
-        <v>1022</v>
+        <v>1002</v>
       </c>
       <c r="D368" s="1" t="s">
-        <v>1023</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="369" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A369" s="1" t="s">
-        <v>430</v>
+        <v>1006</v>
       </c>
       <c r="B369" s="1" t="s">
-        <v>431</v>
+        <v>1007</v>
       </c>
       <c r="D369" s="1" t="s">
-        <v>432</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="370" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A370" s="1" t="s">
-        <v>433</v>
+        <v>1021</v>
       </c>
       <c r="B370" s="1" t="s">
-        <v>434</v>
+        <v>1022</v>
       </c>
       <c r="D370" s="1" t="s">
-        <v>435</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="371" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A371" s="1" t="s">
-        <v>600</v>
+        <v>430</v>
       </c>
       <c r="B371" s="1" t="s">
-        <v>601</v>
+        <v>431</v>
       </c>
       <c r="D371" s="1" t="s">
-        <v>602</v>
+        <v>432</v>
       </c>
     </row>
     <row r="372" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A372" s="1" t="s">
-        <v>594</v>
+        <v>433</v>
       </c>
       <c r="B372" s="1" t="s">
-        <v>595</v>
+        <v>434</v>
       </c>
       <c r="D372" s="1" t="s">
-        <v>596</v>
+        <v>435</v>
       </c>
     </row>
     <row r="373" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A373" s="1" t="s">
-        <v>671</v>
+        <v>600</v>
       </c>
       <c r="B373" s="1" t="s">
-        <v>672</v>
+        <v>601</v>
       </c>
       <c r="D373" s="1" t="s">
-        <v>673</v>
+        <v>602</v>
       </c>
     </row>
     <row r="374" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A374" s="1" t="s">
-        <v>445</v>
+        <v>594</v>
       </c>
       <c r="B374" s="1" t="s">
-        <v>446</v>
+        <v>595</v>
       </c>
       <c r="D374" s="1" t="s">
-        <v>446</v>
+        <v>596</v>
       </c>
     </row>
     <row r="375" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A375" s="1" t="s">
-        <v>597</v>
+        <v>671</v>
       </c>
       <c r="B375" s="1" t="s">
-        <v>598</v>
+        <v>672</v>
       </c>
       <c r="D375" s="1" t="s">
-        <v>599</v>
+        <v>673</v>
       </c>
     </row>
     <row r="376" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A376" s="1" t="s">
-        <v>543</v>
+        <v>445</v>
       </c>
       <c r="B376" s="1" t="s">
-        <v>544</v>
+        <v>446</v>
       </c>
       <c r="D376" s="1" t="s">
-        <v>545</v>
+        <v>446</v>
       </c>
     </row>
     <row r="377" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A377" s="1" t="s">
-        <v>465</v>
+        <v>597</v>
       </c>
       <c r="B377" s="1" t="s">
-        <v>466</v>
+        <v>598</v>
       </c>
       <c r="D377" s="1" t="s">
-        <v>467</v>
+        <v>599</v>
       </c>
     </row>
     <row r="378" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A378" s="1" t="s">
-        <v>620</v>
+        <v>543</v>
       </c>
       <c r="B378" s="1" t="s">
-        <v>621</v>
+        <v>544</v>
       </c>
       <c r="D378" s="1" t="s">
-        <v>622</v>
+        <v>545</v>
       </c>
     </row>
     <row r="379" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A379" s="1" t="s">
-        <v>403</v>
+        <v>465</v>
       </c>
       <c r="B379" s="1" t="s">
-        <v>404</v>
+        <v>466</v>
       </c>
       <c r="D379" s="1" t="s">
-        <v>405</v>
+        <v>467</v>
       </c>
     </row>
     <row r="380" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A380" s="1" t="s">
-        <v>406</v>
+        <v>620</v>
       </c>
       <c r="B380" s="1" t="s">
-        <v>407</v>
+        <v>621</v>
       </c>
       <c r="D380" s="1" t="s">
-        <v>408</v>
+        <v>622</v>
       </c>
     </row>
     <row r="381" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A381" s="1" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="B381" s="1" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="D381" s="1" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
     </row>
     <row r="382" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A382" s="1" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="B382" s="1" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="D382" s="1" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
     </row>
     <row r="383" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A383" s="1" t="s">
-        <v>848</v>
+        <v>409</v>
       </c>
       <c r="B383" s="1" t="s">
-        <v>849</v>
+        <v>410</v>
       </c>
       <c r="D383" s="1" t="s">
-        <v>850</v>
+        <v>411</v>
       </c>
     </row>
     <row r="384" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A384" s="1" t="s">
-        <v>827</v>
+        <v>412</v>
       </c>
       <c r="B384" s="1" t="s">
-        <v>828</v>
+        <v>413</v>
       </c>
       <c r="D384" s="1" t="s">
-        <v>829</v>
+        <v>414</v>
       </c>
     </row>
     <row r="385" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A385" s="1" t="s">
-        <v>1168</v>
+        <v>848</v>
       </c>
       <c r="B385" s="1" t="s">
-        <v>1169</v>
+        <v>849</v>
       </c>
       <c r="D385" s="1" t="s">
-        <v>1170</v>
+        <v>850</v>
       </c>
     </row>
     <row r="386" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A386" s="1" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
       <c r="B386" s="1" t="s">
-        <v>831</v>
+        <v>828</v>
       </c>
       <c r="D386" s="1" t="s">
-        <v>832</v>
+        <v>829</v>
       </c>
     </row>
     <row r="387" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A387" s="1" t="s">
-        <v>1157</v>
+        <v>1168</v>
       </c>
       <c r="B387" s="1" t="s">
-        <v>1156</v>
+        <v>1169</v>
       </c>
       <c r="D387" s="1" t="s">
-        <v>1155</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="388" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A388" s="1" t="s">
-        <v>1161</v>
+        <v>830</v>
       </c>
       <c r="B388" s="1" t="s">
-        <v>1162</v>
+        <v>831</v>
       </c>
       <c r="D388" s="1" t="s">
-        <v>1160</v>
+        <v>832</v>
       </c>
     </row>
     <row r="389" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A389" s="1" t="s">
-        <v>727</v>
+        <v>1157</v>
       </c>
       <c r="B389" s="1" t="s">
-        <v>728</v>
+        <v>1156</v>
       </c>
       <c r="D389" s="1" t="s">
-        <v>729</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="390" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A390" s="1" t="s">
-        <v>724</v>
+        <v>1161</v>
       </c>
       <c r="B390" s="1" t="s">
-        <v>725</v>
+        <v>1162</v>
       </c>
       <c r="D390" s="1" t="s">
-        <v>726</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="391" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A391" s="1" t="s">
-        <v>516</v>
+        <v>727</v>
       </c>
       <c r="B391" s="1" t="s">
-        <v>517</v>
+        <v>728</v>
       </c>
       <c r="D391" s="1" t="s">
-        <v>518</v>
+        <v>729</v>
       </c>
     </row>
     <row r="392" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A392" s="1" t="s">
-        <v>591</v>
+        <v>724</v>
       </c>
       <c r="B392" s="1" t="s">
-        <v>592</v>
+        <v>725</v>
       </c>
       <c r="D392" s="1" t="s">
-        <v>593</v>
+        <v>726</v>
       </c>
     </row>
     <row r="393" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A393" s="1" t="s">
-        <v>674</v>
+        <v>516</v>
       </c>
       <c r="B393" s="1" t="s">
-        <v>675</v>
+        <v>517</v>
       </c>
       <c r="D393" s="1" t="s">
-        <v>676</v>
+        <v>518</v>
       </c>
     </row>
     <row r="394" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A394" s="1" t="s">
-        <v>654</v>
+        <v>591</v>
       </c>
       <c r="B394" s="1" t="s">
-        <v>655</v>
+        <v>592</v>
       </c>
       <c r="D394" s="1" t="s">
-        <v>1035</v>
+        <v>593</v>
       </c>
     </row>
     <row r="395" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A395" s="1" t="s">
-        <v>1045</v>
+        <v>674</v>
       </c>
       <c r="B395" s="1" t="s">
-        <v>1046</v>
+        <v>675</v>
       </c>
       <c r="D395" s="1" t="s">
-        <v>1047</v>
+        <v>676</v>
       </c>
     </row>
     <row r="396" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A396" s="1" t="s">
-        <v>1028</v>
+        <v>654</v>
       </c>
       <c r="B396" s="1" t="s">
-        <v>1027</v>
+        <v>655</v>
       </c>
       <c r="D396" s="1" t="s">
-        <v>1029</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="397" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A397" s="1" t="s">
-        <v>842</v>
+        <v>1045</v>
       </c>
       <c r="B397" s="1" t="s">
-        <v>843</v>
+        <v>1046</v>
       </c>
       <c r="D397" s="1" t="s">
-        <v>844</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="398" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A398" s="1" t="s">
-        <v>866</v>
+        <v>1028</v>
       </c>
       <c r="B398" s="1" t="s">
-        <v>867</v>
+        <v>1027</v>
       </c>
       <c r="D398" s="1" t="s">
-        <v>868</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="399" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A399" s="1" t="s">
-        <v>471</v>
+        <v>842</v>
       </c>
       <c r="B399" s="1" t="s">
-        <v>472</v>
+        <v>843</v>
       </c>
       <c r="D399" s="1" t="s">
-        <v>473</v>
+        <v>844</v>
       </c>
     </row>
     <row r="400" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A400" s="1" t="s">
-        <v>975</v>
+        <v>866</v>
       </c>
       <c r="B400" s="1" t="s">
-        <v>922</v>
+        <v>867</v>
       </c>
       <c r="D400" s="1" t="s">
-        <v>1004</v>
+        <v>868</v>
       </c>
     </row>
     <row r="401" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A401" s="1" t="s">
-        <v>558</v>
+        <v>471</v>
       </c>
       <c r="B401" s="1" t="s">
-        <v>559</v>
+        <v>472</v>
       </c>
       <c r="D401" s="1" t="s">
-        <v>560</v>
+        <v>473</v>
       </c>
     </row>
     <row r="402" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A402" s="1" t="s">
-        <v>972</v>
+        <v>975</v>
       </c>
       <c r="B402" s="1" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="D402" s="1" t="s">
-        <v>974</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="403" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A403" s="1" t="s">
-        <v>495</v>
+        <v>558</v>
       </c>
       <c r="B403" s="1" t="s">
-        <v>496</v>
+        <v>559</v>
       </c>
       <c r="D403" s="1" t="s">
-        <v>497</v>
+        <v>560</v>
       </c>
     </row>
     <row r="404" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A404" s="1" t="s">
-        <v>1175</v>
+        <v>972</v>
       </c>
       <c r="B404" s="1" t="s">
-        <v>1176</v>
+        <v>921</v>
       </c>
       <c r="D404" s="1" t="s">
-        <v>1177</v>
+        <v>974</v>
       </c>
     </row>
     <row r="405" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A405" s="1" t="s">
-        <v>991</v>
+        <v>495</v>
       </c>
       <c r="B405" s="1" t="s">
-        <v>992</v>
+        <v>496</v>
       </c>
       <c r="D405" s="1" t="s">
-        <v>993</v>
+        <v>497</v>
       </c>
     </row>
     <row r="406" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A406" s="1" t="s">
-        <v>983</v>
+        <v>1175</v>
       </c>
       <c r="B406" s="1" t="s">
-        <v>919</v>
+        <v>1176</v>
       </c>
       <c r="D406" s="1" t="s">
-        <v>976</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="407" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A407" s="1" t="s">
-        <v>982</v>
+        <v>991</v>
       </c>
       <c r="B407" s="1" t="s">
-        <v>918</v>
+        <v>992</v>
       </c>
       <c r="D407" s="1" t="s">
-        <v>977</v>
+        <v>993</v>
       </c>
     </row>
     <row r="408" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A408" s="1" t="s">
-        <v>901</v>
+        <v>983</v>
       </c>
       <c r="B408" s="1" t="s">
-        <v>902</v>
+        <v>919</v>
       </c>
       <c r="D408" s="1" t="s">
-        <v>903</v>
+        <v>976</v>
       </c>
     </row>
     <row r="409" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A409" s="1" t="s">
-        <v>480</v>
+        <v>982</v>
       </c>
       <c r="B409" s="1" t="s">
-        <v>481</v>
+        <v>918</v>
       </c>
       <c r="D409" s="1" t="s">
-        <v>482</v>
+        <v>977</v>
       </c>
     </row>
     <row r="410" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A410" s="1" t="s">
-        <v>1073</v>
+        <v>901</v>
       </c>
       <c r="B410" s="1" t="s">
-        <v>1074</v>
+        <v>902</v>
       </c>
       <c r="D410" s="1" t="s">
-        <v>1014</v>
+        <v>903</v>
       </c>
     </row>
     <row r="411" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A411" s="1" t="s">
-        <v>498</v>
+        <v>480</v>
       </c>
       <c r="B411" s="1" t="s">
-        <v>499</v>
+        <v>481</v>
       </c>
       <c r="D411" s="1" t="s">
-        <v>500</v>
+        <v>482</v>
       </c>
     </row>
     <row r="412" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A412" s="1" t="s">
-        <v>483</v>
+        <v>1073</v>
       </c>
       <c r="B412" s="1" t="s">
-        <v>484</v>
+        <v>1074</v>
       </c>
       <c r="D412" s="1" t="s">
-        <v>485</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="413" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A413" s="1" t="s">
-        <v>1165</v>
+        <v>498</v>
       </c>
       <c r="B413" s="1" t="s">
-        <v>1166</v>
+        <v>499</v>
       </c>
       <c r="D413" s="1" t="s">
-        <v>1167</v>
+        <v>500</v>
       </c>
     </row>
     <row r="414" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A414" s="1" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="B414" s="1" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="D414" s="1" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
     </row>
     <row r="415" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A415" s="1" t="s">
-        <v>944</v>
+        <v>1165</v>
       </c>
       <c r="B415" s="1" t="s">
-        <v>945</v>
+        <v>1166</v>
       </c>
       <c r="D415" s="1" t="s">
-        <v>946</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="416" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A416" s="1" t="s">
-        <v>704</v>
+        <v>486</v>
       </c>
       <c r="B416" s="1" t="s">
-        <v>705</v>
+        <v>487</v>
       </c>
       <c r="D416" s="1" t="s">
-        <v>706</v>
+        <v>488</v>
       </c>
     </row>
     <row r="417" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A417" s="1" t="s">
-        <v>800</v>
+        <v>944</v>
       </c>
       <c r="B417" s="1" t="s">
-        <v>801</v>
+        <v>945</v>
       </c>
       <c r="D417" s="1" t="s">
-        <v>802</v>
+        <v>946</v>
       </c>
     </row>
     <row r="418" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A418" s="1" t="s">
-        <v>531</v>
+        <v>704</v>
       </c>
       <c r="B418" s="1" t="s">
-        <v>532</v>
+        <v>705</v>
       </c>
       <c r="D418" s="1" t="s">
-        <v>533</v>
+        <v>706</v>
       </c>
     </row>
     <row r="419" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A419" s="1" t="s">
-        <v>501</v>
+        <v>800</v>
       </c>
       <c r="B419" s="1" t="s">
-        <v>502</v>
+        <v>801</v>
       </c>
       <c r="D419" s="1" t="s">
-        <v>503</v>
+        <v>802</v>
       </c>
     </row>
     <row r="420" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A420" s="1" t="s">
-        <v>415</v>
+        <v>531</v>
       </c>
       <c r="B420" s="1" t="s">
-        <v>416</v>
+        <v>532</v>
       </c>
       <c r="D420" s="1" t="s">
-        <v>417</v>
+        <v>533</v>
       </c>
     </row>
     <row r="421" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A421" s="1" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="B421" s="1" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="D421" s="1" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
     </row>
     <row r="422" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A422" s="1" t="s">
-        <v>721</v>
+        <v>415</v>
       </c>
       <c r="B422" s="1" t="s">
-        <v>722</v>
+        <v>416</v>
       </c>
       <c r="D422" s="1" t="s">
-        <v>723</v>
+        <v>417</v>
       </c>
     </row>
     <row r="423" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A423" s="1" t="s">
-        <v>555</v>
+        <v>504</v>
       </c>
       <c r="B423" s="1" t="s">
-        <v>556</v>
+        <v>505</v>
       </c>
       <c r="D423" s="1" t="s">
-        <v>557</v>
+        <v>506</v>
       </c>
     </row>
     <row r="424" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A424" s="1" t="s">
-        <v>561</v>
+        <v>721</v>
       </c>
       <c r="B424" s="1" t="s">
-        <v>562</v>
+        <v>722</v>
       </c>
       <c r="D424" s="1" t="s">
-        <v>563</v>
+        <v>723</v>
       </c>
     </row>
     <row r="425" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A425" s="1" t="s">
-        <v>549</v>
+        <v>555</v>
       </c>
       <c r="B425" s="1" t="s">
-        <v>550</v>
+        <v>556</v>
       </c>
       <c r="D425" s="1" t="s">
-        <v>551</v>
+        <v>557</v>
       </c>
     </row>
     <row r="426" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A426" s="1" t="s">
-        <v>763</v>
+        <v>561</v>
       </c>
       <c r="B426" s="1" t="s">
-        <v>764</v>
+        <v>562</v>
       </c>
       <c r="D426" s="1" t="s">
-        <v>551</v>
+        <v>563</v>
       </c>
     </row>
     <row r="427" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A427" s="1" t="s">
-        <v>618</v>
+        <v>549</v>
       </c>
       <c r="B427" s="1" t="s">
-        <v>619</v>
+        <v>550</v>
       </c>
       <c r="D427" s="1" t="s">
-        <v>1011</v>
+        <v>551</v>
       </c>
     </row>
     <row r="428" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A428" s="1" t="s">
-        <v>606</v>
+        <v>763</v>
       </c>
       <c r="B428" s="1" t="s">
-        <v>607</v>
+        <v>764</v>
       </c>
       <c r="D428" s="1" t="s">
-        <v>608</v>
+        <v>551</v>
       </c>
     </row>
     <row r="429" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A429" s="1" t="s">
-        <v>1184</v>
+        <v>618</v>
       </c>
       <c r="B429" s="1" t="s">
-        <v>1191</v>
+        <v>619</v>
       </c>
       <c r="D429" s="1" t="s">
-        <v>1198</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="430" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A430" s="1" t="s">
-        <v>1185</v>
+        <v>606</v>
       </c>
       <c r="B430" s="1" t="s">
-        <v>1192</v>
+        <v>607</v>
       </c>
       <c r="D430" s="1" t="s">
-        <v>1199</v>
+        <v>608</v>
       </c>
     </row>
     <row r="431" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A431" s="1" t="s">
-        <v>450</v>
+        <v>1184</v>
       </c>
       <c r="B431" s="1" t="s">
-        <v>451</v>
+        <v>1191</v>
       </c>
       <c r="D431" s="1" t="s">
-        <v>452</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="432" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A432" s="1" t="s">
-        <v>1171</v>
+        <v>1185</v>
       </c>
       <c r="B432" s="1" t="s">
-        <v>1172</v>
+        <v>1192</v>
       </c>
       <c r="D432" s="1" t="s">
-        <v>1173</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="433" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A433" s="1" t="s">
-        <v>1186</v>
+        <v>450</v>
       </c>
       <c r="B433" s="1" t="s">
-        <v>1193</v>
+        <v>451</v>
       </c>
       <c r="D433" s="1" t="s">
-        <v>1200</v>
+        <v>452</v>
       </c>
     </row>
     <row r="434" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A434" s="1" t="s">
-        <v>1187</v>
+        <v>1171</v>
       </c>
       <c r="B434" s="1" t="s">
-        <v>1194</v>
+        <v>1172</v>
       </c>
       <c r="D434" s="1" t="s">
-        <v>1201</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="435" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A435" s="1" t="s">
-        <v>689</v>
+        <v>1186</v>
       </c>
       <c r="B435" s="1" t="s">
-        <v>690</v>
+        <v>1193</v>
       </c>
       <c r="D435" s="1" t="s">
-        <v>691</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="436" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A436" s="1" t="s">
-        <v>453</v>
+        <v>1187</v>
       </c>
       <c r="B436" s="1" t="s">
-        <v>454</v>
+        <v>1194</v>
       </c>
       <c r="D436" s="1" t="s">
-        <v>455</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="437" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A437" s="1" t="s">
-        <v>1205</v>
+        <v>689</v>
       </c>
       <c r="B437" s="1" t="s">
-        <v>1206</v>
+        <v>690</v>
       </c>
       <c r="D437" s="1" t="s">
-        <v>1207</v>
+        <v>691</v>
       </c>
     </row>
     <row r="438" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A438" s="1" t="s">
-        <v>765</v>
+        <v>453</v>
       </c>
       <c r="B438" s="1" t="s">
-        <v>766</v>
+        <v>454</v>
       </c>
       <c r="D438" s="1" t="s">
-        <v>767</v>
+        <v>455</v>
       </c>
     </row>
     <row r="439" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A439" s="1" t="s">
-        <v>1051</v>
+        <v>1205</v>
       </c>
       <c r="B439" s="1" t="s">
-        <v>1052</v>
+        <v>1206</v>
       </c>
       <c r="D439" s="1" t="s">
-        <v>1053</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="440" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A440" s="1" t="s">
-        <v>821</v>
+        <v>765</v>
       </c>
       <c r="B440" s="1" t="s">
-        <v>822</v>
+        <v>766</v>
       </c>
       <c r="D440" s="1" t="s">
-        <v>823</v>
+        <v>767</v>
       </c>
     </row>
     <row r="441" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A441" s="1" t="s">
-        <v>421</v>
+        <v>1051</v>
       </c>
       <c r="B441" s="1" t="s">
-        <v>422</v>
+        <v>1052</v>
       </c>
       <c r="D441" s="1" t="s">
-        <v>423</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="442" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A442" s="1" t="s">
-        <v>1016</v>
+        <v>821</v>
       </c>
       <c r="B442" s="1" t="s">
-        <v>1017</v>
+        <v>822</v>
       </c>
       <c r="D442" s="1" t="s">
-        <v>1018</v>
+        <v>823</v>
       </c>
     </row>
     <row r="443" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A443" s="1" t="s">
-        <v>744</v>
+        <v>421</v>
       </c>
       <c r="B443" s="1" t="s">
-        <v>745</v>
+        <v>422</v>
       </c>
       <c r="D443" s="1" t="s">
-        <v>746</v>
+        <v>423</v>
       </c>
     </row>
     <row r="444" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A444" s="1" t="s">
-        <v>905</v>
+        <v>1016</v>
       </c>
       <c r="B444" s="1" t="s">
-        <v>904</v>
+        <v>1017</v>
       </c>
       <c r="D444" s="1" t="s">
-        <v>906</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="445" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A445" s="1" t="s">
-        <v>907</v>
+        <v>744</v>
       </c>
       <c r="B445" s="1" t="s">
-        <v>908</v>
+        <v>745</v>
       </c>
       <c r="D445" s="1" t="s">
-        <v>909</v>
+        <v>746</v>
       </c>
     </row>
     <row r="446" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A446" s="1" t="s">
-        <v>540</v>
+        <v>905</v>
       </c>
       <c r="B446" s="1" t="s">
-        <v>541</v>
+        <v>904</v>
       </c>
       <c r="D446" s="1" t="s">
-        <v>542</v>
+        <v>906</v>
       </c>
     </row>
     <row r="447" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A447" s="1" t="s">
-        <v>662</v>
+        <v>907</v>
       </c>
       <c r="B447" s="1" t="s">
-        <v>663</v>
+        <v>908</v>
       </c>
       <c r="D447" s="1" t="s">
-        <v>664</v>
+        <v>909</v>
       </c>
     </row>
     <row r="448" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A448" s="1" t="s">
-        <v>692</v>
+        <v>540</v>
       </c>
       <c r="B448" s="1" t="s">
-        <v>693</v>
+        <v>541</v>
       </c>
       <c r="D448" s="1" t="s">
-        <v>694</v>
+        <v>542</v>
       </c>
     </row>
     <row r="449" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A449" s="1" t="s">
-        <v>967</v>
+        <v>662</v>
       </c>
       <c r="B449" s="1" t="s">
-        <v>926</v>
+        <v>663</v>
       </c>
       <c r="D449" s="1" t="s">
-        <v>912</v>
+        <v>664</v>
       </c>
     </row>
     <row r="450" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A450" s="1" t="s">
-        <v>786</v>
+        <v>692</v>
       </c>
       <c r="B450" s="1" t="s">
-        <v>787</v>
+        <v>693</v>
       </c>
       <c r="D450" s="1" t="s">
-        <v>788</v>
+        <v>694</v>
       </c>
     </row>
     <row r="451" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A451" s="1" t="s">
-        <v>623</v>
+        <v>967</v>
       </c>
       <c r="B451" s="1" t="s">
-        <v>624</v>
+        <v>926</v>
       </c>
       <c r="D451" s="1" t="s">
-        <v>625</v>
+        <v>912</v>
       </c>
     </row>
     <row r="452" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A452" s="1" t="s">
-        <v>836</v>
+        <v>786</v>
       </c>
       <c r="B452" s="1" t="s">
-        <v>837</v>
+        <v>787</v>
       </c>
       <c r="D452" s="1" t="s">
-        <v>838</v>
+        <v>788</v>
       </c>
     </row>
     <row r="453" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A453" s="1" t="s">
-        <v>686</v>
+        <v>623</v>
       </c>
       <c r="B453" s="1" t="s">
-        <v>687</v>
+        <v>624</v>
       </c>
       <c r="D453" s="1" t="s">
-        <v>688</v>
+        <v>625</v>
       </c>
     </row>
     <row r="454" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A454" s="1" t="s">
-        <v>896</v>
+        <v>836</v>
       </c>
       <c r="B454" s="1" t="s">
-        <v>897</v>
+        <v>837</v>
+      </c>
+      <c r="D454" s="1" t="s">
+        <v>838</v>
       </c>
     </row>
     <row r="455" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A455" s="1" t="s">
-        <v>971</v>
+        <v>686</v>
       </c>
       <c r="B455" s="1" t="s">
-        <v>920</v>
+        <v>687</v>
       </c>
       <c r="D455" s="1" t="s">
-        <v>973</v>
+        <v>688</v>
       </c>
     </row>
     <row r="456" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A456" s="1" t="s">
-        <v>950</v>
+        <v>896</v>
       </c>
       <c r="B456" s="1" t="s">
-        <v>951</v>
-      </c>
-      <c r="D456" s="1" t="s">
-        <v>952</v>
+        <v>897</v>
       </c>
     </row>
     <row r="457" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A457" s="1" t="s">
-        <v>474</v>
+        <v>971</v>
       </c>
       <c r="B457" s="1" t="s">
-        <v>475</v>
+        <v>920</v>
       </c>
       <c r="D457" s="1" t="s">
-        <v>476</v>
+        <v>973</v>
       </c>
     </row>
     <row r="458" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A458" s="1" t="s">
-        <v>567</v>
+        <v>950</v>
       </c>
       <c r="B458" s="1" t="s">
-        <v>568</v>
+        <v>951</v>
       </c>
       <c r="D458" s="1" t="s">
-        <v>569</v>
+        <v>952</v>
       </c>
     </row>
     <row r="459" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A459" s="1" t="s">
-        <v>768</v>
+        <v>474</v>
       </c>
       <c r="B459" s="1" t="s">
-        <v>769</v>
+        <v>475</v>
       </c>
       <c r="D459" s="1" t="s">
-        <v>770</v>
+        <v>476</v>
       </c>
     </row>
     <row r="460" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A460" s="1" t="s">
-        <v>771</v>
+        <v>567</v>
       </c>
       <c r="B460" s="1" t="s">
-        <v>772</v>
+        <v>568</v>
       </c>
       <c r="D460" s="1" t="s">
-        <v>354</v>
+        <v>569</v>
       </c>
     </row>
     <row r="461" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A461" s="1" t="s">
-        <v>712</v>
+        <v>768</v>
       </c>
       <c r="B461" s="1" t="s">
-        <v>713</v>
+        <v>769</v>
       </c>
       <c r="D461" s="1" t="s">
-        <v>714</v>
+        <v>770</v>
       </c>
     </row>
     <row r="462" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A462" s="1" t="s">
-        <v>881</v>
+        <v>771</v>
       </c>
       <c r="B462" s="1" t="s">
-        <v>882</v>
+        <v>772</v>
       </c>
       <c r="D462" s="1" t="s">
-        <v>883</v>
+        <v>354</v>
       </c>
     </row>
     <row r="463" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A463" s="1" t="s">
-        <v>1147</v>
+        <v>712</v>
       </c>
       <c r="B463" s="1" t="s">
-        <v>1148</v>
+        <v>713</v>
       </c>
       <c r="D463" s="1" t="s">
-        <v>1146</v>
+        <v>714</v>
       </c>
     </row>
     <row r="464" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A464" s="1" t="s">
-        <v>953</v>
+        <v>881</v>
       </c>
       <c r="B464" s="1" t="s">
-        <v>955</v>
+        <v>882</v>
       </c>
       <c r="D464" s="1" t="s">
-        <v>956</v>
+        <v>883</v>
       </c>
     </row>
     <row r="465" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A465" s="1" t="s">
-        <v>747</v>
+        <v>1147</v>
       </c>
       <c r="B465" s="1" t="s">
-        <v>748</v>
+        <v>1148</v>
       </c>
       <c r="D465" s="1" t="s">
-        <v>749</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="466" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A466" s="1" t="s">
-        <v>576</v>
+        <v>953</v>
       </c>
       <c r="B466" s="1" t="s">
-        <v>577</v>
+        <v>955</v>
       </c>
       <c r="D466" s="1" t="s">
-        <v>578</v>
+        <v>956</v>
       </c>
     </row>
     <row r="467" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A467" s="1" t="s">
-        <v>824</v>
+        <v>747</v>
       </c>
       <c r="B467" s="1" t="s">
-        <v>825</v>
+        <v>748</v>
       </c>
       <c r="D467" s="1" t="s">
-        <v>826</v>
+        <v>749</v>
       </c>
     </row>
     <row r="468" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A468" s="1" t="s">
-        <v>1024</v>
+        <v>576</v>
       </c>
       <c r="B468" s="1" t="s">
-        <v>1025</v>
+        <v>577</v>
       </c>
       <c r="D468" s="1" t="s">
-        <v>1026</v>
+        <v>578</v>
       </c>
     </row>
     <row r="469" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A469" s="1" t="s">
-        <v>427</v>
+        <v>824</v>
       </c>
       <c r="B469" s="1" t="s">
-        <v>428</v>
+        <v>825</v>
       </c>
       <c r="D469" s="1" t="s">
-        <v>429</v>
+        <v>826</v>
       </c>
     </row>
     <row r="470" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A470" s="1" t="s">
-        <v>626</v>
+        <v>1024</v>
       </c>
       <c r="B470" s="1" t="s">
-        <v>627</v>
+        <v>1025</v>
       </c>
       <c r="D470" s="1" t="s">
-        <v>628</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="471" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A471" s="1" t="s">
-        <v>418</v>
+        <v>427</v>
       </c>
       <c r="B471" s="1" t="s">
-        <v>419</v>
+        <v>428</v>
       </c>
       <c r="D471" s="1" t="s">
-        <v>420</v>
+        <v>429</v>
       </c>
     </row>
     <row r="472" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A472" s="1" t="s">
-        <v>932</v>
+        <v>626</v>
       </c>
       <c r="B472" s="1" t="s">
-        <v>933</v>
+        <v>627</v>
       </c>
       <c r="D472" s="1" t="s">
-        <v>934</v>
+        <v>628</v>
       </c>
     </row>
     <row r="473" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A473" s="1" t="s">
-        <v>735</v>
+        <v>418</v>
       </c>
       <c r="B473" s="1" t="s">
-        <v>736</v>
+        <v>419</v>
       </c>
       <c r="D473" s="1" t="s">
-        <v>737</v>
+        <v>420</v>
       </c>
     </row>
     <row r="474" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A474" s="1" t="s">
-        <v>738</v>
+        <v>932</v>
       </c>
       <c r="B474" s="1" t="s">
-        <v>739</v>
+        <v>933</v>
       </c>
       <c r="D474" s="1" t="s">
-        <v>740</v>
+        <v>934</v>
       </c>
     </row>
     <row r="475" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A475" s="1" t="s">
-        <v>741</v>
+        <v>735</v>
       </c>
       <c r="B475" s="1" t="s">
-        <v>742</v>
+        <v>736</v>
       </c>
       <c r="D475" s="1" t="s">
-        <v>743</v>
+        <v>737</v>
       </c>
     </row>
     <row r="476" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A476" s="1" t="s">
-        <v>629</v>
+        <v>738</v>
       </c>
       <c r="B476" s="1" t="s">
-        <v>630</v>
+        <v>739</v>
       </c>
       <c r="D476" s="1" t="s">
-        <v>631</v>
+        <v>740</v>
       </c>
     </row>
     <row r="477" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A477" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="B477" s="1" t="s">
+        <v>742</v>
+      </c>
+      <c r="D477" s="1" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="478" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A478" s="1" t="s">
+        <v>629</v>
+      </c>
+      <c r="B478" s="1" t="s">
+        <v>630</v>
+      </c>
+      <c r="D478" s="1" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="479" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A479" s="1" t="s">
         <v>632</v>
       </c>
-      <c r="B477" s="1" t="s">
+      <c r="B479" s="1" t="s">
         <v>633</v>
       </c>
-      <c r="D477" s="1" t="s">
+      <c r="D479" s="1" t="s">
         <v>634</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Follow Font Awesome v5.0.13
</commit_message>
<xml_diff>
--- a/conf/messages.xlsx
+++ b/conf/messages.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10505"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hiro/github/FinePlay/conf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C9D92922-05AD-3143-B62B-1804C0583823}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AF33AF20-FCB9-6F41-878E-E532F6632405}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4940" yWindow="740" windowWidth="33460" windowHeight="21560" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1338" uniqueCount="1281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1344" uniqueCount="1287">
   <si>
     <t>key</t>
   </si>
@@ -4401,6 +4401,36 @@
   </si>
   <si>
     <t>スライド</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>optional</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>任意</t>
+    <rPh sb="0" eb="2">
+      <t>ニン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Optional</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>eternal</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Eternal</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>永遠</t>
+    <rPh sb="0" eb="2">
+      <t>エイエn</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -5138,10 +5168,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G502"/>
+  <dimension ref="A1:G504"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A435" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D445" sqref="D445"/>
+    <sheetView tabSelected="1" topLeftCell="A300" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E312" sqref="E312"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -8080,353 +8110,353 @@
     </row>
     <row r="317" spans="1:4">
       <c r="A317" s="1" t="s">
-        <v>802</v>
+        <v>1284</v>
       </c>
       <c r="B317" s="1" t="s">
-        <v>803</v>
+        <v>1285</v>
       </c>
       <c r="D317" s="1" t="s">
-        <v>804</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="318" spans="1:4">
       <c r="A318" s="1" t="s">
-        <v>1184</v>
+        <v>802</v>
       </c>
       <c r="B318" s="1" t="s">
-        <v>1191</v>
+        <v>803</v>
       </c>
       <c r="D318" s="1" t="s">
-        <v>1198</v>
+        <v>804</v>
       </c>
     </row>
     <row r="319" spans="1:4">
       <c r="A319" s="1" t="s">
-        <v>455</v>
+        <v>1184</v>
       </c>
       <c r="B319" s="1" t="s">
-        <v>456</v>
+        <v>1191</v>
       </c>
       <c r="D319" s="1" t="s">
-        <v>457</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="320" spans="1:4">
       <c r="A320" s="1" t="s">
-        <v>838</v>
+        <v>455</v>
       </c>
       <c r="B320" s="1" t="s">
-        <v>839</v>
+        <v>456</v>
       </c>
       <c r="D320" s="1" t="s">
-        <v>840</v>
+        <v>457</v>
       </c>
     </row>
     <row r="321" spans="1:4">
       <c r="A321" s="1" t="s">
-        <v>1037</v>
+        <v>838</v>
       </c>
       <c r="B321" s="1" t="s">
-        <v>1038</v>
+        <v>839</v>
       </c>
       <c r="D321" s="1" t="s">
-        <v>1039</v>
+        <v>840</v>
       </c>
     </row>
     <row r="322" spans="1:4">
       <c r="A322" s="1" t="s">
-        <v>714</v>
+        <v>1037</v>
       </c>
       <c r="B322" s="1" t="s">
-        <v>715</v>
+        <v>1038</v>
       </c>
       <c r="D322" s="1" t="s">
-        <v>716</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="323" spans="1:4">
       <c r="A323" s="1" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="B323" s="1" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
       <c r="D323" s="1" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
     </row>
     <row r="324" spans="1:4">
       <c r="A324" s="1" t="s">
-        <v>614</v>
+        <v>717</v>
       </c>
       <c r="B324" s="1" t="s">
-        <v>615</v>
+        <v>718</v>
       </c>
       <c r="D324" s="1" t="s">
-        <v>616</v>
+        <v>719</v>
       </c>
     </row>
     <row r="325" spans="1:4">
       <c r="A325" s="1" t="s">
-        <v>584</v>
+        <v>614</v>
       </c>
       <c r="B325" s="1" t="s">
-        <v>585</v>
+        <v>615</v>
       </c>
       <c r="D325" s="1" t="s">
-        <v>586</v>
+        <v>616</v>
       </c>
     </row>
     <row r="326" spans="1:4">
       <c r="A326" s="1" t="s">
-        <v>611</v>
+        <v>584</v>
       </c>
       <c r="B326" s="1" t="s">
-        <v>612</v>
+        <v>585</v>
       </c>
       <c r="D326" s="1" t="s">
-        <v>613</v>
+        <v>586</v>
       </c>
     </row>
     <row r="327" spans="1:4">
       <c r="A327" s="1" t="s">
-        <v>755</v>
+        <v>611</v>
       </c>
       <c r="B327" s="1" t="s">
-        <v>756</v>
+        <v>612</v>
       </c>
       <c r="D327" s="1" t="s">
-        <v>757</v>
+        <v>613</v>
       </c>
     </row>
     <row r="328" spans="1:4">
       <c r="A328" s="1" t="s">
-        <v>890</v>
+        <v>755</v>
       </c>
       <c r="B328" s="1" t="s">
-        <v>891</v>
+        <v>756</v>
+      </c>
+      <c r="D328" s="1" t="s">
+        <v>757</v>
       </c>
     </row>
     <row r="329" spans="1:4">
       <c r="A329" s="1" t="s">
-        <v>700</v>
+        <v>890</v>
       </c>
       <c r="B329" s="1" t="s">
-        <v>701</v>
-      </c>
-      <c r="D329" s="1" t="s">
-        <v>702</v>
+        <v>891</v>
       </c>
     </row>
     <row r="330" spans="1:4">
       <c r="A330" s="1" t="s">
-        <v>682</v>
+        <v>700</v>
       </c>
       <c r="B330" s="1" t="s">
-        <v>683</v>
+        <v>701</v>
       </c>
       <c r="D330" s="1" t="s">
-        <v>684</v>
+        <v>702</v>
       </c>
     </row>
     <row r="331" spans="1:4">
       <c r="A331" s="1" t="s">
-        <v>791</v>
+        <v>682</v>
       </c>
       <c r="B331" s="1" t="s">
-        <v>792</v>
+        <v>683</v>
       </c>
       <c r="D331" s="1" t="s">
-        <v>958</v>
+        <v>684</v>
       </c>
     </row>
     <row r="332" spans="1:4">
       <c r="A332" s="1" t="s">
-        <v>774</v>
+        <v>791</v>
       </c>
       <c r="B332" s="1" t="s">
-        <v>775</v>
+        <v>792</v>
       </c>
       <c r="D332" s="1" t="s">
-        <v>431</v>
+        <v>958</v>
       </c>
     </row>
     <row r="333" spans="1:4">
       <c r="A333" s="1" t="s">
-        <v>832</v>
+        <v>774</v>
       </c>
       <c r="B333" s="1" t="s">
-        <v>833</v>
+        <v>775</v>
       </c>
       <c r="D333" s="1" t="s">
-        <v>834</v>
+        <v>431</v>
       </c>
     </row>
     <row r="334" spans="1:4">
       <c r="A334" s="1" t="s">
-        <v>1203</v>
+        <v>832</v>
       </c>
       <c r="B334" s="1" t="s">
-        <v>1204</v>
+        <v>833</v>
       </c>
       <c r="D334" s="1" t="s">
-        <v>1205</v>
+        <v>834</v>
       </c>
     </row>
     <row r="335" spans="1:4">
       <c r="A335" s="1" t="s">
-        <v>637</v>
+        <v>1203</v>
       </c>
       <c r="B335" s="1" t="s">
-        <v>638</v>
+        <v>1204</v>
       </c>
       <c r="D335" s="1" t="s">
-        <v>639</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="336" spans="1:4">
       <c r="A336" s="1" t="s">
-        <v>551</v>
+        <v>637</v>
       </c>
       <c r="B336" s="1" t="s">
-        <v>552</v>
+        <v>638</v>
       </c>
       <c r="D336" s="1" t="s">
-        <v>553</v>
+        <v>639</v>
       </c>
     </row>
     <row r="337" spans="1:4">
       <c r="A337" s="1" t="s">
-        <v>955</v>
+        <v>551</v>
       </c>
       <c r="B337" s="1" t="s">
-        <v>956</v>
+        <v>552</v>
       </c>
       <c r="D337" s="1" t="s">
-        <v>957</v>
+        <v>553</v>
       </c>
     </row>
     <row r="338" spans="1:4">
       <c r="A338" s="1" t="s">
-        <v>1026</v>
+        <v>955</v>
       </c>
       <c r="B338" s="1" t="s">
-        <v>1025</v>
+        <v>956</v>
       </c>
       <c r="D338" s="1" t="s">
-        <v>1027</v>
+        <v>957</v>
       </c>
     </row>
     <row r="339" spans="1:4">
       <c r="A339" s="1" t="s">
-        <v>694</v>
+        <v>1026</v>
       </c>
       <c r="B339" s="1" t="s">
-        <v>695</v>
+        <v>1025</v>
       </c>
       <c r="D339" s="1" t="s">
-        <v>696</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="340" spans="1:4">
       <c r="A340" s="1" t="s">
-        <v>676</v>
+        <v>694</v>
       </c>
       <c r="B340" s="1" t="s">
-        <v>677</v>
+        <v>695</v>
       </c>
       <c r="D340" s="1" t="s">
-        <v>678</v>
+        <v>696</v>
       </c>
     </row>
     <row r="341" spans="1:4">
       <c r="A341" s="1" t="s">
-        <v>871</v>
+        <v>676</v>
       </c>
       <c r="B341" s="1" t="s">
-        <v>872</v>
+        <v>677</v>
       </c>
       <c r="D341" s="1" t="s">
-        <v>873</v>
+        <v>678</v>
       </c>
     </row>
     <row r="342" spans="1:4">
       <c r="A342" s="1" t="s">
-        <v>954</v>
+        <v>871</v>
       </c>
       <c r="B342" s="1" t="s">
-        <v>953</v>
+        <v>872</v>
       </c>
       <c r="D342" s="1" t="s">
-        <v>758</v>
+        <v>873</v>
       </c>
     </row>
     <row r="343" spans="1:4">
       <c r="A343" s="1" t="s">
-        <v>1005</v>
+        <v>954</v>
       </c>
       <c r="B343" s="1" t="s">
-        <v>1006</v>
+        <v>953</v>
       </c>
       <c r="D343" s="1" t="s">
-        <v>950</v>
+        <v>758</v>
       </c>
     </row>
     <row r="344" spans="1:4">
       <c r="A344" s="1" t="s">
-        <v>882</v>
+        <v>1005</v>
       </c>
       <c r="B344" s="1" t="s">
-        <v>883</v>
+        <v>1006</v>
+      </c>
+      <c r="D344" s="1" t="s">
+        <v>950</v>
       </c>
     </row>
     <row r="345" spans="1:4">
       <c r="A345" s="1" t="s">
-        <v>856</v>
+        <v>882</v>
       </c>
       <c r="B345" s="1" t="s">
-        <v>857</v>
-      </c>
-      <c r="D345" s="1" t="s">
-        <v>858</v>
+        <v>883</v>
       </c>
     </row>
     <row r="346" spans="1:4">
       <c r="A346" s="1" t="s">
-        <v>880</v>
+        <v>856</v>
       </c>
       <c r="B346" s="1" t="s">
-        <v>881</v>
+        <v>857</v>
+      </c>
+      <c r="D346" s="1" t="s">
+        <v>858</v>
       </c>
     </row>
     <row r="347" spans="1:4">
       <c r="A347" s="1" t="s">
-        <v>752</v>
+        <v>880</v>
       </c>
       <c r="B347" s="1" t="s">
-        <v>753</v>
-      </c>
-      <c r="D347" s="1" t="s">
-        <v>754</v>
+        <v>881</v>
       </c>
     </row>
     <row r="348" spans="1:4">
       <c r="A348" s="1" t="s">
-        <v>572</v>
+        <v>752</v>
       </c>
       <c r="B348" s="1" t="s">
-        <v>573</v>
+        <v>753</v>
       </c>
       <c r="D348" s="1" t="s">
-        <v>574</v>
+        <v>754</v>
       </c>
     </row>
     <row r="349" spans="1:4">
       <c r="A349" s="1" t="s">
-        <v>776</v>
+        <v>572</v>
       </c>
       <c r="B349" s="1" t="s">
-        <v>777</v>
+        <v>573</v>
       </c>
       <c r="D349" s="1" t="s">
         <v>574</v>
@@ -8434,1680 +8464,1702 @@
     </row>
     <row r="350" spans="1:4">
       <c r="A350" s="1" t="s">
-        <v>509</v>
+        <v>776</v>
       </c>
       <c r="B350" s="1" t="s">
-        <v>510</v>
+        <v>777</v>
       </c>
       <c r="D350" s="1" t="s">
-        <v>511</v>
+        <v>574</v>
       </c>
     </row>
     <row r="351" spans="1:4">
       <c r="A351" s="1" t="s">
-        <v>981</v>
+        <v>509</v>
       </c>
       <c r="B351" s="1" t="s">
-        <v>912</v>
+        <v>510</v>
       </c>
       <c r="D351" s="1" t="s">
-        <v>975</v>
+        <v>511</v>
       </c>
     </row>
     <row r="352" spans="1:4">
       <c r="A352" s="1" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="B352" s="1" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="D352" s="1" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
     </row>
     <row r="353" spans="1:4">
       <c r="A353" s="1" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="B353" s="1" t="s">
-        <v>910</v>
+        <v>913</v>
       </c>
       <c r="D353" s="1" t="s">
-        <v>977</v>
+        <v>974</v>
       </c>
     </row>
     <row r="354" spans="1:4">
       <c r="A354" s="1" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="B354" s="1" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="D354" s="1" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
     </row>
     <row r="355" spans="1:4">
       <c r="A355" s="1" t="s">
-        <v>759</v>
+        <v>983</v>
       </c>
       <c r="B355" s="1" t="s">
-        <v>760</v>
+        <v>911</v>
       </c>
       <c r="D355" s="1" t="s">
-        <v>761</v>
+        <v>976</v>
       </c>
     </row>
     <row r="356" spans="1:4">
       <c r="A356" s="1" t="s">
-        <v>884</v>
+        <v>759</v>
       </c>
       <c r="B356" s="1" t="s">
-        <v>885</v>
+        <v>760</v>
+      </c>
+      <c r="D356" s="1" t="s">
+        <v>761</v>
       </c>
     </row>
     <row r="357" spans="1:4">
       <c r="A357" s="1" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="B357" s="1" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
     </row>
     <row r="358" spans="1:4">
       <c r="A358" s="1" t="s">
-        <v>964</v>
+        <v>886</v>
       </c>
       <c r="B358" s="1" t="s">
-        <v>921</v>
-      </c>
-      <c r="D358" s="1" t="s">
-        <v>907</v>
+        <v>887</v>
       </c>
     </row>
     <row r="359" spans="1:4">
       <c r="A359" s="1" t="s">
-        <v>0</v>
+        <v>964</v>
       </c>
       <c r="B359" s="1" t="s">
-        <v>709</v>
+        <v>921</v>
       </c>
       <c r="D359" s="1" t="s">
-        <v>710</v>
+        <v>907</v>
       </c>
     </row>
     <row r="360" spans="1:4">
       <c r="A360" s="1" t="s">
-        <v>810</v>
+        <v>0</v>
       </c>
       <c r="B360" s="1" t="s">
-        <v>811</v>
+        <v>709</v>
       </c>
       <c r="D360" s="1" t="s">
-        <v>896</v>
+        <v>710</v>
       </c>
     </row>
     <row r="361" spans="1:4">
       <c r="A361" s="1" t="s">
-        <v>587</v>
+        <v>810</v>
       </c>
       <c r="B361" s="1" t="s">
-        <v>588</v>
+        <v>811</v>
       </c>
       <c r="D361" s="1" t="s">
-        <v>589</v>
+        <v>896</v>
       </c>
     </row>
     <row r="362" spans="1:4">
       <c r="A362" s="1" t="s">
-        <v>812</v>
+        <v>587</v>
       </c>
       <c r="B362" s="1" t="s">
-        <v>813</v>
+        <v>588</v>
       </c>
       <c r="D362" s="1" t="s">
-        <v>526</v>
+        <v>589</v>
       </c>
     </row>
     <row r="363" spans="1:4">
       <c r="A363" s="1" t="s">
-        <v>939</v>
+        <v>812</v>
       </c>
       <c r="B363" s="1" t="s">
-        <v>937</v>
+        <v>813</v>
       </c>
       <c r="D363" s="1" t="s">
-        <v>938</v>
+        <v>526</v>
       </c>
     </row>
     <row r="364" spans="1:4">
       <c r="A364" s="1" t="s">
-        <v>805</v>
+        <v>939</v>
       </c>
       <c r="B364" s="1" t="s">
-        <v>806</v>
+        <v>937</v>
       </c>
       <c r="D364" s="1" t="s">
-        <v>807</v>
+        <v>938</v>
       </c>
     </row>
     <row r="365" spans="1:4">
       <c r="A365" s="1" t="s">
-        <v>1066</v>
+        <v>805</v>
       </c>
       <c r="B365" s="1" t="s">
-        <v>1067</v>
+        <v>806</v>
       </c>
       <c r="D365" s="1" t="s">
-        <v>784</v>
+        <v>807</v>
       </c>
     </row>
     <row r="366" spans="1:4">
       <c r="A366" s="1" t="s">
-        <v>865</v>
+        <v>1066</v>
       </c>
       <c r="B366" s="1" t="s">
-        <v>866</v>
+        <v>1067</v>
       </c>
       <c r="D366" s="1" t="s">
-        <v>867</v>
+        <v>784</v>
       </c>
     </row>
     <row r="367" spans="1:4">
       <c r="A367" s="1" t="s">
-        <v>640</v>
+        <v>865</v>
       </c>
       <c r="B367" s="1" t="s">
-        <v>641</v>
+        <v>866</v>
       </c>
       <c r="D367" s="1" t="s">
-        <v>642</v>
+        <v>867</v>
       </c>
     </row>
     <row r="368" spans="1:4">
       <c r="A368" s="1" t="s">
-        <v>527</v>
+        <v>640</v>
       </c>
       <c r="B368" s="1" t="s">
-        <v>528</v>
+        <v>641</v>
       </c>
       <c r="D368" s="1" t="s">
-        <v>529</v>
+        <v>642</v>
       </c>
     </row>
     <row r="369" spans="1:4">
       <c r="A369" s="1" t="s">
-        <v>435</v>
+        <v>527</v>
       </c>
       <c r="B369" s="1" t="s">
-        <v>436</v>
+        <v>528</v>
       </c>
       <c r="D369" s="1" t="s">
-        <v>437</v>
+        <v>529</v>
       </c>
     </row>
     <row r="370" spans="1:4">
       <c r="A370" s="1" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B370" s="1" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D370" s="1" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="371" spans="1:4">
       <c r="A371" s="1" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="B371" s="1" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="D371" s="1" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="372" spans="1:4">
       <c r="A372" s="1" t="s">
-        <v>808</v>
+        <v>441</v>
       </c>
       <c r="B372" s="1" t="s">
-        <v>809</v>
+        <v>442</v>
       </c>
       <c r="D372" s="1" t="s">
-        <v>990</v>
+        <v>443</v>
       </c>
     </row>
     <row r="373" spans="1:4">
       <c r="A373" s="1" t="s">
-        <v>646</v>
+        <v>808</v>
       </c>
       <c r="B373" s="1" t="s">
-        <v>647</v>
+        <v>809</v>
       </c>
       <c r="D373" s="1" t="s">
-        <v>648</v>
+        <v>990</v>
       </c>
     </row>
     <row r="374" spans="1:4">
       <c r="A374" s="1" t="s">
-        <v>925</v>
+        <v>646</v>
       </c>
       <c r="B374" s="1" t="s">
-        <v>926</v>
+        <v>647</v>
       </c>
       <c r="D374" s="1" t="s">
-        <v>927</v>
+        <v>648</v>
       </c>
     </row>
     <row r="375" spans="1:4">
       <c r="A375" s="1" t="s">
-        <v>991</v>
+        <v>925</v>
       </c>
       <c r="B375" s="1" t="s">
-        <v>992</v>
+        <v>926</v>
       </c>
       <c r="D375" s="1" t="s">
-        <v>993</v>
+        <v>927</v>
       </c>
     </row>
     <row r="376" spans="1:4">
       <c r="A376" s="1" t="s">
-        <v>994</v>
+        <v>991</v>
       </c>
       <c r="B376" s="1" t="s">
-        <v>995</v>
+        <v>992</v>
       </c>
       <c r="D376" s="1" t="s">
-        <v>996</v>
+        <v>993</v>
       </c>
     </row>
     <row r="377" spans="1:4">
       <c r="A377" s="1" t="s">
-        <v>1001</v>
+        <v>994</v>
       </c>
       <c r="B377" s="1" t="s">
-        <v>729</v>
+        <v>995</v>
       </c>
       <c r="D377" s="1" t="s">
-        <v>730</v>
+        <v>996</v>
       </c>
     </row>
     <row r="378" spans="1:4">
       <c r="A378" s="1" t="s">
-        <v>853</v>
+        <v>1001</v>
       </c>
       <c r="B378" s="1" t="s">
-        <v>854</v>
+        <v>729</v>
       </c>
       <c r="D378" s="1" t="s">
-        <v>855</v>
+        <v>730</v>
       </c>
     </row>
     <row r="379" spans="1:4">
       <c r="A379" s="1" t="s">
-        <v>664</v>
+        <v>853</v>
       </c>
       <c r="B379" s="1" t="s">
-        <v>665</v>
+        <v>854</v>
       </c>
       <c r="D379" s="1" t="s">
-        <v>666</v>
+        <v>855</v>
       </c>
     </row>
     <row r="380" spans="1:4">
       <c r="A380" s="1" t="s">
-        <v>962</v>
+        <v>664</v>
       </c>
       <c r="B380" s="1" t="s">
-        <v>923</v>
+        <v>665</v>
       </c>
       <c r="D380" s="1" t="s">
-        <v>906</v>
+        <v>666</v>
       </c>
     </row>
     <row r="381" spans="1:4">
       <c r="A381" s="1" t="s">
-        <v>997</v>
+        <v>962</v>
       </c>
       <c r="B381" s="1" t="s">
-        <v>998</v>
+        <v>923</v>
       </c>
       <c r="D381" s="1" t="s">
-        <v>999</v>
+        <v>906</v>
       </c>
     </row>
     <row r="382" spans="1:4">
       <c r="A382" s="1" t="s">
-        <v>1002</v>
+        <v>997</v>
       </c>
       <c r="B382" s="1" t="s">
-        <v>1003</v>
+        <v>998</v>
       </c>
       <c r="D382" s="1" t="s">
-        <v>1004</v>
+        <v>999</v>
       </c>
     </row>
     <row r="383" spans="1:4">
       <c r="A383" s="1" t="s">
-        <v>1016</v>
+        <v>1002</v>
       </c>
       <c r="B383" s="1" t="s">
-        <v>1017</v>
+        <v>1003</v>
       </c>
       <c r="D383" s="1" t="s">
-        <v>1018</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="384" spans="1:4">
       <c r="A384" s="1" t="s">
-        <v>429</v>
+        <v>1016</v>
       </c>
       <c r="B384" s="1" t="s">
-        <v>430</v>
+        <v>1017</v>
       </c>
       <c r="D384" s="1" t="s">
-        <v>431</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="385" spans="1:4">
       <c r="A385" s="1" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B385" s="1" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="D385" s="1" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="386" spans="1:4">
       <c r="A386" s="1" t="s">
-        <v>599</v>
+        <v>432</v>
       </c>
       <c r="B386" s="1" t="s">
-        <v>600</v>
+        <v>433</v>
       </c>
       <c r="D386" s="1" t="s">
-        <v>601</v>
+        <v>434</v>
       </c>
     </row>
     <row r="387" spans="1:4">
       <c r="A387" s="1" t="s">
-        <v>593</v>
+        <v>599</v>
       </c>
       <c r="B387" s="1" t="s">
-        <v>594</v>
+        <v>600</v>
       </c>
       <c r="D387" s="1" t="s">
-        <v>595</v>
+        <v>601</v>
       </c>
     </row>
     <row r="388" spans="1:4">
       <c r="A388" s="1" t="s">
-        <v>670</v>
+        <v>593</v>
       </c>
       <c r="B388" s="1" t="s">
-        <v>671</v>
+        <v>594</v>
       </c>
       <c r="D388" s="1" t="s">
-        <v>672</v>
+        <v>595</v>
       </c>
     </row>
     <row r="389" spans="1:4">
       <c r="A389" s="1" t="s">
-        <v>444</v>
+        <v>670</v>
       </c>
       <c r="B389" s="1" t="s">
-        <v>445</v>
+        <v>671</v>
       </c>
       <c r="D389" s="1" t="s">
-        <v>445</v>
+        <v>672</v>
       </c>
     </row>
     <row r="390" spans="1:4">
       <c r="A390" s="1" t="s">
-        <v>596</v>
+        <v>444</v>
       </c>
       <c r="B390" s="1" t="s">
-        <v>597</v>
+        <v>445</v>
       </c>
       <c r="D390" s="1" t="s">
-        <v>598</v>
+        <v>445</v>
       </c>
     </row>
     <row r="391" spans="1:4">
       <c r="A391" s="1" t="s">
-        <v>542</v>
+        <v>596</v>
       </c>
       <c r="B391" s="1" t="s">
-        <v>543</v>
+        <v>597</v>
       </c>
       <c r="D391" s="1" t="s">
-        <v>544</v>
+        <v>598</v>
       </c>
     </row>
     <row r="392" spans="1:4">
       <c r="A392" s="1" t="s">
-        <v>464</v>
+        <v>542</v>
       </c>
       <c r="B392" s="1" t="s">
-        <v>465</v>
+        <v>543</v>
       </c>
       <c r="D392" s="1" t="s">
-        <v>466</v>
+        <v>544</v>
       </c>
     </row>
     <row r="393" spans="1:4">
       <c r="A393" s="1" t="s">
-        <v>619</v>
+        <v>464</v>
       </c>
       <c r="B393" s="1" t="s">
-        <v>620</v>
+        <v>465</v>
       </c>
       <c r="D393" s="1" t="s">
-        <v>621</v>
+        <v>466</v>
       </c>
     </row>
     <row r="394" spans="1:4">
       <c r="A394" s="1" t="s">
-        <v>402</v>
+        <v>619</v>
       </c>
       <c r="B394" s="1" t="s">
-        <v>403</v>
+        <v>620</v>
       </c>
       <c r="D394" s="1" t="s">
-        <v>404</v>
+        <v>621</v>
       </c>
     </row>
     <row r="395" spans="1:4">
       <c r="A395" s="1" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="B395" s="1" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D395" s="1" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="396" spans="1:4">
       <c r="A396" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B396" s="1" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="D396" s="1" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="397" spans="1:4">
       <c r="A397" s="1" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="B397" s="1" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="D397" s="1" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
     </row>
     <row r="398" spans="1:4">
       <c r="A398" s="1" t="s">
-        <v>847</v>
+        <v>411</v>
       </c>
       <c r="B398" s="1" t="s">
-        <v>848</v>
+        <v>412</v>
       </c>
       <c r="D398" s="1" t="s">
-        <v>849</v>
+        <v>413</v>
       </c>
     </row>
     <row r="399" spans="1:4">
       <c r="A399" s="1" t="s">
-        <v>1219</v>
+        <v>847</v>
       </c>
       <c r="B399" s="1" t="s">
-        <v>1220</v>
+        <v>848</v>
       </c>
       <c r="D399" s="1" t="s">
-        <v>1202</v>
+        <v>849</v>
       </c>
     </row>
     <row r="400" spans="1:4">
       <c r="A400" s="1" t="s">
-        <v>826</v>
+        <v>1281</v>
       </c>
       <c r="B400" s="1" t="s">
-        <v>827</v>
+        <v>1283</v>
       </c>
       <c r="D400" s="1" t="s">
-        <v>828</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="401" spans="1:4">
       <c r="A401" s="1" t="s">
-        <v>1163</v>
+        <v>1219</v>
       </c>
       <c r="B401" s="1" t="s">
-        <v>1164</v>
+        <v>1220</v>
       </c>
       <c r="D401" s="1" t="s">
-        <v>1165</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="402" spans="1:4">
       <c r="A402" s="1" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
       <c r="B402" s="1" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
       <c r="D402" s="1" t="s">
-        <v>831</v>
+        <v>828</v>
       </c>
     </row>
     <row r="403" spans="1:4">
       <c r="A403" s="1" t="s">
-        <v>1152</v>
+        <v>1163</v>
       </c>
       <c r="B403" s="1" t="s">
-        <v>1151</v>
+        <v>1164</v>
       </c>
       <c r="D403" s="1" t="s">
-        <v>1150</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="404" spans="1:4">
       <c r="A404" s="1" t="s">
-        <v>1156</v>
+        <v>829</v>
       </c>
       <c r="B404" s="1" t="s">
-        <v>1157</v>
+        <v>830</v>
       </c>
       <c r="D404" s="1" t="s">
-        <v>1155</v>
+        <v>831</v>
       </c>
     </row>
     <row r="405" spans="1:4">
       <c r="A405" s="1" t="s">
-        <v>726</v>
+        <v>1152</v>
       </c>
       <c r="B405" s="1" t="s">
-        <v>727</v>
+        <v>1151</v>
       </c>
       <c r="D405" s="1" t="s">
-        <v>728</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="406" spans="1:4">
       <c r="A406" s="1" t="s">
-        <v>723</v>
+        <v>1156</v>
       </c>
       <c r="B406" s="1" t="s">
-        <v>724</v>
+        <v>1157</v>
       </c>
       <c r="D406" s="1" t="s">
-        <v>725</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="407" spans="1:4">
       <c r="A407" s="1" t="s">
-        <v>515</v>
+        <v>726</v>
       </c>
       <c r="B407" s="1" t="s">
-        <v>516</v>
+        <v>727</v>
       </c>
       <c r="D407" s="1" t="s">
-        <v>517</v>
+        <v>728</v>
       </c>
     </row>
     <row r="408" spans="1:4">
       <c r="A408" s="1" t="s">
-        <v>590</v>
+        <v>723</v>
       </c>
       <c r="B408" s="1" t="s">
-        <v>591</v>
+        <v>724</v>
       </c>
       <c r="D408" s="1" t="s">
-        <v>592</v>
+        <v>725</v>
       </c>
     </row>
     <row r="409" spans="1:4">
       <c r="A409" s="1" t="s">
-        <v>673</v>
+        <v>515</v>
       </c>
       <c r="B409" s="1" t="s">
-        <v>674</v>
+        <v>516</v>
       </c>
       <c r="D409" s="1" t="s">
-        <v>675</v>
+        <v>517</v>
       </c>
     </row>
     <row r="410" spans="1:4">
       <c r="A410" s="1" t="s">
-        <v>653</v>
+        <v>590</v>
       </c>
       <c r="B410" s="1" t="s">
-        <v>654</v>
+        <v>591</v>
       </c>
       <c r="D410" s="1" t="s">
-        <v>1030</v>
+        <v>592</v>
       </c>
     </row>
     <row r="411" spans="1:4">
       <c r="A411" s="1" t="s">
-        <v>1040</v>
+        <v>673</v>
       </c>
       <c r="B411" s="1" t="s">
-        <v>1041</v>
+        <v>674</v>
       </c>
       <c r="D411" s="1" t="s">
-        <v>1042</v>
+        <v>675</v>
       </c>
     </row>
     <row r="412" spans="1:4">
       <c r="A412" s="1" t="s">
-        <v>1023</v>
+        <v>653</v>
       </c>
       <c r="B412" s="1" t="s">
-        <v>1022</v>
+        <v>654</v>
       </c>
       <c r="D412" s="1" t="s">
-        <v>1024</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="413" spans="1:4">
       <c r="A413" s="1" t="s">
-        <v>841</v>
+        <v>1040</v>
       </c>
       <c r="B413" s="1" t="s">
-        <v>842</v>
+        <v>1041</v>
       </c>
       <c r="D413" s="1" t="s">
-        <v>843</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="414" spans="1:4">
       <c r="A414" s="1" t="s">
-        <v>1254</v>
+        <v>1023</v>
       </c>
       <c r="B414" s="1" t="s">
-        <v>1255</v>
+        <v>1022</v>
       </c>
       <c r="D414" s="1" t="s">
-        <v>1256</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="415" spans="1:4">
       <c r="A415" s="1" t="s">
-        <v>1251</v>
+        <v>841</v>
       </c>
       <c r="B415" s="1" t="s">
-        <v>1252</v>
+        <v>842</v>
       </c>
       <c r="D415" s="1" t="s">
-        <v>1253</v>
+        <v>843</v>
       </c>
     </row>
     <row r="416" spans="1:4">
       <c r="A416" s="1" t="s">
-        <v>470</v>
+        <v>1254</v>
       </c>
       <c r="B416" s="1" t="s">
-        <v>471</v>
+        <v>1255</v>
       </c>
       <c r="D416" s="1" t="s">
-        <v>472</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="417" spans="1:4">
       <c r="A417" s="1" t="s">
-        <v>971</v>
+        <v>1251</v>
       </c>
       <c r="B417" s="1" t="s">
-        <v>918</v>
+        <v>1252</v>
       </c>
       <c r="D417" s="1" t="s">
-        <v>1000</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="418" spans="1:4">
       <c r="A418" s="1" t="s">
-        <v>557</v>
+        <v>470</v>
       </c>
       <c r="B418" s="1" t="s">
-        <v>558</v>
+        <v>471</v>
       </c>
       <c r="D418" s="1" t="s">
-        <v>559</v>
+        <v>472</v>
       </c>
     </row>
     <row r="419" spans="1:4">
       <c r="A419" s="1" t="s">
-        <v>1233</v>
+        <v>971</v>
       </c>
       <c r="B419" s="1" t="s">
-        <v>1234</v>
+        <v>918</v>
       </c>
       <c r="D419" s="1" t="s">
-        <v>1235</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="420" spans="1:4">
       <c r="A420" s="1" t="s">
-        <v>968</v>
+        <v>557</v>
       </c>
       <c r="B420" s="1" t="s">
-        <v>917</v>
+        <v>558</v>
       </c>
       <c r="D420" s="1" t="s">
-        <v>970</v>
+        <v>559</v>
       </c>
     </row>
     <row r="421" spans="1:4">
       <c r="A421" s="1" t="s">
-        <v>494</v>
+        <v>1233</v>
       </c>
       <c r="B421" s="1" t="s">
-        <v>495</v>
+        <v>1234</v>
       </c>
       <c r="D421" s="1" t="s">
-        <v>496</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="422" spans="1:4">
       <c r="A422" s="1" t="s">
-        <v>1170</v>
+        <v>968</v>
       </c>
       <c r="B422" s="1" t="s">
-        <v>1171</v>
+        <v>917</v>
       </c>
       <c r="D422" s="1" t="s">
-        <v>1172</v>
+        <v>970</v>
       </c>
     </row>
     <row r="423" spans="1:4">
       <c r="A423" s="1" t="s">
-        <v>987</v>
+        <v>494</v>
       </c>
       <c r="B423" s="1" t="s">
-        <v>988</v>
+        <v>495</v>
       </c>
       <c r="D423" s="1" t="s">
-        <v>989</v>
+        <v>496</v>
       </c>
     </row>
     <row r="424" spans="1:4">
       <c r="A424" s="1" t="s">
-        <v>979</v>
+        <v>1170</v>
       </c>
       <c r="B424" s="1" t="s">
-        <v>915</v>
+        <v>1171</v>
       </c>
       <c r="D424" s="1" t="s">
-        <v>972</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="425" spans="1:4">
       <c r="A425" s="1" t="s">
-        <v>978</v>
+        <v>987</v>
       </c>
       <c r="B425" s="1" t="s">
-        <v>914</v>
+        <v>988</v>
       </c>
       <c r="D425" s="1" t="s">
-        <v>973</v>
+        <v>989</v>
       </c>
     </row>
     <row r="426" spans="1:4">
       <c r="A426" s="1" t="s">
-        <v>897</v>
+        <v>979</v>
       </c>
       <c r="B426" s="1" t="s">
-        <v>898</v>
+        <v>915</v>
       </c>
       <c r="D426" s="1" t="s">
-        <v>899</v>
+        <v>972</v>
       </c>
     </row>
     <row r="427" spans="1:4">
       <c r="A427" s="1" t="s">
-        <v>479</v>
+        <v>978</v>
       </c>
       <c r="B427" s="1" t="s">
-        <v>480</v>
+        <v>914</v>
       </c>
       <c r="D427" s="1" t="s">
-        <v>481</v>
+        <v>973</v>
       </c>
     </row>
     <row r="428" spans="1:4">
       <c r="A428" s="1" t="s">
-        <v>1068</v>
+        <v>897</v>
       </c>
       <c r="B428" s="1" t="s">
-        <v>1069</v>
+        <v>898</v>
       </c>
       <c r="D428" s="1" t="s">
-        <v>1010</v>
+        <v>899</v>
       </c>
     </row>
     <row r="429" spans="1:4">
       <c r="A429" s="1" t="s">
-        <v>497</v>
+        <v>479</v>
       </c>
       <c r="B429" s="1" t="s">
-        <v>498</v>
+        <v>480</v>
       </c>
       <c r="D429" s="1" t="s">
-        <v>499</v>
+        <v>481</v>
       </c>
     </row>
     <row r="430" spans="1:4">
       <c r="A430" s="1" t="s">
-        <v>482</v>
+        <v>1068</v>
       </c>
       <c r="B430" s="1" t="s">
-        <v>483</v>
+        <v>1069</v>
       </c>
       <c r="D430" s="1" t="s">
-        <v>484</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="431" spans="1:4">
       <c r="A431" s="1" t="s">
-        <v>1160</v>
+        <v>497</v>
       </c>
       <c r="B431" s="1" t="s">
-        <v>1161</v>
+        <v>498</v>
       </c>
       <c r="D431" s="1" t="s">
-        <v>1162</v>
+        <v>499</v>
       </c>
     </row>
     <row r="432" spans="1:4">
       <c r="A432" s="1" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="B432" s="1" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="D432" s="1" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
     </row>
     <row r="433" spans="1:4">
       <c r="A433" s="1" t="s">
-        <v>940</v>
+        <v>1160</v>
       </c>
       <c r="B433" s="1" t="s">
-        <v>941</v>
+        <v>1161</v>
       </c>
       <c r="D433" s="1" t="s">
-        <v>942</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="434" spans="1:4">
       <c r="A434" s="1" t="s">
-        <v>703</v>
+        <v>485</v>
       </c>
       <c r="B434" s="1" t="s">
-        <v>704</v>
+        <v>486</v>
       </c>
       <c r="D434" s="1" t="s">
-        <v>705</v>
+        <v>487</v>
       </c>
     </row>
     <row r="435" spans="1:4">
       <c r="A435" s="1" t="s">
-        <v>799</v>
+        <v>940</v>
       </c>
       <c r="B435" s="1" t="s">
-        <v>800</v>
+        <v>941</v>
       </c>
       <c r="D435" s="1" t="s">
-        <v>801</v>
+        <v>942</v>
       </c>
     </row>
     <row r="436" spans="1:4">
       <c r="A436" s="1" t="s">
-        <v>530</v>
+        <v>703</v>
       </c>
       <c r="B436" s="1" t="s">
-        <v>531</v>
+        <v>704</v>
       </c>
       <c r="D436" s="1" t="s">
-        <v>532</v>
+        <v>705</v>
       </c>
     </row>
     <row r="437" spans="1:4">
       <c r="A437" s="1" t="s">
-        <v>500</v>
+        <v>799</v>
       </c>
       <c r="B437" s="1" t="s">
-        <v>501</v>
+        <v>800</v>
       </c>
       <c r="D437" s="1" t="s">
-        <v>502</v>
+        <v>801</v>
       </c>
     </row>
     <row r="438" spans="1:4">
       <c r="A438" s="1" t="s">
-        <v>414</v>
+        <v>530</v>
       </c>
       <c r="B438" s="1" t="s">
-        <v>415</v>
+        <v>531</v>
       </c>
       <c r="D438" s="1" t="s">
-        <v>416</v>
+        <v>532</v>
       </c>
     </row>
     <row r="439" spans="1:4">
       <c r="A439" s="1" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="B439" s="1" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="D439" s="1" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="440" spans="1:4">
       <c r="A440" s="1" t="s">
-        <v>720</v>
+        <v>414</v>
       </c>
       <c r="B440" s="1" t="s">
-        <v>721</v>
+        <v>415</v>
       </c>
       <c r="D440" s="1" t="s">
-        <v>722</v>
+        <v>416</v>
       </c>
     </row>
     <row r="441" spans="1:4">
       <c r="A441" s="1" t="s">
-        <v>554</v>
+        <v>503</v>
       </c>
       <c r="B441" s="1" t="s">
-        <v>555</v>
+        <v>504</v>
       </c>
       <c r="D441" s="1" t="s">
-        <v>556</v>
+        <v>505</v>
       </c>
     </row>
     <row r="442" spans="1:4">
       <c r="A442" s="1" t="s">
-        <v>560</v>
+        <v>720</v>
       </c>
       <c r="B442" s="1" t="s">
-        <v>561</v>
+        <v>721</v>
       </c>
       <c r="D442" s="1" t="s">
-        <v>562</v>
+        <v>722</v>
       </c>
     </row>
     <row r="443" spans="1:4">
       <c r="A443" s="1" t="s">
-        <v>548</v>
+        <v>554</v>
       </c>
       <c r="B443" s="1" t="s">
-        <v>549</v>
+        <v>555</v>
       </c>
       <c r="D443" s="1" t="s">
-        <v>550</v>
+        <v>556</v>
       </c>
     </row>
     <row r="444" spans="1:4">
       <c r="A444" s="1" t="s">
-        <v>762</v>
+        <v>560</v>
       </c>
       <c r="B444" s="1" t="s">
-        <v>763</v>
+        <v>561</v>
       </c>
       <c r="D444" s="1" t="s">
-        <v>550</v>
+        <v>562</v>
       </c>
     </row>
     <row r="445" spans="1:4">
       <c r="A445" s="1" t="s">
-        <v>1278</v>
+        <v>548</v>
       </c>
       <c r="B445" s="1" t="s">
-        <v>1279</v>
+        <v>549</v>
       </c>
       <c r="D445" s="1" t="s">
-        <v>1280</v>
+        <v>550</v>
       </c>
     </row>
     <row r="446" spans="1:4">
       <c r="A446" s="1" t="s">
-        <v>617</v>
+        <v>762</v>
       </c>
       <c r="B446" s="1" t="s">
-        <v>618</v>
+        <v>763</v>
       </c>
       <c r="D446" s="1" t="s">
-        <v>1007</v>
+        <v>550</v>
       </c>
     </row>
     <row r="447" spans="1:4">
       <c r="A447" s="1" t="s">
-        <v>605</v>
+        <v>1278</v>
       </c>
       <c r="B447" s="1" t="s">
-        <v>606</v>
+        <v>1279</v>
       </c>
       <c r="D447" s="1" t="s">
-        <v>607</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="448" spans="1:4">
       <c r="A448" s="1" t="s">
-        <v>1179</v>
+        <v>617</v>
       </c>
       <c r="B448" s="1" t="s">
-        <v>1186</v>
+        <v>618</v>
       </c>
       <c r="D448" s="1" t="s">
-        <v>1193</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="449" spans="1:4">
       <c r="A449" s="1" t="s">
-        <v>1180</v>
+        <v>605</v>
       </c>
       <c r="B449" s="1" t="s">
-        <v>1187</v>
+        <v>606</v>
       </c>
       <c r="D449" s="1" t="s">
-        <v>1194</v>
+        <v>607</v>
       </c>
     </row>
     <row r="450" spans="1:4">
       <c r="A450" s="1" t="s">
-        <v>449</v>
+        <v>1179</v>
       </c>
       <c r="B450" s="1" t="s">
-        <v>450</v>
+        <v>1186</v>
       </c>
       <c r="D450" s="1" t="s">
-        <v>451</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="451" spans="1:4">
       <c r="A451" s="1" t="s">
-        <v>1166</v>
+        <v>1180</v>
       </c>
       <c r="B451" s="1" t="s">
-        <v>1167</v>
+        <v>1187</v>
       </c>
       <c r="D451" s="1" t="s">
-        <v>1168</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="452" spans="1:4">
       <c r="A452" s="1" t="s">
-        <v>1181</v>
+        <v>449</v>
       </c>
       <c r="B452" s="1" t="s">
-        <v>1188</v>
+        <v>450</v>
       </c>
       <c r="D452" s="1" t="s">
-        <v>1195</v>
+        <v>451</v>
       </c>
     </row>
     <row r="453" spans="1:4">
       <c r="A453" s="1" t="s">
-        <v>1182</v>
+        <v>1166</v>
       </c>
       <c r="B453" s="1" t="s">
-        <v>1189</v>
+        <v>1167</v>
       </c>
       <c r="D453" s="1" t="s">
-        <v>1196</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="454" spans="1:4">
       <c r="A454" s="1" t="s">
-        <v>688</v>
+        <v>1181</v>
       </c>
       <c r="B454" s="1" t="s">
-        <v>689</v>
+        <v>1188</v>
       </c>
       <c r="D454" s="1" t="s">
-        <v>690</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="455" spans="1:4">
       <c r="A455" s="1" t="s">
-        <v>452</v>
+        <v>1182</v>
       </c>
       <c r="B455" s="1" t="s">
-        <v>453</v>
+        <v>1189</v>
       </c>
       <c r="D455" s="1" t="s">
-        <v>454</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="456" spans="1:4">
       <c r="A456" s="1" t="s">
-        <v>1200</v>
+        <v>688</v>
       </c>
       <c r="B456" s="1" t="s">
-        <v>1201</v>
+        <v>689</v>
       </c>
       <c r="D456" s="1" t="s">
-        <v>1218</v>
+        <v>690</v>
       </c>
     </row>
     <row r="457" spans="1:4">
       <c r="A457" s="1" t="s">
-        <v>764</v>
+        <v>452</v>
       </c>
       <c r="B457" s="1" t="s">
-        <v>765</v>
+        <v>453</v>
       </c>
       <c r="D457" s="1" t="s">
-        <v>766</v>
+        <v>454</v>
       </c>
     </row>
     <row r="458" spans="1:4">
       <c r="A458" s="1" t="s">
-        <v>1248</v>
+        <v>1200</v>
       </c>
       <c r="B458" s="1" t="s">
-        <v>1249</v>
+        <v>1201</v>
       </c>
       <c r="D458" s="1" t="s">
-        <v>1250</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="459" spans="1:4">
       <c r="A459" s="1" t="s">
-        <v>1046</v>
+        <v>764</v>
       </c>
       <c r="B459" s="1" t="s">
-        <v>1047</v>
+        <v>765</v>
       </c>
       <c r="D459" s="1" t="s">
-        <v>1048</v>
+        <v>766</v>
       </c>
     </row>
     <row r="460" spans="1:4">
       <c r="A460" s="1" t="s">
-        <v>820</v>
+        <v>1248</v>
       </c>
       <c r="B460" s="1" t="s">
-        <v>821</v>
+        <v>1249</v>
       </c>
       <c r="D460" s="1" t="s">
-        <v>822</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="461" spans="1:4">
       <c r="A461" s="1" t="s">
-        <v>420</v>
+        <v>1046</v>
       </c>
       <c r="B461" s="1" t="s">
-        <v>421</v>
+        <v>1047</v>
       </c>
       <c r="D461" s="1" t="s">
-        <v>422</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="462" spans="1:4">
       <c r="A462" s="1" t="s">
-        <v>1011</v>
+        <v>820</v>
       </c>
       <c r="B462" s="1" t="s">
-        <v>1012</v>
+        <v>821</v>
       </c>
       <c r="D462" s="1" t="s">
-        <v>1013</v>
+        <v>822</v>
       </c>
     </row>
     <row r="463" spans="1:4">
       <c r="A463" s="1" t="s">
-        <v>743</v>
+        <v>420</v>
       </c>
       <c r="B463" s="1" t="s">
-        <v>744</v>
+        <v>421</v>
       </c>
       <c r="D463" s="1" t="s">
-        <v>745</v>
+        <v>422</v>
       </c>
     </row>
     <row r="464" spans="1:4">
       <c r="A464" s="1" t="s">
-        <v>901</v>
+        <v>1011</v>
       </c>
       <c r="B464" s="1" t="s">
-        <v>900</v>
+        <v>1012</v>
       </c>
       <c r="D464" s="1" t="s">
-        <v>902</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="465" spans="1:4">
       <c r="A465" s="1" t="s">
-        <v>903</v>
+        <v>743</v>
       </c>
       <c r="B465" s="1" t="s">
-        <v>904</v>
+        <v>744</v>
       </c>
       <c r="D465" s="1" t="s">
-        <v>905</v>
+        <v>745</v>
       </c>
     </row>
     <row r="466" spans="1:4">
       <c r="A466" s="1" t="s">
-        <v>539</v>
+        <v>901</v>
       </c>
       <c r="B466" s="1" t="s">
-        <v>540</v>
+        <v>900</v>
       </c>
       <c r="D466" s="1" t="s">
-        <v>541</v>
+        <v>902</v>
       </c>
     </row>
     <row r="467" spans="1:4">
       <c r="A467" s="1" t="s">
-        <v>661</v>
+        <v>903</v>
       </c>
       <c r="B467" s="1" t="s">
-        <v>662</v>
+        <v>904</v>
       </c>
       <c r="D467" s="1" t="s">
-        <v>663</v>
+        <v>905</v>
       </c>
     </row>
     <row r="468" spans="1:4">
       <c r="A468" s="1" t="s">
-        <v>691</v>
+        <v>539</v>
       </c>
       <c r="B468" s="1" t="s">
-        <v>692</v>
+        <v>540</v>
       </c>
       <c r="D468" s="1" t="s">
-        <v>693</v>
+        <v>541</v>
       </c>
     </row>
     <row r="469" spans="1:4">
       <c r="A469" s="1" t="s">
-        <v>963</v>
+        <v>661</v>
       </c>
       <c r="B469" s="1" t="s">
-        <v>922</v>
+        <v>662</v>
       </c>
       <c r="D469" s="1" t="s">
-        <v>908</v>
+        <v>663</v>
       </c>
     </row>
     <row r="470" spans="1:4">
       <c r="A470" s="1" t="s">
-        <v>785</v>
+        <v>691</v>
       </c>
       <c r="B470" s="1" t="s">
-        <v>786</v>
+        <v>692</v>
       </c>
       <c r="D470" s="1" t="s">
-        <v>787</v>
+        <v>693</v>
       </c>
     </row>
     <row r="471" spans="1:4">
       <c r="A471" s="1" t="s">
-        <v>622</v>
+        <v>963</v>
       </c>
       <c r="B471" s="1" t="s">
-        <v>623</v>
+        <v>922</v>
       </c>
       <c r="D471" s="1" t="s">
-        <v>624</v>
+        <v>908</v>
       </c>
     </row>
     <row r="472" spans="1:4">
       <c r="A472" s="1" t="s">
-        <v>835</v>
+        <v>785</v>
       </c>
       <c r="B472" s="1" t="s">
-        <v>836</v>
+        <v>786</v>
       </c>
       <c r="D472" s="1" t="s">
-        <v>837</v>
+        <v>787</v>
       </c>
     </row>
     <row r="473" spans="1:4">
       <c r="A473" s="1" t="s">
-        <v>685</v>
+        <v>622</v>
       </c>
       <c r="B473" s="1" t="s">
-        <v>686</v>
+        <v>623</v>
       </c>
       <c r="D473" s="1" t="s">
-        <v>687</v>
+        <v>624</v>
       </c>
     </row>
     <row r="474" spans="1:4">
       <c r="A474" s="1" t="s">
-        <v>892</v>
+        <v>835</v>
       </c>
       <c r="B474" s="1" t="s">
-        <v>893</v>
+        <v>836</v>
+      </c>
+      <c r="D474" s="1" t="s">
+        <v>837</v>
       </c>
     </row>
     <row r="475" spans="1:4">
       <c r="A475" s="1" t="s">
-        <v>967</v>
+        <v>685</v>
       </c>
       <c r="B475" s="1" t="s">
-        <v>916</v>
+        <v>686</v>
       </c>
       <c r="D475" s="1" t="s">
-        <v>969</v>
+        <v>687</v>
       </c>
     </row>
     <row r="476" spans="1:4">
       <c r="A476" s="1" t="s">
-        <v>946</v>
+        <v>892</v>
       </c>
       <c r="B476" s="1" t="s">
-        <v>947</v>
-      </c>
-      <c r="D476" s="1" t="s">
-        <v>948</v>
+        <v>893</v>
       </c>
     </row>
     <row r="477" spans="1:4">
       <c r="A477" s="1" t="s">
-        <v>473</v>
+        <v>967</v>
       </c>
       <c r="B477" s="1" t="s">
-        <v>474</v>
+        <v>916</v>
       </c>
       <c r="D477" s="1" t="s">
-        <v>475</v>
+        <v>969</v>
       </c>
     </row>
     <row r="478" spans="1:4">
       <c r="A478" s="1" t="s">
-        <v>566</v>
+        <v>946</v>
       </c>
       <c r="B478" s="1" t="s">
-        <v>567</v>
+        <v>947</v>
       </c>
       <c r="D478" s="1" t="s">
-        <v>568</v>
+        <v>948</v>
       </c>
     </row>
     <row r="479" spans="1:4">
       <c r="A479" s="1" t="s">
-        <v>767</v>
+        <v>473</v>
       </c>
       <c r="B479" s="1" t="s">
-        <v>768</v>
+        <v>474</v>
       </c>
       <c r="D479" s="1" t="s">
-        <v>769</v>
+        <v>475</v>
       </c>
     </row>
     <row r="480" spans="1:4">
       <c r="A480" s="1" t="s">
-        <v>770</v>
+        <v>566</v>
       </c>
       <c r="B480" s="1" t="s">
-        <v>771</v>
+        <v>567</v>
       </c>
       <c r="D480" s="1" t="s">
-        <v>353</v>
+        <v>568</v>
       </c>
     </row>
     <row r="481" spans="1:4">
       <c r="A481" s="1" t="s">
-        <v>711</v>
+        <v>767</v>
       </c>
       <c r="B481" s="1" t="s">
-        <v>712</v>
+        <v>768</v>
       </c>
       <c r="D481" s="1" t="s">
-        <v>713</v>
+        <v>769</v>
       </c>
     </row>
     <row r="482" spans="1:4">
       <c r="A482" s="1" t="s">
-        <v>877</v>
+        <v>770</v>
       </c>
       <c r="B482" s="1" t="s">
-        <v>878</v>
+        <v>771</v>
       </c>
       <c r="D482" s="1" t="s">
-        <v>879</v>
+        <v>353</v>
       </c>
     </row>
     <row r="483" spans="1:4">
       <c r="A483" s="1" t="s">
-        <v>1142</v>
+        <v>711</v>
       </c>
       <c r="B483" s="1" t="s">
-        <v>1143</v>
+        <v>712</v>
       </c>
       <c r="D483" s="1" t="s">
-        <v>1141</v>
+        <v>713</v>
       </c>
     </row>
     <row r="484" spans="1:4">
       <c r="A484" s="1" t="s">
-        <v>949</v>
+        <v>877</v>
       </c>
       <c r="B484" s="1" t="s">
-        <v>951</v>
+        <v>878</v>
       </c>
       <c r="D484" s="1" t="s">
-        <v>952</v>
+        <v>879</v>
       </c>
     </row>
     <row r="485" spans="1:4">
       <c r="A485" s="1" t="s">
-        <v>746</v>
+        <v>1142</v>
       </c>
       <c r="B485" s="1" t="s">
-        <v>747</v>
+        <v>1143</v>
       </c>
       <c r="D485" s="1" t="s">
-        <v>748</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="486" spans="1:4">
       <c r="A486" s="1" t="s">
-        <v>1227</v>
+        <v>949</v>
       </c>
       <c r="B486" s="1" t="s">
-        <v>1228</v>
+        <v>951</v>
       </c>
       <c r="D486" s="1" t="s">
-        <v>1229</v>
+        <v>952</v>
       </c>
     </row>
     <row r="487" spans="1:4">
       <c r="A487" s="1" t="s">
-        <v>575</v>
+        <v>746</v>
       </c>
       <c r="B487" s="1" t="s">
-        <v>576</v>
+        <v>747</v>
       </c>
       <c r="D487" s="1" t="s">
-        <v>577</v>
+        <v>748</v>
       </c>
     </row>
     <row r="488" spans="1:4">
       <c r="A488" s="1" t="s">
-        <v>823</v>
+        <v>1227</v>
       </c>
       <c r="B488" s="1" t="s">
-        <v>824</v>
+        <v>1228</v>
       </c>
       <c r="D488" s="1" t="s">
-        <v>825</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="489" spans="1:4">
       <c r="A489" s="1" t="s">
-        <v>1019</v>
+        <v>575</v>
       </c>
       <c r="B489" s="1" t="s">
-        <v>1020</v>
+        <v>576</v>
       </c>
       <c r="D489" s="1" t="s">
-        <v>1021</v>
+        <v>577</v>
       </c>
     </row>
     <row r="490" spans="1:4">
       <c r="A490" s="1" t="s">
-        <v>426</v>
+        <v>823</v>
       </c>
       <c r="B490" s="1" t="s">
-        <v>427</v>
+        <v>824</v>
       </c>
       <c r="D490" s="1" t="s">
-        <v>428</v>
+        <v>825</v>
       </c>
     </row>
     <row r="491" spans="1:4">
       <c r="A491" s="1" t="s">
-        <v>625</v>
+        <v>1019</v>
       </c>
       <c r="B491" s="1" t="s">
-        <v>626</v>
+        <v>1020</v>
       </c>
       <c r="D491" s="1" t="s">
-        <v>627</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="492" spans="1:4">
       <c r="A492" s="1" t="s">
-        <v>417</v>
+        <v>426</v>
       </c>
       <c r="B492" s="1" t="s">
-        <v>418</v>
+        <v>427</v>
       </c>
       <c r="D492" s="1" t="s">
-        <v>419</v>
+        <v>428</v>
       </c>
     </row>
     <row r="493" spans="1:4">
       <c r="A493" s="1" t="s">
-        <v>928</v>
+        <v>625</v>
       </c>
       <c r="B493" s="1" t="s">
-        <v>929</v>
+        <v>626</v>
       </c>
       <c r="D493" s="1" t="s">
-        <v>930</v>
+        <v>627</v>
       </c>
     </row>
     <row r="494" spans="1:4">
       <c r="A494" s="1" t="s">
-        <v>1263</v>
+        <v>417</v>
       </c>
       <c r="B494" s="1" t="s">
-        <v>1264</v>
+        <v>418</v>
       </c>
       <c r="D494" s="1" t="s">
-        <v>1265</v>
+        <v>419</v>
       </c>
     </row>
     <row r="495" spans="1:4">
       <c r="A495" s="1" t="s">
-        <v>1239</v>
+        <v>928</v>
       </c>
       <c r="B495" s="1" t="s">
-        <v>1242</v>
+        <v>929</v>
       </c>
       <c r="D495" s="1" t="s">
-        <v>1244</v>
+        <v>930</v>
       </c>
     </row>
     <row r="496" spans="1:4">
       <c r="A496" s="1" t="s">
-        <v>734</v>
+        <v>1263</v>
       </c>
       <c r="B496" s="1" t="s">
-        <v>735</v>
+        <v>1264</v>
       </c>
       <c r="D496" s="1" t="s">
-        <v>736</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="497" spans="1:4">
       <c r="A497" s="1" t="s">
-        <v>737</v>
+        <v>1239</v>
       </c>
       <c r="B497" s="1" t="s">
-        <v>738</v>
+        <v>1242</v>
       </c>
       <c r="D497" s="1" t="s">
-        <v>739</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="498" spans="1:4">
       <c r="A498" s="1" t="s">
-        <v>1240</v>
+        <v>734</v>
       </c>
       <c r="B498" s="1" t="s">
-        <v>1247</v>
+        <v>735</v>
       </c>
       <c r="D498" s="1" t="s">
-        <v>1246</v>
+        <v>736</v>
       </c>
     </row>
     <row r="499" spans="1:4">
       <c r="A499" s="1" t="s">
-        <v>1241</v>
+        <v>737</v>
       </c>
       <c r="B499" s="1" t="s">
-        <v>1243</v>
+        <v>738</v>
       </c>
       <c r="D499" s="1" t="s">
-        <v>1245</v>
+        <v>739</v>
       </c>
     </row>
     <row r="500" spans="1:4">
       <c r="A500" s="1" t="s">
-        <v>740</v>
+        <v>1240</v>
       </c>
       <c r="B500" s="1" t="s">
-        <v>741</v>
+        <v>1247</v>
       </c>
       <c r="D500" s="1" t="s">
-        <v>742</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="501" spans="1:4">
       <c r="A501" s="1" t="s">
-        <v>628</v>
+        <v>1241</v>
       </c>
       <c r="B501" s="1" t="s">
-        <v>629</v>
+        <v>1243</v>
       </c>
       <c r="D501" s="1" t="s">
-        <v>630</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="502" spans="1:4">
       <c r="A502" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="B502" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="D502" s="1" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="503" spans="1:4">
+      <c r="A503" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="B503" s="1" t="s">
+        <v>629</v>
+      </c>
+      <c r="D503" s="1" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="504" spans="1:4">
+      <c r="A504" s="1" t="s">
         <v>631</v>
       </c>
-      <c r="B502" s="1" t="s">
+      <c r="B504" s="1" t="s">
         <v>632</v>
       </c>
-      <c r="D502" s="1" t="s">
+      <c r="D504" s="1" t="s">
         <v>633</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A224:G433">
+  <sortState ref="A224:G435">
     <sortCondition ref="A224"/>
   </sortState>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
Follow Play Framework v2.7.0-RC9
</commit_message>
<xml_diff>
--- a/conf/messages.xlsx
+++ b/conf/messages.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hiro/github/FinePlay/conf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13DE5706-8CB2-8D4C-A3D5-5DF26A5AAD49}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA208F38-A2A7-F84A-BE84-548BC1162BE6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3740" yWindow="920" windowWidth="33460" windowHeight="21560" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1461" uniqueCount="1391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1467" uniqueCount="1397">
   <si>
     <t>key</t>
   </si>
@@ -4891,6 +4891,36 @@
   </si>
   <si>
     <t>SMS</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>clear</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Clear</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>消去</t>
+    <rPh sb="0" eb="2">
+      <t>ショウky</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>strict</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Strict</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>厳密</t>
+    <rPh sb="0" eb="2">
+      <t>ゲンミt</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -5635,10 +5665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G540"/>
+  <dimension ref="A1:G542"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A457" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F478" sqref="F478"/>
+    <sheetView tabSelected="1" topLeftCell="A467" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D488" sqref="D488"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -8198,925 +8228,925 @@
     </row>
     <row r="279" spans="1:4">
       <c r="A279" s="1" t="s">
-        <v>563</v>
+        <v>1391</v>
       </c>
       <c r="B279" s="1" t="s">
-        <v>564</v>
+        <v>1392</v>
       </c>
       <c r="D279" s="1" t="s">
-        <v>565</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="280" spans="1:4">
       <c r="A280" s="1" t="s">
-        <v>1229</v>
+        <v>563</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>1230</v>
+        <v>564</v>
       </c>
       <c r="D280" s="1" t="s">
-        <v>1231</v>
+        <v>565</v>
       </c>
     </row>
     <row r="281" spans="1:4">
       <c r="A281" s="1" t="s">
-        <v>545</v>
+        <v>1229</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>546</v>
+        <v>1230</v>
       </c>
       <c r="D281" s="1" t="s">
-        <v>547</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="282" spans="1:4">
       <c r="A282" s="1" t="s">
-        <v>868</v>
+        <v>545</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>869</v>
+        <v>546</v>
       </c>
       <c r="D282" s="1" t="s">
-        <v>870</v>
+        <v>547</v>
       </c>
     </row>
     <row r="283" spans="1:4">
       <c r="A283" s="1" t="s">
-        <v>1274</v>
+        <v>868</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>1275</v>
+        <v>869</v>
       </c>
       <c r="D283" s="1" t="s">
-        <v>1276</v>
+        <v>870</v>
       </c>
     </row>
     <row r="284" spans="1:4">
       <c r="A284" s="1" t="s">
-        <v>706</v>
+        <v>1274</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>707</v>
+        <v>1275</v>
       </c>
       <c r="D284" s="1" t="s">
-        <v>708</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="285" spans="1:4">
       <c r="A285" s="1" t="s">
-        <v>393</v>
+        <v>706</v>
       </c>
       <c r="B285" s="1" t="s">
-        <v>394</v>
+        <v>707</v>
       </c>
       <c r="D285" s="1" t="s">
-        <v>395</v>
+        <v>708</v>
       </c>
     </row>
     <row r="286" spans="1:4">
       <c r="A286" s="1" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="D286" s="1" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="287" spans="1:4">
       <c r="A287" s="1" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="B287" s="1" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="D287" s="1" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
     <row r="288" spans="1:4">
       <c r="A288" s="1" t="s">
-        <v>458</v>
+        <v>399</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>459</v>
+        <v>400</v>
       </c>
       <c r="D288" s="1" t="s">
-        <v>460</v>
+        <v>401</v>
       </c>
     </row>
     <row r="289" spans="1:4">
       <c r="A289" s="1" t="s">
-        <v>1182</v>
+        <v>458</v>
       </c>
       <c r="B289" s="1" t="s">
-        <v>1189</v>
+        <v>459</v>
       </c>
       <c r="D289" s="1" t="s">
-        <v>1196</v>
+        <v>460</v>
       </c>
     </row>
     <row r="290" spans="1:4">
       <c r="A290" s="1" t="s">
-        <v>817</v>
+        <v>1182</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>818</v>
+        <v>1189</v>
       </c>
       <c r="D290" s="1" t="s">
-        <v>819</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="291" spans="1:4">
       <c r="A291" s="1" t="s">
-        <v>634</v>
+        <v>817</v>
       </c>
       <c r="B291" s="1" t="s">
-        <v>635</v>
+        <v>818</v>
       </c>
       <c r="D291" s="1" t="s">
-        <v>636</v>
+        <v>819</v>
       </c>
     </row>
     <row r="292" spans="1:4">
       <c r="A292" s="1" t="s">
-        <v>655</v>
+        <v>634</v>
       </c>
       <c r="B292" s="1" t="s">
-        <v>656</v>
+        <v>635</v>
       </c>
       <c r="D292" s="1" t="s">
-        <v>657</v>
+        <v>636</v>
       </c>
     </row>
     <row r="293" spans="1:4">
       <c r="A293" s="1" t="s">
-        <v>1299</v>
+        <v>655</v>
       </c>
       <c r="B293" s="1" t="s">
-        <v>1300</v>
+        <v>656</v>
       </c>
       <c r="D293" s="1" t="s">
-        <v>1301</v>
+        <v>657</v>
       </c>
     </row>
     <row r="294" spans="1:4">
       <c r="A294" s="1" t="s">
-        <v>781</v>
+        <v>1299</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>782</v>
+        <v>1300</v>
       </c>
       <c r="D294" s="1" t="s">
-        <v>783</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="295" spans="1:4">
       <c r="A295" s="1" t="s">
-        <v>697</v>
+        <v>781</v>
       </c>
       <c r="B295" s="1" t="s">
-        <v>698</v>
+        <v>782</v>
       </c>
       <c r="D295" s="1" t="s">
-        <v>699</v>
+        <v>783</v>
       </c>
     </row>
     <row r="296" spans="1:4">
       <c r="A296" s="1" t="s">
-        <v>1205</v>
+        <v>697</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>1206</v>
+        <v>698</v>
       </c>
       <c r="D296" s="1" t="s">
-        <v>1207</v>
+        <v>699</v>
       </c>
     </row>
     <row r="297" spans="1:4">
       <c r="A297" s="1" t="s">
-        <v>1148</v>
+        <v>1205</v>
       </c>
       <c r="B297" s="1" t="s">
-        <v>1147</v>
+        <v>1206</v>
       </c>
       <c r="D297" s="1" t="s">
-        <v>1146</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="298" spans="1:4">
       <c r="A298" s="1" t="s">
-        <v>467</v>
+        <v>1148</v>
       </c>
       <c r="B298" s="1" t="s">
-        <v>468</v>
+        <v>1147</v>
       </c>
       <c r="D298" s="1" t="s">
-        <v>469</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="299" spans="1:4">
       <c r="A299" s="1" t="s">
-        <v>778</v>
+        <v>467</v>
       </c>
       <c r="B299" s="1" t="s">
-        <v>779</v>
+        <v>468</v>
       </c>
       <c r="D299" s="1" t="s">
-        <v>780</v>
+        <v>469</v>
       </c>
     </row>
     <row r="300" spans="1:4">
       <c r="A300" s="1" t="s">
-        <v>1143</v>
+        <v>778</v>
       </c>
       <c r="B300" s="1" t="s">
-        <v>1144</v>
+        <v>779</v>
       </c>
       <c r="D300" s="1" t="s">
-        <v>1145</v>
+        <v>780</v>
       </c>
     </row>
     <row r="301" spans="1:4">
       <c r="A301" s="1" t="s">
-        <v>578</v>
+        <v>1143</v>
       </c>
       <c r="B301" s="1" t="s">
-        <v>579</v>
+        <v>1144</v>
       </c>
       <c r="D301" s="1" t="s">
-        <v>580</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="302" spans="1:4">
       <c r="A302" s="1" t="s">
-        <v>536</v>
+        <v>578</v>
       </c>
       <c r="B302" s="1" t="s">
-        <v>537</v>
+        <v>579</v>
       </c>
       <c r="D302" s="1" t="s">
-        <v>538</v>
+        <v>580</v>
       </c>
     </row>
     <row r="303" spans="1:4">
       <c r="A303" s="1" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="B303" s="1" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="D303" s="1" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
     </row>
     <row r="304" spans="1:4">
       <c r="A304" s="1" t="s">
-        <v>1014</v>
+        <v>533</v>
       </c>
       <c r="B304" s="1" t="s">
-        <v>1015</v>
+        <v>534</v>
       </c>
       <c r="D304" s="1" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="305" spans="1:4">
       <c r="A305" s="1" t="s">
-        <v>1210</v>
+        <v>1014</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>1209</v>
+        <v>1015</v>
       </c>
       <c r="D305" s="1" t="s">
-        <v>1208</v>
+        <v>538</v>
       </c>
     </row>
     <row r="306" spans="1:4">
       <c r="A306" s="1" t="s">
-        <v>1</v>
+        <v>1210</v>
       </c>
       <c r="B306" s="1" t="s">
-        <v>5</v>
+        <v>1209</v>
       </c>
       <c r="D306" s="1" t="s">
-        <v>221</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="307" spans="1:4">
       <c r="A307" s="1" t="s">
-        <v>476</v>
+        <v>1</v>
       </c>
       <c r="B307" s="1" t="s">
-        <v>477</v>
+        <v>5</v>
       </c>
       <c r="D307" s="1" t="s">
-        <v>478</v>
+        <v>221</v>
       </c>
     </row>
     <row r="308" spans="1:4">
       <c r="A308" s="1" t="s">
-        <v>667</v>
+        <v>476</v>
       </c>
       <c r="B308" s="1" t="s">
-        <v>668</v>
+        <v>477</v>
       </c>
       <c r="D308" s="1" t="s">
-        <v>669</v>
+        <v>478</v>
       </c>
     </row>
     <row r="309" spans="1:4">
       <c r="A309" s="1" t="s">
-        <v>506</v>
+        <v>667</v>
       </c>
       <c r="B309" s="1" t="s">
-        <v>507</v>
+        <v>668</v>
       </c>
       <c r="D309" s="1" t="s">
-        <v>508</v>
+        <v>669</v>
       </c>
     </row>
     <row r="310" spans="1:4">
       <c r="A310" s="1" t="s">
-        <v>850</v>
+        <v>506</v>
       </c>
       <c r="B310" s="1" t="s">
-        <v>851</v>
+        <v>507</v>
       </c>
       <c r="D310" s="1" t="s">
-        <v>852</v>
+        <v>508</v>
       </c>
     </row>
     <row r="311" spans="1:4">
       <c r="A311" s="1" t="s">
-        <v>643</v>
+        <v>850</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>644</v>
+        <v>851</v>
       </c>
       <c r="D311" s="1" t="s">
-        <v>645</v>
+        <v>852</v>
       </c>
     </row>
     <row r="312" spans="1:4">
       <c r="A312" s="1" t="s">
-        <v>788</v>
+        <v>643</v>
       </c>
       <c r="B312" s="1" t="s">
-        <v>789</v>
+        <v>644</v>
       </c>
       <c r="D312" s="1" t="s">
-        <v>790</v>
+        <v>645</v>
       </c>
     </row>
     <row r="313" spans="1:4">
       <c r="A313" s="1" t="s">
-        <v>1323</v>
+        <v>788</v>
       </c>
       <c r="B313" s="1" t="s">
-        <v>1324</v>
+        <v>789</v>
       </c>
       <c r="D313" s="1" t="s">
-        <v>1325</v>
+        <v>790</v>
       </c>
     </row>
     <row r="314" spans="1:4">
       <c r="A314" s="1" t="s">
-        <v>679</v>
+        <v>1323</v>
       </c>
       <c r="B314" s="1" t="s">
-        <v>680</v>
+        <v>1324</v>
       </c>
       <c r="D314" s="1" t="s">
-        <v>681</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="315" spans="1:4">
       <c r="A315" s="1" t="s">
-        <v>423</v>
+        <v>679</v>
       </c>
       <c r="B315" s="1" t="s">
-        <v>424</v>
+        <v>680</v>
       </c>
       <c r="D315" s="1" t="s">
-        <v>425</v>
+        <v>681</v>
       </c>
     </row>
     <row r="316" spans="1:4">
       <c r="A316" s="1" t="s">
-        <v>943</v>
+        <v>423</v>
       </c>
       <c r="B316" s="1" t="s">
-        <v>944</v>
+        <v>424</v>
       </c>
       <c r="D316" s="1" t="s">
-        <v>945</v>
+        <v>425</v>
       </c>
     </row>
     <row r="317" spans="1:4">
       <c r="A317" s="1" t="s">
-        <v>569</v>
+        <v>943</v>
       </c>
       <c r="B317" s="1" t="s">
-        <v>570</v>
+        <v>944</v>
       </c>
       <c r="D317" s="1" t="s">
-        <v>571</v>
+        <v>945</v>
       </c>
     </row>
     <row r="318" spans="1:4">
       <c r="A318" s="1" t="s">
-        <v>518</v>
+        <v>569</v>
       </c>
       <c r="B318" s="1" t="s">
-        <v>519</v>
+        <v>570</v>
       </c>
       <c r="D318" s="1" t="s">
-        <v>520</v>
+        <v>571</v>
       </c>
     </row>
     <row r="319" spans="1:4">
       <c r="A319" s="1" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="B319" s="1" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="D319" s="1" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="320" spans="1:4">
       <c r="A320" s="1" t="s">
-        <v>1031</v>
+        <v>521</v>
       </c>
       <c r="B320" s="1" t="s">
-        <v>1032</v>
+        <v>522</v>
       </c>
       <c r="D320" s="1" t="s">
-        <v>1033</v>
+        <v>523</v>
       </c>
     </row>
     <row r="321" spans="1:4">
       <c r="A321" s="1" t="s">
-        <v>491</v>
+        <v>1031</v>
       </c>
       <c r="B321" s="1" t="s">
-        <v>492</v>
+        <v>1032</v>
       </c>
       <c r="D321" s="1" t="s">
-        <v>493</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="322" spans="1:4">
       <c r="A322" s="1" t="s">
-        <v>772</v>
+        <v>491</v>
       </c>
       <c r="B322" s="1" t="s">
-        <v>23</v>
+        <v>492</v>
       </c>
       <c r="D322" s="1" t="s">
-        <v>773</v>
+        <v>493</v>
       </c>
     </row>
     <row r="323" spans="1:4">
       <c r="A323" s="1" t="s">
-        <v>461</v>
+        <v>772</v>
       </c>
       <c r="B323" s="1" t="s">
-        <v>462</v>
+        <v>23</v>
       </c>
       <c r="D323" s="1" t="s">
-        <v>463</v>
+        <v>773</v>
       </c>
     </row>
     <row r="324" spans="1:4">
       <c r="A324" s="1" t="s">
-        <v>608</v>
+        <v>461</v>
       </c>
       <c r="B324" s="1" t="s">
-        <v>609</v>
+        <v>462</v>
       </c>
       <c r="D324" s="1" t="s">
-        <v>610</v>
+        <v>463</v>
       </c>
     </row>
     <row r="325" spans="1:4">
       <c r="A325" s="1" t="s">
-        <v>1331</v>
+        <v>608</v>
       </c>
       <c r="B325" s="1" t="s">
-        <v>1330</v>
+        <v>609</v>
       </c>
       <c r="D325" s="1" t="s">
-        <v>1346</v>
+        <v>610</v>
       </c>
     </row>
     <row r="326" spans="1:4">
       <c r="A326" s="1" t="s">
-        <v>793</v>
+        <v>1331</v>
       </c>
       <c r="B326" s="1" t="s">
-        <v>794</v>
+        <v>1330</v>
       </c>
       <c r="D326" s="1" t="s">
-        <v>795</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="327" spans="1:4">
       <c r="A327" s="1" t="s">
-        <v>581</v>
+        <v>793</v>
       </c>
       <c r="B327" s="1" t="s">
-        <v>582</v>
+        <v>794</v>
       </c>
       <c r="D327" s="1" t="s">
-        <v>583</v>
+        <v>795</v>
       </c>
     </row>
     <row r="328" spans="1:4">
       <c r="A328" s="1" t="s">
-        <v>1008</v>
+        <v>581</v>
       </c>
       <c r="B328" s="1" t="s">
-        <v>1009</v>
+        <v>582</v>
       </c>
       <c r="D328" s="1" t="s">
-        <v>1010</v>
+        <v>583</v>
       </c>
     </row>
     <row r="329" spans="1:4">
       <c r="A329" s="1" t="s">
-        <v>1283</v>
+        <v>1008</v>
       </c>
       <c r="B329" s="1" t="s">
-        <v>1284</v>
+        <v>1009</v>
       </c>
       <c r="D329" s="1" t="s">
-        <v>1285</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="330" spans="1:4">
       <c r="A330" s="1" t="s">
-        <v>802</v>
+        <v>1283</v>
       </c>
       <c r="B330" s="1" t="s">
-        <v>803</v>
+        <v>1284</v>
       </c>
       <c r="D330" s="1" t="s">
-        <v>804</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="331" spans="1:4">
       <c r="A331" s="1" t="s">
-        <v>1183</v>
+        <v>802</v>
       </c>
       <c r="B331" s="1" t="s">
-        <v>1190</v>
+        <v>803</v>
       </c>
       <c r="D331" s="1" t="s">
-        <v>1197</v>
+        <v>804</v>
       </c>
     </row>
     <row r="332" spans="1:4">
       <c r="A332" s="1" t="s">
-        <v>455</v>
+        <v>1183</v>
       </c>
       <c r="B332" s="1" t="s">
-        <v>456</v>
+        <v>1190</v>
       </c>
       <c r="D332" s="1" t="s">
-        <v>457</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="333" spans="1:4">
       <c r="A333" s="1" t="s">
-        <v>838</v>
+        <v>455</v>
       </c>
       <c r="B333" s="1" t="s">
-        <v>839</v>
+        <v>456</v>
       </c>
       <c r="D333" s="1" t="s">
-        <v>840</v>
+        <v>457</v>
       </c>
     </row>
     <row r="334" spans="1:4">
       <c r="A334" s="1" t="s">
-        <v>1037</v>
+        <v>838</v>
       </c>
       <c r="B334" s="1" t="s">
-        <v>1038</v>
+        <v>839</v>
       </c>
       <c r="D334" s="1" t="s">
-        <v>1039</v>
+        <v>840</v>
       </c>
     </row>
     <row r="335" spans="1:4">
       <c r="A335" s="1" t="s">
-        <v>714</v>
+        <v>1037</v>
       </c>
       <c r="B335" s="1" t="s">
-        <v>715</v>
+        <v>1038</v>
       </c>
       <c r="D335" s="1" t="s">
-        <v>716</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="336" spans="1:4">
       <c r="A336" s="1" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="B336" s="1" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
       <c r="D336" s="1" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
     </row>
     <row r="337" spans="1:4">
       <c r="A337" s="1" t="s">
-        <v>614</v>
+        <v>717</v>
       </c>
       <c r="B337" s="1" t="s">
-        <v>615</v>
+        <v>718</v>
       </c>
       <c r="D337" s="1" t="s">
-        <v>616</v>
+        <v>719</v>
       </c>
     </row>
     <row r="338" spans="1:4">
       <c r="A338" s="1" t="s">
-        <v>584</v>
+        <v>614</v>
       </c>
       <c r="B338" s="1" t="s">
-        <v>585</v>
+        <v>615</v>
       </c>
       <c r="D338" s="1" t="s">
-        <v>586</v>
+        <v>616</v>
       </c>
     </row>
     <row r="339" spans="1:4">
       <c r="A339" s="1" t="s">
-        <v>611</v>
+        <v>584</v>
       </c>
       <c r="B339" s="1" t="s">
-        <v>612</v>
+        <v>585</v>
       </c>
       <c r="D339" s="1" t="s">
-        <v>613</v>
+        <v>586</v>
       </c>
     </row>
     <row r="340" spans="1:4">
       <c r="A340" s="1" t="s">
-        <v>755</v>
+        <v>611</v>
       </c>
       <c r="B340" s="1" t="s">
-        <v>756</v>
+        <v>612</v>
       </c>
       <c r="D340" s="1" t="s">
-        <v>757</v>
+        <v>613</v>
       </c>
     </row>
     <row r="341" spans="1:4">
       <c r="A341" s="1" t="s">
-        <v>890</v>
+        <v>755</v>
       </c>
       <c r="B341" s="1" t="s">
-        <v>891</v>
+        <v>756</v>
+      </c>
+      <c r="D341" s="1" t="s">
+        <v>757</v>
       </c>
     </row>
     <row r="342" spans="1:4">
       <c r="A342" s="1" t="s">
-        <v>700</v>
+        <v>890</v>
       </c>
       <c r="B342" s="1" t="s">
-        <v>701</v>
-      </c>
-      <c r="D342" s="1" t="s">
-        <v>702</v>
+        <v>891</v>
       </c>
     </row>
     <row r="343" spans="1:4">
       <c r="A343" s="1" t="s">
-        <v>682</v>
+        <v>700</v>
       </c>
       <c r="B343" s="1" t="s">
-        <v>683</v>
+        <v>701</v>
       </c>
       <c r="D343" s="1" t="s">
-        <v>684</v>
+        <v>702</v>
       </c>
     </row>
     <row r="344" spans="1:4">
       <c r="A344" s="1" t="s">
-        <v>1313</v>
+        <v>682</v>
       </c>
       <c r="B344" s="1" t="s">
-        <v>1315</v>
+        <v>683</v>
       </c>
       <c r="D344" s="1" t="s">
-        <v>1314</v>
+        <v>684</v>
       </c>
     </row>
     <row r="345" spans="1:4">
       <c r="A345" s="1" t="s">
-        <v>791</v>
+        <v>1313</v>
       </c>
       <c r="B345" s="1" t="s">
-        <v>792</v>
+        <v>1315</v>
       </c>
       <c r="D345" s="1" t="s">
-        <v>958</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="346" spans="1:4">
       <c r="A346" s="1" t="s">
-        <v>774</v>
+        <v>791</v>
       </c>
       <c r="B346" s="1" t="s">
-        <v>775</v>
+        <v>792</v>
       </c>
       <c r="D346" s="1" t="s">
-        <v>431</v>
+        <v>958</v>
       </c>
     </row>
     <row r="347" spans="1:4">
       <c r="A347" s="1" t="s">
-        <v>832</v>
+        <v>774</v>
       </c>
       <c r="B347" s="1" t="s">
-        <v>833</v>
+        <v>775</v>
       </c>
       <c r="D347" s="1" t="s">
-        <v>834</v>
+        <v>431</v>
       </c>
     </row>
     <row r="348" spans="1:4">
       <c r="A348" s="1" t="s">
-        <v>1202</v>
+        <v>832</v>
       </c>
       <c r="B348" s="1" t="s">
-        <v>1203</v>
+        <v>833</v>
       </c>
       <c r="D348" s="1" t="s">
-        <v>1204</v>
+        <v>834</v>
       </c>
     </row>
     <row r="349" spans="1:4">
       <c r="A349" s="1" t="s">
-        <v>637</v>
+        <v>1202</v>
       </c>
       <c r="B349" s="1" t="s">
-        <v>638</v>
+        <v>1203</v>
       </c>
       <c r="D349" s="1" t="s">
-        <v>639</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="350" spans="1:4">
       <c r="A350" s="1" t="s">
-        <v>551</v>
+        <v>637</v>
       </c>
       <c r="B350" s="1" t="s">
-        <v>552</v>
+        <v>638</v>
       </c>
       <c r="D350" s="1" t="s">
-        <v>553</v>
+        <v>639</v>
       </c>
     </row>
     <row r="351" spans="1:4">
       <c r="A351" s="1" t="s">
-        <v>955</v>
+        <v>551</v>
       </c>
       <c r="B351" s="1" t="s">
-        <v>956</v>
+        <v>552</v>
       </c>
       <c r="D351" s="1" t="s">
-        <v>957</v>
+        <v>553</v>
       </c>
     </row>
     <row r="352" spans="1:4">
       <c r="A352" s="1" t="s">
-        <v>1026</v>
+        <v>955</v>
       </c>
       <c r="B352" s="1" t="s">
-        <v>1025</v>
+        <v>956</v>
       </c>
       <c r="D352" s="1" t="s">
-        <v>1027</v>
+        <v>957</v>
       </c>
     </row>
     <row r="353" spans="1:4">
       <c r="A353" s="1" t="s">
-        <v>694</v>
+        <v>1026</v>
       </c>
       <c r="B353" s="1" t="s">
-        <v>695</v>
+        <v>1025</v>
       </c>
       <c r="D353" s="1" t="s">
-        <v>696</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="354" spans="1:4">
       <c r="A354" s="1" t="s">
-        <v>676</v>
+        <v>694</v>
       </c>
       <c r="B354" s="1" t="s">
-        <v>677</v>
+        <v>695</v>
       </c>
       <c r="D354" s="1" t="s">
-        <v>678</v>
+        <v>696</v>
       </c>
     </row>
     <row r="355" spans="1:4">
       <c r="A355" s="1" t="s">
-        <v>871</v>
+        <v>676</v>
       </c>
       <c r="B355" s="1" t="s">
-        <v>872</v>
+        <v>677</v>
       </c>
       <c r="D355" s="1" t="s">
-        <v>873</v>
+        <v>678</v>
       </c>
     </row>
     <row r="356" spans="1:4">
       <c r="A356" s="1" t="s">
-        <v>954</v>
+        <v>871</v>
       </c>
       <c r="B356" s="1" t="s">
-        <v>953</v>
+        <v>872</v>
       </c>
       <c r="D356" s="1" t="s">
-        <v>758</v>
+        <v>873</v>
       </c>
     </row>
     <row r="357" spans="1:4">
       <c r="A357" s="1" t="s">
-        <v>1005</v>
+        <v>954</v>
       </c>
       <c r="B357" s="1" t="s">
-        <v>1006</v>
+        <v>953</v>
       </c>
       <c r="D357" s="1" t="s">
-        <v>950</v>
+        <v>758</v>
       </c>
     </row>
     <row r="358" spans="1:4">
       <c r="A358" s="1" t="s">
-        <v>882</v>
+        <v>1005</v>
       </c>
       <c r="B358" s="1" t="s">
-        <v>883</v>
+        <v>1006</v>
+      </c>
+      <c r="D358" s="1" t="s">
+        <v>950</v>
       </c>
     </row>
     <row r="359" spans="1:4">
       <c r="A359" s="1" t="s">
-        <v>856</v>
+        <v>882</v>
       </c>
       <c r="B359" s="1" t="s">
-        <v>857</v>
-      </c>
-      <c r="D359" s="1" t="s">
-        <v>858</v>
+        <v>883</v>
       </c>
     </row>
     <row r="360" spans="1:4">
       <c r="A360" s="1" t="s">
-        <v>880</v>
+        <v>856</v>
       </c>
       <c r="B360" s="1" t="s">
-        <v>881</v>
+        <v>857</v>
+      </c>
+      <c r="D360" s="1" t="s">
+        <v>858</v>
       </c>
     </row>
     <row r="361" spans="1:4">
       <c r="A361" s="1" t="s">
-        <v>752</v>
+        <v>880</v>
       </c>
       <c r="B361" s="1" t="s">
-        <v>753</v>
-      </c>
-      <c r="D361" s="1" t="s">
-        <v>754</v>
+        <v>881</v>
       </c>
     </row>
     <row r="362" spans="1:4">
       <c r="A362" s="1" t="s">
-        <v>572</v>
+        <v>752</v>
       </c>
       <c r="B362" s="1" t="s">
-        <v>573</v>
+        <v>753</v>
       </c>
       <c r="D362" s="1" t="s">
-        <v>574</v>
+        <v>754</v>
       </c>
     </row>
     <row r="363" spans="1:4">
       <c r="A363" s="1" t="s">
-        <v>776</v>
+        <v>572</v>
       </c>
       <c r="B363" s="1" t="s">
-        <v>777</v>
+        <v>573</v>
       </c>
       <c r="D363" s="1" t="s">
         <v>574</v>
@@ -9124,606 +9154,606 @@
     </row>
     <row r="364" spans="1:4">
       <c r="A364" s="1" t="s">
-        <v>509</v>
+        <v>776</v>
       </c>
       <c r="B364" s="1" t="s">
-        <v>510</v>
+        <v>777</v>
       </c>
       <c r="D364" s="1" t="s">
-        <v>511</v>
+        <v>574</v>
       </c>
     </row>
     <row r="365" spans="1:4">
       <c r="A365" s="1" t="s">
-        <v>981</v>
+        <v>509</v>
       </c>
       <c r="B365" s="1" t="s">
-        <v>912</v>
+        <v>510</v>
       </c>
       <c r="D365" s="1" t="s">
-        <v>975</v>
+        <v>511</v>
       </c>
     </row>
     <row r="366" spans="1:4">
       <c r="A366" s="1" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="B366" s="1" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="D366" s="1" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
     </row>
     <row r="367" spans="1:4">
       <c r="A367" s="1" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="B367" s="1" t="s">
-        <v>910</v>
+        <v>913</v>
       </c>
       <c r="D367" s="1" t="s">
-        <v>977</v>
+        <v>974</v>
       </c>
     </row>
     <row r="368" spans="1:4">
       <c r="A368" s="1" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="B368" s="1" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="D368" s="1" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
     </row>
     <row r="369" spans="1:4">
       <c r="A369" s="1" t="s">
-        <v>759</v>
+        <v>983</v>
       </c>
       <c r="B369" s="1" t="s">
-        <v>760</v>
+        <v>911</v>
       </c>
       <c r="D369" s="1" t="s">
-        <v>761</v>
+        <v>976</v>
       </c>
     </row>
     <row r="370" spans="1:4">
       <c r="A370" s="1" t="s">
-        <v>884</v>
+        <v>759</v>
       </c>
       <c r="B370" s="1" t="s">
-        <v>885</v>
+        <v>760</v>
+      </c>
+      <c r="D370" s="1" t="s">
+        <v>761</v>
       </c>
     </row>
     <row r="371" spans="1:4">
       <c r="A371" s="1" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="B371" s="1" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
     </row>
     <row r="372" spans="1:4">
       <c r="A372" s="1" t="s">
-        <v>964</v>
+        <v>886</v>
       </c>
       <c r="B372" s="1" t="s">
-        <v>921</v>
-      </c>
-      <c r="D372" s="1" t="s">
-        <v>907</v>
+        <v>887</v>
       </c>
     </row>
     <row r="373" spans="1:4">
       <c r="A373" s="1" t="s">
-        <v>0</v>
+        <v>964</v>
       </c>
       <c r="B373" s="1" t="s">
-        <v>709</v>
+        <v>921</v>
       </c>
       <c r="D373" s="1" t="s">
-        <v>710</v>
+        <v>907</v>
       </c>
     </row>
     <row r="374" spans="1:4">
       <c r="A374" s="1" t="s">
-        <v>1339</v>
+        <v>0</v>
       </c>
       <c r="B374" s="1" t="s">
-        <v>1338</v>
+        <v>709</v>
       </c>
       <c r="D374" s="1" t="s">
-        <v>1337</v>
+        <v>710</v>
       </c>
     </row>
     <row r="375" spans="1:4">
       <c r="A375" s="1" t="s">
-        <v>810</v>
+        <v>1339</v>
       </c>
       <c r="B375" s="1" t="s">
-        <v>811</v>
+        <v>1338</v>
       </c>
       <c r="D375" s="1" t="s">
-        <v>896</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="376" spans="1:4">
       <c r="A376" s="1" t="s">
-        <v>587</v>
+        <v>810</v>
       </c>
       <c r="B376" s="1" t="s">
-        <v>588</v>
+        <v>811</v>
       </c>
       <c r="D376" s="1" t="s">
-        <v>589</v>
+        <v>896</v>
       </c>
     </row>
     <row r="377" spans="1:4">
       <c r="A377" s="1" t="s">
-        <v>812</v>
+        <v>587</v>
       </c>
       <c r="B377" s="1" t="s">
-        <v>813</v>
+        <v>588</v>
       </c>
       <c r="D377" s="1" t="s">
-        <v>526</v>
+        <v>589</v>
       </c>
     </row>
     <row r="378" spans="1:4">
       <c r="A378" s="1" t="s">
-        <v>939</v>
+        <v>812</v>
       </c>
       <c r="B378" s="1" t="s">
-        <v>937</v>
+        <v>813</v>
       </c>
       <c r="D378" s="1" t="s">
-        <v>938</v>
+        <v>526</v>
       </c>
     </row>
     <row r="379" spans="1:4">
       <c r="A379" s="1" t="s">
-        <v>805</v>
+        <v>939</v>
       </c>
       <c r="B379" s="1" t="s">
-        <v>806</v>
+        <v>937</v>
       </c>
       <c r="D379" s="1" t="s">
-        <v>807</v>
+        <v>938</v>
       </c>
     </row>
     <row r="380" spans="1:4">
       <c r="A380" s="1" t="s">
-        <v>1066</v>
+        <v>805</v>
       </c>
       <c r="B380" s="1" t="s">
-        <v>1067</v>
+        <v>806</v>
       </c>
       <c r="D380" s="1" t="s">
-        <v>784</v>
+        <v>807</v>
       </c>
     </row>
     <row r="381" spans="1:4">
       <c r="A381" s="1" t="s">
-        <v>865</v>
+        <v>1066</v>
       </c>
       <c r="B381" s="1" t="s">
-        <v>866</v>
+        <v>1067</v>
       </c>
       <c r="D381" s="1" t="s">
-        <v>867</v>
+        <v>784</v>
       </c>
     </row>
     <row r="382" spans="1:4">
       <c r="A382" s="1" t="s">
-        <v>640</v>
+        <v>865</v>
       </c>
       <c r="B382" s="1" t="s">
-        <v>641</v>
+        <v>866</v>
       </c>
       <c r="D382" s="1" t="s">
-        <v>642</v>
+        <v>867</v>
       </c>
     </row>
     <row r="383" spans="1:4">
       <c r="A383" s="1" t="s">
-        <v>527</v>
+        <v>640</v>
       </c>
       <c r="B383" s="1" t="s">
-        <v>528</v>
+        <v>641</v>
       </c>
       <c r="D383" s="1" t="s">
-        <v>529</v>
+        <v>642</v>
       </c>
     </row>
     <row r="384" spans="1:4">
       <c r="A384" s="1" t="s">
-        <v>435</v>
+        <v>527</v>
       </c>
       <c r="B384" s="1" t="s">
-        <v>436</v>
+        <v>528</v>
       </c>
       <c r="D384" s="1" t="s">
-        <v>437</v>
+        <v>529</v>
       </c>
     </row>
     <row r="385" spans="1:4">
       <c r="A385" s="1" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B385" s="1" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D385" s="1" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="386" spans="1:4">
       <c r="A386" s="1" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="B386" s="1" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="D386" s="1" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="387" spans="1:4">
       <c r="A387" s="1" t="s">
-        <v>1343</v>
+        <v>441</v>
       </c>
       <c r="B387" s="1" t="s">
-        <v>1344</v>
+        <v>442</v>
       </c>
       <c r="D387" s="1" t="s">
-        <v>1345</v>
+        <v>443</v>
       </c>
     </row>
     <row r="388" spans="1:4">
       <c r="A388" s="1" t="s">
-        <v>808</v>
+        <v>1343</v>
       </c>
       <c r="B388" s="1" t="s">
-        <v>809</v>
+        <v>1344</v>
       </c>
       <c r="D388" s="1" t="s">
-        <v>990</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="389" spans="1:4">
       <c r="A389" s="1" t="s">
-        <v>646</v>
+        <v>808</v>
       </c>
       <c r="B389" s="1" t="s">
-        <v>647</v>
+        <v>809</v>
       </c>
       <c r="D389" s="1" t="s">
-        <v>648</v>
+        <v>990</v>
       </c>
     </row>
     <row r="390" spans="1:4">
       <c r="A390" s="1" t="s">
-        <v>925</v>
+        <v>646</v>
       </c>
       <c r="B390" s="1" t="s">
-        <v>926</v>
+        <v>647</v>
       </c>
       <c r="D390" s="1" t="s">
-        <v>927</v>
+        <v>648</v>
       </c>
     </row>
     <row r="391" spans="1:4">
       <c r="A391" s="1" t="s">
-        <v>991</v>
+        <v>925</v>
       </c>
       <c r="B391" s="1" t="s">
-        <v>992</v>
+        <v>926</v>
       </c>
       <c r="D391" s="1" t="s">
-        <v>993</v>
+        <v>927</v>
       </c>
     </row>
     <row r="392" spans="1:4">
       <c r="A392" s="1" t="s">
-        <v>994</v>
+        <v>991</v>
       </c>
       <c r="B392" s="1" t="s">
-        <v>995</v>
+        <v>992</v>
       </c>
       <c r="D392" s="1" t="s">
-        <v>996</v>
+        <v>993</v>
       </c>
     </row>
     <row r="393" spans="1:4">
       <c r="A393" s="1" t="s">
-        <v>1001</v>
+        <v>994</v>
       </c>
       <c r="B393" s="1" t="s">
-        <v>729</v>
+        <v>995</v>
       </c>
       <c r="D393" s="1" t="s">
-        <v>730</v>
+        <v>996</v>
       </c>
     </row>
     <row r="394" spans="1:4">
       <c r="A394" s="1" t="s">
-        <v>853</v>
+        <v>1001</v>
       </c>
       <c r="B394" s="1" t="s">
-        <v>854</v>
+        <v>729</v>
       </c>
       <c r="D394" s="1" t="s">
-        <v>855</v>
+        <v>730</v>
       </c>
     </row>
     <row r="395" spans="1:4">
       <c r="A395" s="1" t="s">
-        <v>664</v>
+        <v>853</v>
       </c>
       <c r="B395" s="1" t="s">
-        <v>665</v>
+        <v>854</v>
       </c>
       <c r="D395" s="1" t="s">
-        <v>666</v>
+        <v>855</v>
       </c>
     </row>
     <row r="396" spans="1:4">
       <c r="A396" s="1" t="s">
-        <v>962</v>
+        <v>664</v>
       </c>
       <c r="B396" s="1" t="s">
-        <v>923</v>
+        <v>665</v>
       </c>
       <c r="D396" s="1" t="s">
-        <v>906</v>
+        <v>666</v>
       </c>
     </row>
     <row r="397" spans="1:4">
       <c r="A397" s="1" t="s">
-        <v>997</v>
+        <v>962</v>
       </c>
       <c r="B397" s="1" t="s">
-        <v>998</v>
+        <v>923</v>
       </c>
       <c r="D397" s="1" t="s">
-        <v>999</v>
+        <v>906</v>
       </c>
     </row>
     <row r="398" spans="1:4">
       <c r="A398" s="1" t="s">
-        <v>1002</v>
+        <v>997</v>
       </c>
       <c r="B398" s="1" t="s">
-        <v>1003</v>
+        <v>998</v>
       </c>
       <c r="D398" s="1" t="s">
-        <v>1004</v>
+        <v>999</v>
       </c>
     </row>
     <row r="399" spans="1:4">
       <c r="A399" s="1" t="s">
-        <v>1016</v>
+        <v>1002</v>
       </c>
       <c r="B399" s="1" t="s">
-        <v>1017</v>
+        <v>1003</v>
       </c>
       <c r="D399" s="1" t="s">
-        <v>1018</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="400" spans="1:4">
       <c r="A400" s="1" t="s">
-        <v>429</v>
+        <v>1016</v>
       </c>
       <c r="B400" s="1" t="s">
-        <v>430</v>
+        <v>1017</v>
       </c>
       <c r="D400" s="1" t="s">
-        <v>431</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="401" spans="1:4">
       <c r="A401" s="1" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B401" s="1" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="D401" s="1" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="402" spans="1:4">
       <c r="A402" s="1" t="s">
-        <v>1316</v>
+        <v>432</v>
       </c>
       <c r="B402" s="1" t="s">
-        <v>1317</v>
+        <v>433</v>
       </c>
       <c r="D402" s="1" t="s">
-        <v>1318</v>
+        <v>434</v>
       </c>
     </row>
     <row r="403" spans="1:4">
       <c r="A403" s="1" t="s">
-        <v>599</v>
+        <v>1316</v>
       </c>
       <c r="B403" s="1" t="s">
-        <v>600</v>
+        <v>1317</v>
       </c>
       <c r="D403" s="1" t="s">
-        <v>601</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="404" spans="1:4">
       <c r="A404" s="1" t="s">
-        <v>593</v>
+        <v>599</v>
       </c>
       <c r="B404" s="1" t="s">
-        <v>594</v>
+        <v>600</v>
       </c>
       <c r="D404" s="1" t="s">
-        <v>595</v>
+        <v>601</v>
       </c>
     </row>
     <row r="405" spans="1:4">
       <c r="A405" s="1" t="s">
-        <v>670</v>
+        <v>593</v>
       </c>
       <c r="B405" s="1" t="s">
-        <v>671</v>
+        <v>594</v>
       </c>
       <c r="D405" s="1" t="s">
-        <v>672</v>
+        <v>595</v>
       </c>
     </row>
     <row r="406" spans="1:4">
       <c r="A406" s="1" t="s">
-        <v>444</v>
+        <v>670</v>
       </c>
       <c r="B406" s="1" t="s">
-        <v>445</v>
+        <v>671</v>
       </c>
       <c r="D406" s="1" t="s">
-        <v>445</v>
+        <v>672</v>
       </c>
     </row>
     <row r="407" spans="1:4">
       <c r="A407" s="1" t="s">
-        <v>596</v>
+        <v>444</v>
       </c>
       <c r="B407" s="1" t="s">
-        <v>597</v>
+        <v>445</v>
       </c>
       <c r="D407" s="1" t="s">
-        <v>598</v>
+        <v>445</v>
       </c>
     </row>
     <row r="408" spans="1:4">
       <c r="A408" s="1" t="s">
-        <v>542</v>
+        <v>596</v>
       </c>
       <c r="B408" s="1" t="s">
-        <v>543</v>
+        <v>597</v>
       </c>
       <c r="D408" s="1" t="s">
-        <v>544</v>
+        <v>598</v>
       </c>
     </row>
     <row r="409" spans="1:4">
       <c r="A409" s="1" t="s">
-        <v>464</v>
+        <v>542</v>
       </c>
       <c r="B409" s="1" t="s">
-        <v>465</v>
+        <v>543</v>
       </c>
       <c r="D409" s="1" t="s">
-        <v>466</v>
+        <v>544</v>
       </c>
     </row>
     <row r="410" spans="1:4">
       <c r="A410" s="1" t="s">
-        <v>619</v>
+        <v>464</v>
       </c>
       <c r="B410" s="1" t="s">
-        <v>620</v>
+        <v>465</v>
       </c>
       <c r="D410" s="1" t="s">
-        <v>621</v>
+        <v>466</v>
       </c>
     </row>
     <row r="411" spans="1:4">
       <c r="A411" s="1" t="s">
-        <v>402</v>
+        <v>619</v>
       </c>
       <c r="B411" s="1" t="s">
-        <v>403</v>
+        <v>620</v>
       </c>
       <c r="D411" s="1" t="s">
-        <v>404</v>
+        <v>621</v>
       </c>
     </row>
     <row r="412" spans="1:4">
       <c r="A412" s="1" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="B412" s="1" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D412" s="1" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="413" spans="1:4">
       <c r="A413" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B413" s="1" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="D413" s="1" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="414" spans="1:4">
       <c r="A414" s="1" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="B414" s="1" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="D414" s="1" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
     </row>
     <row r="415" spans="1:4">
       <c r="A415" s="1" t="s">
-        <v>847</v>
+        <v>411</v>
       </c>
       <c r="B415" s="1" t="s">
-        <v>848</v>
+        <v>412</v>
       </c>
       <c r="D415" s="1" t="s">
-        <v>849</v>
+        <v>413</v>
       </c>
     </row>
     <row r="416" spans="1:4">
       <c r="A416" s="1" t="s">
-        <v>1308</v>
+        <v>847</v>
       </c>
       <c r="B416" s="1" t="s">
-        <v>1309</v>
+        <v>848</v>
+      </c>
+      <c r="D416" s="1" t="s">
+        <v>849</v>
       </c>
     </row>
     <row r="417" spans="1:4">
       <c r="A417" s="1" t="s">
-        <v>1280</v>
+        <v>1308</v>
       </c>
       <c r="B417" s="1" t="s">
-        <v>1282</v>
-      </c>
-      <c r="D417" s="1" t="s">
-        <v>1281</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="418" spans="1:4">
       <c r="A418" s="1" t="s">
-        <v>1218</v>
+        <v>1280</v>
       </c>
       <c r="B418" s="1" t="s">
-        <v>1219</v>
+        <v>1282</v>
       </c>
       <c r="D418" s="1" t="s">
-        <v>1201</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="419" spans="1:4">
       <c r="A419" s="1" t="s">
-        <v>1332</v>
+        <v>1218</v>
       </c>
       <c r="B419" s="1" t="s">
-        <v>1333</v>
+        <v>1219</v>
       </c>
       <c r="D419" s="1" t="s">
         <v>1201</v>
@@ -9731,601 +9761,601 @@
     </row>
     <row r="420" spans="1:4">
       <c r="A420" s="1" t="s">
-        <v>826</v>
+        <v>1332</v>
       </c>
       <c r="B420" s="1" t="s">
-        <v>827</v>
+        <v>1333</v>
       </c>
       <c r="D420" s="1" t="s">
-        <v>828</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="421" spans="1:4">
       <c r="A421" s="1" t="s">
-        <v>1359</v>
+        <v>826</v>
       </c>
       <c r="B421" s="1" t="s">
-        <v>1360</v>
+        <v>827</v>
       </c>
       <c r="D421" s="1" t="s">
-        <v>1361</v>
+        <v>828</v>
       </c>
     </row>
     <row r="422" spans="1:4">
       <c r="A422" s="1" t="s">
-        <v>1162</v>
+        <v>1359</v>
       </c>
       <c r="B422" s="1" t="s">
-        <v>1163</v>
+        <v>1360</v>
       </c>
       <c r="D422" s="1" t="s">
-        <v>1164</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="423" spans="1:4">
       <c r="A423" s="1" t="s">
-        <v>829</v>
+        <v>1162</v>
       </c>
       <c r="B423" s="1" t="s">
-        <v>830</v>
+        <v>1163</v>
       </c>
       <c r="D423" s="1" t="s">
-        <v>831</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="424" spans="1:4">
       <c r="A424" s="1" t="s">
-        <v>1151</v>
+        <v>829</v>
       </c>
       <c r="B424" s="1" t="s">
-        <v>1150</v>
+        <v>830</v>
       </c>
       <c r="D424" s="1" t="s">
-        <v>1149</v>
+        <v>831</v>
       </c>
     </row>
     <row r="425" spans="1:4">
       <c r="A425" s="1" t="s">
-        <v>1305</v>
+        <v>1151</v>
       </c>
       <c r="B425" s="1" t="s">
-        <v>1306</v>
+        <v>1150</v>
       </c>
       <c r="D425" s="1" t="s">
-        <v>1307</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="426" spans="1:4">
       <c r="A426" s="1" t="s">
-        <v>1386</v>
+        <v>1305</v>
       </c>
       <c r="B426" s="1" t="s">
-        <v>1387</v>
+        <v>1306</v>
       </c>
       <c r="D426" s="1" t="s">
-        <v>1388</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="427" spans="1:4">
       <c r="A427" s="1" t="s">
-        <v>1353</v>
+        <v>1386</v>
       </c>
       <c r="B427" s="1" t="s">
-        <v>1354</v>
+        <v>1387</v>
+      </c>
+      <c r="D427" s="1" t="s">
+        <v>1388</v>
       </c>
     </row>
     <row r="428" spans="1:4">
       <c r="A428" s="1" t="s">
-        <v>1383</v>
+        <v>1353</v>
       </c>
       <c r="B428" s="1" t="s">
-        <v>1384</v>
-      </c>
-      <c r="D428" s="1" t="s">
-        <v>1385</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="429" spans="1:4">
       <c r="A429" s="1" t="s">
-        <v>1155</v>
+        <v>1383</v>
       </c>
       <c r="B429" s="1" t="s">
-        <v>1156</v>
+        <v>1384</v>
       </c>
       <c r="D429" s="1" t="s">
-        <v>1154</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="430" spans="1:4">
       <c r="A430" s="1" t="s">
-        <v>726</v>
+        <v>1155</v>
       </c>
       <c r="B430" s="1" t="s">
-        <v>727</v>
+        <v>1156</v>
       </c>
       <c r="D430" s="1" t="s">
-        <v>728</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="431" spans="1:4">
       <c r="A431" s="1" t="s">
-        <v>723</v>
+        <v>726</v>
       </c>
       <c r="B431" s="1" t="s">
-        <v>724</v>
+        <v>727</v>
       </c>
       <c r="D431" s="1" t="s">
-        <v>725</v>
+        <v>728</v>
       </c>
     </row>
     <row r="432" spans="1:4">
       <c r="A432" s="1" t="s">
-        <v>515</v>
+        <v>723</v>
       </c>
       <c r="B432" s="1" t="s">
-        <v>516</v>
+        <v>724</v>
       </c>
       <c r="D432" s="1" t="s">
-        <v>517</v>
+        <v>725</v>
       </c>
     </row>
     <row r="433" spans="1:4">
       <c r="A433" s="1" t="s">
-        <v>590</v>
+        <v>515</v>
       </c>
       <c r="B433" s="1" t="s">
-        <v>591</v>
+        <v>516</v>
       </c>
       <c r="D433" s="1" t="s">
-        <v>592</v>
+        <v>517</v>
       </c>
     </row>
     <row r="434" spans="1:4">
       <c r="A434" s="1" t="s">
-        <v>1377</v>
+        <v>590</v>
       </c>
       <c r="B434" s="1" t="s">
-        <v>1378</v>
+        <v>591</v>
       </c>
       <c r="D434" s="1" t="s">
-        <v>1379</v>
+        <v>592</v>
       </c>
     </row>
     <row r="435" spans="1:4">
       <c r="A435" s="1" t="s">
-        <v>673</v>
+        <v>1377</v>
       </c>
       <c r="B435" s="1" t="s">
-        <v>674</v>
+        <v>1378</v>
       </c>
       <c r="D435" s="1" t="s">
-        <v>675</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="436" spans="1:4">
       <c r="A436" s="1" t="s">
-        <v>653</v>
+        <v>673</v>
       </c>
       <c r="B436" s="1" t="s">
-        <v>654</v>
+        <v>674</v>
       </c>
       <c r="D436" s="1" t="s">
-        <v>1030</v>
+        <v>675</v>
       </c>
     </row>
     <row r="437" spans="1:4">
       <c r="A437" s="1" t="s">
-        <v>1374</v>
+        <v>653</v>
       </c>
       <c r="B437" s="1" t="s">
-        <v>1375</v>
+        <v>654</v>
       </c>
       <c r="D437" s="1" t="s">
-        <v>1376</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="438" spans="1:4">
       <c r="A438" s="1" t="s">
-        <v>1040</v>
+        <v>1374</v>
       </c>
       <c r="B438" s="1" t="s">
-        <v>1041</v>
+        <v>1375</v>
       </c>
       <c r="D438" s="1" t="s">
-        <v>1042</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="439" spans="1:4">
       <c r="A439" s="1" t="s">
-        <v>1023</v>
+        <v>1040</v>
       </c>
       <c r="B439" s="1" t="s">
-        <v>1022</v>
+        <v>1041</v>
       </c>
       <c r="D439" s="1" t="s">
-        <v>1024</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="440" spans="1:4">
       <c r="A440" s="1" t="s">
-        <v>841</v>
+        <v>1023</v>
       </c>
       <c r="B440" s="1" t="s">
-        <v>842</v>
+        <v>1022</v>
       </c>
       <c r="D440" s="1" t="s">
-        <v>843</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="441" spans="1:4">
       <c r="A441" s="1" t="s">
-        <v>1253</v>
+        <v>841</v>
       </c>
       <c r="B441" s="1" t="s">
-        <v>1254</v>
+        <v>842</v>
       </c>
       <c r="D441" s="1" t="s">
-        <v>1255</v>
+        <v>843</v>
       </c>
     </row>
     <row r="442" spans="1:4">
       <c r="A442" s="1" t="s">
-        <v>1250</v>
+        <v>1253</v>
       </c>
       <c r="B442" s="1" t="s">
-        <v>1251</v>
+        <v>1254</v>
       </c>
       <c r="D442" s="1" t="s">
-        <v>1252</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="443" spans="1:4">
       <c r="A443" s="1" t="s">
-        <v>470</v>
+        <v>1250</v>
       </c>
       <c r="B443" s="1" t="s">
-        <v>471</v>
+        <v>1251</v>
       </c>
       <c r="D443" s="1" t="s">
-        <v>472</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="444" spans="1:4">
       <c r="A444" s="1" t="s">
-        <v>971</v>
+        <v>470</v>
       </c>
       <c r="B444" s="1" t="s">
-        <v>918</v>
+        <v>471</v>
       </c>
       <c r="D444" s="1" t="s">
-        <v>1000</v>
+        <v>472</v>
       </c>
     </row>
     <row r="445" spans="1:4">
       <c r="A445" s="1" t="s">
-        <v>1365</v>
+        <v>971</v>
       </c>
       <c r="B445" s="1" t="s">
-        <v>1367</v>
+        <v>918</v>
       </c>
       <c r="D445" s="1" t="s">
-        <v>1366</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="446" spans="1:4">
       <c r="A446" s="1" t="s">
-        <v>557</v>
+        <v>1365</v>
       </c>
       <c r="B446" s="1" t="s">
-        <v>558</v>
+        <v>1367</v>
       </c>
       <c r="D446" s="1" t="s">
-        <v>559</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="447" spans="1:4">
       <c r="A447" s="1" t="s">
-        <v>1232</v>
+        <v>557</v>
       </c>
       <c r="B447" s="1" t="s">
-        <v>1233</v>
+        <v>558</v>
       </c>
       <c r="D447" s="1" t="s">
-        <v>1234</v>
+        <v>559</v>
       </c>
     </row>
     <row r="448" spans="1:4">
       <c r="A448" s="1" t="s">
-        <v>968</v>
+        <v>1232</v>
       </c>
       <c r="B448" s="1" t="s">
-        <v>917</v>
+        <v>1233</v>
       </c>
       <c r="D448" s="1" t="s">
-        <v>970</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="449" spans="1:4">
       <c r="A449" s="1" t="s">
-        <v>494</v>
+        <v>968</v>
       </c>
       <c r="B449" s="1" t="s">
-        <v>495</v>
+        <v>917</v>
       </c>
       <c r="D449" s="1" t="s">
-        <v>496</v>
+        <v>970</v>
       </c>
     </row>
     <row r="450" spans="1:4">
       <c r="A450" s="1" t="s">
-        <v>1169</v>
+        <v>494</v>
       </c>
       <c r="B450" s="1" t="s">
-        <v>1170</v>
+        <v>495</v>
       </c>
       <c r="D450" s="1" t="s">
-        <v>1171</v>
+        <v>496</v>
       </c>
     </row>
     <row r="451" spans="1:4">
       <c r="A451" s="1" t="s">
-        <v>987</v>
+        <v>1169</v>
       </c>
       <c r="B451" s="1" t="s">
-        <v>988</v>
+        <v>1170</v>
       </c>
       <c r="D451" s="1" t="s">
-        <v>989</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="452" spans="1:4">
       <c r="A452" s="1" t="s">
-        <v>979</v>
+        <v>987</v>
       </c>
       <c r="B452" s="1" t="s">
-        <v>915</v>
+        <v>988</v>
       </c>
       <c r="D452" s="1" t="s">
-        <v>972</v>
+        <v>989</v>
       </c>
     </row>
     <row r="453" spans="1:4">
       <c r="A453" s="1" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="B453" s="1" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="D453" s="1" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="454" spans="1:4">
       <c r="A454" s="1" t="s">
-        <v>897</v>
+        <v>978</v>
       </c>
       <c r="B454" s="1" t="s">
-        <v>898</v>
+        <v>914</v>
       </c>
       <c r="D454" s="1" t="s">
-        <v>899</v>
+        <v>973</v>
       </c>
     </row>
     <row r="455" spans="1:4">
       <c r="A455" s="1" t="s">
-        <v>479</v>
+        <v>897</v>
       </c>
       <c r="B455" s="1" t="s">
-        <v>480</v>
+        <v>898</v>
       </c>
       <c r="D455" s="1" t="s">
-        <v>481</v>
+        <v>899</v>
       </c>
     </row>
     <row r="456" spans="1:4">
       <c r="A456" s="1" t="s">
-        <v>1068</v>
+        <v>479</v>
       </c>
       <c r="B456" s="1" t="s">
-        <v>1069</v>
+        <v>480</v>
       </c>
       <c r="D456" s="1" t="s">
-        <v>1010</v>
+        <v>481</v>
       </c>
     </row>
     <row r="457" spans="1:4">
       <c r="A457" s="1" t="s">
-        <v>497</v>
+        <v>1068</v>
       </c>
       <c r="B457" s="1" t="s">
-        <v>498</v>
+        <v>1069</v>
       </c>
       <c r="D457" s="1" t="s">
-        <v>499</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="458" spans="1:4">
       <c r="A458" s="1" t="s">
-        <v>482</v>
+        <v>497</v>
       </c>
       <c r="B458" s="1" t="s">
-        <v>483</v>
+        <v>498</v>
       </c>
       <c r="D458" s="1" t="s">
-        <v>484</v>
+        <v>499</v>
       </c>
     </row>
     <row r="459" spans="1:4">
       <c r="A459" s="1" t="s">
-        <v>1159</v>
+        <v>482</v>
       </c>
       <c r="B459" s="1" t="s">
-        <v>1160</v>
+        <v>483</v>
       </c>
       <c r="D459" s="1" t="s">
-        <v>1161</v>
+        <v>484</v>
       </c>
     </row>
     <row r="460" spans="1:4">
       <c r="A460" s="1" t="s">
-        <v>485</v>
+        <v>1159</v>
       </c>
       <c r="B460" s="1" t="s">
-        <v>486</v>
+        <v>1160</v>
       </c>
       <c r="D460" s="1" t="s">
-        <v>487</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="461" spans="1:4">
       <c r="A461" s="1" t="s">
-        <v>940</v>
+        <v>485</v>
       </c>
       <c r="B461" s="1" t="s">
-        <v>941</v>
+        <v>486</v>
       </c>
       <c r="D461" s="1" t="s">
-        <v>942</v>
+        <v>487</v>
       </c>
     </row>
     <row r="462" spans="1:4">
       <c r="A462" s="1" t="s">
-        <v>703</v>
+        <v>940</v>
       </c>
       <c r="B462" s="1" t="s">
-        <v>704</v>
+        <v>941</v>
       </c>
       <c r="D462" s="1" t="s">
-        <v>705</v>
+        <v>942</v>
       </c>
     </row>
     <row r="463" spans="1:4">
       <c r="A463" s="1" t="s">
-        <v>799</v>
+        <v>703</v>
       </c>
       <c r="B463" s="1" t="s">
-        <v>800</v>
+        <v>704</v>
       </c>
       <c r="D463" s="1" t="s">
-        <v>801</v>
+        <v>705</v>
       </c>
     </row>
     <row r="464" spans="1:4">
       <c r="A464" s="1" t="s">
-        <v>530</v>
+        <v>799</v>
       </c>
       <c r="B464" s="1" t="s">
-        <v>531</v>
+        <v>800</v>
       </c>
       <c r="D464" s="1" t="s">
-        <v>532</v>
+        <v>801</v>
       </c>
     </row>
     <row r="465" spans="1:4">
       <c r="A465" s="1" t="s">
-        <v>1296</v>
+        <v>530</v>
       </c>
       <c r="B465" s="1" t="s">
-        <v>1298</v>
+        <v>531</v>
       </c>
       <c r="D465" s="1" t="s">
-        <v>1297</v>
+        <v>532</v>
       </c>
     </row>
     <row r="466" spans="1:4">
       <c r="A466" s="1" t="s">
-        <v>500</v>
+        <v>1296</v>
       </c>
       <c r="B466" s="1" t="s">
-        <v>501</v>
+        <v>1298</v>
       </c>
       <c r="D466" s="1" t="s">
-        <v>502</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="467" spans="1:4">
       <c r="A467" s="1" t="s">
-        <v>1334</v>
+        <v>500</v>
       </c>
       <c r="B467" s="1" t="s">
-        <v>1335</v>
+        <v>501</v>
       </c>
       <c r="D467" s="1" t="s">
-        <v>1336</v>
+        <v>502</v>
       </c>
     </row>
     <row r="468" spans="1:4">
       <c r="A468" s="1" t="s">
-        <v>414</v>
+        <v>1334</v>
       </c>
       <c r="B468" s="1" t="s">
-        <v>415</v>
+        <v>1335</v>
       </c>
       <c r="D468" s="1" t="s">
-        <v>416</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="469" spans="1:4">
       <c r="A469" s="1" t="s">
-        <v>503</v>
+        <v>414</v>
       </c>
       <c r="B469" s="1" t="s">
-        <v>504</v>
+        <v>415</v>
       </c>
       <c r="D469" s="1" t="s">
-        <v>505</v>
+        <v>416</v>
       </c>
     </row>
     <row r="470" spans="1:4">
       <c r="A470" s="1" t="s">
-        <v>720</v>
+        <v>503</v>
       </c>
       <c r="B470" s="1" t="s">
-        <v>721</v>
+        <v>504</v>
       </c>
       <c r="D470" s="1" t="s">
-        <v>722</v>
+        <v>505</v>
       </c>
     </row>
     <row r="471" spans="1:4">
       <c r="A471" s="1" t="s">
-        <v>554</v>
+        <v>720</v>
       </c>
       <c r="B471" s="1" t="s">
-        <v>555</v>
+        <v>721</v>
       </c>
       <c r="D471" s="1" t="s">
-        <v>556</v>
+        <v>722</v>
       </c>
     </row>
     <row r="472" spans="1:4">
       <c r="A472" s="1" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="B472" s="1" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="D472" s="1" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
     </row>
     <row r="473" spans="1:4">
       <c r="A473" s="1" t="s">
-        <v>548</v>
+        <v>560</v>
       </c>
       <c r="B473" s="1" t="s">
-        <v>549</v>
+        <v>561</v>
       </c>
       <c r="D473" s="1" t="s">
-        <v>550</v>
+        <v>562</v>
       </c>
     </row>
     <row r="474" spans="1:4">
       <c r="A474" s="1" t="s">
-        <v>762</v>
+        <v>548</v>
       </c>
       <c r="B474" s="1" t="s">
-        <v>763</v>
+        <v>549</v>
       </c>
       <c r="D474" s="1" t="s">
         <v>550</v>
@@ -10333,723 +10363,745 @@
     </row>
     <row r="475" spans="1:4">
       <c r="A475" s="1" t="s">
-        <v>1362</v>
+        <v>762</v>
       </c>
       <c r="B475" s="1" t="s">
-        <v>1363</v>
+        <v>763</v>
       </c>
       <c r="D475" s="1" t="s">
-        <v>1364</v>
+        <v>550</v>
       </c>
     </row>
     <row r="476" spans="1:4">
       <c r="A476" s="1" t="s">
-        <v>1277</v>
+        <v>1362</v>
       </c>
       <c r="B476" s="1" t="s">
-        <v>1278</v>
+        <v>1363</v>
       </c>
       <c r="D476" s="1" t="s">
-        <v>1279</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="477" spans="1:4">
       <c r="A477" s="1" t="s">
-        <v>1389</v>
+        <v>1277</v>
       </c>
       <c r="B477" s="1" t="s">
-        <v>1390</v>
+        <v>1278</v>
+      </c>
+      <c r="D477" s="1" t="s">
+        <v>1279</v>
       </c>
     </row>
     <row r="478" spans="1:4">
       <c r="A478" s="1" t="s">
-        <v>617</v>
+        <v>1389</v>
       </c>
       <c r="B478" s="1" t="s">
-        <v>618</v>
-      </c>
-      <c r="D478" s="1" t="s">
-        <v>1007</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="479" spans="1:4">
       <c r="A479" s="1" t="s">
-        <v>605</v>
+        <v>617</v>
       </c>
       <c r="B479" s="1" t="s">
-        <v>606</v>
+        <v>618</v>
       </c>
       <c r="D479" s="1" t="s">
-        <v>607</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="480" spans="1:4">
       <c r="A480" s="1" t="s">
-        <v>1178</v>
+        <v>605</v>
       </c>
       <c r="B480" s="1" t="s">
-        <v>1185</v>
+        <v>606</v>
       </c>
       <c r="D480" s="1" t="s">
-        <v>1192</v>
+        <v>607</v>
       </c>
     </row>
     <row r="481" spans="1:4">
       <c r="A481" s="1" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="B481" s="1" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="D481" s="1" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="482" spans="1:4">
       <c r="A482" s="1" t="s">
-        <v>449</v>
+        <v>1179</v>
       </c>
       <c r="B482" s="1" t="s">
-        <v>450</v>
+        <v>1186</v>
       </c>
       <c r="D482" s="1" t="s">
-        <v>451</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="483" spans="1:4">
       <c r="A483" s="1" t="s">
-        <v>1165</v>
+        <v>449</v>
       </c>
       <c r="B483" s="1" t="s">
-        <v>1166</v>
+        <v>450</v>
       </c>
       <c r="D483" s="1" t="s">
-        <v>1167</v>
+        <v>451</v>
       </c>
     </row>
     <row r="484" spans="1:4">
       <c r="A484" s="1" t="s">
-        <v>1180</v>
+        <v>1165</v>
       </c>
       <c r="B484" s="1" t="s">
-        <v>1187</v>
+        <v>1166</v>
       </c>
       <c r="D484" s="1" t="s">
-        <v>1194</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="485" spans="1:4">
       <c r="A485" s="1" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="B485" s="1" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="D485" s="1" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="486" spans="1:4">
       <c r="A486" s="1" t="s">
-        <v>688</v>
+        <v>1181</v>
       </c>
       <c r="B486" s="1" t="s">
-        <v>689</v>
+        <v>1188</v>
       </c>
       <c r="D486" s="1" t="s">
-        <v>690</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="487" spans="1:4">
       <c r="A487" s="1" t="s">
-        <v>1371</v>
+        <v>1394</v>
       </c>
       <c r="B487" s="1" t="s">
-        <v>1372</v>
+        <v>1395</v>
       </c>
       <c r="D487" s="1" t="s">
-        <v>1373</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="488" spans="1:4">
       <c r="A488" s="1" t="s">
-        <v>452</v>
+        <v>688</v>
       </c>
       <c r="B488" s="1" t="s">
-        <v>453</v>
+        <v>689</v>
       </c>
       <c r="D488" s="1" t="s">
-        <v>454</v>
+        <v>690</v>
       </c>
     </row>
     <row r="489" spans="1:4">
       <c r="A489" s="1" t="s">
-        <v>1199</v>
+        <v>1371</v>
       </c>
       <c r="B489" s="1" t="s">
-        <v>1200</v>
+        <v>1372</v>
       </c>
       <c r="D489" s="1" t="s">
-        <v>1217</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="490" spans="1:4">
       <c r="A490" s="1" t="s">
-        <v>1302</v>
+        <v>452</v>
       </c>
       <c r="B490" s="1" t="s">
-        <v>1303</v>
+        <v>453</v>
       </c>
       <c r="D490" s="1" t="s">
-        <v>1304</v>
+        <v>454</v>
       </c>
     </row>
     <row r="491" spans="1:4">
       <c r="A491" s="1" t="s">
-        <v>764</v>
+        <v>1199</v>
       </c>
       <c r="B491" s="1" t="s">
-        <v>765</v>
+        <v>1200</v>
       </c>
       <c r="D491" s="1" t="s">
-        <v>766</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="492" spans="1:4">
       <c r="A492" s="1" t="s">
-        <v>1247</v>
+        <v>1302</v>
       </c>
       <c r="B492" s="1" t="s">
-        <v>1248</v>
+        <v>1303</v>
       </c>
       <c r="D492" s="1" t="s">
-        <v>1249</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="493" spans="1:4">
       <c r="A493" s="1" t="s">
-        <v>1046</v>
+        <v>764</v>
       </c>
       <c r="B493" s="1" t="s">
-        <v>1047</v>
+        <v>765</v>
       </c>
       <c r="D493" s="1" t="s">
-        <v>1048</v>
+        <v>766</v>
       </c>
     </row>
     <row r="494" spans="1:4">
       <c r="A494" s="1" t="s">
-        <v>1293</v>
+        <v>1247</v>
       </c>
       <c r="B494" s="1" t="s">
-        <v>1294</v>
+        <v>1248</v>
       </c>
       <c r="D494" s="1" t="s">
-        <v>1295</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="495" spans="1:4">
       <c r="A495" s="1" t="s">
-        <v>820</v>
+        <v>1046</v>
       </c>
       <c r="B495" s="1" t="s">
-        <v>821</v>
+        <v>1047</v>
       </c>
       <c r="D495" s="1" t="s">
-        <v>822</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="496" spans="1:4">
       <c r="A496" s="1" t="s">
-        <v>420</v>
+        <v>1293</v>
       </c>
       <c r="B496" s="1" t="s">
-        <v>421</v>
+        <v>1294</v>
       </c>
       <c r="D496" s="1" t="s">
-        <v>422</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="497" spans="1:4">
       <c r="A497" s="1" t="s">
-        <v>1380</v>
+        <v>820</v>
       </c>
       <c r="B497" s="1" t="s">
-        <v>1381</v>
+        <v>821</v>
       </c>
       <c r="D497" s="1" t="s">
-        <v>1382</v>
+        <v>822</v>
       </c>
     </row>
     <row r="498" spans="1:4">
       <c r="A498" s="1" t="s">
-        <v>1011</v>
+        <v>420</v>
       </c>
       <c r="B498" s="1" t="s">
-        <v>1012</v>
+        <v>421</v>
       </c>
       <c r="D498" s="1" t="s">
-        <v>1013</v>
+        <v>422</v>
       </c>
     </row>
     <row r="499" spans="1:4">
       <c r="A499" s="1" t="s">
-        <v>743</v>
+        <v>1380</v>
       </c>
       <c r="B499" s="1" t="s">
-        <v>744</v>
+        <v>1381</v>
       </c>
       <c r="D499" s="1" t="s">
-        <v>745</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="500" spans="1:4">
       <c r="A500" s="1" t="s">
-        <v>901</v>
+        <v>1011</v>
       </c>
       <c r="B500" s="1" t="s">
-        <v>900</v>
+        <v>1012</v>
       </c>
       <c r="D500" s="1" t="s">
-        <v>902</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="501" spans="1:4">
       <c r="A501" s="1" t="s">
-        <v>903</v>
+        <v>743</v>
       </c>
       <c r="B501" s="1" t="s">
-        <v>904</v>
+        <v>744</v>
       </c>
       <c r="D501" s="1" t="s">
-        <v>905</v>
+        <v>745</v>
       </c>
     </row>
     <row r="502" spans="1:4">
       <c r="A502" s="1" t="s">
-        <v>539</v>
+        <v>901</v>
       </c>
       <c r="B502" s="1" t="s">
-        <v>540</v>
+        <v>900</v>
       </c>
       <c r="D502" s="1" t="s">
-        <v>541</v>
+        <v>902</v>
       </c>
     </row>
     <row r="503" spans="1:4">
       <c r="A503" s="1" t="s">
-        <v>661</v>
+        <v>903</v>
       </c>
       <c r="B503" s="1" t="s">
-        <v>662</v>
+        <v>904</v>
       </c>
       <c r="D503" s="1" t="s">
-        <v>663</v>
+        <v>905</v>
       </c>
     </row>
     <row r="504" spans="1:4">
       <c r="A504" s="1" t="s">
-        <v>691</v>
+        <v>539</v>
       </c>
       <c r="B504" s="1" t="s">
-        <v>692</v>
+        <v>540</v>
       </c>
       <c r="D504" s="1" t="s">
-        <v>693</v>
+        <v>541</v>
       </c>
     </row>
     <row r="505" spans="1:4">
       <c r="A505" s="1" t="s">
-        <v>963</v>
+        <v>661</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>922</v>
+        <v>662</v>
       </c>
       <c r="D505" s="1" t="s">
-        <v>908</v>
+        <v>663</v>
       </c>
     </row>
     <row r="506" spans="1:4">
       <c r="A506" s="1" t="s">
-        <v>1368</v>
+        <v>691</v>
       </c>
       <c r="B506" s="1" t="s">
-        <v>1369</v>
+        <v>692</v>
       </c>
       <c r="D506" s="1" t="s">
-        <v>1370</v>
+        <v>693</v>
       </c>
     </row>
     <row r="507" spans="1:4">
       <c r="A507" s="1" t="s">
-        <v>785</v>
+        <v>963</v>
       </c>
       <c r="B507" s="1" t="s">
-        <v>786</v>
+        <v>922</v>
       </c>
       <c r="D507" s="1" t="s">
-        <v>787</v>
+        <v>908</v>
       </c>
     </row>
     <row r="508" spans="1:4">
       <c r="A508" s="1" t="s">
-        <v>622</v>
+        <v>1368</v>
       </c>
       <c r="B508" s="1" t="s">
-        <v>623</v>
+        <v>1369</v>
       </c>
       <c r="D508" s="1" t="s">
-        <v>624</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="509" spans="1:4">
       <c r="A509" s="1" t="s">
-        <v>835</v>
+        <v>785</v>
       </c>
       <c r="B509" s="1" t="s">
-        <v>836</v>
+        <v>786</v>
       </c>
       <c r="D509" s="1" t="s">
-        <v>837</v>
+        <v>787</v>
       </c>
     </row>
     <row r="510" spans="1:4">
       <c r="A510" s="1" t="s">
-        <v>685</v>
+        <v>622</v>
       </c>
       <c r="B510" s="1" t="s">
-        <v>686</v>
+        <v>623</v>
       </c>
       <c r="D510" s="1" t="s">
-        <v>687</v>
+        <v>624</v>
       </c>
     </row>
     <row r="511" spans="1:4">
       <c r="A511" s="1" t="s">
-        <v>892</v>
+        <v>835</v>
       </c>
       <c r="B511" s="1" t="s">
-        <v>893</v>
+        <v>836</v>
+      </c>
+      <c r="D511" s="1" t="s">
+        <v>837</v>
       </c>
     </row>
     <row r="512" spans="1:4">
       <c r="A512" s="1" t="s">
-        <v>967</v>
+        <v>685</v>
       </c>
       <c r="B512" s="1" t="s">
-        <v>916</v>
+        <v>686</v>
       </c>
       <c r="D512" s="1" t="s">
-        <v>969</v>
+        <v>687</v>
       </c>
     </row>
     <row r="513" spans="1:4">
       <c r="A513" s="1" t="s">
-        <v>946</v>
+        <v>892</v>
       </c>
       <c r="B513" s="1" t="s">
-        <v>947</v>
-      </c>
-      <c r="D513" s="1" t="s">
-        <v>948</v>
+        <v>893</v>
       </c>
     </row>
     <row r="514" spans="1:4">
       <c r="A514" s="1" t="s">
-        <v>473</v>
+        <v>967</v>
       </c>
       <c r="B514" s="1" t="s">
-        <v>474</v>
+        <v>916</v>
       </c>
       <c r="D514" s="1" t="s">
-        <v>475</v>
+        <v>969</v>
       </c>
     </row>
     <row r="515" spans="1:4">
       <c r="A515" s="1" t="s">
-        <v>566</v>
+        <v>946</v>
       </c>
       <c r="B515" s="1" t="s">
-        <v>567</v>
+        <v>947</v>
       </c>
       <c r="D515" s="1" t="s">
-        <v>568</v>
+        <v>948</v>
       </c>
     </row>
     <row r="516" spans="1:4">
       <c r="A516" s="1" t="s">
-        <v>767</v>
+        <v>473</v>
       </c>
       <c r="B516" s="1" t="s">
-        <v>768</v>
+        <v>474</v>
       </c>
       <c r="D516" s="1" t="s">
-        <v>769</v>
+        <v>475</v>
       </c>
     </row>
     <row r="517" spans="1:4">
       <c r="A517" s="1" t="s">
-        <v>770</v>
+        <v>566</v>
       </c>
       <c r="B517" s="1" t="s">
-        <v>771</v>
+        <v>567</v>
       </c>
       <c r="D517" s="1" t="s">
-        <v>353</v>
+        <v>568</v>
       </c>
     </row>
     <row r="518" spans="1:4">
       <c r="A518" s="1" t="s">
-        <v>1347</v>
+        <v>767</v>
       </c>
       <c r="B518" s="1" t="s">
-        <v>1348</v>
+        <v>768</v>
+      </c>
+      <c r="D518" s="1" t="s">
+        <v>769</v>
       </c>
     </row>
     <row r="519" spans="1:4">
       <c r="A519" s="1" t="s">
-        <v>711</v>
+        <v>770</v>
       </c>
       <c r="B519" s="1" t="s">
-        <v>712</v>
+        <v>771</v>
       </c>
       <c r="D519" s="1" t="s">
-        <v>713</v>
+        <v>353</v>
       </c>
     </row>
     <row r="520" spans="1:4">
       <c r="A520" s="1" t="s">
-        <v>877</v>
+        <v>1347</v>
       </c>
       <c r="B520" s="1" t="s">
-        <v>878</v>
-      </c>
-      <c r="D520" s="1" t="s">
-        <v>879</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="521" spans="1:4">
       <c r="A521" s="1" t="s">
-        <v>1141</v>
+        <v>711</v>
       </c>
       <c r="B521" s="1" t="s">
-        <v>1142</v>
+        <v>712</v>
       </c>
       <c r="D521" s="1" t="s">
-        <v>1140</v>
+        <v>713</v>
       </c>
     </row>
     <row r="522" spans="1:4">
       <c r="A522" s="1" t="s">
-        <v>949</v>
+        <v>877</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>951</v>
+        <v>878</v>
       </c>
       <c r="D522" s="1" t="s">
-        <v>952</v>
+        <v>879</v>
       </c>
     </row>
     <row r="523" spans="1:4">
       <c r="A523" s="1" t="s">
-        <v>746</v>
+        <v>1141</v>
       </c>
       <c r="B523" s="1" t="s">
-        <v>747</v>
+        <v>1142</v>
       </c>
       <c r="D523" s="1" t="s">
-        <v>748</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="524" spans="1:4">
       <c r="A524" s="1" t="s">
-        <v>1226</v>
+        <v>949</v>
       </c>
       <c r="B524" s="1" t="s">
-        <v>1227</v>
+        <v>951</v>
       </c>
       <c r="D524" s="1" t="s">
-        <v>1228</v>
+        <v>952</v>
       </c>
     </row>
     <row r="525" spans="1:4">
       <c r="A525" s="1" t="s">
-        <v>575</v>
+        <v>746</v>
       </c>
       <c r="B525" s="1" t="s">
-        <v>576</v>
+        <v>747</v>
       </c>
       <c r="D525" s="1" t="s">
-        <v>577</v>
+        <v>748</v>
       </c>
     </row>
     <row r="526" spans="1:4">
       <c r="A526" s="1" t="s">
-        <v>823</v>
+        <v>1226</v>
       </c>
       <c r="B526" s="1" t="s">
-        <v>824</v>
+        <v>1227</v>
       </c>
       <c r="D526" s="1" t="s">
-        <v>825</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="527" spans="1:4">
       <c r="A527" s="1" t="s">
-        <v>1019</v>
+        <v>575</v>
       </c>
       <c r="B527" s="1" t="s">
-        <v>1020</v>
+        <v>576</v>
       </c>
       <c r="D527" s="1" t="s">
-        <v>1021</v>
+        <v>577</v>
       </c>
     </row>
     <row r="528" spans="1:4">
       <c r="A528" s="1" t="s">
-        <v>426</v>
+        <v>823</v>
       </c>
       <c r="B528" s="1" t="s">
-        <v>427</v>
+        <v>824</v>
       </c>
       <c r="D528" s="1" t="s">
-        <v>428</v>
+        <v>825</v>
       </c>
     </row>
     <row r="529" spans="1:4">
       <c r="A529" s="1" t="s">
-        <v>625</v>
+        <v>1019</v>
       </c>
       <c r="B529" s="1" t="s">
-        <v>626</v>
+        <v>1020</v>
       </c>
       <c r="D529" s="1" t="s">
-        <v>627</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="530" spans="1:4">
       <c r="A530" s="1" t="s">
-        <v>417</v>
+        <v>426</v>
       </c>
       <c r="B530" s="1" t="s">
-        <v>418</v>
+        <v>427</v>
       </c>
       <c r="D530" s="1" t="s">
-        <v>419</v>
+        <v>428</v>
       </c>
     </row>
     <row r="531" spans="1:4">
       <c r="A531" s="1" t="s">
-        <v>928</v>
+        <v>625</v>
       </c>
       <c r="B531" s="1" t="s">
-        <v>929</v>
+        <v>626</v>
       </c>
       <c r="D531" s="1" t="s">
-        <v>930</v>
+        <v>627</v>
       </c>
     </row>
     <row r="532" spans="1:4">
       <c r="A532" s="1" t="s">
-        <v>1262</v>
+        <v>417</v>
       </c>
       <c r="B532" s="1" t="s">
-        <v>1263</v>
+        <v>418</v>
       </c>
       <c r="D532" s="1" t="s">
-        <v>1264</v>
+        <v>419</v>
       </c>
     </row>
     <row r="533" spans="1:4">
       <c r="A533" s="1" t="s">
-        <v>1238</v>
+        <v>928</v>
       </c>
       <c r="B533" s="1" t="s">
-        <v>1241</v>
+        <v>929</v>
       </c>
       <c r="D533" s="1" t="s">
-        <v>1243</v>
+        <v>930</v>
       </c>
     </row>
     <row r="534" spans="1:4">
       <c r="A534" s="1" t="s">
-        <v>734</v>
+        <v>1262</v>
       </c>
       <c r="B534" s="1" t="s">
-        <v>735</v>
+        <v>1263</v>
       </c>
       <c r="D534" s="1" t="s">
-        <v>736</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="535" spans="1:4">
       <c r="A535" s="1" t="s">
-        <v>737</v>
+        <v>1238</v>
       </c>
       <c r="B535" s="1" t="s">
-        <v>738</v>
+        <v>1241</v>
       </c>
       <c r="D535" s="1" t="s">
-        <v>739</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="536" spans="1:4">
       <c r="A536" s="1" t="s">
-        <v>1239</v>
+        <v>734</v>
       </c>
       <c r="B536" s="1" t="s">
-        <v>1246</v>
+        <v>735</v>
       </c>
       <c r="D536" s="1" t="s">
-        <v>1245</v>
+        <v>736</v>
       </c>
     </row>
     <row r="537" spans="1:4">
       <c r="A537" s="1" t="s">
-        <v>1240</v>
+        <v>737</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>1242</v>
+        <v>738</v>
       </c>
       <c r="D537" s="1" t="s">
-        <v>1244</v>
+        <v>739</v>
       </c>
     </row>
     <row r="538" spans="1:4">
       <c r="A538" s="1" t="s">
-        <v>740</v>
+        <v>1239</v>
       </c>
       <c r="B538" s="1" t="s">
-        <v>741</v>
+        <v>1246</v>
       </c>
       <c r="D538" s="1" t="s">
-        <v>742</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="539" spans="1:4">
       <c r="A539" s="1" t="s">
-        <v>628</v>
+        <v>1240</v>
       </c>
       <c r="B539" s="1" t="s">
-        <v>629</v>
+        <v>1242</v>
       </c>
       <c r="D539" s="1" t="s">
-        <v>630</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="540" spans="1:4">
       <c r="A540" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="B540" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="D540" s="1" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="541" spans="1:4">
+      <c r="A541" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="B541" s="1" t="s">
+        <v>629</v>
+      </c>
+      <c r="D541" s="1" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="542" spans="1:4">
+      <c r="A542" s="1" t="s">
         <v>631</v>
       </c>
-      <c r="B540" s="1" t="s">
+      <c r="B542" s="1" t="s">
         <v>632</v>
       </c>
-      <c r="D540" s="1" t="s">
+      <c r="D542" s="1" t="s">
         <v>633</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A230:G461">
+  <sortState ref="A230:G462">
     <sortCondition ref="A230"/>
   </sortState>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
Follow Play Framework v2.8.0
</commit_message>
<xml_diff>
--- a/conf/messages.xlsx
+++ b/conf/messages.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hiro/github/FinePlay/conf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75332F0A-1D50-AD4C-A984-E8005F918D1B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D8A77F8-EF66-5346-9438-70D5D8047CB5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3740" yWindow="920" windowWidth="33460" windowHeight="21560" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4342,14 +4342,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t># Copyright (C) 2009-2018 Lightbend Inc. &lt;https://www.lightbend.com&gt;</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t># Japanese messages Copyright (C) 2017-2018 hiro20v. &lt;https://github.com/hiro20v&gt;</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>map.rotate.lambda</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -5045,6 +5037,14 @@
   </si>
   <si>
     <t>スキャン</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t># Copyright (C) 2009-2019 Lightbend Inc. &lt;https://www.lightbend.com&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t># Japanese messages Copyright (C) 2017-2019 hiro20v. &lt;https://github.com/hiro20v&gt;</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -5791,9 +5791,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G553"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A456" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D476" sqref="D476"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
@@ -5816,7 +5814,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -5833,7 +5831,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -5850,7 +5848,7 @@
         <v>895</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -5860,10 +5858,10 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>1268</v>
+        <v>1424</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>1269</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -7053,24 +7051,24 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="1" t="s">
+        <v>1287</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>1288</v>
+      </c>
+      <c r="D149" s="1" t="s">
         <v>1289</v>
-      </c>
-      <c r="B149" s="1" t="s">
-        <v>1290</v>
-      </c>
-      <c r="D149" s="1" t="s">
-        <v>1291</v>
       </c>
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="1" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>1288</v>
+        <v>1286</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>1286</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="152" spans="1:4">
@@ -7097,18 +7095,18 @@
         <v>229</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>1357</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="1" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>1354</v>
+        <v>1352</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>1355</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="158" spans="1:4">
@@ -7138,7 +7136,7 @@
         <v>235</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="163" spans="1:5">
@@ -7152,15 +7150,15 @@
         <v>242</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="164" spans="1:5">
       <c r="A164" s="1" t="s">
-        <v>1405</v>
+        <v>1403</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="165" spans="1:5">
@@ -7171,7 +7169,7 @@
         <v>235</v>
       </c>
       <c r="E165" s="1" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="166" spans="1:5">
@@ -7185,12 +7183,12 @@
         <v>1029</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="167" spans="1:5">
       <c r="A167" s="1" t="s">
-        <v>1320</v>
+        <v>1318</v>
       </c>
       <c r="C167" s="1" t="s">
         <v>2</v>
@@ -7199,15 +7197,15 @@
         <v>3</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="168" spans="1:5">
       <c r="A168" s="1" t="s">
-        <v>1412</v>
+        <v>1410</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
       <c r="D168" s="1" t="s">
         <v>1153</v>
@@ -7215,19 +7213,19 @@
     </row>
     <row r="169" spans="1:5">
       <c r="A169" s="1" t="s">
-        <v>1417</v>
+        <v>1415</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D169" s="1" t="s">
         <v>1029</v>
       </c>
       <c r="E169" s="1" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="170" spans="1:5">
@@ -7241,7 +7239,7 @@
         <v>235</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="171" spans="1:5">
@@ -7258,7 +7256,7 @@
         <v>235</v>
       </c>
       <c r="E171" s="1" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="172" spans="1:5">
@@ -7269,7 +7267,7 @@
         <v>237</v>
       </c>
       <c r="E172" s="1" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="173" spans="1:5">
@@ -7283,7 +7281,7 @@
         <v>235</v>
       </c>
       <c r="E173" s="1" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="174" spans="1:5">
@@ -7305,15 +7303,15 @@
         <v>1153</v>
       </c>
       <c r="E175" s="1" t="s">
-        <v>1321</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="176" spans="1:5">
       <c r="A176" s="1" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D176" s="1" t="s">
         <v>1029</v>
@@ -7332,41 +7330,41 @@
     </row>
     <row r="179" spans="1:4">
       <c r="A179" s="1" t="s">
-        <v>1413</v>
+        <v>1411</v>
       </c>
       <c r="B179" s="1" t="s">
         <v>1267</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>1419</v>
+        <v>1417</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>1415</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="180" spans="1:4">
       <c r="A180" s="1" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="B180" s="1" t="s">
         <v>1267</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>1418</v>
+        <v>1416</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>1416</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="182" spans="1:4">
       <c r="A182" s="1" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
       <c r="B182" s="1" t="s">
         <v>1267</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>1273</v>
+        <v>1271</v>
       </c>
       <c r="D182" s="1" t="s">
         <v>1266</v>
@@ -7374,7 +7372,7 @@
     </row>
     <row r="183" spans="1:4">
       <c r="A183" s="1" t="s">
-        <v>1271</v>
+        <v>1269</v>
       </c>
       <c r="B183" s="1" t="s">
         <v>1267</v>
@@ -7388,7 +7386,7 @@
     </row>
     <row r="184" spans="1:4">
       <c r="A184" s="1" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
       <c r="B184" s="1" t="s">
         <v>1267</v>
@@ -8199,13 +8197,13 @@
     </row>
     <row r="265" spans="1:4">
       <c r="A265" s="1" t="s">
+        <v>1307</v>
+      </c>
+      <c r="B265" s="1" t="s">
+        <v>1308</v>
+      </c>
+      <c r="D265" s="1" t="s">
         <v>1309</v>
-      </c>
-      <c r="B265" s="1" t="s">
-        <v>1310</v>
-      </c>
-      <c r="D265" s="1" t="s">
-        <v>1311</v>
       </c>
     </row>
     <row r="266" spans="1:4">
@@ -8284,13 +8282,13 @@
     </row>
     <row r="273" spans="1:5">
       <c r="A273" s="1" t="s">
+        <v>1337</v>
+      </c>
+      <c r="B273" s="1" t="s">
+        <v>1338</v>
+      </c>
+      <c r="D273" s="1" t="s">
         <v>1339</v>
-      </c>
-      <c r="B273" s="1" t="s">
-        <v>1340</v>
-      </c>
-      <c r="D273" s="1" t="s">
-        <v>1341</v>
       </c>
     </row>
     <row r="274" spans="1:5">
@@ -8304,7 +8302,7 @@
         <v>861</v>
       </c>
       <c r="E274" s="1" t="s">
-        <v>1396</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="275" spans="1:5">
@@ -8342,13 +8340,13 @@
     </row>
     <row r="278" spans="1:5">
       <c r="A278" s="1" t="s">
+        <v>1418</v>
+      </c>
+      <c r="B278" s="1" t="s">
+        <v>1419</v>
+      </c>
+      <c r="D278" s="1" t="s">
         <v>1420</v>
-      </c>
-      <c r="B278" s="1" t="s">
-        <v>1421</v>
-      </c>
-      <c r="D278" s="1" t="s">
-        <v>1422</v>
       </c>
     </row>
     <row r="279" spans="1:5">
@@ -8397,13 +8395,13 @@
     </row>
     <row r="283" spans="1:5">
       <c r="A283" s="1" t="s">
+        <v>1324</v>
+      </c>
+      <c r="B283" s="1" t="s">
+        <v>1325</v>
+      </c>
+      <c r="D283" s="1" t="s">
         <v>1326</v>
-      </c>
-      <c r="B283" s="1" t="s">
-        <v>1327</v>
-      </c>
-      <c r="D283" s="1" t="s">
-        <v>1328</v>
       </c>
     </row>
     <row r="284" spans="1:5">
@@ -8419,13 +8417,13 @@
     </row>
     <row r="285" spans="1:5">
       <c r="A285" s="1" t="s">
+        <v>1388</v>
+      </c>
+      <c r="B285" s="1" t="s">
+        <v>1389</v>
+      </c>
+      <c r="D285" s="1" t="s">
         <v>1390</v>
-      </c>
-      <c r="B285" s="1" t="s">
-        <v>1391</v>
-      </c>
-      <c r="D285" s="1" t="s">
-        <v>1392</v>
       </c>
     </row>
     <row r="286" spans="1:5">
@@ -8474,13 +8472,13 @@
     </row>
     <row r="290" spans="1:4">
       <c r="A290" s="1" t="s">
+        <v>1272</v>
+      </c>
+      <c r="B290" s="1" t="s">
+        <v>1273</v>
+      </c>
+      <c r="D290" s="1" t="s">
         <v>1274</v>
-      </c>
-      <c r="B290" s="1" t="s">
-        <v>1275</v>
-      </c>
-      <c r="D290" s="1" t="s">
-        <v>1276</v>
       </c>
     </row>
     <row r="291" spans="1:4">
@@ -8584,13 +8582,13 @@
     </row>
     <row r="300" spans="1:4">
       <c r="A300" s="1" t="s">
+        <v>1296</v>
+      </c>
+      <c r="B300" s="1" t="s">
+        <v>1297</v>
+      </c>
+      <c r="D300" s="1" t="s">
         <v>1298</v>
-      </c>
-      <c r="B300" s="1" t="s">
-        <v>1299</v>
-      </c>
-      <c r="D300" s="1" t="s">
-        <v>1300</v>
       </c>
     </row>
     <row r="301" spans="1:4">
@@ -8628,13 +8626,13 @@
     </row>
     <row r="304" spans="1:4">
       <c r="A304" s="1" t="s">
-        <v>1403</v>
+        <v>1401</v>
       </c>
       <c r="B304" s="1" t="s">
+        <v>1400</v>
+      </c>
+      <c r="D304" s="1" t="s">
         <v>1402</v>
-      </c>
-      <c r="D304" s="1" t="s">
-        <v>1404</v>
       </c>
     </row>
     <row r="305" spans="1:4">
@@ -8815,13 +8813,13 @@
     </row>
     <row r="321" spans="1:4">
       <c r="A321" s="1" t="s">
+        <v>1320</v>
+      </c>
+      <c r="B321" s="1" t="s">
+        <v>1321</v>
+      </c>
+      <c r="D321" s="1" t="s">
         <v>1322</v>
-      </c>
-      <c r="B321" s="1" t="s">
-        <v>1323</v>
-      </c>
-      <c r="D321" s="1" t="s">
-        <v>1324</v>
       </c>
     </row>
     <row r="322" spans="1:4">
@@ -8947,13 +8945,13 @@
     </row>
     <row r="333" spans="1:4">
       <c r="A333" s="1" t="s">
-        <v>1330</v>
+        <v>1328</v>
       </c>
       <c r="B333" s="1" t="s">
-        <v>1329</v>
+        <v>1327</v>
       </c>
       <c r="D333" s="1" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="334" spans="1:4">
@@ -8991,13 +8989,13 @@
     </row>
     <row r="337" spans="1:4">
       <c r="A337" s="1" t="s">
+        <v>1281</v>
+      </c>
+      <c r="B337" s="1" t="s">
+        <v>1282</v>
+      </c>
+      <c r="D337" s="1" t="s">
         <v>1283</v>
-      </c>
-      <c r="B337" s="1" t="s">
-        <v>1284</v>
-      </c>
-      <c r="D337" s="1" t="s">
-        <v>1285</v>
       </c>
     </row>
     <row r="338" spans="1:4">
@@ -9153,13 +9151,13 @@
     </row>
     <row r="352" spans="1:4">
       <c r="A352" s="1" t="s">
+        <v>1310</v>
+      </c>
+      <c r="B352" s="1" t="s">
         <v>1312</v>
       </c>
-      <c r="B352" s="1" t="s">
-        <v>1314</v>
-      </c>
       <c r="D352" s="1" t="s">
-        <v>1313</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="353" spans="1:4">
@@ -9378,13 +9376,13 @@
     </row>
     <row r="373" spans="1:4">
       <c r="A373" s="1" t="s">
+        <v>1404</v>
+      </c>
+      <c r="B373" s="1" t="s">
+        <v>1405</v>
+      </c>
+      <c r="D373" s="1" t="s">
         <v>1406</v>
-      </c>
-      <c r="B373" s="1" t="s">
-        <v>1407</v>
-      </c>
-      <c r="D373" s="1" t="s">
-        <v>1408</v>
       </c>
     </row>
     <row r="374" spans="1:4">
@@ -9482,13 +9480,13 @@
     </row>
     <row r="383" spans="1:4">
       <c r="A383" s="1" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="B383" s="1" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="D383" s="1" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="384" spans="1:4">
@@ -9625,13 +9623,13 @@
     </row>
     <row r="396" spans="1:4">
       <c r="A396" s="1" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B396" s="1" t="s">
+        <v>1341</v>
+      </c>
+      <c r="D396" s="1" t="s">
         <v>1342</v>
-      </c>
-      <c r="B396" s="1" t="s">
-        <v>1343</v>
-      </c>
-      <c r="D396" s="1" t="s">
-        <v>1344</v>
       </c>
     </row>
     <row r="397" spans="1:4">
@@ -9790,13 +9788,13 @@
     </row>
     <row r="411" spans="1:5">
       <c r="A411" s="1" t="s">
+        <v>1313</v>
+      </c>
+      <c r="B411" s="1" t="s">
+        <v>1314</v>
+      </c>
+      <c r="D411" s="1" t="s">
         <v>1315</v>
-      </c>
-      <c r="B411" s="1" t="s">
-        <v>1316</v>
-      </c>
-      <c r="D411" s="1" t="s">
-        <v>1317</v>
       </c>
     </row>
     <row r="412" spans="1:5">
@@ -9810,7 +9808,7 @@
         <v>601</v>
       </c>
       <c r="E412" s="1" t="s">
-        <v>1397</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="413" spans="1:5">
@@ -9857,7 +9855,7 @@
         <v>598</v>
       </c>
       <c r="E416" s="1" t="s">
-        <v>1398</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="417" spans="1:4">
@@ -9950,21 +9948,21 @@
     </row>
     <row r="425" spans="1:4">
       <c r="A425" s="1" t="s">
-        <v>1307</v>
+        <v>1305</v>
       </c>
       <c r="B425" s="1" t="s">
-        <v>1308</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="426" spans="1:4">
       <c r="A426" s="1" t="s">
+        <v>1278</v>
+      </c>
+      <c r="B426" s="1" t="s">
         <v>1280</v>
       </c>
-      <c r="B426" s="1" t="s">
-        <v>1282</v>
-      </c>
       <c r="D426" s="1" t="s">
-        <v>1281</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="427" spans="1:4">
@@ -9980,21 +9978,21 @@
     </row>
     <row r="428" spans="1:4">
       <c r="A428" s="1" t="s">
-        <v>1410</v>
+        <v>1408</v>
       </c>
       <c r="B428" s="1" t="s">
-        <v>1411</v>
+        <v>1409</v>
       </c>
       <c r="D428" s="1" t="s">
-        <v>1409</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="429" spans="1:4">
       <c r="A429" s="1" t="s">
-        <v>1331</v>
+        <v>1329</v>
       </c>
       <c r="B429" s="1" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="D429" s="1" t="s">
         <v>1201</v>
@@ -10013,13 +10011,13 @@
     </row>
     <row r="431" spans="1:4">
       <c r="A431" s="1" t="s">
+        <v>1356</v>
+      </c>
+      <c r="B431" s="1" t="s">
+        <v>1357</v>
+      </c>
+      <c r="D431" s="1" t="s">
         <v>1358</v>
-      </c>
-      <c r="B431" s="1" t="s">
-        <v>1359</v>
-      </c>
-      <c r="D431" s="1" t="s">
-        <v>1360</v>
       </c>
     </row>
     <row r="432" spans="1:4">
@@ -10057,43 +10055,43 @@
     </row>
     <row r="435" spans="1:4">
       <c r="A435" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="B435" s="1" t="s">
+        <v>1303</v>
+      </c>
+      <c r="D435" s="1" t="s">
         <v>1304</v>
-      </c>
-      <c r="B435" s="1" t="s">
-        <v>1305</v>
-      </c>
-      <c r="D435" s="1" t="s">
-        <v>1306</v>
       </c>
     </row>
     <row r="436" spans="1:4">
       <c r="A436" s="1" t="s">
+        <v>1383</v>
+      </c>
+      <c r="B436" s="1" t="s">
+        <v>1384</v>
+      </c>
+      <c r="D436" s="1" t="s">
         <v>1385</v>
-      </c>
-      <c r="B436" s="1" t="s">
-        <v>1386</v>
-      </c>
-      <c r="D436" s="1" t="s">
-        <v>1387</v>
       </c>
     </row>
     <row r="437" spans="1:4">
       <c r="A437" s="1" t="s">
-        <v>1352</v>
+        <v>1350</v>
       </c>
       <c r="B437" s="1" t="s">
-        <v>1353</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="438" spans="1:4">
       <c r="A438" s="1" t="s">
+        <v>1380</v>
+      </c>
+      <c r="B438" s="1" t="s">
+        <v>1381</v>
+      </c>
+      <c r="D438" s="1" t="s">
         <v>1382</v>
-      </c>
-      <c r="B438" s="1" t="s">
-        <v>1383</v>
-      </c>
-      <c r="D438" s="1" t="s">
-        <v>1384</v>
       </c>
     </row>
     <row r="439" spans="1:4">
@@ -10153,13 +10151,13 @@
     </row>
     <row r="444" spans="1:4">
       <c r="A444" s="1" t="s">
+        <v>1374</v>
+      </c>
+      <c r="B444" s="1" t="s">
+        <v>1375</v>
+      </c>
+      <c r="D444" s="1" t="s">
         <v>1376</v>
-      </c>
-      <c r="B444" s="1" t="s">
-        <v>1377</v>
-      </c>
-      <c r="D444" s="1" t="s">
-        <v>1378</v>
       </c>
     </row>
     <row r="445" spans="1:4">
@@ -10186,13 +10184,13 @@
     </row>
     <row r="447" spans="1:4">
       <c r="A447" s="1" t="s">
+        <v>1371</v>
+      </c>
+      <c r="B447" s="1" t="s">
+        <v>1372</v>
+      </c>
+      <c r="D447" s="1" t="s">
         <v>1373</v>
-      </c>
-      <c r="B447" s="1" t="s">
-        <v>1374</v>
-      </c>
-      <c r="D447" s="1" t="s">
-        <v>1375</v>
       </c>
     </row>
     <row r="448" spans="1:4">
@@ -10274,13 +10272,13 @@
     </row>
     <row r="455" spans="1:4">
       <c r="A455" s="1" t="s">
+        <v>1362</v>
+      </c>
+      <c r="B455" s="1" t="s">
         <v>1364</v>
       </c>
-      <c r="B455" s="1" t="s">
-        <v>1366</v>
-      </c>
       <c r="D455" s="1" t="s">
-        <v>1365</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="456" spans="1:4">
@@ -10494,24 +10492,24 @@
     </row>
     <row r="475" spans="1:4">
       <c r="A475" s="1" t="s">
+        <v>1421</v>
+      </c>
+      <c r="B475" s="1" t="s">
+        <v>1422</v>
+      </c>
+      <c r="D475" s="1" t="s">
         <v>1423</v>
-      </c>
-      <c r="B475" s="1" t="s">
-        <v>1424</v>
-      </c>
-      <c r="D475" s="1" t="s">
-        <v>1425</v>
       </c>
     </row>
     <row r="476" spans="1:4">
       <c r="A476" s="1" t="s">
+        <v>1293</v>
+      </c>
+      <c r="B476" s="1" t="s">
         <v>1295</v>
       </c>
-      <c r="B476" s="1" t="s">
-        <v>1297</v>
-      </c>
       <c r="D476" s="1" t="s">
-        <v>1296</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="477" spans="1:4">
@@ -10527,13 +10525,13 @@
     </row>
     <row r="478" spans="1:4">
       <c r="A478" s="1" t="s">
+        <v>1331</v>
+      </c>
+      <c r="B478" s="1" t="s">
+        <v>1332</v>
+      </c>
+      <c r="D478" s="1" t="s">
         <v>1333</v>
-      </c>
-      <c r="B478" s="1" t="s">
-        <v>1334</v>
-      </c>
-      <c r="D478" s="1" t="s">
-        <v>1335</v>
       </c>
     </row>
     <row r="479" spans="1:4">
@@ -10615,43 +10613,43 @@
     </row>
     <row r="486" spans="1:4">
       <c r="A486" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="B486" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="D486" s="1" t="s">
         <v>1399</v>
-      </c>
-      <c r="B486" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="D486" s="1" t="s">
-        <v>1401</v>
       </c>
     </row>
     <row r="487" spans="1:4">
       <c r="A487" s="1" t="s">
+        <v>1359</v>
+      </c>
+      <c r="B487" s="1" t="s">
+        <v>1360</v>
+      </c>
+      <c r="D487" s="1" t="s">
         <v>1361</v>
-      </c>
-      <c r="B487" s="1" t="s">
-        <v>1362</v>
-      </c>
-      <c r="D487" s="1" t="s">
-        <v>1363</v>
       </c>
     </row>
     <row r="488" spans="1:4">
       <c r="A488" s="1" t="s">
+        <v>1275</v>
+      </c>
+      <c r="B488" s="1" t="s">
+        <v>1276</v>
+      </c>
+      <c r="D488" s="1" t="s">
         <v>1277</v>
-      </c>
-      <c r="B488" s="1" t="s">
-        <v>1278</v>
-      </c>
-      <c r="D488" s="1" t="s">
-        <v>1279</v>
       </c>
     </row>
     <row r="489" spans="1:4">
       <c r="A489" s="1" t="s">
-        <v>1388</v>
+        <v>1386</v>
       </c>
       <c r="B489" s="1" t="s">
-        <v>1389</v>
+        <v>1387</v>
       </c>
     </row>
     <row r="490" spans="1:4">
@@ -10744,13 +10742,13 @@
     </row>
     <row r="498" spans="1:4">
       <c r="A498" s="1" t="s">
+        <v>1391</v>
+      </c>
+      <c r="B498" s="1" t="s">
+        <v>1392</v>
+      </c>
+      <c r="D498" s="1" t="s">
         <v>1393</v>
-      </c>
-      <c r="B498" s="1" t="s">
-        <v>1394</v>
-      </c>
-      <c r="D498" s="1" t="s">
-        <v>1395</v>
       </c>
     </row>
     <row r="499" spans="1:4">
@@ -10766,13 +10764,13 @@
     </row>
     <row r="500" spans="1:4">
       <c r="A500" s="1" t="s">
+        <v>1368</v>
+      </c>
+      <c r="B500" s="1" t="s">
+        <v>1369</v>
+      </c>
+      <c r="D500" s="1" t="s">
         <v>1370</v>
-      </c>
-      <c r="B500" s="1" t="s">
-        <v>1371</v>
-      </c>
-      <c r="D500" s="1" t="s">
-        <v>1372</v>
       </c>
     </row>
     <row r="501" spans="1:4">
@@ -10799,13 +10797,13 @@
     </row>
     <row r="503" spans="1:4">
       <c r="A503" s="1" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B503" s="1" t="s">
+        <v>1300</v>
+      </c>
+      <c r="D503" s="1" t="s">
         <v>1301</v>
-      </c>
-      <c r="B503" s="1" t="s">
-        <v>1302</v>
-      </c>
-      <c r="D503" s="1" t="s">
-        <v>1303</v>
       </c>
     </row>
     <row r="504" spans="1:4">
@@ -10843,13 +10841,13 @@
     </row>
     <row r="507" spans="1:4">
       <c r="A507" s="1" t="s">
+        <v>1290</v>
+      </c>
+      <c r="B507" s="1" t="s">
+        <v>1291</v>
+      </c>
+      <c r="D507" s="1" t="s">
         <v>1292</v>
-      </c>
-      <c r="B507" s="1" t="s">
-        <v>1293</v>
-      </c>
-      <c r="D507" s="1" t="s">
-        <v>1294</v>
       </c>
     </row>
     <row r="508" spans="1:4">
@@ -10876,13 +10874,13 @@
     </row>
     <row r="510" spans="1:4">
       <c r="A510" s="1" t="s">
+        <v>1377</v>
+      </c>
+      <c r="B510" s="1" t="s">
+        <v>1378</v>
+      </c>
+      <c r="D510" s="1" t="s">
         <v>1379</v>
-      </c>
-      <c r="B510" s="1" t="s">
-        <v>1380</v>
-      </c>
-      <c r="D510" s="1" t="s">
-        <v>1381</v>
       </c>
     </row>
     <row r="511" spans="1:4">
@@ -10975,13 +10973,13 @@
     </row>
     <row r="519" spans="1:4">
       <c r="A519" s="1" t="s">
+        <v>1365</v>
+      </c>
+      <c r="B519" s="1" t="s">
+        <v>1366</v>
+      </c>
+      <c r="D519" s="1" t="s">
         <v>1367</v>
-      </c>
-      <c r="B519" s="1" t="s">
-        <v>1368</v>
-      </c>
-      <c r="D519" s="1" t="s">
-        <v>1369</v>
       </c>
     </row>
     <row r="520" spans="1:4">
@@ -11104,10 +11102,10 @@
     </row>
     <row r="531" spans="1:4">
       <c r="A531" s="1" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="B531" s="1" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="532" spans="1:4">

</xml_diff>